<commit_message>
headers ready (some ajustments later)
</commit_message>
<xml_diff>
--- a/downloads/მარაბდა.xlsx
+++ b/downloads/მარაბდა.xlsx
@@ -12,9 +12,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>რიგითი №</t>
+  </si>
+  <si>
+    <t>ავტო ბაზა</t>
+  </si>
+  <si>
+    <t xml:space="preserve">მარშრუტის. № </t>
+  </si>
+  <si>
+    <t>ავტობუსების მარშრუტების მოძრაობის სქემა</t>
+  </si>
+  <si>
+    <t>მარშრუტის ბრუნის სიგრძე, კმ</t>
+  </si>
+  <si>
+    <t>ავტობუსის ტიპი</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>ინტერვალი, წთ</t>
+  </si>
+  <si>
+    <t>ბრუნის დრო</t>
+  </si>
+  <si>
+    <t>ბრუნების ჯამური რაოდენობა</t>
+  </si>
+  <si>
+    <t>დაწყების დრო</t>
+  </si>
+  <si>
+    <t>დასრულების დრო</t>
+  </si>
+  <si>
+    <t>ხაზზე დასრულების დრო</t>
+  </si>
+  <si>
+    <t>საგარანტიო გასვლები</t>
+  </si>
+  <si>
+    <t xml:space="preserve">შენიშვნა </t>
+  </si>
+  <si>
+    <t>მომუშავე ავტობუსების რაოდენობა</t>
+  </si>
+  <si>
+    <t>პუნქტი "A"</t>
+  </si>
+  <si>
+    <t>გასვლები "A" პუნქტიდან</t>
+  </si>
+  <si>
+    <t>პუნქტი "B"</t>
+  </si>
+  <si>
+    <t>გასვლები "B" პუნქტიდან</t>
   </si>
 </sst>
 </file>
@@ -31,7 +88,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -40,16 +97,26 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor rgb="DEDEDE"/>
+        <fgColor rgb="DDD9C3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="DEDEDE"/>
+        <fgColor rgb="DDD9C3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -57,14 +124,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true">
       <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true">
+      <alignment textRotation="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="true" applyBorder="true">
+      <alignment textRotation="0"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -72,20 +163,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="3.515625" customWidth="true"/>
+    <col min="2" max="2" width="3.515625" customWidth="true"/>
+    <col min="3" max="3" width="3.515625" customWidth="true"/>
+    <col min="4" max="4" width="35.15625" customWidth="true"/>
+    <col min="5" max="5" width="5.078125" customWidth="true"/>
+    <col min="6" max="6" width="5.078125" customWidth="true"/>
+    <col min="7" max="7" width="5.078125" customWidth="true"/>
+    <col min="8" max="8" width="5.078125" customWidth="true"/>
+    <col min="9" max="9" width="5.078125" customWidth="true"/>
+    <col min="10" max="10" width="5.078125" customWidth="true"/>
+    <col min="11" max="11" width="5.078125" customWidth="true"/>
+    <col min="12" max="12" width="5.078125" customWidth="true"/>
+    <col min="13" max="13" width="5.078125" customWidth="true"/>
+    <col min="14" max="14" width="5.078125" customWidth="true"/>
+    <col min="20" max="20" width="5.078125" customWidth="true"/>
+    <col min="15" max="15" width="5.078125" customWidth="true"/>
+    <col min="17" max="17" width="5.078125" customWidth="true"/>
+    <col min="18" max="18" width="5.078125" customWidth="true"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="50.0" customHeight="true">
+    <row r="1" ht="20.0" customHeight="true">
       <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
+      <c r="B1" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s" s="1">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+      <c r="S1"/>
+      <c r="T1" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" ht="20.0" customHeight="true">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2" t="s" s="1">
+        <v>15</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+    </row>
+    <row r="3" ht="80.0" customHeight="true">
+      <c r="N3" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="O3" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="P3"/>
+      <c r="Q3" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="R3" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="S3"/>
+      <c r="T3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="15">
     <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="J1:J3"/>
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="L1:L3"/>
+    <mergeCell ref="M1:M3"/>
+    <mergeCell ref="N1:S2"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
guaranty routes READY, with database and everything
</commit_message>
<xml_diff>
--- a/downloads/მარაბდა.xlsx
+++ b/downloads/მარაბდა.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="240">
   <si>
     <t>რიგითი №</t>
   </si>
@@ -77,19 +77,754 @@
     <t/>
   </si>
   <si>
+    <t>როსტომ აბრამიშვილის ქ. #1-3 კორპუსის  მიმდებარედ (მოედანთან) - როსტომ აბრამიშვილის ქ. -  ლილოს დასახლება (ჭირნახულის ქ. - მეფრინველეთა ქ. - თენზიგ სტურუას ქ. - ზურაბ ნამორაძის ქ. - ევგენი აფხაზავას II შესახვევი - ევგენი აფხაზავას ქ. - ჭირნახულის ქ.) - ივანე იუმაშევის ქ. - კახეთის გზატკეცილი - ჯავახეთის ქ. - მოსკოვის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - ქეთევან დედოფლის გამზირი - მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ). 
+უკუმიმართულებით: მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ)  - ვაჟა ჩაჩავას ქ. - აწყურის ქ. - კახეთის I შესახვევი - ქეთევან დედოფლის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - მოსკოვის გამზირი - ჯავახეთის ქ. - კახეთის გზატკეცილი - ივანე იუმაშევის ქ. - ლილოს დასახლება (ჭირნახულის ქ. - ევგენი აფხაზავას ქ. - ევგენი აფხაზავას II შესახვევი - ევგენი აფხაზავას IV შესახვევი -  ევგენი აფხაზავას ქ. - თენზიგ სტურუას ქ. - მეფრინველეთა ქ. - ჭირნახულის ქ. ) - როსტომ აბრამიშვილის ქ. - როსტომ აბრამიშვილის ქ. #1-3 კორპუსის  მიმდებარედ (მოედანთან))</t>
+  </si>
+  <si>
     <t>MAN A-47</t>
   </si>
   <si>
+    <t> ლილო-ლოჭინი</t>
+  </si>
+  <si>
+    <t>მ/ს ისანი</t>
+  </si>
+  <si>
+    <t>ქიზიყის ქ. (#5 კორპუსის მიმდებარედ) - ქიზიყის ქ. - პოლიციის ქ. - აბელ ენუქიძის ქ. - ბესარიონ ჭიჭინაძის ქ. - გუმათჰესის ქ. - ქინძმარაულის ქ. - მოსკოვის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - ქეთევან დედოფლის გამზირი - ნიკოლოზ ბარათაშვილის აღმართი – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. (გაჩერება „კონკის“ მხარეს).
+უკუმიმართულებით:  ნიკოლოზ ბარათაშვილის ქ. (“კონკის“ მხარეს) – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის აღმართი – ქეთევან დედოფლის გამზირი – შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
     <t>BMC Procity</t>
   </si>
   <si>
+    <t>ქიზიყის ქუჩა</t>
+  </si>
+  <si>
+    <t>ბარათაშვილის ქუჩა</t>
+  </si>
+  <si>
+    <t>მ/ს ,,სანდრო ახმეტელის თეატრი' (ალეკო გობრონიძისა და ომარ ხიზანიშვილის ქუჩის გადაკვეთა) - ალეკო გობრონიძის ქ. - აქვსენტ ისააკიანის ქ. - ანაპის 414-ე დივიზიის ქ. (ზღვის უბნის XI მ/რ-ის V-IV კვ.) - ანაპის 414-ე დივიზიის ქ. (ზღვის უბნის XI მ/რ-ის III-II-I კვ - ზღვის უბნის X-X'ბ' კვარტალი) - მ/ს ,,სარაჯიშვილი'- დავით სარაჯიშვილის გამზირი (მობრუნება ქერჩის ქუჩის გადაკვეთასთან) - გიორგი მინდელის ქ. - გიორგი მინდელის ხიდი - ჯორჯ ბალანჩინის ქ.  - აკაკი ბელიაშვილის ქ. - ნოდარ ბოხუას ქ. - ლუბლიანას ქ. - სანდრო ახმეტელის ქ. - რობერტ ბარძიმაშვილის ქ. - ბორის პაიჭაძის ქ. (მიქელაძის ქუჩის გადაკვეთა, #21 პოლიკლინიკის პირდაპირ).
+უკუ მიმართულებით:  ბორის პაიჭაძის ქ. (მიქელაძის ქუჩის გადაკვეთა, #21 პოლიკლინიკის პირდაპირ) - მიქელაძის ქ. - რობერტ ბარძიმაშვილის ქ. - სანდრო ახმეტელის ქ. - ლუბლიანას ქ. - ნოდარ ბოხუას ქ. - აკაკი ბელიაშვილის ქ. - ჯორჯ ბალანჩინის ქ. - გიორგი მინდელის ხიდი - გიორგი მინდელის ქ. - დავით გურამიშვილის გამზირი (მობრუნება შატილის ქუჩის გადაკვეთასთან) - ანაპის 414-ე დივიზიის ქ. (ზღვის უბნის X'ბ'-X კვარტალი - ზღვის უბნის XI მ/რ-ის I-II-III კვ) - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>მ/ს ახმეტელის თეატრი</t>
+  </si>
+  <si>
+    <t>პაიჭაძის ქუჩა (დიღომი)</t>
+  </si>
+  <si>
+    <t>სოფელი წავკისი (რუსთაველის ქ. #86-ის მიმდებარედ, გიორგი ბრწყინვალეს ქუჩის გადაკვეთასთან) - სოფელი წავკისი (რუსთაველის ქ. - დავით აღმაშენებლის ქ.) - თბილისი-კოჯრის ქ. - კოჯრის გზატკეცილი - მარო მაყაშვილის აღმართი - მარო მაყაშვილის ქ. - ამაღლების ქ. - ლადო ასათიანის შესახვევი - ლადო ასათიანის ქ. - შალვა დადიანის ქ. - თავისუფლების მოედანი -ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ). 
+უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – გიორგი ლეონიძის ქ. – მიხეილ ლერმონტოვის ქ. – პაოლო იაშვილის ქ. – ამაღლების ქ. – მარო მაყაშვილის ქ. – მარო მაყაშვილის აღმართი – კოჯრის გზატკეცილი – შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
     <t>Isuzu Novociti Life</t>
   </si>
   <si>
+    <t>წავკისი </t>
+  </si>
+  <si>
+    <t xml:space="preserve">დაბა წყნეთი (მაია წყნეთელის ქუჩისა და მაია წყნეთელის I შესახვევის გადაკვეთის მიმდებარედ) - დაბა წყნეთი (მაია წყნეთელის ქ. - თამარ მეფის ქ. - შოთა რუსთაველის ქ. - დავით აღმაშენებლის ქ. - დიმიტრი ამილახვარის ქ.) - წყნეთის გზატკეცილი -ქაქუცა  ჩოლოყაშვილის გამზირი - მიხეილ თამარაშვილის გამზირი - ვაჟა ფშაველას გამზირი-- ფერდინანდ თავაძის ქ. - სერგო ზაქარიაძის ქ. - ვაჟა ფშაველას I ჩიხი - ვაჟა ფშაველას გამზირი (მ/ს 'დელისი'-ს მიმდებარედ). 
+უკუმიმართულებით:  მ/ს 'დელისი' (ვაჟა ფშაველას გამზირი)  - ვაჟა ფშაველას გამზირი - ალექსანდრე ყაზბეგის გამზირი (პეტრე ქავთარაძის ქ. №1-თან მოხვევით) - მიხეილ თამარაშვილის გამზირი - ქაქუცა ჩოლოყაშვილის გამზირი - წყნეთის გზატკეცილი - დაბა წყნეთი (დიმიტრი ამილახვარის ქ. - დავით აღმაშენებლის ქ. - შოთა რუსთაველის ქ. - თამარ მეფის ქ. - მაია წყნეთელის ქ. - მაია წყნეთელის ქუჩისა და მაია წყნეთელის I შესახვევის გადაკვეთის მიმდებარედ). </t>
+  </si>
+  <si>
+    <t>წყნეთი </t>
+  </si>
+  <si>
+    <t>მ/ს დელისი</t>
+  </si>
+  <si>
+    <t>ანა პოლიტკოვსკაიას ქ. (ანა პოლიტკოვსკაიას ქ. #18-ის მიმდებარედ, მოედანთან) - ზურაბ ანჯაფარიძის ქ. - ელიზბარ მინდელის ქ. (მობრუნება ელიზბარ მინდელის ქ. #9-ის მიმდებარედ) - შალვა ნუცუბიძის ქ. -  სიმონ კანდელაკის ქ- პეკინის გამზირი - ვაჟა ფშაველას გამზირი - ბექას ქ. - ალექსანდრე ყაზბეგის გამზირი - პეკინის გამზირი - მერაბ კოსტავას ქ. - ვარაზისხევის ქ. - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი - თავისუფლების მოედანი - შოთა რუსთაველის გამზირი - გიორგი ჭანტურიას ქ. - სულიკო ვირსალაძის ქ. - მარჯვენა სანაპირო - ბართაშვილის ქ. (#2-ის მიმდებარედ). 
+უკუმიმართულებით: ნიკოლოზ ბართაშვილის ქ. (#2-ის მიმდებარედ) - ალექსანდრე პუშკინის ქ. - თავისუფლების მოედანი - შოთა რუსთაველის გამზირი - მერაბ კოსტავას ქ. - გმირთა მოედანი - მერაბ კოსტავას ქ. - გიორგი მიროტაძის ქ. - პეკინის გამზირი - ზურაბ ჟვანიას მოედანი - სიმონ კანდელაკის ქ. - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>პოლიტკოვსკაიას ქუჩა</t>
+  </si>
+  <si>
+    <t xml:space="preserve">მ/ს 'დიდუბე' (ქვედა გასასვლელი)(ტრანსპორტის ქ. №1-ის მიმდებარედ)აკაკი წერეთლის გამზირი - ჯონ (მალხაზ) შალიკაშვილის ხიდი - გრიგოლ რობაქიძის გამზირი - დავით აღმაშენებლის ხეივანი (მობრუნება გიორგი  ბრწყინვალეს  ქუჩის გადაკვეთამდე, რესტორანი „მონოპოლის“ მიმდებარედ) - მარშალ გელოვანის გამზირი - სოფ. დიღომი (დავით აღმაშენებლის ქ. - დავით სარაჯიშვილის ქ. - დავით აღმაშენებლის ქ.) - პეტრე სარაჯიშვილის ქ. - მარშალ გელოვანის გამზირი -  გრიგოლ რობაქიძის გამზირი - ჯონ (მალხაზ) შალიკაშვილის ხიდი - აკაკი წერეთლის გამზირი - მ/ს 'დიდუბე' (ქვედა) (ტრანსპორტის ქ. №1-ის მიმდებარედ)(წრიული). (წრიული). </t>
+  </si>
+  <si>
+    <t>სოფ. დიღომი</t>
+  </si>
+  <si>
+    <t>მ/ს დიდუბე</t>
+  </si>
+  <si>
+    <t>სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ) - თამარ მეფის გამზირი - გმირთა მოედანი - ვარაზისხევის ქ. - ილია ჭავჭავაძის გამზირი - ჩოლოყაშვილის გამზირი-წყნეთის გზატკეცილი (ბაგების დასახლება) - წყნეთის გზატკეცილი, კორპუსი #2-ის მიდებარედ (თბილისის ივანე ჯავახიშვილის სახ. სუ-ის საერთო სახოვრებელი). 
+უკუმიმართულებით:  წყნეთის გზატკეცილი, კორპუსი #2-ის მიდებარედ (თბილისის ივანე ჯავახიშვილის სახ. სუ-ის საერთო სახოვრებელი) - წყნეთის გზატკეცილი (ბაგების დასახლება) - ჩოლოყაშვილის გამზირი-ილია ჭავჭავაძის გამზირი - პეტრე მელიქიშვილის ქუჩა - მერაბ კოსტავას ქ. - გმირთა მოედანი - თამარ მეფის გამზირი - სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ).</t>
+  </si>
+  <si>
     <t>MAN A-21</t>
   </si>
   <si>
+    <t>სადგურის მოედანი 1</t>
+  </si>
+  <si>
+    <t>ვაკე-ბაგები</t>
+  </si>
+  <si>
+    <t xml:space="preserve">დაბა კოჯორი (ვაჟა ფშაველას ქ. #33-ის მიმდებარედ) - დაბა კოჯორი (ვაჟა ფშაველას ქ. - ალექსანდრე ჩხეიძის ქ. (მობრუნება ალექსანდრე ჩხეიძის ქ. #16-თან) - გრიგოლ ორბელიანის ქ. - ამაღლების ქ. - ზაქარია ბაქრაძის ქ. - იუნკერთა ქ.) - თბილისი-კოჯრის ქ. (სოფ. ტაბახმელას, სოფ. შინდისის, სოფელი წავკისის, წავკისის ველის გავლით) - კოჯრის გზატკეცილი - მარო მაყაშვილის აღმართი - მარო მაყაშვილის ქ. - ამაღლების ქ. - ლადო ასათიანის შესახვევი - ლადო ასათიანის ქ. - შალვა დადიანის ქ. - თავისუფლების მოედანი -ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).
+უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – გიორგი ლეონიძის ქ. – მიხეილ ლერმონტოვის ქ. – პაოლო იაშვილის ქ. – ამაღლების ქ. – მარო მაყაშვილის ქ. – მარო მაყაშვილის აღმართი –  კოჯრის გზატკეცილი -  თბილისი-კოჯრის ქ. (წავკისის ველის, სოფ. წავკისის, სოფ. შინდისის, სოფ. ტაბახმელას გავლით) - დაბა კოჯორი (იუნკერთა ქ. - ზაქარია ბაქრაძის ქ. -  ამაღლების ქ. - გრიგოლ ორბელიანის ქ. - ალექსანდრე ჩხეიძის ქ. (მობრუნება ალექსანდრე ჩხეიძის ქ. #16-თან) - ვაჟა ფშაველას ქ. - აზეულას ქ. (მობრუნება ნიკო კეცხოველის ქუჩის გადაკვეთასთან) - ვჟა ფშაველას ქ. - ვაჟა ფშაველას ქ.#33-ის მიმდებარედ). </t>
+  </si>
+  <si>
+    <t>კოჯორი </t>
+  </si>
+  <si>
+    <t xml:space="preserve">დაბა ზაჰესის დასახლება (ავჭალის ქ., ბენზინ გასამართი სადგურის მიმდებარე ტერიტორია) - ავჭალის ქ. - ელეფთერ ანდრონიკაშვილის ქ. - უწერის ქ. - ლიბანის ქ. - დავით სარაჯიშვილის ქ. - დავით გურამიშვილის გამზირი - თორნიკე ერისთავის ქ. - აკაკი წერეთლის გამზირი - აკაკი წერეთლის გამზირი #2-ის მიმდებარედ (ბორის პაიჭაძის სახ. ეროვნული სტადიონი)
+უკუმიმართულებით:  აკაკი წერეთლის გამზირი #2-ის მიმდებარედ (ბორის პაიჭაძის სახ. ეროვნული სტადიონი) - აკაკი წერეთლის გამზირი (მობრუნება გიორგი ცაბაძის ქუჩის გადაკვეთასთან) - შემდეგ იგივე სქემით. </t>
+  </si>
+  <si>
+    <t>ზაჰესი </t>
+  </si>
+  <si>
+    <t>ეროვნული სტადიონი</t>
+  </si>
+  <si>
+    <t>სოფელი დიდი ლილო (ერეკლე მეორეს და მშვიდობის ქუჩების გადაკვეთა) - ერეკლე მეორეს ქ. (სოფელი დიდი ლილო) - კახეთის გზატკეცილი - ჯავახეთის ქ. - მოსკოვის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - ქეთევან დედოფლის გამზირი - მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ). 
+უკუმიმართულებით: მ/ს 'ისანი' (ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ) - ვაჟა ჩაჩავას ქ. - აწყურის ქ. - კახეთის I შესახვევი - ქეთევან დედოფლის გამზირი -  მ/ს 'სამგორი' (ქვედა გასასვლელი) - მოსკოვის გამზირი - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>დიდი ლილო</t>
+  </si>
+  <si>
+    <t xml:space="preserve">დიდი დიღმის IV მ/რაიონი, კორპუსი #6-ის მიმდებარედ (დემეტრე თავდადებულის ქ.) - დიდი დიღომი  IV მ/რაიონი (დემეტრე თავდადებულის ქ. - არჩილ მეფის ქ.) - დიდი დიღმის III მ/რაიონი (მირიან მეფის ქ.) - პეტრე იბერის ქ. - იოანე პეტრიწის ქ. - ფარნავაზ მეფის გამზირი - დავით აღმაშენებლის ხეივანი  - მარშალ გელოვანის გამზირი - იური გაგარინის ქ. - ზურაბ ჟვანიას მოედანი - სიმონ კანდელაკის ქ. - ჟიული შარტავას ქ. - გიორგი სააკაძის მოედანი - მერაბ კოსტავას ქ. - გიორგი მიროტაძის ქ. - პეკინის გამზირი - მერაბ კოსტავას ქ. - ვარაზისხევის ქ. - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი -  თავისუფლების მოედანი-ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).                                                                                                                                                                                              უკუმიმართულებით:  ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – შოთა რუსთაველის გამზირი – მერაბ კოსტავას ქ. – გმირთა მოედანი – მერაბ კოსტავას ქ. – გიორგი სააკაძის მოედანი – ჟიული შარტავას ქუჩა -  შემდეგ იგივე სქემით. </t>
+  </si>
+  <si>
+    <t>დიდი დიღმის IV მ/რ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">დიდი დიღმის IV მ/რაიონი, კორპუსი #6-ის მიმდებარედ (დემეტრე თავდადებულის ქ.) - დიდი დიღმის IV მ/რაიონი (დემეტრე თავდადებულის ქ. - არჩილ მეფის ქ.) - დიდი დიღმის III მ/რაიონი (მირიან მეფის ქ.)- პეტრე იბერის ქ. - იოანე პეტრიწის ქ. - ფარნავაზ მეფის გამზირი - დავით აღმაშენებლის ხეივანი - გრიგოლ რობაქიძის გამზირი -  შალიკაშვილის ხიდი - აკაკი წერეთლის გამზირი - გიორგი ცაბაძის ქ. - დავით აღმაშენებლის გამზირი - თამარ მეფის გამზირი - სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ).
+უკუ მიმართულებით:  სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ) - თამარ მეფის გამზირი - მიხეილ წინამძღვრიშვილის ქ. - აკაკი წერეთლის გამზირი - შემდეგ იგივე სქემით. </t>
+  </si>
+  <si>
+    <t>მ/ს 'დიდუბე' (ქვედა გასასვლელი)(ტრანსპორტის ქ. #1-ის მიმდებარედ) - აკაკი წერეთლის გამზირი - შალიკაშვილის ხიდი - გრიგოლ რობაქიძის გამზირი - დავით აღმაშენებლის ხეივანი (მობრუნება გიორგი  ბრწყინვალეს  ქუჩის გადაკვეთამდე, რესტორანი „მონოპოლის“ მიმდებარედ) - მარშალ გელოვანის გამზირი - სოფ. დიღომი (დავით აღმაშენებლის ქ. ) - დიდგორის ქ. - მირიან მეფე და ნანა დედოფლის I ჩიხი - სოფელი დიდგორი (ორასი თავდადებული მხედრის ქ. ) - ხოდაბუნების ქ. - მირიან მეფე და ნანა დედოფლის I ჩიხი - სოფელი თელოვანი (ქეთევან დედოფლის ქ. - ქეთევან დედოფლის ქ. #17-19-ის მიმდებარედ).
+უკუმიმართულებით: სოფელი თელოვანი (ქეთევან დედოფლის ქ. #17-19-ის მიმდებარედ - ქეთევან დედოფლის ქ.) - მირიან მეფე და ნანა დედოფლის I ჩიხი - ხოდაბუნების ქ. - სოფელი დიდგორი (ორასი თავდადებული მხედრის ქ. ) - მირიან მეფე და ნანა დედოფლის I ჩიხი - დიდგორის ქ. - სოფ. დიღომი (დავით აღმაშენებლის ქ.) - პეტრე სარაჯიშვილის ქ. - მარშალ გელოვანის გამზირი -  გრიგოლ რობაქიძის გამზირი - ჯონ (მალხაზ) შალიკაშვილის ხიდი - აკაკი წერეთლის გამზირი - მ/ს 'დიდუბე' (ქვედა გასასვლელი) (ტრანსპორტის ქ. #1-ის მიმდებარედ).</t>
+  </si>
+  <si>
+    <t>სოფ. თელოვანი</t>
+  </si>
+  <si>
+    <t>მუხიანის IV 'ბ' მ/რ (კორპუსი #42-ის მიმდებარედ) - ალეკო გობრონიძის ქ. - აქვსენტ ისააკიანის ქ. - გია რომელაშვილის ქ. (ზღვის უბნის III მ/რ-ის III - II - I კვარტალი) - ზღვის უბნის IV მ/რ (მობრუნება სარაჯიშვილის ქ. #1-ის მიმდებარედ) - ჩარგლის ქ. - გუდამაყრის ქ. - დავით გურამიშვილის გამზირი - ცოტნე დადიანის ქ. -  (მობრუნება ფიროსმანის მოედანზე) - დავით გურამიშვილის გამზირი  - გუდამაყრის ქ. - ჩარგლის ქ. - ზღვის უბნის IV მ/რ - გია რომელაშვილის ქ. (ზღვის უბნის III მ/რ-ის III - II - I კვარტალი) -  აქვსენტ ისააკიანის ქ. - ალეკო გობრონიძის ქ. - მუხიანის IV 'ბ' მ/რ (კორპუსი #42-ის მიმდებარედ)(წრიული)</t>
+  </si>
+  <si>
+    <t>მუხიანის IV ბ მ/რ</t>
+  </si>
+  <si>
+    <t>გადასასვლელი ხიდი</t>
+  </si>
+  <si>
+    <t>სოფელი პატარა ლილო (თამარ მეფის ქ. #72-ის მიმდებარედ) - სოფელი პატარა ლილო (თამარ მეფის ქ. - დავით აღმაშენებლის ქ.) - ვარკეთილის მეურნეობა (ალექსანდრე ყაზბეგის ქ. - მეგობრობის ქ. - გრიგოლ რობაქიძის გამზირი - მშვიდობის ქ.) - ევგენია მაისურაძის ქ. - მიხეილ გახოკიძის ქ. - საქართველოს ერთიანობისთვის მებრძოლთა ქ. - ჯავახეთის ქ. - მოსკოვის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - ქეთევან დედოფლის გამზირი - მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ). 
+უკუმიმართულებით: მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ)  - ვაჟა ჩაჩავას ქ. - აწყურის ქ. - კახეთის I შესახვევი - ქეთევან დედოფლის გამზირი -  მ/ს 'სამგორი' (ქვედა გასასვლელი) - მოსკოვის გამზირი - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>პატარა ლილო</t>
+  </si>
+  <si>
+    <t>დიღმის მასივი, ლუბლიანას ქ. #21“ა“-ს მიმდებარე ტერიტორია - ლუბლიანას ქ. - სანდრო ახმეტელის ქ. - რობერტ ბარძიმაშვილის ქ. - ბორის პაიჭაძის ქ. - გრიგოლ რობაქიძის გამზირი - შალიკაშვილის ხიდი - აკაკი წერეთლის გამზირი - გიორგი ცაბაძის ქ. - დავით აღმაშენებლის გამზირი - ჭოროხის ქ. - დიმიტრი უზნაძის ქ. - ზაარბრიუკენის მოედანი - ჩუღურეთის ხიდი – მშრალი ხიდი – გიორგი ათონელის ქ. – სულიკო ვირსალაძის ქ. – მტკვრის მარჯვენა სანაპირო – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).                                                                              უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ)- ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – შოთა რუსთაველის გამზირი – გიორგი ჭანტურიას ქ. – გიორგი ათონელის ქ. – მშრალი ხიდი – ჩუღურეთის ხიდი – ზაარბრუკენის მოედანი – მტკვრის მარცხენა სანაპირო – კოტე მარჯანიშვილის ქ. – კოტე მარჯანიშვილის მოედანი – დავით აღმაშენებლის გამზირი – გიორგი ცაბაძის ქ. – აკაკი წერეთლის გამზირი – შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>დიღმის მასივი</t>
+  </si>
+  <si>
+    <t xml:space="preserve">დიდი დიღმის IV მ/რაიონი, კორპუსი №6-ის მიმდებარედ (დემეტრე თავდადებულის ქ.) - დიდი დიღმის IV მ/რაიონი (დემეტრე თავდადებულის ქ. - არჩილ მეფის ქ.) - დიდი დიღმის III მ/რაიონი (მირიან მეფის ქ.) - პეტრე იბერის ქ. - იოანე პეტრიწის ქ. - ფარნავაზ მეფის გამზირი - ჯორჯ ბალანჩინის ქ. - აკაკი ბელიაშვილის ქ. - ნოდარ ბოხუას ქ. - ლუბლიანას ქ. - სანდრო ახმეტელის ქ. - რობერტ ბარძიმაშვილის ქ. - ბორის პაიჭაძის ქ. - გრიგოლ რობაქიძის გამზირი - შალიკაშვილის ხიდი - აკაკი წერეთლის გამზირი - გიორგი წინამძღვრიშვილის ქ. - თამარ მეფის გამზირი - გმირთა მოედანი - ვარაზისხევის ქ. - ილია ჭავჭავაძის გამზირი - მიხეილ თამარაშვილის გამზირი - ვაჟა ფშაველას გამზირი - ზურაბ ანჯაფარიძის ქ. -ივანე  ჯავახიშვილის სახ. თსუ-ის  X კორპუსი (მაღლივი კორპუსი)
+უკუმიმართულებით: ივანე  ჯავახიშვილის სახ. თსუ-ის  X კორპუსი (მაღლივი კორპუსი) - ზურაბ ანჯაფარიძის ქ.  - ვაჟა ფშაველას გამზირი - ალექსანდრე ყაზბეგის გამზირი (პეტრე ქავთარაძის ქ. №1-თან მოხვევით) - მიხეილ თამარაშვილის გამზირი - ილია ჭავჭავაძის გამზირი - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - გმირთა მოედანი - თამარ მეფის გამზირი - მიხეილ წინამძღვრიშვილის ქ. - აკაკი წერეთლის გამზირი - შალიკაშვილის ხიდი - გრიგოლ რობაქიძის გამზირი - ბორის პაიჭაძის ქ. - ევგენი მიქელაძის ქ. -  რობერტ ბარძიმაშვილის ქ. - სანდრო ახმეტელის ქ. - ლუბლიანას ქ. - ნოდარ ბოხუას ქ. - აკაკი ბელიაშვილის ქ. - შემდეგ იგივე სქემით.
+</t>
+  </si>
+  <si>
+    <t>სახ. უნივერსიტეტის მ/კ</t>
+  </si>
+  <si>
+    <t>სოფელი ნასაგური (აფხაზეთის და ნახშირგორას ქუჩების გადაკვეთის მიმდებარედ) - სოფელი ნასაგური (აფხაზეთის ქ. - იორის ქ. - აკაკი მგელაძის ქ.) - კახეთის გზატკეცილი - ჯავახეთის ქ. - მოსკოვის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - ქეთევან დედოფლის გამზირი - მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ). 
+უკუმიმართულებით: მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ)  - ვაჟა ჩაჩავას ქ. - აწყურის ქ. - კახეთის I შესახვევი - ქეთევან დედოფლის გამზირი -  მ/ს 'სამგორი' (ქვედა გასასვლელი) - მოსკოვის გამზირი - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>სოფელი ნასაგური</t>
+  </si>
+  <si>
+    <t>ომარ ხიზანიშვილის ქ.  (გლდანის VII - VIII მ/რ-ის დამაკავშირებული გზა)  - ილია ვეკუას ქ. (გლდანის VII - V - III - I მ/რ) - მ/ს 'ახმეტელის თეატრი' - აკაკი ვასაძის ქ. - ქერჩის ქ - დავით გურამიშვილის გამზირი - ცოტნე დადიანის ქ. - გიორგი ჩიტაიას ქ. - გიორგი მაზნიაშვილის ქ. - ივანე ჯავახიშვილის ქ. -  მოსე გოგიბერიძის ქ. – ზაარბრუკენის მოედანი – ჩუღურეთის ხიდი – მშრალი ხიდი – გიორგი ათონელის ქ. – სულიკო ვირსალაძის ქ. – მტკვრის მარჯვენა სანაპირო – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).    უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – შოთა რუსთაველის გამზირი – გიორგი ჭანტურიას ქ. – გიორგი ათონელის ქ. – მშრალი ხიდი – ჩუღურეთის ხიდი – მოსე გოგიბერიძის ქ. – არნოლდ ჩიქობავას ქ. – გიორგი ჩიტაიას ქ. – ცოტნე დადიანის ქ. – დავით გურამიშვილის გამზირი – ქერჩის ქ. – აკაკი ვასაძის ქ. – მ/ს „ახმეტელის თეატრი“ – ომარ ხიზანიშვილის ქ. (გლდანის II – IV – VI – VIII მ/რ) – ომარ ხიზანიშვილის ქ.  (გლდანის VII – VIII მ/რ-ის დამაკავშირებელი გზა)</t>
+  </si>
+  <si>
+    <t>გლდანის VII-VIII მ/რ</t>
+  </si>
+  <si>
+    <t>ომარ ხიზანიშვილის ქ.  (გლდანის VII - VIII მ/რ-ის დამაკავშირებული გზა) - ილია ვეკუას ქ. (გლდანის VII - V - III - I მ/რ) - მ/ს 'ახმეტელის თეატრი' - აკაკი ვასაძის ქ. - ქერჩის ქ - გიორგი მინდელის ქ. - გიორგი მინდელის ხიდი - ჯორჯ ბალანჩინის ქ. - აკაკი ბელიაშვილის ქ. - ნოდარ ბოხუას ქ. - ლუბლიანას ქ. - სანდრო ახმეტელის ქ. - რობერტ ბარძიმაშვილის ქ. - ბორის პაიჭაძის ქ. - გრიგოლ რობაქიძის გამზირი - დავით აღმაშენებლის ხეივანი (მობრუნება გიორგი  ბრწყინვალეს ქუჩის გადაკვეთამდე, რესტორანი „მონოპოლის“ მიმდებარედ) - მარშალ გელოვანის გამზირი - იური გაგარინის ქ. - პეკინის გამზირი - ვაჟა ფშაველას გამზირი - პეტრე ქავთარაძის ქ. (პეტრე ქავთარაძის ქ. #1-თან მოხვევით) - ივანე ჯავახიშვილის სახ. თსუ-ის  X კორპუსი (მაღლივი კორპუსი)
+უკუ მიმართულებით: ივანე ჯავახიშვილის სახ. თსუ-ის  X კორპუსი (მაღლივი კორპუსი) - პეტრე ქავთარაძის ქ. - ალექსანდრე ყაზბეგის გამზირი - იონა ვაკელის ქ. - ბუდაპეშტის ქ. - გურამ ფანჯიკიძის ქ. - პეკინის გამზირი - ზურაბ ჟვანიას მოედანი - იური გაგარინის ქუჩა - მარშალ გელოვანის გამზირი - გრიგოლ რობაქიძის გამზირი - ბორის პაიჭაძის ქ. - მიქელაძის ქ. -  რობერტ ბარძიმაშვილის ქ. - სანდრო ახმეტელის ქ. - ლუბლიანას ქ. -  ნოდარ ბოხუას ქ. - აკაკი ბელიაშვილის ქ. - ჯორჯ ბალანჩინის ქ. - გიორგი მინდელის ხიდი - გიორგი მინდელის ქ. - მ/ს 'სარაჯიშვილი' - დავით გურამიშვილის გამზირი - ქერჩის ქ. - აკაკი ვასაძის ქ. - მ/ს 'ახმეტელის თეატრი' - ომარ ხიზანიშვილის ქ.  (გლდანის II – IV – VI – VIII მ/რ) – ომარ ხიზანიშვილის ქ.  (გლდანის VII – VIII მ/რ-ის დამაკავშირებელი გზა)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ვაზისუბანი II მ/რ (#23 კორპუსის მიმდებარედ) - ვაზისუბნის III მ/რ I კვ.(#3,4,5,6 კორპუსების გავლით) - ვაზისუბნის I მ/რ (#15,14,13 კორპუსების გავლით) - თეოფანე დავითაიას ქ. - შანდორ პეტეფის ქ. - 17 შინდისელი გმირის ქ. - ჯავახეთის ქ. - მოსკოვის გამზირი - ქეთევან დედოფლის გამზირი -  ნიკოლოზ ბარათაშვილის აღმართი – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – ალექსანდრე პუშკინის ქ. – ბარათაშვილის ქ. (გაჩერება „კონკის“ მხარეს).                                       უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (“კონკის“ მხარეს)  – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის აღმართი – მ/ს `ავლაბარი“ – ქეთევან დედოფლის გამზირი – მოსკოვის გამზირი – ჯავახეთის ქ. (მობრუნება მ/ს „ვარკეთილთან“) – 17 შინდისელი გმირის ქ. – შანდორ პეტეფის ქ. – შემდეგ იგივე სქემით (წრიული) </t>
+  </si>
+  <si>
+    <t>ვაზისუბნის II მ/რ</t>
+  </si>
+  <si>
+    <t>ზურგოვანა (მერაბ კოსტავას ქ. - თავისუფლების ქ.) - ასი ათასი მოწამის ქ. - ფარნავაზ მეფის გამზირი - ჯორჯ ბალანჩინის ქ. - აკაკი ბელიაშვილის ქ. - ნოდარ ბოხუას ქ. - ლუბლიანას ქ. - სანდრო ახმეტელის ქ. - რობერტ ბარძიმაშვილის ქ. - ბორის პაიჭაძის ქ. - გრიგოლ რობაქიძის გამზირი - შალიკაშვილის ხიდი - აკაკი წერეთლის გამზირი - მ/ს 'დიდუბე' (ქვედა გასასვლელი) (ბაზრობა 'ჩემპიონის' პირდაპირ) 
+უკუ მიმართულებით: მ/ს 'დიდუბე' (ქვედა გასასვლელი) (ბაზრობა 'ჩემპიონის' პირდაპირ) - აკაკი წერეთლის გამზირი - შალიკაშვილის ხიდი - გრიგოლ რობაქიძის გამზირი - ბორის პაიჭაძის ქ. - ევგენი მიქელაძის ქ. -  რობერტ ბარძიმაშვილის ქ. - სანდრო ახმეტელის ქ. - ლუბლიანას ქ. - ნოდარ ბოხუას ქ. - აკაკი ბელიაშვილის ქ. - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>ზურგოვანა</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ვაშლიჯვრის დასახლება IV ზონა (#11 კორპუსის მიმდებარედ) - ვასო გოძიაშვილის II შესახვევი - ვასო გოძიაშვილის ქ. - პეტრე სარაჯიშვილის ქ. - მარშალ გელოვანის გამზირი - გრიგოლ რობაქიძის გამზირი - შალიკაშვილის ხიდი - აკაკი წერეთლის გამზირი - მიხეილ  წინამძღვრიშვილის ქ. - აბასთუმნის ქ. - ვაგზლის მოედნისა და აბასთუმნის ქუჩის გადაკვეთის მიმდებრედ (ყოფილი სასტუმრო „კოლხეთის' მიმდებარედ).
+უკუმიმართულებით: სადგურის მოედნისა და აბასთუმნის ქუჩის გადაკვეთის მიმდებარედ (ყოფილი სასტუმრო „კოლხეთის“ მიმდებარედ) – სადგურის მოედანი აბასთუმნის ქ. – მიხეილ წინამძღვრიშვილის ქ. – აკაკი წერეთლის გამზირი – შალიკაშვილის ხიდი – გრიგოლ რობაქიძის გამზირი – დავით აღმაშენებლის ხეივანი (მობრუნება გიორგი  ბრწყინვალეს  ქუჩის გადაკვეთამდე, რესტორანი „მონოპოლის“ მიმდებარედ) – მარშალ გელოვანის გამზირი – დავით აღმაშენებლის ქ. – თეთრი დუქნის ქ. – პეტრე სარაჯიშვილის ქ. – ვასო გოძიაშვილის ქ. – ვაშლიჯვრის დასახლება II – III ზონა – ვასო გოძიაშვილის II შესახვევი  – ვაშლიჯვრის დასახლება IV ზონა (№11 კორპუსის მიმდებარედ).
+</t>
+  </si>
+  <si>
+    <t>ვაშლიჯვრის დასახლება</t>
+  </si>
+  <si>
+    <t>სადგურის მოედანი 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">კოტე მარჯანიშვილის ქუჩისა და კოტე მარჯანიშვილის მოედნის გადაკვეთის მიმდებარედ- კოტე მარჯანიშვილის ქ. - მიხეილ წინამძღვრიშვილის ქ. - კიტა აბაშიძის ქ. - არნოლდ ჩიქობავას მოედანი - ტერენტი გრანელის ქ. - ლამის ქ. - პაატა სააკაძის ქ. - მნათობის ქ. #73-ის პირდაპირ.
+უკუ მიმართულებით: მნათობის ქ. #73-ის პირდაპირ - პაატა სააკაძის ქ. - ლამის ქ. - ტერენტი გრანელის ქ. - არნოლდ ჩიქობავას მოედანი - გიორგი მაზნიაშვილის ქ. - კიევის ქ. - დავით აღმაშენებლის გამზირი - კოტე მარჯანიშვილის მოედანი - კოტე მარჯანიშვილის ქუჩისა და კოტე მარჯანიშვილის მოედნის გადაკვეთის მიმდებარედ.
+</t>
+  </si>
+  <si>
+    <t>მნათობის ქუჩა</t>
+  </si>
+  <si>
+    <t>მარჯანიშვილის მ-ნი</t>
+  </si>
+  <si>
+    <t>ვაგზლის მოედნისა და აბასთუმნის ქუჩის გადაკვეთის მიმდებარედ (ყოფილი სასტუმრო „კოლხეთის“ მიმდებარედ) – თამარ მეფის გამზირი – გმირთა მოედანი – მერაბ კოსტავას ქ. – სააკაძის მოედანი – ჟიული შარტავას ქ. – ზურაბ ჟვანიას მოედანი – სიმონ კანდელაკის ქ. – ბუდაპეშტის ქ. – ივანე ბერიტაშვილის ქ. – ლევან კვაჭაძის ქ.- ონკოლოგიის კვლ. ცენტრი (მობრუნება) – ლევან კვაჭაძის ქ.- ფერმწერთა ქ. - ავტო ვარაზის ქ. - თხინვალას ქ. - იოსებ კეჭაყმაძის ქ. – ლევან კვაჭაძის ქ. – ფერმწერთა ქ. (მობრუნება ნუცუბიძის IV მ/რ, №42 კორპუსის მიმდებარედ) – ლევან კვაჭაძის ქ.- ონკოლოგიის კვლ. ცენტრი (მობრუნება) – ლევან კვაჭაძის ქ.- ივანე ბერიტაშვილის ქ. – ბუდაპეშტის ქ. – სიმონ კანდელაკის ქ. – ჟიული შარტავას ქ. – გიორგი სააკაძის მოედანი – მერაბ კოსტავას ქ. – გიორგი მიროტაძის ქ. – პეკინის გამზირი – მერაბ კოსტავას ქ. – გმირთა მოედანი – თამარ მეფის გამზირი (მობრუნება ვაგზლის მოედნის გადაკვეთასთან) – თევდორე მღვდლის ქ. – ვაგზლის მოედნისა და აბასთუმნის ქუჩის გადაკვეთის მიმდებრედ (ყოფილი სასტუმრო „კოლხეთის“ მიმდებარედ)(წრიული).</t>
+  </si>
+  <si>
+    <t>სოფ. თხინვალი</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ქიზიყის ქ. (#34-ის მიმდებარედ) - ქიზიყის ქ. - პოლიციის ქ. - გრიგოლ ლორთქიფანიძის ქ. - ჯავახეთის ქ. - მოსკოვის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - ქეთევან დედოფლის გამზირი - მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ)
+უკუმიმართულებით: მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ)  - ვაჟა ჩაჩავას ქ. - აწყურის ქ. - კახეთის I შესახვევი - ქეთევან დედოფლის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - მოსკოვის გამზირი - ჯავახეთის ქ. - გრიგოლ ლორთქიფანიძის ქ. - შემდეგ იგივე სქემით.
+</t>
+  </si>
+  <si>
     <t>ბოგდან А092, A093</t>
+  </si>
+  <si>
+    <t>სადგურის მოედანი (“თბილისი ცენტრალი“-ს პირდაპირ) – თამარ მეფის გამზირი – გმირთა მოედანი – ვარაზისხევის ქ. – პეტრე მელიქიშვილის ქ. – მერაბ კოსტავას ქ. – შოთა რუსთაველის გამზირი – თავისუფლების მოედანი – შოთა რუსთაველის გამზირი – გიორგი ჭანტურიას ქ. – სოლიკო ვირსალაძის ქ. – მარჯვენა სანაპირო – ნიკოლოზ ბარათაშვილის ქ. (მობრუნება ნიკოლოზ ბარათაშვილისა და ალექსანდრე პუშკინის ქუჩების გადაკვეთასთან) – მარჯვენა სანაპირო – ვახტანგ გორგასალის ქ. – კრწანისის ქ.  (მობრუნება გრიგოლ ვოლსკის ქუჩის გადაკვეთასთან) -კრწანისის ქ. (№63-ის მიმდებარედ). უკუმიმართულებით: კრწანისის ქ. (№63-ის მიმდებარედ)  – კრწანისის ქ. (მობრუნება გრიგოლ ვოლსკის ქუჩის გადაკვეთასთან) – ვახტანგ გორგასალის ქ. – წმინდა ასი ათასი ქართველი მოწამის სახელობის მეტეხის ხიდი – ევროპის მოედანი – რიყე – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის  ხიდი – ნიკოლოზ ბარათაშვილის ქ. – ალექსანდრე პუშკინის ქ. – თავისუფლების  მოედანი – შოთა რუსთაველის გამზირი – მერაბ კოსტავას ქ. – გმირთა მოედანი – თამარ მეფის გამზირი – სადგურის მოედანი (“თბილისი ცენტრალი“-ს პირდაპირ).</t>
+  </si>
+  <si>
+    <t>კრწანისის ქუჩა</t>
+  </si>
+  <si>
+    <t>ომარ ხიზანიშვილის ქ.  (გლდანის VII - VIII მ/რ-ის დამაკავშირებული გზა)  - ილია ვეკუას ქ. (გლდანის VII - V - III - I მ/რ) - მ/ს 'ახმეტელის თეატრი' - აკაკი ვასაძის ქ. - ქერჩის ქ - სარაჯიშვილის გამზირი - თენგიზ შეშელიძის ქ. - ჯორჯ ბალანჩინის ქ. - მირიან მეფის ქ. - ფარნავაზ მეფის გამზირი - გიორგი ბრწყინვალეს ქ. (მობრუნება ფარნავაზ მეფის გამზირზე) - პეტრე იბერის ქ. - მირიან მეფის ქ. - დიდი დიღომი III  მ/რ (მირიან მეფის ქ.) - დიდი დიღმის IV მ/რაიონი ( არჩილ მეფის ქ. - დემეტრე თავდადებულის ქ.) - დიდი დიღმის IV მ/რაიონი, კორპუსი #6-ის მიმდებარედ (დემეტრე თავდადებულის ქ.)
+უკუმიმართულებით: დიდი დიღმის IV მ/რაიონი, კორპუსი #6-ის მიმდებარედ (დემეტრე თავდადებულის ქ.) -  დიდი დიღმის IV მ/რაიონი (დემეტრე თავდადებულის ქ. - არჩილ მეფის ქ.) - დიდი დიღომი III  მ/რ (მირიან მეფის ქ.) - პეტრე იბერის ქ. - გიორგი ბრწყინვალეს ქ. - ფარნავაზ მეფის გამზირი - მირიან მეფის ქ. - ჯორჯ ბალანჩინის ქ. - გიორგი მინდელის ქ. - თენგიზ შეშელიძის ქ. - მ/ს 'სარაჯიშვილი' - ქერჩის ქ. – აკაკი ვასაძის ქ. – მ/ს „ახმეტელის თეატრი“ – ომარ ხიზანიშვილის ქ. (გლდანის II – IV – VI – VIII მ/რ) – ომარ ხიზანიშვილის ქ.  (გლდანის VII – VIII მ/რ-ის დამაკავშირებელი გზა)</t>
+  </si>
+  <si>
+    <t>დიდი დიღომი IV მ/რ</t>
+  </si>
+  <si>
+    <t>ომარ ხიზანიშვილის ქ.  (გლდანის VII - VIII მ/რ-ის დამაკავშირებული გზა)  - ილია ვეკუას ქ. (გლდანის VII - V - III - I მ/რ) - მ/ს  ახმეტელის თეატრი' - აკაკი ვასაძის ქ. - ქერჩის ქ. - დავით გურამიშვილის გამზირი - თორნიკე ერისთავის ქ. - აკაკი წერეთლის გამზირი - გიორგი ცაბაძის ქ. - დავით აღმაშენებლის გამზირი - კოტე მარჯანიშვილის ქ. - მიხეილ ჯავახიშვილის ქ. - პირველი რესპუბლიკის მოედანი - შოთა რუსთაველის გამზირი - თავისუფლების მოედანი - ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ). 
+უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების  მოედანი – შოთა რუსთაველის გამზირი – მერაბ კოსტავას ქ – გმირთა მოედანი – თამარ მეფის გამზირი – მიხეილ წინამძღვრიშვილის ქ. – აკაკი წერეთლის გამზირი – თორნიკე ერისთავის ქ. – დავით გურამიშვილის გამზირი – მ/ს „სარაჯიშვილი“ – ქერჩის ქ. – აკაკი ვასაძის ქ. – მ/ს „ახმეტელის თეატრი“ – ომარ ხიზანიშვილის ქ.  (გლდანის II – IV – VI – VIII მ/რ) – ომარ ხიზანიშვილის ქ.  (გლდანის VII – VIII მ/რ-ის დამაკავშირებელი გზა)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ) - თამარ მეფის გამზირი - გმირთა მოედანი - ვარაზისხევის ქ. - ილია ჭავჭავაძის გამზირი - ჩოლოყაშვილის გამზირი - წყნეთის გზატკეცილი - დაბა წყნეთი (შოთა რუსთაველის ქ. - აფხაზეთის ქ. - გაგრის ქ. - აფხაზეთის ქ. - შოთა რუსთაველის ქ.) - დაბა წყნეთი (შოთა რუსთაველის  და ბატუ კრავეიშვილის ქუჩის გადაკვეთის პირდაპირ). 
+უკუმიმართულებით: დაბა წყნეთი (შოთა რუსთაველის  და ბატუ კრავეიშვილის ქუჩის გადაკვეთის პირდაპირ) - დაბა წყნეთი (შოთა რუსთაველის ქ. - აფხაზეთის ქ. - გაგრის ქ. - აფხაზეთის ქ. - შოთა რუსთაველის ქ. - დავით აღმაშენებლის ქ. - დიმიტრი ამილახვარის ქ.) - წყნეთის გზატკეცილი - ჩოლოყაშვილის გამზირი - ილია ჭავჭავაძის გამზირი - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - გმირთა მოედანი - თამარ მეფის გამზირი - სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ).
+</t>
+  </si>
+  <si>
+    <t>წყნეთი</t>
+  </si>
+  <si>
+    <t>ზღვის უბნის დასახლება, მე-2 მ/რაიონი, კორპუსი #204-ის მიმდებარედ (ლოტკინის მთა) - დავით იოსელიანის ქ. - გარეჯის ქ. - ნიკოლოზ ხუდადოვის ქ. - ცოტნე დადიანის ქ. - რკინიგზის გადასასვლელი ხიდი (მიმდებარედ). 
+უკუმიმართულებით: რკინიგზის გადასასვლელი ხიდი (მიმდებარედ) - ცოტნე დადიანის ქ. - ნიკოლოზ ხუდადოვის ქ. - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>ზღვის უბანი II მ/რ</t>
+  </si>
+  <si>
+    <t>რკინიგზის გადასასვლელი ხიდი</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ავიაქიმიის ქ. (#53-ის მიმდებარედ) - ავიაქიმიის ქ. - სანავარდოს ქ. - წერონისის ქ. - კლდეკარის ქ. - სამღერეთის ქ. - რევაზ ურიდიას ქ. - ცოტნე დადიანის ქ. - რკინიგზის გადასასვლელი ხიდი (მიმდებარედ).
+უკუმიმართულებით: რკინიგზის გადასასვლელი ხიდი (მიმდებარედ) - ცოტნე დადიანის ქ. - შემდეგ იგივე სქემით.
+</t>
+  </si>
+  <si>
+    <t>ავიაქიმიის ქუჩა</t>
+  </si>
+  <si>
+    <t xml:space="preserve">სადგურის მოედანი (“თბილისი ცენტრალი“-ს პირდაპირ) – თამარ მეფის გამზირი – გმირთა მოედანი – ვარაზისხევის ქ. – პეტრე მელიქიშვილის ქ. – მერაბ კოსტავას ქ. – შოთა რუსთაველის გამზირი – თავისუფლების მოედანი – ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის აღმართი – ქეთევან დედოფლის გამზირი – ლეხ კაჩინსკის ქ. – ჯორჯ ბუშის ქ. – კახეთის გზატკეცილი – ევროპის ქ. – თბილისის შოთა რუსთაველის სახელობის საერთაშორისო აეროპორტი. უკუმიმართულებით: თბილისის შოთა რუსთაველის სახელობის საერთაშორისო აეროპორტი – ევროპის ქ. – კახეთის გზატკეცილი – ჯორჯ ბუშის ქ. – ლეხ კაჩინსკის ქ. – ქეთევან დედოფლის გამზირი – ნიკოლოზ ბარათაშვილის აღმართი – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – შოთა რუსთაველის გამზირი – მერაბ კოსტავას ქ. – გმირთა მოედანი – თამარ მეფის გამზირი – სადგურის მოედანი (“თბილისი ცენტრალი“-ს პირდაპირ).
+</t>
+  </si>
+  <si>
+    <t>აეროპორტი</t>
+  </si>
+  <si>
+    <t>აგრარული უნივერსიტეტი - დავით აღმაშენებლის ხეივანი - გრიგოლ რობაქიძის გამზირი - შალიკაშვილის ხიდი - აკაკი წერეთლის გამზირი - მ/ს 'დიდუბე' (მიმდებარე ტერიტორია, აკაკი წერეთლის გამზირი) - აკაკი წერეთლის გამზირი - შალიკაშვილის ხიდი - გრიგოლ რობაქიძის გამზირი - დავით აღმაშენებლის ხეივანი - აგრარული უნივერსიტეტი (მობრუნება გურამ ნიჟარაძის ქუჩის მოპირდაპირედ)(წრიული)</t>
+  </si>
+  <si>
+    <t>აგრარული უნივერსიტეტი</t>
+  </si>
+  <si>
+    <t>წრიული</t>
+  </si>
+  <si>
+    <t>სესილია თაყაიშვილის ქ. (ვარკეთილის IV მ/რ #418 კორპ.) - ვიქტორ კუპრაძის ქ. (მობრუნება ვარკეთილის IV მ/რ, ვიქტორ კუპრაძის და იოთამ ზედგენიძის ქუჩების გადაკვეთასთან) - ჯავახეთის ქ. - მოსკოვის გამზირი - ქეთევან დედოფლის გამზირი -ნიკოლოზ ბარათაშვილის აღმართი – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – ალექსანდრე პუშკინის ქ. – ბარათაშვილის ქ. (გაჩერება „კონკის“ მხარეს).   უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (“კონკის“ მხარეს) – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის აღმართი – მ/ს „ავლაბარი“ – ქეთევან დედოფლის გამზირი – მოსკოვის გამზირი –  ჯავახეთის ქ. – ილია სუხიშვილის ქ. – სესილია თაყაიშვილის ქ. (ვარკეთილის IV მ/რ №403 კორპ.).</t>
+  </si>
+  <si>
+    <t>ვარკეთილის IV მ/რ</t>
+  </si>
+  <si>
+    <t>ვარკეთილის მეურნეობა (შოთა რუსთაველის ქ. #16 - მეგობრობის ქ.) - ვარკეთილის მეურნეობა (მშვიდობის ქ. - გრიგოლ რობაქიძის გამზირი (მობრუნება აკაკი წერეთლის გადაკვეთასთან) - მშვიდობის ქ. - ევგენია მაისურაძის ქ. - მიხეილ გახოკიძის ქ. - საქართველოს ერთიანობისთვის მებრძოლთა ქ. - ჯავახეთის ქ. - მოსკოვის გამზირი -  მ/ს 'სამგორი' (ქვედა გასასვლელი) - ქეთევან დედოფლის გამზირი - მ/ს 'ისანი'  - ნავთლუღის ქ. - ვლადიმერ ლობჟანიძის ქ. - ვლადიმერ ლობჟანიძის ქ.  (#41-42-ის მიმდებარედ)   
+უკუმიმართულებით: ვლადიმერ ლობჟანიძის ქ. (#41-42-ის მიმდებარედ) - ვლადიმერ ლობჟანიძის ქ. - ნავთლუღის ქ. - მ/ს 'ისანი' - ქეთევან დედოფლის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - მოსკოვის გამზირი - ჯავახეთის ქ. - რომანოზ ხომლელის ქ. - მიხეილ გახოკიძის ქ. - ევგენია მაისურაძის ქ. - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>ვარკეთილის მეურნეობა</t>
+  </si>
+  <si>
+    <t>ექიმის გასასვლელი</t>
+  </si>
+  <si>
+    <t xml:space="preserve">სოფელი წინუბანი (მშვიდობისა და გუდამაყარის ქუჩის გადაკვეთის მიმდებარედ) - მშვიდობის ქ. - კახეთის გზატკეცილი - ჯავახეთის ქ. - მოსკოვის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - ქეთევან დედოფლის გამზირი - მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ). 
+უკუმიმართულებით: მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ)  - ვაჟა ჩაჩავას ქ. - აწყურის ქ. - კახეთის I შესახვევი - ქეთევან დედოფლის გამზირი -  მ/ს 'სამგორი' (ქვედა გასასვლელი) - მოსკოვის გამზირი -ჯავახეთის ქ. - კახეთის გზატკეცილი - მშვიდობის ქ. -სოფელი წინუბანი (მშვიდობის ქ. - იალნოს ქ. (მობრუნება იალნოს მე-5 შესახვევთან) - მერი მდივანის ქ. (მობრუნება ხიდამდე) - მშვიდობისა და გუდამაყარის ქუჩის გადაკვეთის მიმდებარედ. 
+</t>
+  </si>
+  <si>
+    <t>სოფელი წინუბანი</t>
+  </si>
+  <si>
+    <t>იყალთოს მთა (#40-ის მიმდებარე ტერიტორია) - ზაზა  ფანასკერტელ-ციციშვილის ქ. (#25,21,19,22,20,16 კორპუსების გავლით) - ბახტრიონის ქ. - პეკინის გამზირი - მერაბ კოსტავას ქ. - ვარაზისხევის ქ. - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი - თავისუფლების მოედანი - შოთა რუსთაველის გამზირი - გიორგი ჭანტურიას ქ. – სოლიკო ვირსალაძის ქ. – მარჯვენა სანაპირო – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).                                                უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – შოთა რუსთაველის გამზირი – მერაბ კოსტავას - გმირთა მოედანი - მერაბ კოსტავას ქ. - ვახტანგ ჭაბუკიანის ქ. - პეკინის გამზირი - ბახტრიონის ქ. - ფანასკერტელ-ციციშვილის ქ. (#16,20,22,19,21,25 კორპუსების გავლით) - იყალთოს მთა (#40-ის მიმდებარე ტერიტორია). (წრიული)</t>
+  </si>
+  <si>
+    <t>იყალთოს გორა</t>
+  </si>
+  <si>
+    <t>ყვარლისა და თევდორე უშაკოვის ქ-ების გადაკვეთა (ყვარლის ქ. #126, მეტრომშენის დასახლება) - ყვარლის ქ. - კაკაბეთის ქ. - კახეთის გზატკეცილი - ვაჟა ჩაჩავას ქ. - მ/ს ,,ისანი' - ქეთევან დედოფლის გამზირი -ნიკოლოზ ბარათაშვილის აღმართი – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – ალექსანდრე პუშკინის ქ. – ბარათაშვილის ქ. (გაჩერება „კონკის“ მხარეს).                                                                   უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (“კონკის“ მხარეს) – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის აღმართი – მ/ს ,,ავლაბარი“   ქეთევან დედოფლის გამზირი - მ/ს ,,ისანი' - ვაჟა ჩაჩავას ქ. -  კახეთის გზატკეცილი - კაკაბეთის ქ. - ტვიშის ქ. - თევდორე უშაკოვის ქ. - ყვარლისა და თევდორე უშაკოვის ქ-ების გადაკვეთა (ყვარლის ქ. #126, მეტრომშენის დასახლება). (წრიული)</t>
+  </si>
+  <si>
+    <t>ყვარელის ქუჩა</t>
+  </si>
+  <si>
+    <t>სოფელ გლდანი (ბორის პაიჭაძის ქ. №18 სახლის მიმდებარედ) – სოფელი გლდანი (ბორის პაიჭაძის ქ. – ვიტალი დარასელიას ქ. – ვახტანგ გორგასალის ქ. – 26 მაისის ქ.).   – თიანეთის გზატკეცილი – ქერჩის ქ. – აკაკი ვასაძის ქ. – ომარ ხიხანიშვილის ქ. – მ/ს „ახმეტელის თეატრი“ (მიმდებარე ტერიტორია).
+უკუმიმართულებით: მ/ს 'ახმეტელის თეატრი' (მიმდებარე ტერიტორია) - ილია ვეკუას ქ. - აკაკი ვასაძის ქ. - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>სოფელი გლდანი</t>
+  </si>
+  <si>
+    <t>სოფელ გლდანი (ბორის პაიჭაძის ქ. #18 სახლის მიმდებარედ) - სოფელი გლდანი (ბორის პაიჭაძის ქ. - ვიტალი დარასელიას ქ. - ვახტანგ გორგასალის ქ. – 26 მაისის ქ.).   - ლიბანის შესახვევი - ლიბანის ქუჩა - იპოლიტე-ივანოვის ქუჩა ქერჩის ქუჩა - აკაკი ვასაძის ქუჩა - ომარ ხიხანიშვილის ქ. - მ/ს 'ახმეტელის თეატრი' (მიმდებარე ტერიტორია).
+უკუ მიმართულებით: მ/ს 'ახმეტელის თეატრი' (მიმდებარე ტერიტორია) - ილია ვეკუას ქ.  - აკაკი ვასაძის ქ. - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>სოფელ გლდანი (26 მაისის ქ. #83- 26 მაისის ქუჩა).   - ლიბანის შესახვევი - ლიბანის ქუჩა - იპოლიტე-ივანოვის ქუჩა -  ქერჩის ქუჩა - აკაკი ვასაძის ქუჩა - ომარ ხიხანიშვილის ქ. - მ/ს 'ახმეტელის თეატრი' (მიმდებარე ტერიტორია).
+უკუ მიმართულებით: მ/ს 'ახმეტელის თეატრი' (მიმდებარე ტერიტორია) - ილია ვეკუას ქ. - აკაკი ვასაძის ქ. - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">აკაკი ბელიაშვილის ქ. (#40-ის მიმდებარედ) - აკაკი ბელიაშვილის ქ. - სანდრო ახმეტელის ქ - რობერტ ბარძიმაშვილის ქ. - პაიჭაძის ქ. (მობრუნება პაიჭაძის ქ. #5'ა'-სთან) - ევგენი მიქელაძის ქ. - აკაკი ბელიაშვილის ქ. - აკაკი ბაქრაძის ქ. - გრიგოლ რობაქიძის გამზირი - შალიკაშვილის ხიდი - აკაკი წერეთლის გამზირი - გიორგი ცაბაძის ქ. - დავით აღმაშენებლის გამზირი - თამარ მეფის გამზირი - გმირთა მოედანი - ვარაზისხევის ქ. - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი - თავისუფლების მოედანი - ალექსანდრე პუშკინის ქ. - ნიკოლოზ ბარათაშვილის ქ. - ნიკოლოზ ბარათაშვილის ხიდი - ნიკოლოზ ბარათაშვილის აღმართი - მ/ს ,,ავლაბარი' (მიმდებარედ).
+უკუმიმართულებით: მ/ს ,,ავლაბარი' (მიმდებარედ) - ნიკოლოზ ბარათაშვილის აღმართი - ნიკოლოზ ბარათაშვილის ხიდი - მარჯვენა სანაპირო - მიხეილ ჯავახიშვილის ქუჩა - რუსთაველის გამზირი - მერაბ კოსტავას ქ. - გმირთა მოედანი - თამარ მეფის გამზირი - მიხეილ წინამძღვრიშვილის ქ. - აკაკი წერეთლის გამზირი - შალიკაშვილის ხიდი  - აკაკი ბელიაშვილის ქ. (მობრუნება ჯორჯ ბალანჩინის ქუჩაზე, 'Mcdonald's'-ის მიმდებარედ) - აკაკი ბელიაშვილის ქ. (#40-ის მიმდებარედ).
+</t>
+  </si>
+  <si>
+    <t>ბელიაშვილის ქუჩა</t>
+  </si>
+  <si>
+    <t>მ/ს ავლაბარი</t>
+  </si>
+  <si>
+    <t>თავისუფალი უნივერსიტეტი (შალვა ნუცუბიძის I მ/რ) - ბედიას ქ. (შალვა ნუცუბიძის I მ/რ) - შალვა ნუცუბიძის ქ. - ფერდინანდ თავაძის ქ. -  მ/ს ,,დელისი' - ვაჟა ფშაველას გამზირი - ალექსანდრე ყაზბეგის გამზირი (პეტრე ქავთარაძის ქ. #1-თან მოხვევით) - იონა ვაკელის ქ. - ადამ მიცკევიჩის ქ. - დავით გამრეკელის ქ. - ალექსანდრე ყაზბეგის გამზირი - პეკინის გამზირი - მერაბ კოსტავას ქ. - გმირთა მოედანი - თამარ მეფის გამზირი (მობრუნება ვაგზლის მოედნის გადაკვეთასთან) - თევდორე მღვდლის ქ. - ვაგზლის მოედნისა და აბასთუმნის ქუჩის გადაკვეთის მიმდებრედ (ყოფილი სასტუმრო „კოლხეთის“ მიმდებარედ)
+უკუ მიმართულებით: ვაგზლის მოედნისა და აბასთუმნის ქუჩის გადაკვეთის მიმდებრედ (ყოფილი სასტუმრო „კოლხეთის“ მიმდებარედ) - თამარ მეფის გამზირი - თამარ მეფის გამზირი - გმირთა მოედანი - მერაბ კოსტავას ქ. - გიორგი მიროტაძის ქ. - პეკინის გამზირი - ვაჟა ფშაველას გამზირი - ბექას ქ. - დავით გამრეკელის ქ. - ადამ მიცკევიჩის ქ. - იონა ვაკელის ქ. - ვაჟა ფშაველას გამზირი - მარიჯანის ქ. - შალვა ნუცუბიძის ქ. - ბედიას ქ. (შალვა ნუცუბიძის I მ/რ)  - თავისუფალი უნივერსიტეტი (შალვა ნუცუბიძის I მ/რ).</t>
+  </si>
+  <si>
+    <t>ნუცუბიძის I მ/რ</t>
+  </si>
+  <si>
+    <t>სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ) - თამარ მეფის გამზირი - მერაბ კოსტავას ქ. - გიორგი სააკაძის მოედანი - ჟიული შარტავას ქ.- ანა კალანდაძის ქ. - პეკინის გამზირი - ვაჟა ფშაველას გამზირი  - მ/ს ,,დელისი' - ფერდინანდ თავაძის ქ. - შალვა ნუცუბიძის ქ. - რამაზ ჩხიკვაძის ქ. (შალვა ნუცუბიძის III მ/რ) - შალვა ნუცუბიძის III მ/რ-ის II კვ. #5-2-1 კორპუსების გავლით (რამაზ ჩხიკვაძის ქ.) - შალვა ნუცუბიძის III მ/რ IIIკვ. #3-5 კორპუსების გავლით (რამაზ ჩხიკვაძის ქ.) - შალვა ნუცუბიძის III მ/რ IIკვ. #8-9 კორპუსების გავლით (რამაზ ჩხიკვაძის ქ.) - შალვა ნუცუბიძის III მ/რ I კვ. #8-7 კორპუსების გავლით (ძოწენიძის ქ.) - რამაზ ჩხიკვაძის ქ. - შალვა ნუცუბიძის ქ. - ფერდინანდ  თავაძის ქ. -  მ/ს ,,დელისი'  - ვაჟა ფშაველას გამზირი - ალექსანდრე ყაზბეგის გამზირი (პეტრე ქავთარაძის ქ. #1-თან მოხვევით) - პეკინის გამზირი - თინა იოსებიძის ქ. - დები იშხნელების ქ. - ჟიული შარტავას ქ. - გიორგი სააკაძის მოედანი - მერაბ კოსტავას ქ. - გიორგი მიროტაძის ქ. - პეკინის გამზირი - მერაბ კოსტავას ქ. - გმირთა მოედანი - თამარ მეფის გამზირი - სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ) (წრიული).</t>
+  </si>
+  <si>
+    <t>ნუცუბიძის პლატო III მ/რ</t>
+  </si>
+  <si>
+    <t>საერთაშორისო სავაჭრო ცენტრი "თბილისის ზღვის პლაზა"-ს მიმდებარე ტერიტორია (ს/კ: 404934381). - პატარიძის ქ. (ვაზისუბნის III მ/რ, II კვ.) - თეოფანე დავითაიას ქ. - შანდორ პეტეფის ქ. - ლიზა ნაკაშიძე-ბოლქვაძის ქ.  – მ/ს „ვარკეთილი“ - ჯავახეთის ქ. - მოსკოვის გამზირი - ქეთევან დედოფლის გამზირი - მ/ს "ისანი" - ნავთლუღის ქ. - რიჩარდ ჰოლბრუკის ქ. - დიმიტრი გულიას ქ. - დიმიტრი გულიას მოედანი - ვახტანგ გორგასალის ქ. - მარჯვენა სანაპირო - წმინდა ასი ათასი ქართველი მოწამის სახელობის მეტეხის ხიდი - ევროპის მოედანი - წმინდა ასი ათასი ქართველი მოწამის სახელობის მეტეხის ხიდი -კოტე აფხაზის ქ. - თავისუფლების მოედანი - ალექსანდრე პუშკინის ქ. - ნიკოლოზ ბარათაშვილის ქ. (გაჩერება "კონკის" მხარეს).
+უკუ მიმართულებით: ნიკოლოზ ბარათაშვილის ქ. ("კონკის" მხარეს) - მარჯვენა სანაპირო - ვახტანგ გორგასალის ქუჩა - დიმიტრი გულიას მოედანი - დიმიტრი გულიას ქ. - რიჩარდ ჰოლბრუკის ქ. - ნავთლუღის ქ. - ქეთევან დედოფლის გამზირი - მოსკოვის გამზირი - ჯავახეთის ქ. (მობრუნება მ/ს "ვარკეთილთან") - 17 შინდისელი გმირის ქ. - შანდორ პეტეფის ქ. - თეოფანე დავითაიას ქ. - ვაზისუბნის III მ/რ, II კვარტლი (წრეზე მოძრაობით) - საერთაშორისო სავაჭრო ცენტრი "თბილისის ზღვის პლაზა"-ს მიმდებარე ტერიტორია (ს/კ: 404934381).</t>
+  </si>
+  <si>
+    <t>ვაზისუბნის III მ/რ, II კვ</t>
+  </si>
+  <si>
+    <t>გლდანულას დასახლება (#4 კორპუსის მიმდებარედ) - გლდანისხევის ქ. - შოთა მიქატაძის ქ. - კონსტანტინე ლესელიძის ქ. (გლდანის VI-VIII მ/რ-ს გამყოფი გზა)  - ომარ ხიზანიშვილის ქ. (გლდანის VIII მ/რ) - ილია ვეკუას ქ. (გლდანის VII - V - III - I მ/რ) - მ/ს 'ახმეტელის თეატრი' - აკაკი ვასაძის ქ. - ქერჩის ქ - სარაჯიშვილის გამზირი - თენგიზ შეშელიძის ქ. - ჯორჯ ბალანჩინის ქ. - აკაკი ბელიაშვილის ქ. - ნოდარ ბოხუას ქ. - ლუბლიანას ქ. - სანდრო ახმეტელის ქ. - რობერტ ბარძიმაშვილის ქ. - ბორის პაიჭაძის ქ. - გრიგოლ რობაქიძის გამზირი - ჯონ (მალხაზ) შალიკაშვილის ხიდი - აკაკი წერეთლის გამზირი - ქუთაისის ქ. - ვახუშტი ბაგრატიონის ხიდი - გიორგი სააკაძის დაღმართი - გიორგი სააკაძის მოედანი - მერაბ კოსტავას ქ. - გიორგი მიროტაძის ქ. -  პეკინის გამზირი - მერაბ კოსტავას ქ. - ვარაზისხევის ქ. - ილია ჭავჭავაძის გამზირი - ჩოლოყაშვილის გამზირი - წყნეთის გზატკეცილი (ბაგების დასახლება) - წყნეთის გზატკეცილი, კორპუსი #2-ის მიმდებარედ (უნივერსიტეტის საერთო საცხოვრებელი)
+უკუ მიმართულებით:  წყნეთის გზატკეცილი, კორპუსი №2-ის მიმდებარედ (უნივერსიტეტის საერთო საცხოვრებელი) – წყნეთის გზატკეცილი (ბაგების დასახლება) – ჩოლოყაშვილის გამზირი - ილია ჭავჭავაძის გამზირი – პეტრე მელიქიშვილის ქ. – მერაბ კოსტავას ქ. – გიორგი სააკაძის მოედანი – გიორგი სააკაძის დაღმართი – ვახუშტი ბაგრატიონის  ხიდი – ვახუშტი ბაგრატიონის ქ. – აკაკი წერეთლის გამზირი – შალიკაშვილის ხიდი – გრიგოლ რობაქიძის გამზირი – ბორის პაიჭაძის ქ. – მიქელაძის ქ. – რობერტ ბარძიმაშვილის ქ. – სანდრო ახმეტელის ქ. – ლუბლიანას ქ. – ნოდარ ბოხუას ქ. – აკაკი ბელიაშვილის ქ. – ჯორჯ ბალანჩინის ქ. – გიორგი მინდელის ქ. – თენგიზ შეშელიძის ქ.  - მ/ს 'სარაჯიშვილი' - ქერჩის ქ. - აკაკი ვასაძის ქ. –  მ/ს „ახმეტელის თეატრი“ – ომარ ხიზანიშვილის ქ. (გლდანის II – IV – VI მ/რ)  – კონსტანტინე ლესელიძის ქ. – შოთა მიქატაძის ქ. – გლდანისხევის ქ. -გლდანულას დასახლება (№4 კორპუსის მიმდებარედ).</t>
+  </si>
+  <si>
+    <t>გლდანულა </t>
+  </si>
+  <si>
+    <t>ვიქტორ დოლიძის ქ. (#89-ის მიმდებარედ) - ვიქტორ დოლიძის ქ. - მელიტონ და ანდრია ბალანჩივაძის ქ. - მერაბ კოსტავას ქ. - გმირთა მოედანი - ვარაზისხევის ქ. - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი - თავისუფლების მოედანი - შოთა რუსთაველის გამზირი -გიორგი ჭანტურიას ქ. – სოლიკო ვირსალაძის ქ. – მარჯვენა სანაპირო – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).                                                                                            უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – შოთა რუსთაველის გამზირი – მერაბ კოსტავას ქ. – მერაბ კოსტავას ქ. – გიორგი მიროტაძის ქ. – პეკინის გამზირი – დოლიძის ქ. (№89-ის მიმდებარედ). (წრიული)</t>
+  </si>
+  <si>
+    <t>დოლიძის ქუჩა </t>
+  </si>
+  <si>
+    <t>ცაიშის ქ. (კუკიის დასახლება, ქვის დამამუშავებელი საამქროს მიმდებარედ) - ატოცის ქ.  - ნორიოს აღმართი - ართვინის ქ. (მობრუნება ართვინის ქ. #71-ის მიმდებარედ) - მერაბ მამარდაშვილის ქ. - არნოლდ ჩიქობავას მოედანი - გიორგი მაზნიაშვილის ქ. - კიევის ქ. - დავით აღმაშენებლის გამზირი - თამარ მეფის გამზირი - სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ).
+უკუმიმართულებით: სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ) - თამარ მეფის გამზირი - დავით აღმაშენებლის გამზირი - კორტე მარჯანიშვილის მოედანი - კოტე მარჯანიშვილის ქ. - მიხეილ წინამძღვრიშვილის ქ. - კიტა აბაშიძის ქ. - არნოლდ ჩიქობავას მოედანი - მერაბ მამარდაშვილის ქ. - ართვინის ქ. (მობრუნება ართვინის ქ. #71-ის მიმდებარედ) - ნორიოს აღმართი - ატოცის ქ. - ცაიშის ქ. (ქვის დამამუშავებელი საამქროს მიმდებარედ).</t>
+  </si>
+  <si>
+    <t>კუკიის დასახლება </t>
+  </si>
+  <si>
+    <t>დიდი დიღმის IV მ/რაიონი, კორპუსი #6-ის მიმდებარედ (დემეტრე თავდადებულის ქ.) - დიდი დიღმის IV მ/რაიონი (დემეტრე თავდადებულის ქ. - არჩილ მეფის ქ.)  - დიდი დიღმის III მ/რაიონი (მირიან მეფის ქ.) - პეტრე იბერის ქ. - იოანე პეტრიწის ქ. - ფარნავაზ მეფის გამზირი - დავით აღმაშენებლის ხეივანი - მარშალ გელოვანის გამზირი - იური გაგარინის ქ. - ზურაბ ჟვანიას მოედანი - პეკინის გამზირი - ვაჟა ფშაველას გამზირი - ზურაბ ანჯაფარიძის ქ. - ივანე ჯავახიშვილის სახ. თსუ-ის  X კორპუსი (მაღლივი კორპუსი)
+უკუმიმართულებით:  ივანე ჯავახიშვილის სახ. თსუ-ის  X კორპუსი (მაღლივი კორპუსი) - ზურაბ ანჯაფარიძის ქ. - ვაჟა ფშაველას გამზირი - ალექსანდრე ყაზბეგის გამზირი - პეკინის გამზირი - ზურაბ ჟვანიას მოედანი - გაგარინის ქ. - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>ორხევის დასახლება (თენგიზ ჩანტლაძის ქ., #5-ის მიმდებარედ) - ორხევის დასახლება (თენგიზ ჩანტლაძის ქ. -  კობა ახვლედიანის ქ. - გიორგი ახვლედიანის ქ. - გიორგი მუხაძის ქ. - თენგიზ ჩანტლაძის ქ.) - კახეთის გზატკეცილი - გიორგი აბაშვილის ქ. - კალოუბნის ქ. - ჯავახეთის ქ. (მობრუნება მ/ს 'ვარკეთილის' მიმდებარედ) - მოსკოვის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - ქეთევან დედოფლის გამზირი - მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ). 
+უკუმიმართულებით: მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ)  - ვაჟა ჩაჩავას ქ. - აწყურის ქ. - კახეთის I შესახვევი - ქეთევან დედოფლის გამზირი -  მ/ს 'სამგორი' (ქვედა გასასვლელი) - მოსკოვის გამზირი - ჯავახეთის ქ. - კახეთის გზატკეცილი - ორხევის დასახლება ( თენგიზ ჩანტლაძის ქ. - გიორგი მუხაძის ქ. - გიორგი ახვლედიანის ქ. - თენგიზ ჩანტლაძის ქ.) - ორხევის დასახლება (თენგიზ ჩანტლაძის ქ., #5-ის მიმდებარედ)</t>
+  </si>
+  <si>
+    <t>ორხევი </t>
+  </si>
+  <si>
+    <t>კრწანისის ქ.  (გრიგოლ ვოლსკის ქუჩის გადაკვეთის მიმდებარე ტერიტორია) - კრწანისის ქ. - ორთაჭალის ქ. - ვახტანგ გორგასალის ქ. - დიმიტრი გულიას მოედანი - დიმიტრი გულიას ქ. - რიჩარდ ჰოლბრუკის ქ. - ნავთლუღის ქ. - ქეთევან დედოფლის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - მოსკოვის გამზირი - სამგორის ქ. (#2-ის მიმდებარედ)
+უკუმიმართულებით: სამგორის ქ. (#2-ის მიმდებარედ) - მოსკოვის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - ქეთევან დედოფლის გამზირი - ნავთლუღის ქ. - რიჩარდ ჰოლბრუკის ქ. - დიმიტრი გულიას ქ. - გია გულუას ქ. - ვახტანგ გორგასალის ქ. - ორთაჭალის ქ. - კრწანისის ქ. - კრწანისის ქ.  (გრიგოლ ვოლსკის ქუჩის გადაკვეთის მიმდებარე ტერიტორია).</t>
+  </si>
+  <si>
+    <t>სამგორის ქუჩა</t>
+  </si>
+  <si>
+    <t>ნუგზარ ენდელაძის მოედანი (ილია ჭავჭავაძის გადაკვეთის მიმდებარედ) - ქაქუცა ჩოლოყაშვილის გამზირი - მიხეილ თამარაშვილის გამზირი - ალექსანდრე ყაზბეგის გამზირი - გივი კარტოზიას ქ. - ვლადიმერ და არჩილ ასათიანების ქ. (მობრუნება გვირაბთან) - სულხან ცინცაძის ქ. - პეკინის გამზირი - 26 მაისის მოედანი - მერაბ კოსტავას ქ. - გმირთა მოედანი - ვარაზისხევის ქ. - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი - თავისუფლების მოედანი - ალექსანდრე პუშკინის ქ. - ნიკოლოზ ბარათაშვილის ქ. - ნიკოლოზ ბარათაშვილის ხიდი -  მარცხენა სანაპირო - ნიკოლოზ ბარათაშვილის ხიდი - ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).                                                                                       უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) -  ალექსანდრე პუშკინის ქ. - თავისუფლების მოედანი - შოთა რუსთაველის გამზირი - მერაბ კოსტავას ქ. - მიროტაძის ქ. - პეკინის გამზირი - ვაჟა-ფშაველას გამზირი - ბექას ქ. - ალექსანდრე ყაზბეგის გამზირი - პეკინის გამზირი - სულხან ცინცაძის ქ. - გივი კარტოზიას ქ. - მიხეილ ასათიანის ქ. - ვაჟა-ფშაველას გამზირი - მიხეილ თამარაშვილის გამზირი - ქაქუცა ჩოლოყაშვილის გამზირი - ნუგზარ ენდელაძის მოედანი (ილია ჭავჭავაძის გადაკვეთის მიმდებარედ).</t>
+  </si>
+  <si>
+    <t>ილია ჭავჭავაძის გამზირი (ვაკე)</t>
+  </si>
+  <si>
+    <t>ნიკოლოზ ბარათაშვილის ქ. (გაჩერება 'კონკის' მხარეს)- ნიკოლოზ ბარათაშვილის ხიდი - მარცხენა სანაპირო - ნიკოლოზ ბარათაშვილის პანდუსი (მობრუნება ნიკოლოზ ბარათაშვილის ხიდის დასაწყისში) - კოსტა ხეთაგუროვის ქ. - მოსე გოგიბერიძის ქ. - ზაარბრიუკენის მოედანი - მარცხენა სანაპირო - კოტე მარჯანიშვილის ქ.  (მობრუნება კოტე მარჯანიშვილის მოედანზე) - გალაქტიონ ტაბიძის ხიდი - მიხეილ ჯავახიშვილის ქ. - ვარდების რევოლუციის მოედანი - შოთა რუსთაველის გამზირი - მერაბ კოსტავას ქ. - ვარაზისხევის ქ. - ილია ჭავჭავაძის გამზირი -ჩოლოყაშვილის გამზირი -  წყნეთის გზატკეცილი (ბაგების დასახლება) - წყნეთის გზატკეცილი, კორპუსი #4-2 კორპუსი (უნივერსიტეტის საერთო საცხოვრებელი)
+უკუმიმართულებით:  წყნეთის გზატკეცილი, კორპუსი #2-ის მიმდებარედ (უნივერსიტეტის საერთო საცხოვრებელი) - წყნეთის გზატკეცილი (ბაგების დასახლება) - ჩოლოყაშვილის გამზირი - ილია ჭავჭავაძის გამზირი - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი (მობრუნება ზეთის ხილის ხესთან) - მიხეილ ჯავახიშვილის ქ. - გალაქტიონ ტაბიძის ხიდი - კოტე მარჯანიშვილის ქ. - კოტე მარჯანიშვილის მოედანი - დავით აღმაშენებელის გამზირი - ჭოროხის ქ. - დიმიტრი უზნაძის ქ. - ზაარბრიუკენის მოედანი - ლევ ტოლსტოის ქ. - წმ. ნიკოლოზის ქ. - ხეთაგუროვის ქ. - ნიოლოზ ბარათაშვილის პანდუსი - ნიკოლოზ ბარათაშვილის ხიდი - ნიკოლოზ ბარათაშვილის ქ. - ალექსანდრე პუშკინის ქ. - თავისუფლების მოედანი - ალექსანდრე პუშკინის ქ. - ნიკოლოზ ბარათაშვილის ქ. (გაჩერება 'კონკის' მხარეს).</t>
+  </si>
+  <si>
+    <t>მ/ს ,,ღრმაღელე' (მიმდებარედ) - დავით გურამიშვილის გამზირი - გუდამაყრის ქ. - ჩარგლის ქ. - ანაპის 414-ე დივიზიის ქ. (ზღვის უბნის  XI მ/რ-ის I-II-III კვ.) - უცნობ გმირთა ქ. - ბეშენოვას ქ. - ლიპტოვის ქ. - ნიკოლოზ ხუდადოვის ქ. - რკინიგზის გადასასვლელი ხიდი (მიმდებარე ტერიტორია)
+უკუ მიმართულებით: რკინიგზის გადასასვლელი ხიდი (მიმდებარე ტერიტორია) - ნიკოლოზ ხუდადოვის ქ. -  ლიპტოვის ქ. - ბეშენოვას ქ. - უცნობ გმირთა ქ. - ანაპის დივიზიის ქ. (ზღვის უბნის XI მ/რ-ის III-II-I კვ.) - ჩარგლის ქ. - ლიახვის ქ. - დავით გურამიშვილის გამზირი - მ/ს ,,ღრმაღელე' (მიმდებარედ).</t>
+  </si>
+  <si>
+    <t>მ/ს ღრმაღელე</t>
+  </si>
+  <si>
+    <t>ზღვის უბნის III მ/რ-ის IV კვ. (№65 კორპუსის მიმდებარედ) – ლევან რჩეულიშვილის ქ. (ზღვის უბნის III მ/რ, IV-III კვ.) – ანაპის 414-ე დივიზიის ქ. (ზღვის უბნის XI მ/რ-ის V-IV – III-II-I კვარტალი) – ურეკის ქ. – პეტრე გამყრელიძის ქ. – ალექსანდრე ბარამიძის ქ. – დავით გურამიშვილის გამზირი – ცოტნე დადიანის ქ. – გიორგი ჩიტაიას ქ. – დავით კლდიაშვილის ქ. – ივანე ჯავახიშვილის ქ. – კონსტიტუციის ქ. – გიორგი  ჩუბინაშვილის ქ. – თამარ მეფის გამზირი (მობრუნება ვაგზლის მოედნის გადაკვეთასთან) – თევდორე მღვდლის ქ. – ვაგზლის მოედნისა და აბასთუმნის ქუჩის გადაკვეთის მიმდებრედ (ყოფილი სასტუმრო „კოლხეთის“ მიმდებარედ)
+უკუმიმართულებით: ვაგზლის მოედნისა და აბასთუმნის ქუჩის გადაკვეთის მიმდებრედ (ყოფილი სასტუმრო „კოლხეთის“ მიმდებარედ) – თამარ მეფის გამზირი – ეგნატე ნინოშვილის ქ. – კონსტიტუციის ქ. – მიხეილ წინამძღვრიშვილის ქ. – კოტე მარჯანიშვილის ქ. – გიორგი ჩიტაიას ქ. – შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>ზღვის უბნის III მ/რ, IV კვ</t>
+  </si>
+  <si>
+    <t>ცაცა ამირეჯიბის მესამე და მეორე შესახვევების გადაკვეთის მიმდებარედ (360-ე კმ) - ჯამბულ წურწუმიას ქ. (360-ე კმ) - ბესარიონ ჭიჭინაძის ქ. - გუმათჰესის ქ. - ბესარიონ ჭიჭინაძის ქ. - ქინძმარაულის ქ. - გარდაბნის გზატკეცილი - სადგური ველი.
+უკუმიმართულებით: სადგური ველი - გარდაბნის გზატკეცილი - ქინძმარაულის ქ. - ბესარიონ ჭიჭინაძის ქ. - გუმათჰესის ქ. - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>ცაცა ამირეჯიბის ქუჩა </t>
+  </si>
+  <si>
+    <t>სადგური ველი</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ვიქტორ დოლიძის ქ. (#89-ის მიმდებარედ) - დოლიძის ქ. - მელიტონ და ანდრია ბალანჩივაძის ქ. - მერაბ კოსტავას ქ. - გმირთა მოედანი - თამარ მეფის გამზირი - სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ).
+უკუმიმართულებით: სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ) - თამარ მეფის გამზირი - გმირთა მოედანი - მერაბ კოსტავას ქ. - გიორგი მიროტაძის ქ. - პეკინის გამზირი - დოლიძის ქ. (#89-ის მიმდებარედ). </t>
+  </si>
+  <si>
+    <t> დოლიძის ქუჩა</t>
+  </si>
+  <si>
+    <t>ყვარლისა და თევდორე უშაკოვის ქ-ების გადაკვეთა (ყვარლის ქ. #126, მეტრომშენის დასახლება) - ყვარლის ქ. - კაკაბეთის ქ. - კახეთის გზატკეცილი - ვაჟა ჩაჩავას ქ. - მ/ს ,,ისანი' - ქეთევან დედოფლის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - მოსკოვის გამზირი - სამგორის ქ., #2-ის მიმდებარედ.
+უკუმიმართულებით: სამგორის ქ., #2-ის მიმდებარედ - მოსკოვის გამზირი - ქეთევან დედოფლის გამზირი - მ/ს ,,ისანი' - ვაჟა ჩაჩავას ქ. -  კახეთის გზატკეცილი - კაკაბეთის ქ. - მესხეთის ქ. - თევდორე უშაკოვის ქ. - ყვარლისა და თევდორე უშაკოვის ქ-ების გადაკვეთა (ყვარლის ქ. #126, მეტრომშენის დასახლება).</t>
+  </si>
+  <si>
+    <t>უშაკოვის ქუჩა</t>
+  </si>
+  <si>
+    <t>ცაიშის ქ. (ლებარდეს ქუჩის გადაკვეთასთან) - სალხინოს ქ. - ცხრა ძმა ხერხეულიძის ქ. - გიორგი ჩიტაიას ქ. - დავით კლდიაშვილის ქ. - ივანე ჯავახიშვილის ქ. - კონსტიტუციის ქ. - მიხეილ წინამძღვრიშვილის ქ. - თამარ მეფის გამზირი - სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ).
+უკუმიმართულებით: სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ) - თამარ მეფის გამზირი - ეგნატე ნინოშვილის ქ. - კონსტიტუციის ქ. - მიხეილ წინამძღვრიშვილის ქ. - დავით კლდიაშვილის ქ. - გიორგი ჩიტაიას ქ. - ცხრა ძმა ხერხეულიძის ქ. - სალხინოს ქ. - თეკლათის ქ. - ლებარდეს ქ. - დავით გივიშვილის ქ. - სენაკის ქ. - ასხინის ქ. - ცაიშის ქ. (ლებარდეს ქუჩის გადაკვეთასთან).</t>
+  </si>
+  <si>
+    <t>9 ძმის ქუჩა</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ბიჭვინთის ქ. (II-III კორპუსების მიმდებარედ) - ალექსანდრე მანაგაძის ქ. - უწერის ქ. - ლიბანის ქ. - დავით სარაჯიშვილის ქ. -  დავით გურამიშვილის გამზირი - ცოტნე დადიანის ქ. - (მობრუნება ფიროსმანის მოედანზე) - დავით გურამიშვილის გამზირი - დავით სარაჯიშვილის ქ. -  ლიბანის ქ. - უწერის ქ. - ალექსანდრე მანაგაძის ქ.- ბიჭვინთის ქ.  (II-III კორპუსების მიმდებარედ)(წრიული)
+</t>
+  </si>
+  <si>
+    <t>ბიჭვინთის ქუჩა</t>
+  </si>
+  <si>
+    <t>დიმიტრი ალექსიძის ქ. (კორპუსი #403-ის მიმდებარედ) - ვიქტორ კუპრაძის ქ. (ვარკეთილის IV მ/რ-ის #404,406,415,424,420 კორპუსების გავლით) - ვარკეთილის IV მ/რ (#422,421 კორპუსების გავლით) - დიმიტრი ალექსიძის ქ. - საქართველოს ერთიანობისთვის მებრძოლთა ქ. - ხომლელის ქ. - თრიალეთის ქ. - ზაზა ფანასკერტელ-ციციშვილის ქ. - გიორგი აბაშვილის ქ. - კალოუბნის ქ. - ჯავახეთის ქ. (მობრუნება მ/ს 'ვარკეთილთან') - კახეთის გზატკეცილი - მ/ს ,,ისანი' - ნავთლუღის ქ. - რიჩარდ ჰოლბრუკის ქ. - დიმიტრი გულიას ქ. - დიმიტრი გულიას მოედანი - ვახტანგ გორგასალის ქ. - მარჯვენა სანაპირო - წმინდა ასი ათასი ქართველი მოწამის სახელობის მეტეხის ხიდი - ევროპის მოედანი - წმინდა ასი ათასი ქართველი მოწამის სახელობის მეტეხის ხიდი -კოტე აფხაზის ქ. - თავისუფლების მოედანი - ალექსანდრე პუშკინის ქ. - ნიკოლოზ ბარათაშვილის ქ. (გაჩერება 'კონკის' მხარეს) (წრიული).                                                                                                                                                                                                                           უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. ('კონკის' მხარეს) - მარჯვენა სანაპირო - ვახტანგ გორგასალის ქუჩა - დიმიტრი გულიას მოედანი - დიმიტრი გულიას ქ. - რიჩარდ ჰოლბრუკის ქ. - ნავთლუღის ქ. - მ/ს 'ისანი' - კახეთის გზატკეცილი - ჯავახეთის ქ. - კალოუბნის ქ. -  გიორგი აბაშვილის ქ. - ზაზა ფანასკერტელ-ციციშვილის ქ. - თრიალეთის ქ. - ხომლელის ქ. - საქართველოს ერთიანობისთვის მებრძოლთა ქ. - დიმიტრი ალექსიძის ქ. (კორპუსი #403-ის მიმდებარედ).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ძმები ოცხელებისა და ნაკადულის ქუჩების გადაკვეთა  - ილია ბაბუციძის ქ. - ქინძმარაულის შესახვევი - მოსკოვის გამზირი - ქეთევან დედოფლის გამზირი - მ/ს 'ისანი' - ნავთლუღის ქ. - რიჩარდ ჰოლბრუკის ქ. - ბერი გაბრიელ სალოსის გამზირი - ბოგდან ხმელნიცკის ქ. - გარდაბნის გზატკეცილი - წმინდა ბარბარეს სახელობის უბანი (გარდაბნის გზატკეცილისა და დავით ყიფიანის ქუჩის გადაკვეთის მიმდებარედ).
+უკუმიმართულებით: წმინდა ბარბარეს სახელობის უბანი (გარდაბნის გზატკეცილისა და დავით ყიფიანის ქუჩის გადაკვეთის მიმდებარედ) - ბოგდან ხმელნიცკის ქ. - ბერი გაბრიელ სალოსის გამზირი - რიჩარდ ჰოლბრუკის ქ. - ნავთლუღის ქ. -  ქეთევან დედოფლის გამზირი - მოსკოვის გამზირი -  ქინძმარაულის შესახვევი - ძმები ოცხელებისა - ძმები ოცხელებისა და ნაკადულის ქუჩების გადაკვეთა. </t>
+  </si>
+  <si>
+    <t>ნაკადულის ქუჩა</t>
+  </si>
+  <si>
+    <t>წმინდა ბარბარეს უბანი</t>
+  </si>
+  <si>
+    <t>გლდანულას დასახლება (#4 კორპუსის მიმდებარედ) - გლდანის ხევის ქ. - თიანეთის გზატკეცილი - ქერჩის ქ. - აკაკი ვასაძის ქუჩა - ომარ ხიხანიშვილის ქ. - მ/ს 'ახმეტელის თეატრი' (მიმდებარე ტერიტორია).
+უკუმიმართულებით: მ/ს 'ახმეტელის თეატრი' (მიმდებარედ) - ომარ ხიზანიშვილის ქ. - ფორე მოსულიშვილის ქ.- ქერჩის ქ. - თიანეთის გზატკეცილი - გლდანის ხევის ქ. - გლდანულას დასახლება (#4 კორპუსის მიმდებარედ).</t>
+  </si>
+  <si>
+    <t>მაცხოვრის ნათლიღების სახ. მამათა მონასტერი (მიმდებარედ) - მონასტრის ქ. - წყალსადენის ქ. - ფეიქართა ქ. - ქსნის ქ. - დავით გურამიშვილის გამზირი (მობრუნება ერწოს ქუჩის გადაკვეთის მიმდებარედ) - მ/ს 'ღრმაღელე' - მ/ს 'სარაჯიშვილი' (მიმდებარედ).
+უკუმიმართულებით: მ/ს 'სარაჯიშვილი' (მიმდებარედ) - დავით სარაჯიშვილის ქ. (მობრუნება ქერჩის ქუჩის გადაკვეთასთან) - დავით გურამიშვილის გამზირი - ქერჩის ქ. - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>მონასტრის ქუჩა</t>
+  </si>
+  <si>
+    <t>მ/ს სარაჯიშვილი</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ზღვის უბნის III მ/რ-ის IV კვ. (#65 კორპუსის მიმდებარედ) - ლევან რჩეულიშვილის ქ. (თემქის III მ/რ, IV-III კვ.) - გიორგი რომელაშვილის ქ. (ზღვის უბნის III მ/რ-ის III - II - I კვარტალი) - ზღვის უბნის IV მ/რ - მობრუნება სარაჯიშვილის ქ. #1-ის მიმდებარედ - ჩარგლის ქ - ანაპის 414-ე დივიზიის ქ. - მ/ს 'სარაჯიშვილი' (მიმდებარედ).
+უკუმიმართულებით: მ/ს 'სარაჯიშვილი' (მიმდებარედ) - დავით სარაჯიშვილის ქ. (მობრუნება ქერჩის ქუჩის გადაკვეთასთან) - ანაპის 414-ე დივიზიის ქ. - შემდეგ იგივე სქემით. </t>
+  </si>
+  <si>
+    <t>სამშვილდეს ქ. #27-ის მიმდებარედ - გიორგი მარუაშვილის ქ. - აჭარის ქ. (მობრუნება #10-ის მიმდებარედ) - გიორგი მარუაშვილის ქ. - გიორგი ზაზიაშვილის ქ. - გიორგი ჩიტაიას ქ. - დავით კლდიაშვილის ქ. - ივანე ჯავახიშვილის ქ. - კონსტიტუციის ქ. - მიხეილ წინამძღვრიშვილის ქ. - თამარ მეფის გამზირი - სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ).
+უკუმიმართულება: სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ) - თამარ მეფის გამზირი - ეგნატე ნინოშვილის ქ. - კონსტიტუციის ქ. - მიხეილ წინამძღვრიშვილის ქ. - დავით კლდიაშვილის ქ. - გიორგი ჩიტაიას ქ. - გიორგი ზაზიაშვილის ქ. - გიორგი მარუაშვილის ქ. - აჭარის ქ. (მობრუნება #10-ის მიმდებარედ) - გიორგი მარუაშვილის ქ. - სამშვილდეს ქ. #27-ის მიმდებარედ.</t>
+  </si>
+  <si>
+    <t>ტუბდისპანსერი </t>
+  </si>
+  <si>
+    <t>სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ) - თამარ მეფის გამზირი - გმირთა მოედანი - ვარაზისხევის ქ. - პეტრე მელიქიშვილის ქ. -  თამარ ჭოველიძის ქ. - იაკობ გოგებაშვილის ქ. - გურამ რჩეულიშვილის ქ. - ჯაფარიძის ქ. #46 (მიმდებარედ).
+უკუმიმართულებით: ჯაფარიძის ქ. #46 (მიმდებარედ) - ჯაფარიძის ქ. - გურამ რჩეულიშვილის ქ. - იაკობ გოგებაშვილის ქ. - აკაკი შანიძის ქ. - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი (მობრუნება ზეთის ხილის ხესთან) - მერაბ კოსტავას ქ. - გმირთა მოედანი - თამარ მეფის გამზირი - სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ).</t>
+  </si>
+  <si>
+    <t>ჯაფარიძის ქუჩა</t>
+  </si>
+  <si>
+    <t>მუხიანის III მ/რ (#5'ა' კორპუსის მიმდებარედ) - ნოდარ დუმბაძის გამზირი - ნოდარ დუმბაძის გამზირისა და იოსებ ნონეშვილის ქუჩის დამაკავშირებელი გზა -  იოსებ ნონეშვილის ქ.- ალეკო გობრონიძის ქ. - მ/ს 'ახმეტელის თეატრი' (ალეკო გობრონიძისა და ომარ ხიზანიშვილის ქუჩების გადაკვეთა).
+უკუ მიმართულებით: იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>მუხიანის III მ/რ</t>
+  </si>
+  <si>
+    <t>კრწანისის ქ.  (გრიგოლ ვოლსკის ქუჩის გადაკვეთის მიმდებარე ტერიტორია) – კრწანისის ქ. – ორთაჭალის ქ. – ვახტანგ გორგასალის ქ. – დიმიტრი გულიას მოედანი – ვახტანგ გორგასალის ქ. – წმინდა ასი ათასი ქართველი მოწამის სახელობის მეტეხის ხიდი – რიყე – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის  ხიდი – ნიკოლოზ ბარათაშვილის ქ. – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – შოთა რუსთაველის გამზირი (მობრუნება შოთა რუსთაველის გამზირი №42-44-თან) – თავისუფლების მოედანი – ალექსანდრე პუშკინის ქ. – ბარათაშვილის ქ. (№2-ის მოპირდაპირედ, გაჩერება „კონკის“ მხარეს).
+უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. ('კონკის' მხარეს) - მარჯვენა სანაპირო - ვახტანგ გორგასალის ქ. - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>დაბა კიკეთი (9 ძმა ხერხეულიძის ქ. #17-19-ის პირდაპირ) - დაბა კიკეთი (9 ძმა ხერხეულიძის ქ. - ექვთიმე თაყაიშვილის ქ.) - წყნეთი - სამადლოს გზა (სოფ. დიდებაში ჩასვლა-ამოსვლით) - დაბ წყნეთი (რუსთაველის ქ. - რუსთაველისა და დავით აღმაშენებლის ქუჩების გადაკვეთის მიმდებარედ).
+უკუმიმართულებით: იგივე სქემით</t>
+  </si>
+  <si>
+    <t>დაბა კიკეთი</t>
+  </si>
+  <si>
+    <t>დაბა წყნეთი</t>
+  </si>
+  <si>
+    <t>სოფ. ახალდაბა - ახალდაბის ქ. - დაბა წყნეთი (აფხაზეთის ქ. - რუსთაველის ქ. - დიმიტრი ამილახვარის ქ.) - წყნეთის გზატკეცილი - ქაქუცა ჩოლოყაშვილის გამზირი - მიხეილ თამარაშვილის გამზირი - ვაჟა ფშაველას გამზირი (მ/ს 'დელისი')' - ფერდინანდ თავაძის ქ. - სერგო ზაქარიაძის ქ. - ვაჟა ფშაველას I ჩიხი - ვაჟა ფშაველას გამზირი (მ/ს 'დელისი'-ს მიმდებარედ). 
+უკუმიმართულებით: ვაჟა ფშაველას გამზირი (მ/ს 'დელისი'-ს მიმდებარედ)  - ვაჟა ფშაველას გამზირი - ალექსანდრე ყაზბეგის გამზირი (პეტრე ქავთარაძის ქ. №1-თან მოხვევით) - მიხეილ თამარაშვილის გამზირი - ქაქუცა ჩოლოყაშვილის გამზირი - წყნეთის გზატკეცილი - დაბა წყნეთი (რუსთაველის ქ. - აფხაზეთის ქ. ) - ახალდაბის ქ. - სოფ. ახალდაბა.</t>
+  </si>
+  <si>
+    <t>პატარა დიღომი (#1 სახლის მიმდებარედ) - გრიგოლ ფერაძის ქ. (პატარა დიღომი #1-15 სახლი, V- I კორპუსის გავლით) - დავით აღმაშენებლის ხეივანი (მობრუნება 'AUDI'-ს ავტოსერვისის მიმდებარედ) - ასი ათასი მოწამის ქ. - დემეტრე თავდადებულის ქ. - პეტრე იბერის ქ. - იოანე პეტრიწის ქ. - ფარნავაზ მეფის გამზირი - დავით აღმაშენებლის ხეივანი - გრიგოლ რობაქიძის გამზირი - შალიკაშვილის ხიდი - აკაკი წერეთლის გამზირი - გიორგი ცაბაძის ქ. - დავით აღმაშენებლის გამზირი - თამარ მეფის გამზირი - სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ).
+უკუმიმართულებით: სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ) - თამარ მეფის გამზირი - მიხეილ წინამძღვრიშვილის ქ. - აკაკი წერეთლის გამზირი - შალიკაშვილის ხიდი - გრიგოლ რობაქიძის გამზირი - დავით აღმაშენებლის ხეივანი - გრიგოლ ფერაძის ქ. (პატარა დიღომი, I-V კორპუსის, #15-1 სახლის გავლით) - პატარა დიღომი ( #1 სახლი).</t>
+  </si>
+  <si>
+    <t>პატარა დიღომი</t>
+  </si>
+  <si>
+    <t>მუხიანის III მ/რ (#5'ა' კორპუსის მიმდებარედ) - ნოდარ დუმბაძის გამზირი - ალეკო გობრონიძის ქ. - აქვსენტ ისააკიანის ქ. - გიორგი რომელაშვილის ქ. (ზღვის უბნის III მ/რ-ის III - II - I კვარტალი) - ზღვის უბნის IV მ/რ - მობრუნება სარაჯიშვილის ქ. #1-ის მიმდებარედ  - ჩარგლის ქ. - ანაპის დივიზიის ქ. - დავით გურამიშვილის გამზირი - თორნიკე ერისთავის ქ. - აკაკი წერეთლის გამზირი - გიორგი ცაბაძის ქ. - დავით აღმაშენებლის გამზირი - თამარ მეფის გამზირი - სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ).
+უკუმიმართულებით: სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ) - თამარ მეფის გამზირი - მიხეილ წინამძღვრიშვილის ქ. - აკაკი წერეთლის გამზირი - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) - ალექსანდრე პუშკინის ქ. - თავისუფლების მოედანი - შოთა რუსთაველის გამზირი - მერაბ კოსტავას ქ. - გიორგი მიროტაძის ქ. - პეკინის გამზირი - ვაჟა ფშაველას გამზირი - მიხეილ თამარაშვილის გამზირი - ილია ჭავჭავაძის გამზირი - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი - თავისუფლების მოედანი - შოთა რუსთაველის გამზირი - გიორგი ჭანტურიას ქ. - სულიკო ვირსალაძის ქ. - მარჯვენა სანაპირო - ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).</t>
+  </si>
+  <si>
+    <t>შალვა ნუცუბიძის IV მ/რ (შალვა ნუცუბიძის V მ/რ-ის გადასახვევის მიმდებარედ) - ავთო ვარაზის ქ. - შალვა ნუცუბიძის IV მ/რ (№19-20-21-22-29-28-კორპუსების გავლით) - კონსტანტინე კაპანელის ქ. (№14-6-5-4-3-2-1-11 კორპუსების გავლით) - შალვა ნუცუბიძის IV მ/რ ( №12,3,2,1 კორპუსების გავლით) - ნუცუბიძის II მ/რ (ბესარიონ ჟღენტის ქ.) -  შალვა ნუცუბიძის ქ. - მარიჯანის ქ. - პეტრე ქავთარაძის ქ. - ალექსანდრე ყაზბეგის გამზირი - მიხეილ თამარაშვილის გამზირი - ილია ჭავჭავაძის გამზირი - პეტრე მელიქიშვილის ქ. - შოთა რუსთაველის გამზირი - თავისუფლების მოედანი - ალექსანდრე პუშკინის ქ. - ნიკოლოზ ბარათაშვილის ქ. - ნიკოლოზ ბარათაშვილის ხიდი - მარცხენა სანაპირო - ნიკოლოზ ბარათაშვილის ხიდი - ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).
+უკუმიმართულებით:  ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) - ალექსანდრე პუშკინის ქ. - თავისუფლების მოედანი - შოთა რუსთაველის გამზირი - მერაბ კოსტავას ქ. - ვარაზისხევის ქ. - ილია ჭავჭავაძის გამზირი - მიხეილ თამარაშვილის გამზირი - ვაჟა ფშაველას გამზირი - მარიჯანის ქ. - შალვა ნუცუბიძის ქ. - ბესარიონ ჟღენტის ქ. (შალვა ნუცუბიძის II მ/რ) - შალვა ნუცუბიძის IV მ/რ ( №1,2,3,12 კორპუსების გავლით) - კონსტანტინე კაპანელის ქ. (№11-1-2-3-5-6-14 კორპუსების გავლით) - შალვა ნუცუბიძის IV მ/რ ( №28-29-22-21-20-19 კორპუსების გავლით) - ავთო ვარაზის ქ. - შალვა ნუცუბიძის V მ/რ-ის გადასახვევის მიმდებარედ.</t>
+  </si>
+  <si>
+    <t>ნუცუბიძის პლატო IV მ/რ</t>
+  </si>
+  <si>
+    <t>მ/ს 'დიდუბე' (ქვედა გასასვლელი) (ტრანსპორტის ქ. #1-ის მიმდებარედ) - აკაკი წერეთლის გამზირი - გრიგოლ რობაქიძის გამზირი - დავით აღმაშენებლის ხეივანი (მობრუნება გიორგი  ბრწყინვალეს  ქუჩის გადაკვეთამდე, რესტორანი „მონოპოლის“ მიმდებარედ) - მარშალ გელოვანის გამზირი - დავით აღმაშენებლის ქ. - თეთრი დუქნის ქ. - პეტრე სარაჯიშვილის ქ. - ვასო გოძიაშვილის ქ. - მუხრან მაჭავარიანის ქ. - ივანე ბერიტაშვილის ქ. - შალვა ნუცუბიძის ქ. - მიხეილ ასათიანის ქ. - ვაჟა ფშაველას გამზირი - ზურაბ ანჯაფარიძის ქ.  (მ/ს 'სახელმწიფო უნივერსიტეტის' მიმდებარედ).
+უკუმიმართულებით: ზურაბ ანჯაფარიძის ქ.   (მ/ს 'სახელმწიფო უნივერსიტეტის' მიმდებარედ) - ზურაბ ანჯაფარიძის ქ. (მობრუნება ანა პოლიტკოვსკაიას ქუჩის გადაკვეთასთან) - ვაჟა ფშაველას გამზირი - ალექსანდრე ყაზბეგის გამზირი  (პეტრე ქავთარაძის ქ. #1-თან მოხვევით)- მიხეილ თამარაშვილის ქუჩა (მობრუნება მარცხნივ ალ. ყაზბეგის გამზირიდან) - ვაჟა ფშაველას გამზირი - ფერდინანდ თავაძის ქ. - შალვა ნუცუბიძის ქ. - ბუდაპეშტის ქ. - ტაშკენტის ქ. - სიმონ კანდელაკის ქ. - ივანე ბერიტაშვილის ქ. - მუხრან მაჭავარიანის ქ. - ვასო გოძიაშვილის ქ. - პეტრე სარაჯიშვილის ქ. - მარშალ გელოვანის გამზირი - გრიგოლ რობაქიძის გამზირი - აკაკი წერეთლის გამზირი - მ/ს 'დიდუბე' (ქვედა გასასვლელი) (ტრანსპორტის ქ. #1-ის მიმდებარედ)</t>
+  </si>
+  <si>
+    <t>მაჭავარიანის ქუჩა (112)</t>
+  </si>
+  <si>
+    <t>მ/ს სახელმწიფო უნივერსიტეტი</t>
+  </si>
+  <si>
+    <t>ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – გიორგი ლეონიძის ქ. – გერონტი ქიქოძის ქ. – მიხეილ ლერმონტოვის ქ. – პაოლო იაშვილის ქ. – ამაღლების ქ. – მარო მაყაშვილის ქ. – მარო მაყაშვილის აღმართი – კოჯრის გზატკეცილი – ოქროყანის დასახლება (თბილისის ქუჩა, „გ-ბ“ ზონებთან მობრუნება) – მთაწმინდის პარკი.
+უკუმიმართულებით: მთაწმინდის პარკი - ოქროყანის დასახლება ('გ-ბ' ზონებთან მობრუნება, თბილისის ქუჩა) - კოჯრის გზატკეცილი - მარო მაყაშვილის აღმართი - მარო მაყაშვილის ქ. - ამაღლების ქ. - ასათიანის შესახვევი - ლადო ასათიანის ქ. - შალვა დადიანის ქ. - თავისუფლების მოედანი -ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).</t>
+  </si>
+  <si>
+    <t>ოქროყანა </t>
+  </si>
+  <si>
+    <t>მ/ს 'ავლაბარი' - ჰამლეტ გონაშვილის ქ. - ვახტანგ VI ქ. - ვლადიმერ მესხიშვილის ქ. - სამრეკლოს ქ. - მიხეილ ბუხაიძის ქ. - მაქსიმ გორკის ქ. - ივანე ჯავახიშვილის ქ. - მოსე გოგიბერიძის ქ. - ზაარბრიუკენის მოედანი - მარცხენა სანაპირო - კოტე მარჯანიშვილის ქ.  (მობრუნება კოტე მარჯანიშვილის მოედანზე) - გალაქტიონ ტაბიძის ხიდი - მიხეილ ჯავახიშვილის ქ. - მერაბ კოსტავას ქ. - გიორგი სააკაძის მოედანი - ლევან გოთუას ქ. (#26-ის მიმდებარედ).
+უკუმიმართულებით: ლევან გოთუას ქ. (#26-ის მიმდებარედ) - ლევან გოთუას ქ. - გიორგი სააკაძის მოედანი - მერაბ კოსტავას ქ. - გიორგი მიროტაძის ქ. - პეკინის გამზირი - მერაბ კოსტავას ქ. -  გმირთა მოედანი - ვარაზის ხევი - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი (მობრუნება ზეთის ხილის ხესთან) - ივანე ჯავახიშვილის ქ. - გალაქტიონ ტაბიძის ხიდი - კოტე მარჯანიშვილის ქ. - დავით აღმაშენებლის გამზირი - ჭოროხის ქ. - დიმიტრი უზნაძის ქ. - ზაარბრიუკენი მოედანი - ლევ ტოლსტოის ქ. - კოსტა ხეთაგუროვის ქ. - მაქსიმ გორკის ქ. - მიხეილ ბუხაიძის ქ. - სამრეკლოს ქ. - ვლადიმერ მესხიშვილის ქ. - ფაღავას ქ. - მ/ს 'ავლაბარი' (მიმდებარედ).</t>
+  </si>
+  <si>
+    <t>გოთუას ქუჩა</t>
+  </si>
+  <si>
+    <t>სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ) - თამარ მეფის გამზირი - მერაბ კოსტავას ქ. - გიორგი სააკაძის მოედანი - ვახტანგ ჭაბუკიანის ქ. - სულხან ცინცაძის ქ. - გივი კარტოზიას ქ. - მიხეილ ასათიანის ქ. - ვაჟა ფშაველას გამზირი - ზურაბ ანჯაფარიძის ქ. - ივანე ჯავახიშვილის სახ. თსუ-ის  X კორპუსი (მაღლივი კორპუსი)
+უკუმიმართულებით: ივანე ჯავახიშვილის სახ. თსუ-ის  X კორპუსი (მაღლივი კორპუსი) - ზურაბ ანჯაფარიძის ქ. - ვაჟა ფშაველას გამზირი - ალექსანდრე ყაზბეგის გამზირი (პეტრე ქავთარაძის ქ. #1-თან მოხვევით) - გივი კარტოზიას ქ. - ვლადიმერ და არჩილ ასათიანების ქ. (მობრუნება გვირბთან) - სულხან ცინცაძის ქ. - პეკინის გამზირი - მერაბ კოსტავას ქ. - გმირთა მოედანი - თამარ მეფის გამზირი - სადგურის მოედანი ('თბილისი ცენტრალი'-ს პირდაპირ).</t>
+  </si>
+  <si>
+    <t>ზღვის უბნის III მ/რ-ის IV კვ. (#65 კორპუსის მიმდებარედ) - ლევან რჩეულიშვილის ქ. (ზღვის უბნის III მ/რ, IV-III კვ.) - ანაპის 414-ე დივიზიის ქ. (ზღვის უბნის XI მ/რ-ის V-IV - III-II-I კვარტალი) - ჩარგლის ქ. - გუდამაყრის ქ. - დავით გურამიშვილის გამზირი - თორნიკე ერისთავის ქ. - თორნიკე ერისთავის ქ. #1 (მ/ს 'დიდუბე' ზედა გასასვლელი).
+უკუმიმართულებით: თორნიკე ერისთავის ქ. #1 (მ/ს 'დიდუბე' ზედა გასასვლელი) - თორნიკე ერისთავის ქ. - დავით გურამიშვილის გამზირი - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>მ/ს დიდუბე ზედა</t>
+  </si>
+  <si>
+    <t>მუხიანის III მ/რ (№5“ა“ კორპუსის მიმდებარედ) – ნოდარ დუმბაძის გამზირი – მუხიანის III მ/რ (№I-22 კორპუსების გავლით) – იოსებ ნონეშვილის ქ. – ალეკო გობრონიძის ქ. – აქვსენტ ისააკიანის ქ. – ანაპის 414-ე დივიზიის ქ. (ზღვის უბნის XI მ/რ-ის V-IV – III-II-I კვარტალი) – ჩარგლის ქ. – გუდამაყრის ქ. – დავით გურამიშვილის გამზირი – ცოტნე დადიანის ქ. – გიორგი ჩიტაიას ქ. – გიორგი მაზნიაშვილის ქ. – ივანე ჯავახიშვილის ქ. – კოსტა ხეთაგუროვის ქ. – ნიკოლოზ ბარათაშვილის ხიდი –  ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).  უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – ალექსანდრე პუშკინის ქ. - ნიკოლოზ ბარათაშვილის ქ. - ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო  – კოსტა ხეთაგუროვის ქ. – არნოლდ ჩიქობავას ქ. – არნოლდ ჩიქობავას  მოედანი – შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">შალვა ნუცუბიძის V მ/რ (კორპუსი #10-11-ის მიდებარედ)- ავთო ვარაზის ქ. - შალვა ნუცუბიძის IV მ/რ (#19-20-21-22-29-28-კორპუსების გავლით) - კონსტანტინე კაპანელის ქ. (#14-6-5-4-3-2-1-11-12 კორპუსების გავლით) - შალვა ნუცუბიძის II მ/რ (ბესარიონ ჟღენტის ქ.) - შალვა ნუცუბიძის ქ. - ფერდინანდ თავაძის ქ. - სერგო ზაქარიაძის ქ. - ვაჟა ფშაველას ჩიხი - ვაჟა ფშაველას გამზირი (მ/ს 'დელისი'-ს მიმდებარედ).
+უკუმიმართულებით: ვაჟა ფშაველას გამზირი (მ/ს 'დელისი'-ს მიმდებარედ) - ფერდინანდ თავაძის ქ. - შალვა ნუცუბიძის ქ. - შემდეგ იგივე სქემით. </t>
+  </si>
+  <si>
+    <t>ნუცუბიძის V მ/რ</t>
+  </si>
+  <si>
+    <t>ყოფილი ზოოვეტერინარული უნივერსიტეტის საერთო საცხოვრებელი კორპუსები - სოფ. სოღანლუღი - ქვემო ფონიჭალის დასახლება - რუსთავის გზატკეცილი - გორგასალის ქ. - გულიას მ-ნი, ქ. - ბაღდადის ქ. - ნავთლუღის ქ. - მ/ს ,,ისანი' - ქეთევან დედოფლის გამზირი - მოსკოვის გამზირი - ჯავახეთის ქ. - სუხიშვილის ქ - თაყაიშვილის ქ. (ვარკეთილის IV მ/რ, #418-403 კორპუსის მიმდებარედ)
+უკუ მიმართულებით:  იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>აგრარულის საერთო საცხოვრებელი</t>
+  </si>
+  <si>
+    <t>საქართველოს სასჯელაღსრულების, პრობაციისა და იურიდიული დახმარების საკითხთა სამინისტროს სასჯელაღსრულების დეპარტამეტის დაქვემდებარებაში არსებული N6 დაწესებულება - სოფელი კრწანისი - კრწანისის სასწავლო ცენტრი - შსს-ოს აგარაკები - გიგანტის დასახლება - ზოოვეტერინარული ინსტიტუტის დასახლება - სოფ. სოღანლუღი - ქვემო ფონიჭალის დასახლება - რუსთავის გზატკეცილი - გორგასლის ქ. - მეტეხის ხიდი - რიყე - მარცხენა სანაპირო - ბარათაშვილის ქ. (მობრუნება ბარათაშვილისა და პუშკინის ქუჩების გადაკვეთასთან, გაჩერება 'კონკის' მხარეს)
+უკუ მიმართულებით: ბარათაშვილის ქ. ('კონკის' მხარეს) - მარჯვენა სანაპირო - გორგასალის ქ. - შემდეგ იგივე სქემით</t>
+  </si>
+  <si>
+    <t>№6-ე სასჯელ-აღსრულების დაწესებულება</t>
+  </si>
+  <si>
+    <t xml:space="preserve">სოფელი ტაბახმელა (#7 და #6 სახლების გზაგამყოფის მიმდებარედ ) - თბილისი-კოჯრის ქ. (სოფ. შინდისის, სოფელი წავკისის, წავკისის ველის გავლით) - კოჯრის გზატკეცილი - მარო მაყაშვილის აღმართი - მარო მაყაშვილის ქ. - ამაღლების ქ. - ლადო ასათიანის შესახვევი - ლადო ასათიანის ქ. - შალვა დადიანის ქ. - თავისუფლების მოედანი - ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).                                             უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – გიორგი ლეონიძის ქ. – მიხეილ ლერმონტოვის ქ. - პაოლო იაშვილის ქ. - ამაღლების ქ. -  მარო მაყაშვილის ქ. - მარო მაყაშვილის აღმართი - კოჯრის გზატკეცილი - თბილისი-კოჯრის ქ. ( წავკისის ველის, სოფელი წავკისის, სოფ. შინდისის გავლით) - სოფელი ტაბახმელა (კვირაცხოვლის ქ. - საცხოვრებელი კორპუსი - იაშაღაშვილის ქ. - #7,11,12,13,14 სახლი - #6,5,4,3,2,1 სახლი - #7 და #6 სახლების გზაგამყოფის მიმდებარედ). </t>
+  </si>
+  <si>
+    <t>ტაბახმელა </t>
+  </si>
+  <si>
+    <t xml:space="preserve">მ/ს 'დიდუბე' (ქვედა გასასვლელი) (ტრანსპორტის ქ. #1-ის მიმდებარედ)  - წერეთლის გამზირი - შალიკაშვილის ხიდი - გრიგოლ რობაქიძის გამზირი - დავით აღმაშენებლის ხეივანი (მობრუნება გიორგი  ბრწყინვალეს  ქუჩის გადაკვეთამდე, რესტორანი „მონოპოლის“ მიმდებარედ) - მარშალ გელოვანის გამზირი - სოფელი დიღომი (დავით აღმაშენებლის ქ. - კვირაცხოვლის ქ. - ცამეტი ასურელი მამის ქ. - ალექსანდრე ყაზბეგის ქ. - შოთა რუსთაველის ქ. - ფიროსმანის ქ. - ალექსანდრე ყაზბეგის ქ. - ცამეტი ასურელი მამის ქ. - კვირაცხოვლის ქ. - დავით აღმაშენებლის ქ.). - პეტრე სარაჯიშვილის ქ. - მარშალ გელოვანის გამზირი -  გრიგოლ რობაქიძის გამზირი -  შალიკაშვილის ხიდი - აკაკი წერეთლის გამზირი - მ/ს 'დიდუბე' (ქვედა გასასვლელი) (ტრანსპორტის ქ. #1-ის მიმდებარედ, წრიული). </t>
+  </si>
+  <si>
+    <t>სოფელი დიღომი</t>
+  </si>
+  <si>
+    <t>დაბა კიკეთი - თბილისი-კოჯრის გზა (სოფ. დიდება, დაბა კოჯორი, სოფ. ტაბახმელა, სოფ. შინდისი, სოფ. წავკისი, წავკისის ველის გავლით) - კოჯრის გზატკეცილი - მარო მაყაშვილის აღმართი - მარო მაყაშვილის ქ. - ამაღლების ქ. - ლადო ასათიანის შესახვევი - ლადო ასათიანის ქ. - შალვა დადიანის ქ. - თავისუფლების მოედანი -ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ)
+უკუმიმართულებით:  ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – გიორგი ლეონიძის ქ. – მიხეილ ლერმონტოვის ქ. – პაოლო იაშვილის ქ. – ამაღლების ქ. – მარო მაყაშვილის ქ. – მარო მაყაშვილის აღმართი – კოჯრის გზატკეცილი – შემდეგ არსებული სქემით.</t>
+  </si>
+  <si>
+    <t>კიკეთი</t>
+  </si>
+  <si>
+    <t>სოფ. ლისი - სოფ. თხინვალი - ახალი იპოდრომი -  ნუცუბიძის IV-II მ/რ - ჟღენტის ქ. - ნუცუბიძის ქ. - თავაძის ქ. - ზაქარიაძის ქ. - ვაჟა ფშაველას ჩიხი - მ/ს 'დელისი' (მიმდებარედ) 
+უკუ მიმართულებით:  მ/ს 'დელისი' - თავაძის ქ. - ნუცუბიძის ქ. - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>სოფ. გლდანი (26 მაისის და ვახტანგ გორგასალის ქუჩების გადაკვეთის მიმდებარედ-26 მაისის ქ.) – ცენტროლიტის ნაკვეთები (თბილისის შემოვლითი გზა) – ელიფთერ ანდრონიკაშვილის ქ. – უწერის ქ. – ლიბანის ქ. – დავით სარაჯიშვილის ქ. – მ/ს „სარაჯიშვილი“ – ქერჩის ქ – აკაკი ვასაძის ქ. – ომარ ხიხანიშვილის ქ. – მ/ს „ახმეტელის თეატრი“ (მიმდებარედ).
+უკუმიმართულებით: მ/ს „ ახმეტელის თეატრი“ (მიმდებარედ) – ილია ვეკუას ქ. – აკაკი ვასაძის ქ. – ქერჩის ქ. – დავით სარაჯიშვილის ქ. – ლიბანის ქ. – უწერის ქ. – ელიფთერ ანდრონიკაშვილის ქ. – ცენტროლიტის ნაკვეთები (თბილისის შემოვლითი გზა) – სოფ. გლდანი (26 მაისის ქ. – 26 მაისის და ვახტანგ გორგასალის ქუჩების გადაკვეთის მიმდებარედ).</t>
+  </si>
+  <si>
+    <t> სოფ. გლდანი</t>
+  </si>
+  <si>
+    <t xml:space="preserve">მ/ს 'დიდუბე' (ქვედა გასასვლელი)(ტრანსპორტის ქ. #1-ის მიმდებარედ) - აკაკი წერეთლის გამზირი - ჯონ (მალხაზ) შალიკაშვილის ხიდი - გრიგოლ რობაქიძის გამზირი - დავით აღმაშენებლის ხეივანი (მობრუნება გიორგი  ბრწყინვალეს  ქუჩის გადაკვეთამდე, რესტორანი „მონოპოლის“ მიმდებარედ) - მარშალ გელოვანის გამზირი - სოფელი დიღომი (დავით აღმაშენებლის ქ. - კვირაცხოვლის ქ. - მუხრან მაჭავარიანის ქ. - ვაჟა ფშაველას ქ. - კვირაცხოვლის ქ. - ავთანდილ მამუჩაშვილის ქ. - მარიამ უგრეხელიძის ქ. - ცამეტი ასურელი მამის ქ. - კვირაცხოვლის ქ. - დავით აღმაშენებლის ქ.) - პეტრე სარაჯიშვილის ქ. - მარშალ გელოვანის გამზირი -  გრიგოლ რობაქიძის გამზირი - ჯონ (მალხაზ) შალიკაშვილის ხიდი - აკაკი  წერეთლის გამზირი - მ/ს 'დიდუბე' (ქვედა გასასვლელი) (ტრანსპორტის ქ. #1-ის მიმდებარედ). </t>
+  </si>
+  <si>
+    <t>მახათას მთა (კორპუსი #3-ის მიმდებარედ) - მახათას აღმართი -  ნიკოლოზ ხუდადოვის ქ. - ეროსი მანჯგალაძის ქ. - რევაზ ურიდიას ქ. - ცოტნე დადიანის ქ. - რკინიგზის გადასასვლელი ხიდი (მიმდებარე ტერიტორია).
+უკუმიმართულებით: რკინიგზის გადასასვლელი ხიდი (მიმდებარე ტერიტორია) - ნიკოლოზ ხუდადოვის ქ. - შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>მახათას მთა</t>
+  </si>
+  <si>
+    <t>სოფელი შინდისი (ტიციან ტაბიძის ქ. # 25-ის მიმდებარედ) - თბილისი-კოჯრის გზა (სოფ. წავკისის, წავკისის ველის გავლით) - კოჯრის გზატკეცილი - მარო მაყაშვილის აღმართი - მარო მაყაშვილის ქ. - ამაღლების ქ. - ლადო ასათიანის შესახვევი - ლადო ასათიანის ქ. - შალვა დადიანის ქ. - თავისუფლების მოედანი - ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).
+უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. –  თავისუფლების მოედანი – გიორგი ლეონიძის ქ. – მიხეილ ლერმონტოვის ქ. – პაოლო იაშვილის ქ. – ამაღლების ქ. – მარო მაყაშვილის ქ. – მარო მაყაშვილის აღმართი – კოჯრის გზატკეცილი – შემდეგ იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>შინდისი </t>
+  </si>
+  <si>
+    <t>დაბა ზაჰესი (თვისუფლებისა და მიხეილ წინამძღვრიშვილის ქუჩების გადაკვეთის მიმდებარედ) - დაბა ზაჰესის დასახლება (თავისუფლების ქ.- ჭიჭინაძის ქ.- ავჭალის ქ.) - ზაჰესის ხიდი - დავით აღმაშენებლის ხეივანი - ჯორჯ ბალანჩინის ქ. (მობრუნება დიდი დიღომში, ფარნავაზ მეფის გამზირის მიმდებარედ) - აკაკი ბელიაშვილის ქ. - შალიკაშვილის ხიდი - აკაკი წერეთლის გამზირი - მ/ს 'დიდუბე' (ქვედა გასასვლელი) (ტრანსპორტის ქ. #1-ის მიმდებარედ). 
+უკუ მიმართულებით: იგივე სქემით.</t>
+  </si>
+  <si>
+    <t>თამარ მუჯირიშვილის ქ. (№12 კორპუსის მიმდებარედ) – შილდის ქ. – ახალუბნის ქ. – საინგილოს ქ. – გუმბრის ქ. – ვლადიმერ მესხიშვილის ქ. – ნიკოლოზ ბარათაშვილის აღმართი – კოსტა ხეთაგუროვის ქ. – არნოლდ ჩიქობავას ქ. – გიორგი ჩიტაიას ქ. – დავით კლდიაშვილის ქ. – ივანე ჯავახიშვილის ქ. – კონსტიტუციის ქ. – მიხეილ წინამძღვრიშვილის ქ. – თამარ მეფის გამზირი – სადგურის მოედანი (“თბილისი ცენტრალი“-ს პირდაპირ).
+უკუმიმართულებით:  სადგურის მოედანი (“თბილისი ცენტრალი“-ს პირდაპირ) – თამარ მეფის გამზირი – ეგნატე ნინოშვილის ქ. –  კონსტიტუციის ქ. – მიხეილ წინამძღვრიშვილის ქ. – მოსე გოგიბერიძის ქ. – კოსტა ხეთაგუროვის ქ. – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის  ხიდი – ნიკოლოზ ბარათაშვილის ქ. – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მ/ს ,,ავლაბარი“ – ჰამლეტ გონაშვილის ქ. – მეფე ვახტანგ VI-ს ქ. – ვლადიმერ მესხიშვილის ქ. – გუმბრის ქ. – საინგილოს ქ. – ახალუბნის ქ. – შილდის ქ. – თამარ მუჯირიშვილის ქ. (№12 კორპუსის მიმდებარედ).</t>
+  </si>
+  <si>
+    <t>მუჯირიშვილის ქუჩა </t>
+  </si>
+  <si>
+    <t>მ/ს 'რუსთაველი' (Mcdonald's'-ის მიმდებარე ტერიტორია) - შოთა რუსთაველის გამზირი - გიორგი ლეონიძის ქ. - გერონტი ქიქოძის ქ. - მიხეილ ლერმონტოვის ქ. - პაოლო იაშვილის ქ. - ამაღლების ქ. - მარო მაყაშვილის ქ. - მარო მაყაშვილის აღმართი - კოჯრის გზატკეცილი - ოქროყანის დასახლება (შემოვლითი გზით, კოტეჯების მხრიდან) - მთაწმინდის პარკი.
+უკუ მიმართულებით: მთაწმინდის პარკი - ოქროყანის დასახლება (შემოვლითი გზით, კოტეჯების მხრიდან) - კოჯრის გზატკეცილი - მარო მაყაშვილის აღმართი - მარო მაყაშვილის ქ. - ამაღლების ქ. - ლადო ასათიანის შესახვევი - ლადო ასათიანის ქ. - შალვა დადიანის ქ. - თავისუფლების მოედანი - შოთა რუსთაველის გამზირი - მერაბ კოსტავას ქ. (სახ. ფილარმონიასთან მობრუნებით) - მ/ს 'რუსთაველი' (Mcdonald's'-ის მიმდებარე ტერიტორია)</t>
+  </si>
+  <si>
+    <t>მ/ს რუსთაველი</t>
+  </si>
+  <si>
+    <t>მთაწმინდის პარკი</t>
+  </si>
+  <si>
+    <t>ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. –   თავისუფლების მოედანი -  შოთა რუსთაველის გამზირი - მერაბ კოსტავას ქ. - გმირთა მოედანი - მერაბ კოსტავას ქ. - გიორგი სააკაძის მოედანი - ჟიული შარტავას ქ. - ანა კალანდაძის ქ. - პეკინის გამზირი - ვაჟა ფშაველას გამზირი - ზურაბ ანჯაფარიძის ქ. - თბილისის ივანე ჯავახიშვილის სახ. სუ-ის  X კორპუსი (მაღლივი კორპუსი)
+უკუმიმართულებით: თბილისის ივანე ჯავახიშვილის სახ. სუ-ის  X კორპუსი (მაღლივი კორპუსი) - ზურაბ ანჯაფარიძის ქ. - ვაჟა ფშაველას გამზირი - ალექსანდრე ყაზბეგის გამზირი (პეტრე ქავთარაძის ქ. #1-თან მოხვევით) - პეკინის გამზირი - მერაბ კოსტავას ქ. - ვარაზისხევის ქ.  - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი - თავისუფლების მოედანი - ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).</t>
+  </si>
+  <si>
+    <t>ემირ ბურჯანაძის ქ.(დავით ყიფიანის ქუჩის გადაკვეთის მიმდებარედ) - ემირ ბურჯანაძის ქ. - ბოგდან ხმელნიცკის ქ. - ბერი გაბრიელ სალოსის გამზირი - დიმიტრი გულიას ქ. - დიმიტრი გულიას მოედანი - ვახტანგ გორგასალის ქ. - მეტეხის ხიდი - ევროპის მოედანი - მარცხენა სანაპირო - ნიკოლოზ ბარათაშვილის ხიდი - ნიკოლოზ ბარათაშვილის ქ. - ალექსანდრე პუშკინის ქ. - თავისუფლების მოედანი - შოთა რუსთაველის გამზირი - მერაბ კოსტავას ქ. - ვარაზისხევის ქ. - ილია ჭავჭავაძის გამზირი - მიხეილ თამარაშვილის გამზირი - ვაჟა ფშაველას გამზირი - პეტრე ქავთარაძის ქ.  - ანა პოლიტკოვსკაიას ქ. - ანა პოლიტკოვსკაიას ქ. (№16-18-ის მოპირდაპირედ).
+უკუმიმართულებით:  ანა პოლიტკოვსკაიას ქ. (#16-18-ის მოპირდაპირედ) - ანა პოლიტკოვსკაიას ქ. - პეტრე ქავთარაძის ქ. -  ალექსანდრე ყაზბეგის გამზირი - მიხეილ თამარაშვილის გამზირი - ილია ჭავჭავაძის გამზირი - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი - თავისუფლების მოედანი - ნიკოლოზ ბარათშვილის ქ. - მტკვრის მარჯვენა სანაპირო -  ვახტანგ გორგასალის ქ. - დიმიტრი გულიას მოედანი - დიმიტრი გულიას ქ. - ბერი გაბრიელ სალოსის გამზირი - ბოგდან ხმელნიცკის ქ. - ემირ ბურჯანაძის ქ. - ემირ ბურჯანაძის ქ.(დავით ყიფიანის ქუჩის გადაკვეთის მიმდებარედ)</t>
+  </si>
+  <si>
+    <t>დიდი დიღმის IV მ/რაიონი, კორპუსი №6-ის მიმდებარედ (დემეტრე თავდადებულის ქ.) –  დიდი დიღმის IV მ/რაიონი (დემეტრე თავდადებულის ქ. – არჩილ მეფის ქ.) – დიდი დიღომი III-I  მ/რ (მირიან მეფის ქ.) – ჯორჯ ბალანჩინის ქ. – გიორგი მინდელის ქ. – თენგიზ შეშელიძის ქ. – მ/ს „სარაჯიშვილი“ (მიმდებარედ)
+უკუმიმართულებით: მ/ს „სარაჯიშვილი“ (მიმდებარედ) – დავით სარაჯიშვილის გამზირი - თენგიზ შეშელიძის ქ. – ჯორჯ ბალანჩინის ქ. – მირიან მეფის ქ. – დიდი დიღომი III-I  მ/რ (მირიან მეფის ქ.) – დიდი დიღმის IV მ/რაიონი ( არჩილ მეფის ქ. – დემეტრე თავდადებულის ქ.) – დიდი დიღმის IV მ/რაიონი, კორპუსი №6-ის მიმდებარედ (დემეტრე თავდადებულის ქ.)</t>
+  </si>
+  <si>
+    <t>შალვა ნუცუბიძის IV მ/რ (შალვა ნუცუბიძის V მ/რ-ის გადასახვევის მიმდებარედ) - ავთო ვარაზის ქ. - შალვა ნუცუბიძის IV მ/რ (№19-20-21-22-29-28-კორპუსების გავლით) - კონსტანტინე კაპანელის ქ. (№14-6-5-4-3-2-1-11 კორპუსების გავლით) - შალვა ნუცუბიძის IV მ/რ ( №12,3,2,1 კორპუსების გავლით) - ნუცუბიძის II მ/რ (ბესარიონ ჟღენტის ქ.) -  შალვა ნუცუბიძის ქ. - ფერდინანდ თავაძის ქ. - ვაჟა ფშაველას გამზირი - ალექსანდრე ყაზბეგის გამზირი (გადასვლა ვაჟა ფშაველას გამზირი #68-ის მიმდებარე ტერიტორიიდან) - გივი კარტოზიას ქ. – ვლადიმერ და არჩილ ასათიანების ქ. (მობრუნება გვირაბთან) – სულხან ცინცაძის ქ. – პეკინის გამზირი - მერაბ კოსტავას ქ. – გმირთა მოედანი – თამარ მეფის გამზირი – სადგურის მოედანი (“თბილისი ცენტრალი“-ს პირდაპირ).
+უკუმიმართულებით:  სადგურის მოედანი (“თბილისი ცენტრალი“-ს პირდაპირ) – თამარ მეფის გამზირი – მერაბ კოსტავას ქ. – გიორგი მიროტაძის ქ. - პეკინის გამზირი - ვაჟა ფშაველას გამზირი - ბექას ქ. - ალექსანდრე ყაზბეგის გამზირი - გამრეკელის ქ. - სულხან ცინცაძის ქ. - გივი კარტოზიას ქ. - მიხეილ ასათიანის ქ. - ვაჟაა ფშაველას გამზირი - ფერდინანდ თავაძის ქ. - შალვა ნუცუბიძის ქ. - ბესარიონ ჟღენტის ქ. (შალვა ნუცუბიძის II მ/რ) - შალვა ნუცუბიძის IV მ/რ ( №1,2,3,12 კორპუსების გავლით) - კონსტანტინე კაპანელის ქ. (№11-1-2-3-5-6-14 კორპუსების გავლით) - შალვა ნუცუბიძის IV მ/რ ( №28-29-22-21-20-19 კორპუსების გავლით) - ავთო ვარაზის ქ. - შალვა ნუცუბიძის V მ/რ-ის გადასახვევის მიმდებარედ.</t>
+  </si>
+  <si>
+    <t>წყნეთი (შოთა რუსთაველის  და ბათუ კრავეიშვილის ქუჩის გადაკვეთის პირდაპირ) - წყნეთი (შოთა რუსთაველის ქ. - დავით აღმაშენებლის ქ. - დიმიტრი ამილახვრის ქ.) - წყნეთის გზატკეცილი - ქაქუცა ჩოლოყაშვილის გამზირი - მიხეილ თამარაშვილის გამზირი - ვაჟა ფშაველას გამზირი - მ/ს 'დელისი'.
+უკუმიმართულებით:  მ/ს 'დელისი' - ვაჟა ფშაველას გამზირი - ალექსანდრე ყაზბეგის გამზირი (გადასვლა ვაჟა ფშაველას გამზირი #68-ის მიმდებარე ტერიტორიიდან) - მიხეილ თამარაშვილის გამზირი - ქაქუცა ჩოლოყაშვილის გამზირი - წყნეთის გზატკეცილი - წყნეთი (შოთა რუსთაველის ქ.) - წყნეთი (შოთა რუსთაველის  და ბათუ კრავეიშვილის ქუჩის გადაკვეთის პირდაპირ).</t>
+  </si>
+  <si>
+    <t>მ/ს 'ახმეტელის თეატრი' (მიმდებარედ) - ომარ ხიზანიშვილის ქ. (გლდანის II-IV-VI-VIII მ/რ) - ილია ვეკუას ქ. (გლდანის VII-V-III-I მ/რ) - მ/ს 'ახმეტელის თეატრი' (ომარ ხიზანიშვილის ქუჩა) (წრიული)</t>
+  </si>
+  <si>
+    <t>ვაზისუბნის II მ/რ (№23 კორპუსის მიმდებარედ) – ვაზისუბნის II მ/რ (№6-11-4-2 კორპუსების გავლით) -შალვა მშველიძის ქ. – ნიკო მუსხელიშვილის ქ. – დავით კვაჭანტირაძის ქ. – იოსებ და ლეონ ორბელების ქ. – ალექსანდრე წულუკიძის ქ. – ოსიპ მანდელშტამის ქ. – ლიზა ნაკაშიძე-ბოლქვაძის ქ.  – მ/ს „ვარკეთილი“ – ჯავახეთის ქ. – მოსკოვის გამზირი - ქეთევან დედოფლის გამზირი - ნავთლუღის ქ. - რიჩარდ ჰოლბრუკის ქუჩა - დიმიტრი გულიას ქ. - ვახტანგ გორგასალის ქ. -  მარნეულის გზატკეცილი -ზემო ფონიჭალის დასახლება (ანდრო ჟორდანიას ქ. - ლევან ღოღობერიძის ქ. #5,3,2 კორპუსების გავლით) - ზემო ფონიჭალის დასახლება (კორპუსი #28,14,15,19,23,20 კორპუსების გავლით) - მარნეულის გზატკეცილი - ვახტანგ გორგასალის ქ. -  დიმიტრი გულიას ქ. - რიჩარდ ჰოლბრუკის ქუჩა - ნავთლუღის ქ. - ქეთევან დედოფლის გამზირი - მოსკოვის გამზირი - ჯავახეთის ქ. (მობრუნება მ/ს 'ვარკეთილთან') -17 შინდისელი გმირის ქ. – ოსიპ მანდელშტამის ქ. – ალექსანდრე წულუკიძის ქ. – იოსებ და ლეონ ორბელების ქ. – დავით კვაჭანტირაძის ქ. – ნიკო მუსხელიშვილის ქ. – შალვა მშველიძის ქ. – ვაზისუბნის II მ/რ (№2-4-11-6 კორპუსების გავლით) – ვაზისუბნის II მ/რ (№23 კორპუსის მიმდებარედ).</t>
+  </si>
+  <si>
+    <t>ზემო ფონიჭალის დასახლება</t>
+  </si>
+  <si>
+    <t>ნიკოლოზ ბარათაშვილის ქ. (გაჩერება 'კონკის' მხარეს) - ნიკოლოზ ბარათაშვილის ქ. - მტკვრის მარჯვენა სანაპირო - ვახტანგ გორგასალის ქ. - მარნეულის გზატკეცილი -ზემო ფონიჭალის დასახლება (ანდრო ჟორდანიას ქ. - ლევან ღოღობერიძის ქ. #5,3,2 კორპუსების გავლით) - ზემო ფონიჭალის დასახლება (კორპუსი #28,14,15,19,23,20 კორპუსების გავლით) - მარნეულის გზატკეცილი - ვახტანგ გორგასალის ქ. - მეტეხის ხიდი (მობრუნება ევროპის მოედანზე) - კოტე აფხაზის ქ. - თავისუფლების მოედანი - ნიკოლოზ ბარათაშვილის ქ. (გაჩერება 'კონკის' მხარეს).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">რუსთავის გზატკეცილი (ცოტნე დადიანის III ჩიხის მოპირდაპირედ, მობრუნების წრეზე) - ქვემო ფონიჭალის დასახლება (რუსთავის გზატკეცილი) - ვახტანგ გორგასალის ქ. -  მეტეხის ხიდი - ევროპის მოედანი - მტკვრის მარცხენა სანაპირო - ნიკოლოზ ბარათაშვილის ხიდი - ნიკოლოზ ბარათაშვილის ქ. - ალექსანდრე პუშკინის ქ. - თავისუფლების მოედანი - შოთა რუსთაველის გამზირი -მერაბ კოსტავას ქ. - ვარაზისხევის ქ. - ილია ჭავჭავაძის გამზირი - წყნეთის გზატკეცილი - ბაგები (წყნეთის გზატკეცილი, კორპუსი #2-ის მიდებარედ, თბილისის ივანე ჯავახიშვილის სახ. სუ-ის საერთო საცხოვრებელი).
+უკუმიმართულებით:  ბაგები (წყნეთის გზატკეცილი, კორპუსი #2-ის მიდებარედ, თბილისის ივანე ჯავახიშვილის სახ. სუ-ის საერთო საცხოვრებელი) -  წყნეთის გზატკეცილი - ქაქუცა ჩოლოყაშვილის გამზირი - ილია  ჭავჭავაძის გამზირი - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი -თავისუფლების მოედანი -ნიკოლოზ ბარათაშვილის ქ. - მტკვრის მარჯვენა სანაპირო - ვახტანგ  გორგასალის ქ. - რუსთავის გზატკეცილი -ქვემო ფონიჭალის დასახლება (რუსთავის გზატკეცილი) - რუსთავის გზატკეცილი (ცოტნე დადიანის III ჩიხის მოპირდაპირედ, მობრუნების წრეზე). </t>
+  </si>
+  <si>
+    <t>ქვემო ფონიჭალის დასახლება</t>
+  </si>
+  <si>
+    <t>რუსთავის გზატკეცილი (ცოტნე დადიანის III ჩიხის მოპირდაპირედ, მობრუნების წრეზე) - ქვემო ფონიჭალის დასახლება (რუსთავის გზატკეცილი) - ვახტანგ გორგასალის ქ. - დიმიტრი გულიას მოედანი - დიმიტრი გულიას ქ. - რიჩარდ ჰოლბრუკის ქუჩა - ნავთლუღის ქ. - ქეთევან დედოფლის გამზირი - მოსკოვის გამზირი - ჯავახეთის ქ.  - ვიქტორ კუპრაძის ქ. - ზურაბ პატარიძის ქ. - ჰოთელს &amp; პრეფერენს ჰუალინგ თბილისის მიმდებარედ.
+უკუმიმართულებით:  ჰოთელს &amp; პრეფერენს ჰუალინგ თბილისი - ზურაბ პატარიძის ქ. - ვიქტორ კუპრაძის ქ. -  ჯავახეთის ქ. - მოსკოვის გამზირი - ქეთევან დედოფლის გამზირი - ნავთლუღის ქ. - რიჩარდ ჰოლბრუკის ქუჩა - დიმიტრი გულიას ქ. - დიმიტრი გულიას მოედანი - ვახტანგ გორგასალის ქ. - რუსთავის გზატკეცილი - ქვემო ფონიჭალის დასახლება (რუსთავის გზატკეცილი) - რუსთავის გზატკეცილი (ცოტნე დადიანის III ჩიხის მოპირდაპირედ, მობრუნების წრეზე)</t>
+  </si>
+  <si>
+    <t>ჰუალინგ თბილისი</t>
+  </si>
+  <si>
+    <t xml:space="preserve">სოფელი თხინვალი (თხინვალას და ავალიანის ქუჩების გადაკვეთის მიმდებარედ) – კეჭაყმაძის ქ. – ლევან კვაჭაძის ქ. – ფერმწერთა ქ. – ტატა თვალჭრელიძის ქ. (მობრუნება ალექსანდრე ბანძელაძის ქუჩის გადაკვეთასთან) – ფერმწერთა ქ. – ავთო ვარაზის ქ. (ნუცუბიძის IV მ/რაიონი) – ბესარიონ ჟღენტის ქ. (ნუცუბიძის II მ/რაიონი) – შალვა ნუცუბიძის ქ. – ფერდინანდ თავაძის ქ. – სერგო ზაქარიაძის ქ. – ვაჟა-ფშაველას ჩიხი – მ/ს „დელისი“ (ვაჟა-ფშაველას გამზირი) - ალექსანდრე ყაზბეგის გამზირი (მობრუნება ვაჟა ფშაველას გამზირი #68-ის მიმდებარედ) - მიხეილ თამარაშვილის გამზირი - უნივერსიტეტის ქ. (ივანე ჯავახიშვილის სახელობის თსუ-ის მაღლივი კორპუსი).
+უკუმიმართულებით:  უნივერსიტეტის ქ. (ივანე ჯავახიშვილის სახელობის თსუ-ის მაღლივი კორპუსი) - მიხეილ თამარაშვილის გამზირი (მობრუნება ჭაბუა ამირეჯიბის გზატკეცილის პირდაპირ) - მ/ს „დელისი“ (ვაჟა-ფშაველას გამზირი) – ფერდინანდ თავაძის ქ. – შალვა ნუცუბიძის ქ. – ბესარიონ ჟღენტის ქ. ( შალვა ნუცუბიძის II მ/რაიონი) – ავთო ვარაზის ქ. (ნუცუბიძის  IV მ/რაიონი) – ფერმწერთა ქ. – ტატა თვალჭრელიძის ქ. (მობრუნება ალექსანდრე ბანძელაძის ქუჩის გადაკვეთასთან) – ლევან კვაჭაძის ქ. – კეჭაყმაძის ქ. – სოფელი თხინვალი (თხინვალას და ავალიანის ქუჩების გადაკვეთის მიმდებარედ). </t>
+  </si>
+  <si>
+    <t>სოფელი თხინვალი</t>
+  </si>
+  <si>
+    <t>მ/ს „სახელმწიფო უნივერსიტეტი“(მიმდებარედ) - ზურაბ ანჯაფარიძის ქ. - პეტრე ქავთარაძის ქ. - ალექსანდრე ყაზბეგის გამზირი - მიხეილ თამარაშვილის გამზირი - გიორგი წერეთლის ქ. - ქაქუცა ჩოლოყაშვილის გამზირი - ილია ჭავჭავაძის გამზირი - არჩილ მიშველაძის ქ. - ირაკლი აბაშიძის ქ. - მრგვალი ბაღი - ვასილ ბარნოვის ქ. - კოტე მაყაშვილის ქ. - პოლიკარპე კაკაბაძის ქ. - დანიელ ჭონქაძის ქ. - ამაღლების ქ. - ლადო ასათიანის II შესახვევი - ლადო ასათიანის ქ. - შალვა დადიანის ქ. - თავისუფლების მოედანი - ალექსანდრე პუშკინის ქ. - ნიკოლოზ ბარათაშვილის ქ.  (კონკის 'მხარეს'). 
+უკუმიმართულებით:  ნიკოლოზ ბარათაშვილის ქ. (კონკის 'მხარეს') - ნიკოლოზ ბარათაშვილის ხიდი - მტკვრის მარცხენა სანაპირო - ნიკოლოზ ბარათაშვილის ხიდი - ნიკოლოზ ბარათაშვილის ქ. - ალექსანდრე პუშკინის ქ. -თავისუფლების მოედანი - გიორგი ლეონიძის ქ. - მიხეილ ლერმონტოვის ქ. - პაოლო იაშვილის ქ. - ამაღლების ქ. - დანიელ ჭონქაძის ქ. - პოლიკარპე კაკაბაძის ქ. - კოტე მაყაშვილის ქ. - მიხეილ ზანდუკელის ქ. - ვასილ ბარნოვის ქ. - მრგვალი ბაღი - რაფიელ ერისთავის ქ. - ზაქარია ფალიაშვილის ქ. - ნიკოლოზ ბერძენიშვილის ქ. - ილია ჭავჭავაძის გამზირი - მიხეილ თამარაშვილის გამზირი - ვაჟა ფშაველას გამზირი -  პეტრე ქავთარაძის ქ. (გადასვლა ვაჟა ფშაველას გამზირი #68-ის გავლით) - ზურაბ ანჯაფარიძის ქ. - მ/ს „სახელმწიფო უნივერსიტეტი“ (მიმდებარედ).</t>
+  </si>
+  <si>
+    <t>მერაბ კოსტავას ქ. (№68-ის მიმდებარედ) – მერაბ კოსტავას ქ. – ვარაზისხევის ქ. – ილია ჭავჭავაძის გამზირი – მიხეილ თამარაშვილის გამზირი – ალექსანდრე ყაზბეგის გამზირი – პეკინის გამზირი – მერაბ კოსტავას ქ. (№68-ის მიმდებარედ) (წრიული).</t>
+  </si>
+  <si>
+    <t>ვაკე - საბურთალო</t>
+  </si>
+  <si>
+    <t>მერაბ  კოსტავას ქ. (#69-ის მიდებარედ) - გიორგი სააკაძის მოედანი - ჟიული შარტავას ქ. - ანა კალანდაძის ქ. - პეკინის გამზირი - ვაჟა ფშაველას გამზირი - მიხეილ თამარაშვილის გამზირი - ილია ჭავჭავაძის გამზირი  - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ.  (#69-ის მიდებარედ)(წრიული).</t>
+  </si>
+  <si>
+    <t>საბურთალო-ვაკე</t>
   </si>
 </sst>
 </file>
@@ -2096,8 +2831,14 @@
       <c r="C5" t="n" s="8">
         <v>1.0</v>
       </c>
+      <c r="D5" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F5" t="s" s="14">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5" t="n" s="9">
         <v>8.0</v>
@@ -2120,11 +2861,17 @@
       <c r="M5" t="n" s="12">
         <v>0.9770833333333333</v>
       </c>
+      <c r="N5" t="s" s="10">
+        <v>23</v>
+      </c>
       <c r="O5" t="n" s="12">
         <v>0.925</v>
       </c>
       <c r="P5" t="n" s="12">
         <v>0.9423611111111111</v>
+      </c>
+      <c r="Q5" t="s" s="10">
+        <v>24</v>
       </c>
       <c r="R5" t="n" s="12">
         <v>0.9236111111111112</v>
@@ -2143,8 +2890,14 @@
       <c r="C6" t="n" s="8">
         <v>2.0</v>
       </c>
+      <c r="D6" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F6" t="s" s="16">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G6" t="n" s="9">
         <v>11.0</v>
@@ -2167,11 +2920,17 @@
       <c r="M6" t="n" s="12">
         <v>0.9826388888888888</v>
       </c>
+      <c r="N6" t="s" s="10">
+        <v>27</v>
+      </c>
       <c r="O6" t="n" s="12">
         <v>0.9340277777777778</v>
       </c>
       <c r="P6" t="n" s="12">
         <v>0.9409722222222222</v>
+      </c>
+      <c r="Q6" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R6" t="n" s="12">
         <v>0.9305555555555556</v>
@@ -2190,8 +2949,14 @@
       <c r="C7" t="n" s="8">
         <v>3.0</v>
       </c>
+      <c r="D7" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F7" t="s" s="18">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G7" t="n" s="9">
         <v>6.0</v>
@@ -2214,11 +2979,17 @@
       <c r="M7" t="n" s="12">
         <v>0.9736111111111111</v>
       </c>
+      <c r="N7" t="s" s="10">
+        <v>30</v>
+      </c>
       <c r="O7" t="n" s="12">
         <v>0.9180555555555555</v>
       </c>
       <c r="P7" t="n" s="12">
         <v>0.9402777777777778</v>
+      </c>
+      <c r="Q7" t="s" s="10">
+        <v>31</v>
       </c>
       <c r="R7" t="n" s="12">
         <v>0.9180555555555555</v>
@@ -2237,8 +3008,14 @@
       <c r="C8" t="n" s="8">
         <v>4.0</v>
       </c>
+      <c r="D8" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F8" t="s" s="20">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G8" t="n" s="9">
         <v>3.0</v>
@@ -2261,11 +3038,17 @@
       <c r="M8" t="n" s="12">
         <v>0.9840277777777777</v>
       </c>
+      <c r="N8" t="s" s="10">
+        <v>34</v>
+      </c>
       <c r="O8" t="n" s="12">
         <v>0.9145833333333333</v>
       </c>
       <c r="P8" t="n" s="12">
         <v>0.9423611111111111</v>
+      </c>
+      <c r="Q8" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R8" t="n" s="12">
         <v>0.875</v>
@@ -2284,8 +3067,14 @@
       <c r="C9" t="n" s="8">
         <v>5.0</v>
       </c>
+      <c r="D9" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F9" t="s" s="22">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G9" t="n" s="9">
         <v>2.0</v>
@@ -2308,11 +3097,17 @@
       <c r="M9" t="n" s="12">
         <v>0.9583333333333334</v>
       </c>
+      <c r="N9" t="s" s="10">
+        <v>36</v>
+      </c>
       <c r="O9" t="n" s="12">
         <v>0.875</v>
       </c>
       <c r="P9" t="n" s="12">
         <v>0.9166666666666666</v>
+      </c>
+      <c r="Q9" t="s" s="10">
+        <v>37</v>
       </c>
       <c r="R9" t="n" s="12">
         <v>0.8333333333333334</v>
@@ -2331,8 +3126,14 @@
       <c r="C10" t="n" s="8">
         <v>6.0</v>
       </c>
+      <c r="D10" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F10" t="s" s="24">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G10" t="n" s="9">
         <v>7.0</v>
@@ -2355,11 +3156,17 @@
       <c r="M10" t="n" s="12">
         <v>1.0</v>
       </c>
+      <c r="N10" t="s" s="10">
+        <v>28</v>
+      </c>
       <c r="O10" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
       <c r="P10" t="n" s="12">
         <v>0.9444444444444444</v>
+      </c>
+      <c r="Q10" t="s" s="10">
+        <v>39</v>
       </c>
       <c r="R10" t="n" s="12">
         <v>0.9215277777777777</v>
@@ -2378,8 +3185,14 @@
       <c r="C11" t="n" s="8">
         <v>7.0</v>
       </c>
+      <c r="D11" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F11" t="s" s="26">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G11" t="n" s="9">
         <v>3.0</v>
@@ -2402,11 +3215,17 @@
       <c r="M11" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
+      <c r="N11" t="s" s="10">
+        <v>41</v>
+      </c>
       <c r="O11" t="n" s="12">
         <v>0.9375</v>
       </c>
       <c r="P11" t="n" s="12">
         <v>0.9513888888888888</v>
+      </c>
+      <c r="Q11" t="s" s="10">
+        <v>42</v>
       </c>
       <c r="R11" t="n" s="12">
         <v>0.9166666666666666</v>
@@ -2425,8 +3244,14 @@
       <c r="C12" t="n" s="8">
         <v>9.0</v>
       </c>
+      <c r="D12" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F12" t="s" s="28">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G12" t="n" s="9">
         <v>5.0</v>
@@ -2449,11 +3274,17 @@
       <c r="M12" t="n" s="12">
         <v>0.9736111111111111</v>
       </c>
+      <c r="N12" t="s" s="10">
+        <v>45</v>
+      </c>
       <c r="O12" t="n" s="12">
         <v>0.9215277777777777</v>
       </c>
       <c r="P12" t="n" s="12">
         <v>0.9423611111111111</v>
+      </c>
+      <c r="Q12" t="s" s="10">
+        <v>46</v>
       </c>
       <c r="R12" t="n" s="12">
         <v>0.9270833333333334</v>
@@ -2472,8 +3303,14 @@
       <c r="C13" t="n" s="8">
         <v>10.0</v>
       </c>
+      <c r="D13" t="s" s="7">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F13" t="s" s="30">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G13" t="n" s="9">
         <v>4.0</v>
@@ -2496,11 +3333,17 @@
       <c r="M13" t="n" s="12">
         <v>0.9902777777777778</v>
       </c>
+      <c r="N13" t="s" s="10">
+        <v>48</v>
+      </c>
       <c r="O13" t="n" s="12">
         <v>0.9097222222222222</v>
       </c>
       <c r="P13" t="n" s="12">
         <v>0.9368055555555556</v>
+      </c>
+      <c r="Q13" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R13" t="n" s="12">
         <v>0.8840277777777777</v>
@@ -2519,8 +3362,14 @@
       <c r="C14" t="n" s="8">
         <v>11.0</v>
       </c>
+      <c r="D14" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F14" t="s" s="32">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G14" t="n" s="9">
         <v>7.0</v>
@@ -2543,11 +3392,17 @@
       <c r="M14" t="n" s="12">
         <v>0.9923611111111111</v>
       </c>
+      <c r="N14" t="s" s="10">
+        <v>50</v>
+      </c>
       <c r="O14" t="n" s="12">
         <v>0.9236111111111112</v>
       </c>
       <c r="P14" t="n" s="12">
         <v>0.9486111111111111</v>
+      </c>
+      <c r="Q14" t="s" s="10">
+        <v>51</v>
       </c>
       <c r="R14" t="n" s="12">
         <v>0.9173611111111111</v>
@@ -2566,8 +3421,14 @@
       <c r="C15" t="n" s="8">
         <v>12.0</v>
       </c>
+      <c r="D15" t="s" s="7">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F15" t="s" s="34">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G15" t="n" s="9">
         <v>4.0</v>
@@ -2590,11 +3451,17 @@
       <c r="M15" t="n" s="12">
         <v>0.9909722222222223</v>
       </c>
+      <c r="N15" t="s" s="10">
+        <v>53</v>
+      </c>
       <c r="O15" t="n" s="12">
         <v>0.8986111111111111</v>
       </c>
       <c r="P15" t="n" s="12">
         <v>0.9173611111111111</v>
+      </c>
+      <c r="Q15" t="s" s="10">
+        <v>24</v>
       </c>
       <c r="R15" t="n" s="12">
         <v>0.9347222222222222</v>
@@ -2613,8 +3480,14 @@
       <c r="C16" t="n" s="8">
         <v>14.0</v>
       </c>
+      <c r="D16" t="s" s="7">
+        <v>54</v>
+      </c>
+      <c r="E16" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F16" t="s" s="36">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G16" t="n" s="9">
         <v>11.0</v>
@@ -2637,11 +3510,17 @@
       <c r="M16" t="n" s="12">
         <v>0.9958333333333333</v>
       </c>
+      <c r="N16" t="s" s="10">
+        <v>55</v>
+      </c>
       <c r="O16" t="n" s="12">
         <v>0.9055555555555556</v>
       </c>
       <c r="P16" t="n" s="12">
         <v>0.9416666666666667</v>
+      </c>
+      <c r="Q16" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R16" t="n" s="12">
         <v>0.9368055555555556</v>
@@ -2660,8 +3539,14 @@
       <c r="C17" t="n" s="8">
         <v>15.0</v>
       </c>
+      <c r="D17" t="s" s="7">
+        <v>56</v>
+      </c>
+      <c r="E17" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F17" t="s" s="38">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G17" t="n" s="9">
         <v>6.0</v>
@@ -2684,11 +3569,17 @@
       <c r="M17" t="n" s="12">
         <v>0.9791666666666666</v>
       </c>
+      <c r="N17" t="s" s="10">
+        <v>55</v>
+      </c>
       <c r="O17" t="n" s="12">
         <v>0.9097222222222222</v>
       </c>
       <c r="P17" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q17" t="s" s="10">
+        <v>45</v>
       </c>
       <c r="R17" t="n" s="12">
         <v>0.9236111111111112</v>
@@ -2707,8 +3598,14 @@
       <c r="C18" t="n" s="8">
         <v>16.0</v>
       </c>
+      <c r="D18" t="s" s="7">
+        <v>57</v>
+      </c>
+      <c r="E18" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F18" t="s" s="40">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G18" t="n" s="9">
         <v>1.0</v>
@@ -2731,11 +3628,17 @@
       <c r="M18" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
+      <c r="N18" t="s" s="10">
+        <v>58</v>
+      </c>
       <c r="O18" t="n" s="12">
         <v>0.8125</v>
       </c>
       <c r="P18" t="n" s="12">
         <v>0.8854166666666666</v>
+      </c>
+      <c r="Q18" t="s" s="10">
+        <v>42</v>
       </c>
       <c r="R18" t="n" s="12">
         <v>0.7708333333333334</v>
@@ -2754,8 +3657,14 @@
       <c r="C19" t="n" s="8">
         <v>17.0</v>
       </c>
+      <c r="D19" t="s" s="7">
+        <v>59</v>
+      </c>
+      <c r="E19" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F19" t="s" s="42">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G19" t="n" s="9">
         <v>7.0</v>
@@ -2778,11 +3687,17 @@
       <c r="M19" t="n" s="12">
         <v>0.9791666666666666</v>
       </c>
+      <c r="N19" t="s" s="10">
+        <v>60</v>
+      </c>
       <c r="O19" t="n" s="12">
         <v>0.90625</v>
       </c>
       <c r="P19" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q19" t="s" s="10">
+        <v>61</v>
       </c>
       <c r="R19" t="n" s="12">
         <v>0.9201388888888888</v>
@@ -2801,8 +3716,14 @@
       <c r="C20" t="n" s="8">
         <v>18.0</v>
       </c>
+      <c r="D20" t="s" s="7">
+        <v>62</v>
+      </c>
+      <c r="E20" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F20" t="s" s="44">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G20" t="n" s="9">
         <v>3.0</v>
@@ -2825,11 +3746,17 @@
       <c r="M20" t="n" s="12">
         <v>0.9861111111111112</v>
       </c>
+      <c r="N20" t="s" s="10">
+        <v>63</v>
+      </c>
       <c r="O20" t="n" s="12">
         <v>0.9027777777777778</v>
       </c>
       <c r="P20" t="n" s="12">
         <v>0.9305555555555556</v>
+      </c>
+      <c r="Q20" t="s" s="10">
+        <v>24</v>
       </c>
       <c r="R20" t="n" s="12">
         <v>0.8888888888888888</v>
@@ -2848,8 +3775,14 @@
       <c r="C21" t="n" s="8">
         <v>20.0</v>
       </c>
+      <c r="D21" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="E21" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F21" t="s" s="46">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G21" t="n" s="9">
         <v>10.0</v>
@@ -2872,11 +3805,17 @@
       <c r="M21" t="n" s="12">
         <v>0.9868055555555556</v>
       </c>
+      <c r="N21" t="s" s="10">
+        <v>65</v>
+      </c>
       <c r="O21" t="n" s="12">
         <v>0.9333333333333333</v>
       </c>
       <c r="P21" t="n" s="12">
         <v>0.9409722222222222</v>
+      </c>
+      <c r="Q21" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R21" t="n" s="12">
         <v>0.9333333333333333</v>
@@ -2895,8 +3834,14 @@
       <c r="C22" t="n" s="8">
         <v>21.0</v>
       </c>
+      <c r="D22" t="s" s="7">
+        <v>66</v>
+      </c>
+      <c r="E22" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F22" t="s" s="48">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G22" t="n" s="9">
         <v>11.0</v>
@@ -2919,11 +3864,17 @@
       <c r="M22" t="n" s="12">
         <v>1.0118055555555556</v>
       </c>
+      <c r="N22" t="s" s="10">
+        <v>55</v>
+      </c>
       <c r="O22" t="n" s="12">
         <v>0.89375</v>
       </c>
       <c r="P22" t="n" s="12">
         <v>0.9409722222222222</v>
+      </c>
+      <c r="Q22" t="s" s="10">
+        <v>67</v>
       </c>
       <c r="R22" t="n" s="12">
         <v>0.9347222222222222</v>
@@ -2942,8 +3893,14 @@
       <c r="C23" t="n" s="8">
         <v>22.0</v>
       </c>
+      <c r="D23" t="s" s="7">
+        <v>68</v>
+      </c>
+      <c r="E23" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F23" t="s" s="50">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G23" t="n" s="9">
         <v>3.0</v>
@@ -2966,11 +3923,17 @@
       <c r="M23" t="n" s="12">
         <v>0.9861111111111112</v>
       </c>
+      <c r="N23" t="s" s="10">
+        <v>69</v>
+      </c>
       <c r="O23" t="n" s="12">
         <v>0.875</v>
       </c>
       <c r="P23" t="n" s="12">
         <v>0.9027777777777778</v>
+      </c>
+      <c r="Q23" t="s" s="10">
+        <v>24</v>
       </c>
       <c r="R23" t="n" s="12">
         <v>0.9159722222222222</v>
@@ -2989,8 +3952,14 @@
       <c r="C24" t="n" s="8">
         <v>23.0</v>
       </c>
+      <c r="D24" t="s" s="7">
+        <v>70</v>
+      </c>
+      <c r="E24" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F24" t="s" s="52">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G24" t="n" s="9">
         <v>9.0</v>
@@ -3013,11 +3982,17 @@
       <c r="M24" t="n" s="12">
         <v>0.9909722222222223</v>
       </c>
+      <c r="N24" t="s" s="10">
+        <v>71</v>
+      </c>
       <c r="O24" t="n" s="12">
         <v>0.9152777777777777</v>
       </c>
       <c r="P24" t="n" s="12">
         <v>0.9458333333333333</v>
+      </c>
+      <c r="Q24" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R24" t="n" s="12">
         <v>0.9305555555555556</v>
@@ -3036,8 +4011,14 @@
       <c r="C25" t="n" s="8">
         <v>24.0</v>
       </c>
+      <c r="D25" t="s" s="7">
+        <v>72</v>
+      </c>
+      <c r="E25" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F25" t="s" s="54">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G25" t="n" s="9">
         <v>10.0</v>
@@ -3060,11 +4041,17 @@
       <c r="M25" t="n" s="12">
         <v>0.9986111111111111</v>
       </c>
+      <c r="N25" t="s" s="10">
+        <v>71</v>
+      </c>
       <c r="O25" t="n" s="12">
         <v>0.9097222222222222</v>
       </c>
       <c r="P25" t="n" s="12">
         <v>0.9430555555555555</v>
+      </c>
+      <c r="Q25" t="s" s="10">
+        <v>67</v>
       </c>
       <c r="R25" t="n" s="12">
         <v>0.9319444444444445</v>
@@ -3083,8 +4070,14 @@
       <c r="C26" t="n" s="8">
         <v>25.0</v>
       </c>
+      <c r="D26" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="E26" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F26" t="s" s="56">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G26" t="n" s="9">
         <v>8.0</v>
@@ -3107,11 +4100,17 @@
       <c r="M26" t="n" s="12">
         <v>0.9784722222222222</v>
       </c>
+      <c r="N26" t="s" s="10">
+        <v>74</v>
+      </c>
       <c r="O26" t="n" s="12">
         <v>0.9243055555555556</v>
       </c>
       <c r="P26" t="n" s="12">
         <v>0.9423611111111111</v>
+      </c>
+      <c r="Q26" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R26" t="n" s="12">
         <v>0.9243055555555556</v>
@@ -3130,8 +4129,14 @@
       <c r="C27" t="n" s="8">
         <v>26.0</v>
       </c>
+      <c r="D27" t="s" s="7">
+        <v>75</v>
+      </c>
+      <c r="E27" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F27" t="s" s="58">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G27" t="n" s="9">
         <v>1.0</v>
@@ -3154,11 +4159,17 @@
       <c r="M27" t="n" s="12">
         <v>0.9131944444444444</v>
       </c>
+      <c r="N27" t="s" s="10">
+        <v>42</v>
+      </c>
       <c r="O27" t="n" s="12">
         <v>0.8402777777777778</v>
       </c>
       <c r="P27" t="n" s="12">
         <v>0.8888888888888888</v>
+      </c>
+      <c r="Q27" t="s" s="10">
+        <v>76</v>
       </c>
       <c r="R27" t="n" s="12">
         <v>0.8159722222222222</v>
@@ -3177,8 +4188,14 @@
       <c r="C28" t="n" s="8">
         <v>27.0</v>
       </c>
+      <c r="D28" t="s" s="7">
+        <v>77</v>
+      </c>
+      <c r="E28" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F28" t="s" s="60">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G28" t="n" s="9">
         <v>6.0</v>
@@ -3201,11 +4218,17 @@
       <c r="M28" t="n" s="12">
         <v>0.9763888888888889</v>
       </c>
+      <c r="N28" t="s" s="10">
+        <v>78</v>
+      </c>
       <c r="O28" t="n" s="12">
         <v>0.9256944444444445</v>
       </c>
       <c r="P28" t="n" s="12">
         <v>0.9458333333333333</v>
+      </c>
+      <c r="Q28" t="s" s="10">
+        <v>79</v>
       </c>
       <c r="R28" t="n" s="12">
         <v>0.9347222222222222</v>
@@ -3224,8 +4247,14 @@
       <c r="C29" t="n" s="8">
         <v>28.0</v>
       </c>
+      <c r="D29" t="s" s="7">
+        <v>80</v>
+      </c>
+      <c r="E29" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F29" t="s" s="62">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G29" t="n" s="9">
         <v>4.0</v>
@@ -3248,11 +4277,17 @@
       <c r="M29" t="n" s="12">
         <v>0.96875</v>
       </c>
+      <c r="N29" t="s" s="10">
+        <v>81</v>
+      </c>
       <c r="O29" t="n" s="12">
         <v>0.9270833333333334</v>
       </c>
       <c r="P29" t="n" s="12">
         <v>0.9479166666666666</v>
+      </c>
+      <c r="Q29" t="s" s="10">
+        <v>82</v>
       </c>
       <c r="R29" t="n" s="12">
         <v>0.9270833333333334</v>
@@ -3271,8 +4306,14 @@
       <c r="C30" t="n" s="8">
         <v>29.0</v>
       </c>
+      <c r="D30" t="s" s="7">
+        <v>83</v>
+      </c>
+      <c r="E30" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F30" t="s" s="64">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G30" t="n" s="9">
         <v>3.0</v>
@@ -3295,11 +4336,17 @@
       <c r="M30" t="n" s="12">
         <v>0.9791666666666666</v>
       </c>
+      <c r="N30" t="s" s="10">
+        <v>79</v>
+      </c>
       <c r="O30" t="n" s="12">
         <v>0.8986111111111111</v>
       </c>
       <c r="P30" t="n" s="12">
         <v>0.9444444444444444</v>
+      </c>
+      <c r="Q30" t="s" s="10">
+        <v>84</v>
       </c>
       <c r="R30" t="n" s="12">
         <v>0.9104166666666667</v>
@@ -3318,8 +4365,14 @@
       <c r="C31" t="n" s="8">
         <v>30.0</v>
       </c>
+      <c r="D31" t="s" s="7">
+        <v>85</v>
+      </c>
+      <c r="E31" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F31" t="s" s="66">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="G31" t="n" s="9">
         <v>3.0</v>
@@ -3342,11 +4395,17 @@
       <c r="M31" t="n" s="12">
         <v>0.9756944444444444</v>
       </c>
+      <c r="N31" t="s" s="10">
+        <v>27</v>
+      </c>
       <c r="O31" t="n" s="12">
         <v>0.90625</v>
       </c>
       <c r="P31" t="n" s="12">
         <v>0.9444444444444444</v>
+      </c>
+      <c r="Q31" t="s" s="10">
+        <v>24</v>
       </c>
       <c r="R31" t="n" s="12">
         <v>0.9131944444444444</v>
@@ -3365,8 +4424,14 @@
       <c r="C32" t="n" s="8">
         <v>31.0</v>
       </c>
+      <c r="D32" t="s" s="7">
+        <v>87</v>
+      </c>
+      <c r="E32" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F32" t="s" s="68">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G32" t="n" s="9">
         <v>5.0</v>
@@ -3389,11 +4454,17 @@
       <c r="M32" t="n" s="12">
         <v>0.9833333333333333</v>
       </c>
+      <c r="N32" t="s" s="10">
+        <v>88</v>
+      </c>
       <c r="O32" t="n" s="12">
         <v>0.9138888888888889</v>
       </c>
       <c r="P32" t="n" s="12">
         <v>0.9416666666666667</v>
+      </c>
+      <c r="Q32" t="s" s="10">
+        <v>45</v>
       </c>
       <c r="R32" t="n" s="12">
         <v>0.91875</v>
@@ -3412,8 +4483,14 @@
       <c r="C33" t="n" s="8">
         <v>32.0</v>
       </c>
+      <c r="D33" t="s" s="7">
+        <v>89</v>
+      </c>
+      <c r="E33" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F33" t="s" s="70">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G33" t="n" s="9">
         <v>4.0</v>
@@ -3436,11 +4513,17 @@
       <c r="M33" t="n" s="12">
         <v>0.96875</v>
       </c>
+      <c r="N33" t="s" s="10">
+        <v>71</v>
+      </c>
       <c r="O33" t="n" s="12">
         <v>0.9215277777777777</v>
       </c>
       <c r="P33" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q33" t="s" s="10">
+        <v>90</v>
       </c>
       <c r="R33" t="n" s="12">
         <v>0.90625</v>
@@ -3459,8 +4542,14 @@
       <c r="C34" t="n" s="8">
         <v>33.0</v>
       </c>
+      <c r="D34" t="s" s="7">
+        <v>91</v>
+      </c>
+      <c r="E34" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F34" t="s" s="72">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G34" t="n" s="9">
         <v>9.0</v>
@@ -3483,11 +4572,17 @@
       <c r="M34" t="n" s="12">
         <v>0.9951388888888889</v>
       </c>
+      <c r="N34" t="s" s="10">
+        <v>71</v>
+      </c>
       <c r="O34" t="n" s="12">
         <v>0.8951388888888889</v>
       </c>
       <c r="P34" t="n" s="12">
         <v>0.9395833333333333</v>
+      </c>
+      <c r="Q34" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R34" t="n" s="12">
         <v>0.9340277777777778</v>
@@ -3506,8 +4601,14 @@
       <c r="C35" t="n" s="8">
         <v>34.0</v>
       </c>
+      <c r="D35" t="s" s="7">
+        <v>92</v>
+      </c>
+      <c r="E35" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F35" t="s" s="74">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G35" t="n" s="9">
         <v>9.0</v>
@@ -3530,11 +4631,17 @@
       <c r="M35" t="n" s="12">
         <v>0.9923611111111111</v>
       </c>
+      <c r="N35" t="s" s="10">
+        <v>45</v>
+      </c>
       <c r="O35" t="n" s="12">
         <v>0.9215277777777777</v>
       </c>
       <c r="P35" t="n" s="12">
         <v>0.9416666666666667</v>
+      </c>
+      <c r="Q35" t="s" s="10">
+        <v>93</v>
       </c>
       <c r="R35" t="n" s="12">
         <v>0.9263888888888889</v>
@@ -3553,8 +4660,14 @@
       <c r="C36" t="n" s="8">
         <v>35.0</v>
       </c>
+      <c r="D36" t="s" s="7">
+        <v>94</v>
+      </c>
+      <c r="E36" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F36" t="s" s="76">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="G36" t="n" s="9">
         <v>1.0</v>
@@ -3577,11 +4690,17 @@
       <c r="M36" t="n" s="12">
         <v>0.9375</v>
       </c>
+      <c r="N36" t="s" s="10">
+        <v>95</v>
+      </c>
       <c r="O36" t="n" s="12">
         <v>0.8541666666666666</v>
       </c>
       <c r="P36" t="n" s="12">
         <v>0.8958333333333334</v>
+      </c>
+      <c r="Q36" t="s" s="10">
+        <v>96</v>
       </c>
       <c r="R36" t="n" s="12">
         <v>0.875</v>
@@ -3600,8 +4719,14 @@
       <c r="C37" t="n" s="8">
         <v>36.0</v>
       </c>
+      <c r="D37" t="s" s="7">
+        <v>97</v>
+      </c>
+      <c r="E37" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F37" t="s" s="78">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G37" t="n" s="9">
         <v>6.0</v>
@@ -3624,11 +4749,17 @@
       <c r="M37" t="n" s="12">
         <v>0.9583333333333334</v>
       </c>
+      <c r="N37" t="s" s="10">
+        <v>98</v>
+      </c>
       <c r="O37" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
       <c r="P37" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q37" t="s" s="10">
+        <v>61</v>
       </c>
       <c r="R37" t="n" s="12">
         <v>0.9166666666666666</v>
@@ -3647,8 +4778,14 @@
       <c r="C38" t="n" s="8">
         <v>37.0</v>
       </c>
+      <c r="D38" t="s" s="7">
+        <v>99</v>
+      </c>
+      <c r="E38" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F38" t="s" s="80">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G38" t="n" s="9">
         <v>10.0</v>
@@ -3671,11 +4808,17 @@
       <c r="M38" t="n" s="12">
         <v>1.0</v>
       </c>
+      <c r="N38" t="s" s="10">
+        <v>45</v>
+      </c>
       <c r="O38" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
       <c r="P38" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q38" t="s" s="10">
+        <v>100</v>
       </c>
       <c r="R38" t="n" s="12">
         <v>0.9368055555555556</v>
@@ -3694,8 +4837,14 @@
       <c r="C39" t="n" s="8">
         <v>38.0</v>
       </c>
+      <c r="D39" t="s" s="7">
+        <v>101</v>
+      </c>
+      <c r="E39" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F39" t="s" s="82">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G39" t="n" s="9">
         <v>6.0</v>
@@ -3718,11 +4867,17 @@
       <c r="M39" t="n" s="12">
         <v>0.975</v>
       </c>
+      <c r="N39" t="s" s="10">
+        <v>102</v>
+      </c>
       <c r="O39" t="n" s="12">
         <v>0.925</v>
       </c>
       <c r="P39" t="n" s="12">
         <v>0.9416666666666667</v>
+      </c>
+      <c r="Q39" t="s" s="10">
+        <v>103</v>
       </c>
       <c r="R39" t="s" s="12">
         <v>20</v>
@@ -3741,8 +4896,14 @@
       <c r="C40" t="n" s="8">
         <v>39.0</v>
       </c>
+      <c r="D40" t="s" s="7">
+        <v>104</v>
+      </c>
+      <c r="E40" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F40" t="s" s="84">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G40" t="n" s="9">
         <v>10.0</v>
@@ -3765,11 +4926,17 @@
       <c r="M40" t="n" s="12">
         <v>0.9729166666666667</v>
       </c>
+      <c r="N40" t="s" s="10">
+        <v>105</v>
+      </c>
       <c r="O40" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
       <c r="P40" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q40" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R40" t="n" s="12">
         <v>0.9243055555555556</v>
@@ -3788,8 +4955,14 @@
       <c r="C41" t="n" s="8">
         <v>40.0</v>
       </c>
+      <c r="D41" t="s" s="7">
+        <v>106</v>
+      </c>
+      <c r="E41" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F41" t="s" s="86">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G41" t="n" s="9">
         <v>3.0</v>
@@ -3812,11 +4985,17 @@
       <c r="M41" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
+      <c r="N41" t="s" s="10">
+        <v>107</v>
+      </c>
       <c r="O41" t="n" s="12">
         <v>0.9097222222222222</v>
       </c>
       <c r="P41" t="n" s="12">
         <v>0.9430555555555555</v>
+      </c>
+      <c r="Q41" t="s" s="10">
+        <v>108</v>
       </c>
       <c r="R41" t="n" s="12">
         <v>0.9180555555555555</v>
@@ -3835,8 +5014,14 @@
       <c r="C42" t="n" s="8">
         <v>41.0</v>
       </c>
+      <c r="D42" t="s" s="7">
+        <v>109</v>
+      </c>
+      <c r="E42" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F42" t="s" s="88">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G42" t="n" s="9">
         <v>3.0</v>
@@ -3859,11 +5044,17 @@
       <c r="M42" t="n" s="12">
         <v>0.9930555555555556</v>
       </c>
+      <c r="N42" t="s" s="10">
+        <v>110</v>
+      </c>
       <c r="O42" t="n" s="12">
         <v>0.9097222222222222</v>
       </c>
       <c r="P42" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q42" t="s" s="10">
+        <v>24</v>
       </c>
       <c r="R42" t="n" s="12">
         <v>0.9222222222222223</v>
@@ -3882,8 +5073,14 @@
       <c r="C43" t="n" s="8">
         <v>42.0</v>
       </c>
+      <c r="D43" t="s" s="7">
+        <v>111</v>
+      </c>
+      <c r="E43" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F43" t="s" s="90">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G43" t="n" s="9">
         <v>4.0</v>
@@ -3906,11 +5103,17 @@
       <c r="M43" t="n" s="12">
         <v>0.9729166666666667</v>
       </c>
+      <c r="N43" t="s" s="10">
+        <v>112</v>
+      </c>
       <c r="O43" t="n" s="12">
         <v>0.9208333333333333</v>
       </c>
       <c r="P43" t="n" s="12">
         <v>0.9465277777777777</v>
+      </c>
+      <c r="Q43" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R43" t="n" s="12">
         <v>0.9340277777777778</v>
@@ -3929,8 +5132,14 @@
       <c r="C44" t="n" s="8">
         <v>43.0</v>
       </c>
+      <c r="D44" t="s" s="7">
+        <v>113</v>
+      </c>
+      <c r="E44" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F44" t="s" s="92">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G44" t="n" s="9">
         <v>3.0</v>
@@ -3953,11 +5162,17 @@
       <c r="M44" t="n" s="12">
         <v>0.96875</v>
       </c>
+      <c r="N44" t="s" s="10">
+        <v>114</v>
+      </c>
       <c r="O44" t="n" s="12">
         <v>0.8854166666666666</v>
       </c>
       <c r="P44" t="n" s="12">
         <v>0.9270833333333334</v>
+      </c>
+      <c r="Q44" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R44" t="n" s="12">
         <v>0.90625</v>
@@ -3976,8 +5191,14 @@
       <c r="C45" t="n" s="8">
         <v>45.0</v>
       </c>
+      <c r="D45" t="s" s="7">
+        <v>115</v>
+      </c>
+      <c r="E45" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F45" t="s" s="94">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G45" t="n" s="9">
         <v>2.0</v>
@@ -4000,11 +5221,17 @@
       <c r="M45" t="n" s="12">
         <v>0.9527777777777777</v>
       </c>
+      <c r="N45" t="s" s="10">
+        <v>116</v>
+      </c>
       <c r="O45" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
       <c r="P45" t="n" s="12">
         <v>0.9319444444444445</v>
+      </c>
+      <c r="Q45" t="s" s="10">
+        <v>30</v>
       </c>
       <c r="R45" t="n" s="12">
         <v>0.9166666666666666</v>
@@ -4023,8 +5250,14 @@
       <c r="C46" t="n" s="8">
         <v>45.099998474121094</v>
       </c>
+      <c r="D46" t="s" s="7">
+        <v>117</v>
+      </c>
+      <c r="E46" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F46" t="s" s="96">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G46" t="n" s="9">
         <v>1.0</v>
@@ -4047,12 +5280,16 @@
       <c r="M46" t="n" s="12">
         <v>0.9652777777777778</v>
       </c>
+      <c r="N46" t="s" s="10">
+        <v>30</v>
+      </c>
       <c r="O46" t="n" s="12">
         <v>0.9027777777777778</v>
       </c>
       <c r="P46" t="n" s="12">
         <v>0.9444444444444444</v>
       </c>
+      <c r="Q46" s="10"/>
       <c r="R46" t="n" s="12">
         <v>0.8819444444444444</v>
       </c>
@@ -4070,8 +5307,14 @@
       <c r="C47" t="n" s="8">
         <v>45.20000076293945</v>
       </c>
+      <c r="D47" t="s" s="7">
+        <v>118</v>
+      </c>
+      <c r="E47" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F47" t="s" s="98">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="G47" t="n" s="9">
         <v>2.0</v>
@@ -4094,12 +5337,16 @@
       <c r="M47" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
+      <c r="N47" t="s" s="10">
+        <v>30</v>
+      </c>
       <c r="O47" t="n" s="12">
         <v>0.9305555555555556</v>
       </c>
       <c r="P47" t="n" s="12">
         <v>0.9513888888888888</v>
       </c>
+      <c r="Q47" s="10"/>
       <c r="R47" t="n" s="12">
         <v>0.9305555555555556</v>
       </c>
@@ -4117,8 +5364,14 @@
       <c r="C48" t="n" s="8">
         <v>46.0</v>
       </c>
+      <c r="D48" t="s" s="7">
+        <v>119</v>
+      </c>
+      <c r="E48" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F48" t="s" s="100">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G48" t="n" s="9">
         <v>8.0</v>
@@ -4141,11 +5394,17 @@
       <c r="M48" t="n" s="12">
         <v>0.9916666666666667</v>
       </c>
+      <c r="N48" t="s" s="10">
+        <v>120</v>
+      </c>
       <c r="O48" t="n" s="12">
         <v>0.9027777777777778</v>
       </c>
       <c r="P48" t="n" s="12">
         <v>0.9472222222222222</v>
+      </c>
+      <c r="Q48" t="s" s="10">
+        <v>121</v>
       </c>
       <c r="R48" t="n" s="12">
         <v>0.9243055555555556</v>
@@ -4164,8 +5423,14 @@
       <c r="C49" t="n" s="8">
         <v>47.0</v>
       </c>
+      <c r="D49" t="s" s="7">
+        <v>122</v>
+      </c>
+      <c r="E49" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F49" t="s" s="102">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G49" t="n" s="9">
         <v>4.0</v>
@@ -4188,11 +5453,17 @@
       <c r="M49" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
+      <c r="N49" t="s" s="10">
+        <v>123</v>
+      </c>
       <c r="O49" t="n" s="12">
         <v>0.9027777777777778</v>
       </c>
       <c r="P49" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q49" t="s" s="10">
+        <v>79</v>
       </c>
       <c r="R49" t="n" s="12">
         <v>0.9201388888888888</v>
@@ -4211,8 +5482,14 @@
       <c r="C50" t="n" s="8">
         <v>49.0</v>
       </c>
+      <c r="D50" t="s" s="7">
+        <v>124</v>
+      </c>
+      <c r="E50" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F50" t="s" s="104">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G50" t="n" s="9">
         <v>6.0</v>
@@ -4235,11 +5512,17 @@
       <c r="M50" t="n" s="12">
         <v>0.9805555555555555</v>
       </c>
+      <c r="N50" t="s" s="10">
+        <v>125</v>
+      </c>
       <c r="O50" t="n" s="12">
         <v>0.9263888888888889</v>
       </c>
       <c r="P50" t="n" s="12">
         <v>0.9479166666666666</v>
+      </c>
+      <c r="Q50" t="s" s="10">
+        <v>45</v>
       </c>
       <c r="R50" t="n" s="12">
         <v>0.9201388888888888</v>
@@ -4258,8 +5541,14 @@
       <c r="C51" t="n" s="8">
         <v>50.0</v>
       </c>
+      <c r="D51" t="s" s="7">
+        <v>126</v>
+      </c>
+      <c r="E51" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F51" t="s" s="106">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G51" t="n" s="9">
         <v>8.0</v>
@@ -4282,11 +5571,17 @@
       <c r="M51" t="n" s="12">
         <v>0.9861111111111112</v>
       </c>
+      <c r="N51" t="s" s="10">
+        <v>127</v>
+      </c>
       <c r="O51" t="n" s="12">
         <v>0.9236111111111112</v>
       </c>
       <c r="P51" t="n" s="12">
         <v>0.9444444444444444</v>
+      </c>
+      <c r="Q51" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R51" t="n" s="12">
         <v>0.9229166666666667</v>
@@ -4305,8 +5600,14 @@
       <c r="C52" t="n" s="8">
         <v>51.0</v>
       </c>
+      <c r="D52" t="s" s="7">
+        <v>128</v>
+      </c>
+      <c r="E52" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F52" t="s" s="108">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G52" t="n" s="9">
         <v>13.0</v>
@@ -4329,11 +5630,17 @@
       <c r="M52" t="n" s="12">
         <v>1.0104166666666667</v>
       </c>
+      <c r="N52" t="s" s="10">
+        <v>129</v>
+      </c>
       <c r="O52" t="n" s="12">
         <v>0.8854166666666666</v>
       </c>
       <c r="P52" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q52" t="s" s="10">
+        <v>46</v>
       </c>
       <c r="R52" t="n" s="12">
         <v>0.9326388888888889</v>
@@ -4352,8 +5659,14 @@
       <c r="C53" t="n" s="8">
         <v>52.0</v>
       </c>
+      <c r="D53" t="s" s="7">
+        <v>130</v>
+      </c>
+      <c r="E53" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F53" t="s" s="110">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G53" t="n" s="9">
         <v>3.0</v>
@@ -4376,11 +5689,17 @@
       <c r="M53" t="n" s="12">
         <v>0.96875</v>
       </c>
+      <c r="N53" t="s" s="10">
+        <v>131</v>
+      </c>
       <c r="O53" t="n" s="12">
         <v>0.9270833333333334</v>
       </c>
       <c r="P53" t="n" s="12">
         <v>0.9409722222222222</v>
+      </c>
+      <c r="Q53" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R53" t="n" s="12">
         <v>0.9208333333333333</v>
@@ -4399,8 +5718,14 @@
       <c r="C54" t="n" s="8">
         <v>53.0</v>
       </c>
+      <c r="D54" t="s" s="7">
+        <v>132</v>
+      </c>
+      <c r="E54" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F54" t="s" s="112">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G54" t="n" s="9">
         <v>3.0</v>
@@ -4423,11 +5748,17 @@
       <c r="M54" t="n" s="12">
         <v>0.9756944444444444</v>
       </c>
+      <c r="N54" t="s" s="10">
+        <v>133</v>
+      </c>
       <c r="O54" t="n" s="12">
         <v>0.9194444444444444</v>
       </c>
       <c r="P54" t="n" s="12">
         <v>0.9513888888888888</v>
+      </c>
+      <c r="Q54" t="s" s="10">
+        <v>45</v>
       </c>
       <c r="R54" t="n" s="12">
         <v>0.9277777777777778</v>
@@ -4446,8 +5777,14 @@
       <c r="C55" t="n" s="8">
         <v>54.0</v>
       </c>
+      <c r="D55" t="s" s="7">
+        <v>134</v>
+      </c>
+      <c r="E55" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F55" t="s" s="114">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G55" t="n" s="9">
         <v>6.0</v>
@@ -4470,11 +5807,17 @@
       <c r="M55" t="n" s="12">
         <v>0.9979166666666667</v>
       </c>
+      <c r="N55" t="s" s="10">
+        <v>55</v>
+      </c>
       <c r="O55" t="n" s="12">
         <v>0.9020833333333333</v>
       </c>
       <c r="P55" t="n" s="12">
         <v>0.9340277777777778</v>
+      </c>
+      <c r="Q55" t="s" s="10">
+        <v>67</v>
       </c>
       <c r="R55" t="n" s="12">
         <v>0.9333333333333333</v>
@@ -4493,8 +5836,14 @@
       <c r="C56" t="n" s="8">
         <v>56.0</v>
       </c>
+      <c r="D56" t="s" s="7">
+        <v>135</v>
+      </c>
+      <c r="E56" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F56" t="s" s="116">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G56" t="n" s="9">
         <v>5.0</v>
@@ -4517,11 +5866,17 @@
       <c r="M56" t="n" s="12">
         <v>0.9805555555555555</v>
       </c>
+      <c r="N56" t="s" s="10">
+        <v>136</v>
+      </c>
       <c r="O56" t="n" s="12">
         <v>0.9305555555555556</v>
       </c>
       <c r="P56" t="n" s="12">
         <v>0.9430555555555555</v>
+      </c>
+      <c r="Q56" t="s" s="10">
+        <v>24</v>
       </c>
       <c r="R56" t="n" s="12">
         <v>0.9243055555555556</v>
@@ -4540,8 +5895,14 @@
       <c r="C57" t="n" s="8">
         <v>57.0</v>
       </c>
+      <c r="D57" t="s" s="7">
+        <v>137</v>
+      </c>
+      <c r="E57" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F57" t="s" s="118">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G57" t="n" s="9">
         <v>1.0</v>
@@ -4564,11 +5925,17 @@
       <c r="M57" t="n" s="12">
         <v>0.9756944444444444</v>
       </c>
+      <c r="N57" t="s" s="10">
+        <v>88</v>
+      </c>
       <c r="O57" t="n" s="12">
         <v>0.9131944444444444</v>
       </c>
       <c r="P57" t="n" s="12">
         <v>0.9548611111111112</v>
+      </c>
+      <c r="Q57" t="s" s="10">
+        <v>138</v>
       </c>
       <c r="R57" t="n" s="12">
         <v>0.8923611111111112</v>
@@ -4587,8 +5954,14 @@
       <c r="C58" t="n" s="8">
         <v>58.0</v>
       </c>
+      <c r="D58" t="s" s="7">
+        <v>139</v>
+      </c>
+      <c r="E58" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F58" t="s" s="120">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="G58" t="n" s="9">
         <v>4.0</v>
@@ -4611,11 +5984,17 @@
       <c r="M58" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
+      <c r="N58" t="s" s="10">
+        <v>140</v>
+      </c>
       <c r="O58" t="n" s="12">
         <v>0.9027777777777778</v>
       </c>
       <c r="P58" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q58" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R58" t="n" s="12">
         <v>0.9027777777777778</v>
@@ -4634,8 +6013,14 @@
       <c r="C59" t="n" s="8">
         <v>59.0</v>
       </c>
+      <c r="D59" t="s" s="7">
+        <v>141</v>
+      </c>
+      <c r="E59" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F59" t="s" s="122">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G59" t="n" s="9">
         <v>7.0</v>
@@ -4658,11 +6043,17 @@
       <c r="M59" t="n" s="12">
         <v>0.9784722222222222</v>
       </c>
+      <c r="N59" t="s" s="10">
+        <v>28</v>
+      </c>
       <c r="O59" t="n" s="12">
         <v>0.9243055555555556</v>
       </c>
       <c r="P59" t="n" s="12">
         <v>0.94375</v>
+      </c>
+      <c r="Q59" t="s" s="10">
+        <v>46</v>
       </c>
       <c r="R59" t="n" s="12">
         <v>0.9201388888888888</v>
@@ -4681,8 +6072,14 @@
       <c r="C60" t="n" s="8">
         <v>60.0</v>
       </c>
+      <c r="D60" t="s" s="7">
+        <v>142</v>
+      </c>
+      <c r="E60" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F60" t="s" s="124">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G60" t="n" s="9">
         <v>6.0</v>
@@ -4705,11 +6102,17 @@
       <c r="M60" t="n" s="12">
         <v>0.9833333333333333</v>
       </c>
+      <c r="N60" t="s" s="10">
+        <v>143</v>
+      </c>
       <c r="O60" t="n" s="12">
         <v>0.9083333333333333</v>
       </c>
       <c r="P60" t="n" s="12">
         <v>0.9458333333333333</v>
+      </c>
+      <c r="Q60" t="s" s="10">
+        <v>61</v>
       </c>
       <c r="R60" t="n" s="12">
         <v>0.9208333333333333</v>
@@ -4728,8 +6131,14 @@
       <c r="C61" t="n" s="8">
         <v>62.0</v>
       </c>
+      <c r="D61" t="s" s="7">
+        <v>144</v>
+      </c>
+      <c r="E61" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F61" t="s" s="126">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G61" t="n" s="9">
         <v>7.0</v>
@@ -4752,11 +6161,17 @@
       <c r="M61" t="n" s="12">
         <v>0.9881944444444445</v>
       </c>
+      <c r="N61" t="s" s="10">
+        <v>145</v>
+      </c>
       <c r="O61" t="n" s="12">
         <v>0.9055555555555556</v>
       </c>
       <c r="P61" t="n" s="12">
         <v>0.9409722222222222</v>
+      </c>
+      <c r="Q61" t="s" s="10">
+        <v>79</v>
       </c>
       <c r="R61" t="n" s="12">
         <v>0.9347222222222222</v>
@@ -4775,8 +6190,14 @@
       <c r="C62" t="n" s="8">
         <v>64.0</v>
       </c>
+      <c r="D62" t="s" s="7">
+        <v>146</v>
+      </c>
+      <c r="E62" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F62" t="s" s="128">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="G62" t="n" s="9">
         <v>1.0</v>
@@ -4799,11 +6220,17 @@
       <c r="M62" t="n" s="12">
         <v>0.9583333333333334</v>
       </c>
+      <c r="N62" t="s" s="10">
+        <v>147</v>
+      </c>
       <c r="O62" t="n" s="12">
         <v>0.8958333333333334</v>
       </c>
       <c r="P62" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q62" t="s" s="10">
+        <v>148</v>
       </c>
       <c r="R62" t="n" s="12">
         <v>0.875</v>
@@ -4822,8 +6249,14 @@
       <c r="C63" t="n" s="8">
         <v>65.0</v>
       </c>
+      <c r="D63" t="s" s="7">
+        <v>149</v>
+      </c>
+      <c r="E63" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F63" t="s" s="130">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G63" t="n" s="9">
         <v>2.0</v>
@@ -4846,11 +6279,17 @@
       <c r="M63" t="n" s="12">
         <v>0.9458333333333333</v>
       </c>
+      <c r="N63" t="s" s="10">
+        <v>150</v>
+      </c>
       <c r="O63" t="n" s="12">
         <v>0.9125</v>
       </c>
       <c r="P63" t="n" s="12">
         <v>0.9291666666666667</v>
+      </c>
+      <c r="Q63" t="s" s="10">
+        <v>45</v>
       </c>
       <c r="R63" t="n" s="12">
         <v>0.9125</v>
@@ -4869,8 +6308,14 @@
       <c r="C64" t="n" s="8">
         <v>67.0</v>
       </c>
+      <c r="D64" t="s" s="7">
+        <v>151</v>
+      </c>
+      <c r="E64" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F64" t="s" s="132">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="G64" t="n" s="9">
         <v>1.0</v>
@@ -4893,11 +6338,17 @@
       <c r="M64" t="n" s="12">
         <v>0.9326388888888889</v>
       </c>
+      <c r="N64" t="s" s="10">
+        <v>152</v>
+      </c>
       <c r="O64" t="n" s="12">
         <v>0.8854166666666666</v>
       </c>
       <c r="P64" t="n" s="12">
         <v>0.9166666666666666</v>
+      </c>
+      <c r="Q64" t="s" s="10">
+        <v>138</v>
       </c>
       <c r="R64" t="n" s="12">
         <v>0.8701388888888889</v>
@@ -4916,8 +6367,14 @@
       <c r="C65" t="n" s="8">
         <v>68.0</v>
       </c>
+      <c r="D65" t="s" s="7">
+        <v>153</v>
+      </c>
+      <c r="E65" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F65" t="s" s="134">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G65" t="n" s="9">
         <v>3.0</v>
@@ -4940,11 +6397,17 @@
       <c r="M65" t="n" s="12">
         <v>0.9625</v>
       </c>
+      <c r="N65" t="s" s="10">
+        <v>154</v>
+      </c>
       <c r="O65" t="n" s="12">
         <v>0.9215277777777777</v>
       </c>
       <c r="P65" t="n" s="12">
         <v>0.9451388888888889</v>
+      </c>
+      <c r="Q65" t="s" s="10">
+        <v>45</v>
       </c>
       <c r="R65" t="n" s="12">
         <v>0.9270833333333334</v>
@@ -4963,8 +6426,14 @@
       <c r="C66" t="n" s="8">
         <v>70.0</v>
       </c>
+      <c r="D66" t="s" s="7">
+        <v>155</v>
+      </c>
+      <c r="E66" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F66" t="s" s="136">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G66" t="n" s="9">
         <v>7.0</v>
@@ -4987,11 +6456,17 @@
       <c r="M66" t="n" s="12">
         <v>0.9868055555555556</v>
       </c>
+      <c r="N66" t="s" s="10">
+        <v>156</v>
+      </c>
       <c r="O66" t="n" s="12">
         <v>0.9236111111111112</v>
       </c>
       <c r="P66" t="n" s="12">
         <v>0.9479166666666666</v>
+      </c>
+      <c r="Q66" t="s" s="10">
+        <v>61</v>
       </c>
       <c r="R66" t="n" s="12">
         <v>0.9263888888888889</v>
@@ -5010,8 +6485,14 @@
       <c r="C67" t="n" s="8">
         <v>71.0</v>
       </c>
+      <c r="D67" t="s" s="7">
+        <v>157</v>
+      </c>
+      <c r="E67" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F67" t="s" s="138">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G67" t="n" s="9">
         <v>9.0</v>
@@ -5034,11 +6515,17 @@
       <c r="M67" t="n" s="12">
         <v>0.9881944444444445</v>
       </c>
+      <c r="N67" t="s" s="10">
+        <v>105</v>
+      </c>
       <c r="O67" t="n" s="12">
         <v>0.9138888888888889</v>
       </c>
       <c r="P67" t="n" s="12">
         <v>0.9430555555555555</v>
+      </c>
+      <c r="Q67" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R67" t="n" s="12">
         <v>0.9201388888888888</v>
@@ -5057,8 +6544,14 @@
       <c r="C68" t="n" s="8">
         <v>72.0</v>
       </c>
+      <c r="D68" t="s" s="7">
+        <v>158</v>
+      </c>
+      <c r="E68" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F68" t="s" s="140">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G68" t="n" s="9">
         <v>6.0</v>
@@ -5081,11 +6574,17 @@
       <c r="M68" t="n" s="12">
         <v>0.9708333333333333</v>
       </c>
+      <c r="N68" t="s" s="10">
+        <v>159</v>
+      </c>
       <c r="O68" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
       <c r="P68" t="n" s="12">
         <v>0.9381944444444444</v>
+      </c>
+      <c r="Q68" t="s" s="10">
+        <v>160</v>
       </c>
       <c r="R68" t="n" s="12">
         <v>0.9277777777777778</v>
@@ -5104,8 +6603,14 @@
       <c r="C69" t="n" s="8">
         <v>73.0</v>
       </c>
+      <c r="D69" t="s" s="7">
+        <v>161</v>
+      </c>
+      <c r="E69" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F69" t="s" s="142">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G69" t="n" s="9">
         <v>3.0</v>
@@ -5128,11 +6633,17 @@
       <c r="M69" t="n" s="12">
         <v>0.9625</v>
       </c>
+      <c r="N69" t="s" s="10">
+        <v>129</v>
+      </c>
       <c r="O69" t="n" s="12">
         <v>0.9333333333333333</v>
       </c>
       <c r="P69" t="n" s="12">
         <v>0.9430555555555555</v>
+      </c>
+      <c r="Q69" t="s" s="10">
+        <v>30</v>
       </c>
       <c r="R69" t="n" s="12">
         <v>0.9284722222222223</v>
@@ -5151,8 +6662,14 @@
       <c r="C70" t="n" s="8">
         <v>74.0</v>
       </c>
+      <c r="D70" t="s" s="7">
+        <v>162</v>
+      </c>
+      <c r="E70" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F70" t="s" s="144">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G70" t="n" s="9">
         <v>1.0</v>
@@ -5175,11 +6692,17 @@
       <c r="M70" t="n" s="12">
         <v>0.9375</v>
       </c>
+      <c r="N70" t="s" s="10">
+        <v>163</v>
+      </c>
       <c r="O70" t="n" s="12">
         <v>0.8541666666666666</v>
       </c>
       <c r="P70" t="n" s="12">
         <v>0.8958333333333334</v>
+      </c>
+      <c r="Q70" t="s" s="10">
+        <v>164</v>
       </c>
       <c r="R70" t="n" s="12">
         <v>0.875</v>
@@ -5198,8 +6721,14 @@
       <c r="C71" t="n" s="8">
         <v>75.0</v>
       </c>
+      <c r="D71" t="s" s="7">
+        <v>165</v>
+      </c>
+      <c r="E71" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F71" t="s" s="146">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G71" t="n" s="9">
         <v>2.0</v>
@@ -5222,11 +6751,17 @@
       <c r="M71" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
+      <c r="N71" t="s" s="10">
+        <v>145</v>
+      </c>
       <c r="O71" t="n" s="12">
         <v>0.9305555555555556</v>
       </c>
       <c r="P71" t="n" s="12">
         <v>0.9513888888888888</v>
+      </c>
+      <c r="Q71" t="s" s="10">
+        <v>164</v>
       </c>
       <c r="R71" t="n" s="12">
         <v>0.9305555555555556</v>
@@ -5245,8 +6780,14 @@
       <c r="C72" t="n" s="8">
         <v>77.0</v>
       </c>
+      <c r="D72" t="s" s="7">
+        <v>166</v>
+      </c>
+      <c r="E72" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F72" t="s" s="148">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G72" t="n" s="9">
         <v>1.0</v>
@@ -5269,11 +6810,17 @@
       <c r="M72" t="n" s="12">
         <v>0.9618055555555556</v>
       </c>
+      <c r="N72" t="s" s="10">
+        <v>167</v>
+      </c>
       <c r="O72" t="n" s="12">
         <v>0.9097222222222222</v>
       </c>
       <c r="P72" t="n" s="12">
         <v>0.9444444444444444</v>
+      </c>
+      <c r="Q72" t="s" s="10">
+        <v>45</v>
       </c>
       <c r="R72" t="n" s="12">
         <v>0.8923611111111112</v>
@@ -5292,8 +6839,14 @@
       <c r="C73" t="n" s="8">
         <v>78.0</v>
       </c>
+      <c r="D73" t="s" s="7">
+        <v>168</v>
+      </c>
+      <c r="E73" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F73" t="s" s="150">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G73" t="n" s="9">
         <v>4.0</v>
@@ -5316,11 +6869,17 @@
       <c r="M73" t="n" s="12">
         <v>0.9583333333333334</v>
       </c>
+      <c r="N73" t="s" s="10">
+        <v>169</v>
+      </c>
       <c r="O73" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
       <c r="P73" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q73" t="s" s="10">
+        <v>45</v>
       </c>
       <c r="R73" t="n" s="12">
         <v>0.9166666666666666</v>
@@ -5339,8 +6898,14 @@
       <c r="C74" t="n" s="8">
         <v>79.0</v>
       </c>
+      <c r="D74" t="s" s="7">
+        <v>170</v>
+      </c>
+      <c r="E74" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F74" t="s" s="152">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G74" t="n" s="9">
         <v>2.0</v>
@@ -5363,11 +6928,17 @@
       <c r="M74" t="n" s="12">
         <v>0.9583333333333334</v>
       </c>
+      <c r="N74" t="s" s="10">
+        <v>171</v>
+      </c>
       <c r="O74" t="n" s="12">
         <v>0.9361111111111111</v>
       </c>
       <c r="P74" t="n" s="12">
         <v>0.9472222222222222</v>
+      </c>
+      <c r="Q74" t="s" s="10">
+        <v>30</v>
       </c>
       <c r="R74" t="n" s="12">
         <v>0.9361111111111111</v>
@@ -5386,6 +6957,12 @@
       <c r="C75" t="n" s="8">
         <v>80.0</v>
       </c>
+      <c r="D75" t="s" s="7">
+        <v>172</v>
+      </c>
+      <c r="E75" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F75" t="s" s="153">
         <v>20</v>
       </c>
@@ -5410,11 +6987,17 @@
       <c r="M75" t="n" s="12">
         <v>0.9604166666666667</v>
       </c>
+      <c r="N75" t="s" s="10">
+        <v>88</v>
+      </c>
       <c r="O75" t="n" s="12">
         <v>0.8854166666666666</v>
       </c>
       <c r="P75" t="n" s="12">
         <v>0.9340277777777778</v>
+      </c>
+      <c r="Q75" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R75" t="n" s="12">
         <v>0.8631944444444445</v>
@@ -5433,8 +7016,14 @@
       <c r="C76" t="n" s="8">
         <v>81.0</v>
       </c>
+      <c r="D76" t="s" s="7">
+        <v>173</v>
+      </c>
+      <c r="E76" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F76" t="s" s="155">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="G76" t="n" s="9">
         <v>1.0</v>
@@ -5457,11 +7046,17 @@
       <c r="M76" t="n" s="12">
         <v>0.9055555555555556</v>
       </c>
+      <c r="N76" t="s" s="10">
+        <v>174</v>
+      </c>
       <c r="O76" t="n" s="12">
         <v>0.8118055555555556</v>
       </c>
       <c r="P76" t="n" s="12">
         <v>0.8743055555555556</v>
+      </c>
+      <c r="Q76" t="s" s="10">
+        <v>175</v>
       </c>
       <c r="R76" t="n" s="12">
         <v>0.7805555555555556</v>
@@ -5480,8 +7075,14 @@
       <c r="C77" t="n" s="8">
         <v>82.0</v>
       </c>
+      <c r="D77" t="s" s="7">
+        <v>176</v>
+      </c>
+      <c r="E77" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F77" t="s" s="157">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="G77" t="n" s="9">
         <v>2.0</v>
@@ -5504,11 +7105,17 @@
       <c r="M77" t="n" s="12">
         <v>0.9270833333333334</v>
       </c>
+      <c r="N77" t="s" s="10">
+        <v>36</v>
+      </c>
       <c r="O77" t="n" s="12">
         <v>0.84375</v>
       </c>
       <c r="P77" t="n" s="12">
         <v>0.8854166666666666</v>
+      </c>
+      <c r="Q77" t="s" s="10">
+        <v>37</v>
       </c>
       <c r="R77" t="n" s="12">
         <v>0.8020833333333334</v>
@@ -5527,8 +7134,14 @@
       <c r="C78" t="n" s="8">
         <v>84.0</v>
       </c>
+      <c r="D78" t="s" s="7">
+        <v>177</v>
+      </c>
+      <c r="E78" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F78" t="s" s="159">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G78" t="n" s="9">
         <v>4.0</v>
@@ -5551,11 +7164,17 @@
       <c r="M78" t="n" s="12">
         <v>0.9840277777777777</v>
       </c>
+      <c r="N78" t="s" s="10">
+        <v>178</v>
+      </c>
       <c r="O78" t="n" s="12">
         <v>0.9041666666666667</v>
       </c>
       <c r="P78" t="n" s="12">
         <v>0.9416666666666667</v>
+      </c>
+      <c r="Q78" t="s" s="10">
+        <v>45</v>
       </c>
       <c r="R78" t="n" s="12">
         <v>0.9090277777777778</v>
@@ -5574,8 +7193,14 @@
       <c r="C79" t="n" s="8">
         <v>86.0</v>
       </c>
+      <c r="D79" t="s" s="7">
+        <v>179</v>
+      </c>
+      <c r="E79" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F79" t="s" s="161">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G79" t="n" s="9">
         <v>8.0</v>
@@ -5598,11 +7223,17 @@
       <c r="M79" t="n" s="12">
         <v>0.9840277777777777</v>
       </c>
+      <c r="N79" t="s" s="10">
+        <v>171</v>
+      </c>
       <c r="O79" t="n" s="12">
         <v>0.8951388888888889</v>
       </c>
       <c r="P79" t="n" s="12">
         <v>0.9395833333333333</v>
+      </c>
+      <c r="Q79" t="s" s="10">
+        <v>45</v>
       </c>
       <c r="R79" t="n" s="12">
         <v>0.9173611111111111</v>
@@ -5621,8 +7252,14 @@
       <c r="C80" t="n" s="8">
         <v>87.0</v>
       </c>
+      <c r="D80" t="s" s="7">
+        <v>180</v>
+      </c>
+      <c r="E80" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F80" t="s" s="163">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G80" t="n" s="9">
         <v>3.0</v>
@@ -5645,11 +7282,17 @@
       <c r="M80" t="n" s="12">
         <v>0.98125</v>
       </c>
+      <c r="N80" t="s" s="10">
+        <v>28</v>
+      </c>
       <c r="O80" t="n" s="12">
         <v>0.9083333333333333</v>
       </c>
       <c r="P80" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q80" t="s" s="10">
+        <v>103</v>
       </c>
       <c r="R80" t="s" s="12">
         <v>20</v>
@@ -5668,8 +7311,14 @@
       <c r="C81" t="n" s="8">
         <v>88.0</v>
       </c>
+      <c r="D81" t="s" s="7">
+        <v>181</v>
+      </c>
+      <c r="E81" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F81" t="s" s="165">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G81" t="n" s="9">
         <v>10.0</v>
@@ -5692,11 +7341,17 @@
       <c r="M81" t="n" s="12">
         <v>0.9805555555555555</v>
       </c>
+      <c r="N81" t="s" s="10">
+        <v>182</v>
+      </c>
       <c r="O81" t="n" s="12">
         <v>0.9111111111111111</v>
       </c>
       <c r="P81" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q81" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R81" t="n" s="12">
         <v>0.9291666666666667</v>
@@ -5715,8 +7370,14 @@
       <c r="C82" t="n" s="8">
         <v>89.0</v>
       </c>
+      <c r="D82" t="s" s="7">
+        <v>183</v>
+      </c>
+      <c r="E82" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F82" t="s" s="167">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G82" t="n" s="9">
         <v>2.0</v>
@@ -5739,11 +7400,17 @@
       <c r="M82" t="n" s="12">
         <v>0.9583333333333334</v>
       </c>
+      <c r="N82" t="s" s="10">
+        <v>184</v>
+      </c>
       <c r="O82" t="n" s="12">
         <v>0.9090277777777778</v>
       </c>
       <c r="P82" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q82" t="s" s="10">
+        <v>185</v>
       </c>
       <c r="R82" t="n" s="12">
         <v>0.9083333333333333</v>
@@ -5762,8 +7429,14 @@
       <c r="C83" t="n" s="8">
         <v>90.0</v>
       </c>
+      <c r="D83" t="s" s="7">
+        <v>186</v>
+      </c>
+      <c r="E83" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F83" t="s" s="169">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G83" t="n" s="9">
         <v>5.0</v>
@@ -5786,11 +7459,17 @@
       <c r="M83" t="n" s="12">
         <v>0.9729166666666667</v>
       </c>
+      <c r="N83" t="s" s="10">
+        <v>187</v>
+      </c>
       <c r="O83" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
       <c r="P83" t="n" s="12">
         <v>0.9479166666666666</v>
+      </c>
+      <c r="Q83" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R83" t="n" s="12">
         <v>0.9229166666666667</v>
@@ -5809,8 +7488,14 @@
       <c r="C84" t="n" s="8">
         <v>91.0</v>
       </c>
+      <c r="D84" t="s" s="7">
+        <v>188</v>
+      </c>
+      <c r="E84" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F84" t="s" s="171">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="G84" t="n" s="9">
         <v>3.0</v>
@@ -5833,11 +7518,17 @@
       <c r="M84" t="n" s="12">
         <v>0.9666666666666667</v>
       </c>
+      <c r="N84" t="s" s="10">
+        <v>121</v>
+      </c>
       <c r="O84" t="n" s="12">
         <v>0.9020833333333333</v>
       </c>
       <c r="P84" t="n" s="12">
         <v>0.9388888888888889</v>
+      </c>
+      <c r="Q84" t="s" s="10">
+        <v>189</v>
       </c>
       <c r="R84" t="n" s="12">
         <v>0.9111111111111111</v>
@@ -5856,8 +7547,14 @@
       <c r="C85" t="n" s="8">
         <v>92.0</v>
       </c>
+      <c r="D85" t="s" s="7">
+        <v>190</v>
+      </c>
+      <c r="E85" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F85" t="s" s="173">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="G85" t="n" s="9">
         <v>5.0</v>
@@ -5880,11 +7577,17 @@
       <c r="M85" t="n" s="12">
         <v>0.9791666666666666</v>
       </c>
+      <c r="N85" t="s" s="10">
+        <v>45</v>
+      </c>
       <c r="O85" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
       <c r="P85" t="n" s="12">
         <v>0.9416666666666667</v>
+      </c>
+      <c r="Q85" t="s" s="10">
+        <v>67</v>
       </c>
       <c r="R85" t="n" s="12">
         <v>0.9229166666666667</v>
@@ -5903,8 +7606,14 @@
       <c r="C86" t="n" s="8">
         <v>94.0</v>
       </c>
+      <c r="D86" t="s" s="7">
+        <v>191</v>
+      </c>
+      <c r="E86" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F86" t="s" s="175">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G86" t="n" s="9">
         <v>4.0</v>
@@ -5927,11 +7636,17 @@
       <c r="M86" t="n" s="12">
         <v>0.9645833333333333</v>
       </c>
+      <c r="N86" t="s" s="10">
+        <v>145</v>
+      </c>
       <c r="O86" t="n" s="12">
         <v>0.9173611111111111</v>
       </c>
       <c r="P86" t="n" s="12">
         <v>0.9409722222222222</v>
+      </c>
+      <c r="Q86" t="s" s="10">
+        <v>192</v>
       </c>
       <c r="R86" t="n" s="12">
         <v>0.9173611111111111</v>
@@ -5950,8 +7665,14 @@
       <c r="C87" t="n" s="8">
         <v>95.0</v>
       </c>
+      <c r="D87" t="s" s="7">
+        <v>193</v>
+      </c>
+      <c r="E87" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F87" t="s" s="177">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G87" t="n" s="9">
         <v>7.0</v>
@@ -5974,11 +7695,17 @@
       <c r="M87" t="n" s="12">
         <v>0.9958333333333333</v>
       </c>
+      <c r="N87" t="s" s="10">
+        <v>171</v>
+      </c>
       <c r="O87" t="n" s="12">
         <v>0.8965277777777778</v>
       </c>
       <c r="P87" t="n" s="12">
         <v>0.9388888888888889</v>
+      </c>
+      <c r="Q87" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R87" t="n" s="12">
         <v>0.9173611111111111</v>
@@ -5997,8 +7724,14 @@
       <c r="C88" t="n" s="8">
         <v>99.0</v>
       </c>
+      <c r="D88" t="s" s="7">
+        <v>194</v>
+      </c>
+      <c r="E88" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F88" t="s" s="179">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G88" t="n" s="9">
         <v>4.0</v>
@@ -6021,11 +7754,17 @@
       <c r="M88" t="n" s="12">
         <v>0.9652777777777778</v>
       </c>
+      <c r="N88" t="s" s="10">
+        <v>195</v>
+      </c>
       <c r="O88" t="n" s="12">
         <v>0.9236111111111112</v>
       </c>
       <c r="P88" t="n" s="12">
         <v>0.9444444444444444</v>
+      </c>
+      <c r="Q88" t="s" s="10">
+        <v>37</v>
       </c>
       <c r="R88" t="n" s="12">
         <v>0.9236111111111112</v>
@@ -6044,8 +7783,14 @@
       <c r="C89" t="n" s="8">
         <v>101.0</v>
       </c>
+      <c r="D89" t="s" s="7">
+        <v>196</v>
+      </c>
+      <c r="E89" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F89" t="s" s="181">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="G89" t="n" s="9">
         <v>5.0</v>
@@ -6068,11 +7813,17 @@
       <c r="M89" t="n" s="12">
         <v>1.0006944444444446</v>
       </c>
+      <c r="N89" t="s" s="10">
+        <v>197</v>
+      </c>
       <c r="O89" t="n" s="12">
         <v>0.9159722222222222</v>
       </c>
       <c r="P89" t="n" s="12">
         <v>0.9534722222222223</v>
+      </c>
+      <c r="Q89" t="s" s="10">
+        <v>105</v>
       </c>
       <c r="R89" t="n" s="12">
         <v>0.9069444444444444</v>
@@ -6091,8 +7842,14 @@
       <c r="C90" t="n" s="8">
         <v>102.0</v>
       </c>
+      <c r="D90" t="s" s="7">
+        <v>198</v>
+      </c>
+      <c r="E90" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F90" t="s" s="183">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="G90" t="n" s="9">
         <v>5.0</v>
@@ -6115,11 +7872,17 @@
       <c r="M90" t="n" s="12">
         <v>0.9958333333333333</v>
       </c>
+      <c r="N90" t="s" s="10">
+        <v>199</v>
+      </c>
       <c r="O90" t="n" s="12">
         <v>0.9055555555555556</v>
       </c>
       <c r="P90" t="n" s="12">
         <v>0.9416666666666667</v>
+      </c>
+      <c r="Q90" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R90" t="n" s="12">
         <v>0.9145833333333333</v>
@@ -6138,8 +7901,14 @@
       <c r="C91" t="n" s="8">
         <v>103.0</v>
       </c>
+      <c r="D91" t="s" s="7">
+        <v>200</v>
+      </c>
+      <c r="E91" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F91" t="s" s="185">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G91" t="n" s="9">
         <v>3.0</v>
@@ -6162,11 +7931,17 @@
       <c r="M91" t="n" s="12">
         <v>0.9701388888888889</v>
       </c>
+      <c r="N91" t="s" s="10">
+        <v>201</v>
+      </c>
       <c r="O91" t="n" s="12">
         <v>0.9020833333333333</v>
       </c>
       <c r="P91" t="n" s="12">
         <v>0.9298611111111111</v>
+      </c>
+      <c r="Q91" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R91" t="n" s="12">
         <v>0.8611111111111112</v>
@@ -6185,8 +7960,14 @@
       <c r="C92" t="n" s="8">
         <v>104.0</v>
       </c>
+      <c r="D92" t="s" s="7">
+        <v>202</v>
+      </c>
+      <c r="E92" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F92" t="s" s="187">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G92" t="n" s="9">
         <v>2.0</v>
@@ -6209,11 +7990,17 @@
       <c r="M92" t="n" s="12">
         <v>0.9479166666666666</v>
       </c>
+      <c r="N92" t="s" s="10">
+        <v>203</v>
+      </c>
       <c r="O92" t="n" s="12">
         <v>0.8993055555555556</v>
       </c>
       <c r="P92" t="n" s="12">
         <v>0.9236111111111112</v>
+      </c>
+      <c r="Q92" t="s" s="10">
+        <v>42</v>
       </c>
       <c r="R92" t="n" s="12">
         <v>0.875</v>
@@ -6232,8 +8019,14 @@
       <c r="C93" t="n" s="8">
         <v>106.0</v>
       </c>
+      <c r="D93" t="s" s="7">
+        <v>204</v>
+      </c>
+      <c r="E93" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F93" t="s" s="189">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G93" t="n" s="9">
         <v>4.0</v>
@@ -6256,11 +8049,17 @@
       <c r="M93" t="n" s="12">
         <v>0.9861111111111112</v>
       </c>
+      <c r="N93" t="s" s="10">
+        <v>28</v>
+      </c>
       <c r="O93" t="n" s="12">
         <v>0.8756944444444444</v>
       </c>
       <c r="P93" t="n" s="12">
         <v>0.9104166666666667</v>
+      </c>
+      <c r="Q93" t="s" s="10">
+        <v>205</v>
       </c>
       <c r="R93" t="n" s="12">
         <v>0.9027777777777778</v>
@@ -6279,8 +8078,14 @@
       <c r="C94" t="n" s="8">
         <v>107.0</v>
       </c>
+      <c r="D94" t="s" s="7">
+        <v>206</v>
+      </c>
+      <c r="E94" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F94" t="s" s="191">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G94" t="n" s="9">
         <v>1.0</v>
@@ -6303,11 +8108,17 @@
       <c r="M94" t="n" s="12">
         <v>0.9826388888888888</v>
       </c>
+      <c r="N94" t="s" s="10">
+        <v>84</v>
+      </c>
       <c r="O94" t="n" s="12">
         <v>0.8680555555555556</v>
       </c>
       <c r="P94" t="n" s="12">
         <v>0.9444444444444444</v>
+      </c>
+      <c r="Q94" t="s" s="10">
+        <v>37</v>
       </c>
       <c r="R94" t="n" s="12">
         <v>0.8298611111111112</v>
@@ -6326,8 +8137,14 @@
       <c r="C95" t="n" s="8">
         <v>108.0</v>
       </c>
+      <c r="D95" t="s" s="7">
+        <v>207</v>
+      </c>
+      <c r="E95" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F95" t="s" s="193">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G95" t="n" s="9">
         <v>4.0</v>
@@ -6350,11 +8167,17 @@
       <c r="M95" t="n" s="12">
         <v>0.9861111111111112</v>
       </c>
+      <c r="N95" t="s" s="10">
+        <v>208</v>
+      </c>
       <c r="O95" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
       <c r="P95" t="n" s="12">
         <v>0.9340277777777778</v>
+      </c>
+      <c r="Q95" t="s" s="10">
+        <v>30</v>
       </c>
       <c r="R95" t="n" s="12">
         <v>0.9173611111111111</v>
@@ -6373,8 +8196,14 @@
       <c r="C96" t="n" s="8">
         <v>109.0</v>
       </c>
+      <c r="D96" t="s" s="7">
+        <v>209</v>
+      </c>
+      <c r="E96" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F96" t="s" s="195">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="G96" t="n" s="9">
         <v>1.0</v>
@@ -6397,11 +8226,17 @@
       <c r="M96" t="n" s="12">
         <v>0.9666666666666667</v>
       </c>
+      <c r="N96" t="s" s="10">
+        <v>41</v>
+      </c>
       <c r="O96" t="n" s="12">
         <v>0.8958333333333334</v>
       </c>
       <c r="P96" t="n" s="12">
         <v>0.9444444444444444</v>
+      </c>
+      <c r="Q96" t="s" s="10">
+        <v>42</v>
       </c>
       <c r="R96" t="n" s="12">
         <v>0.8694444444444445</v>
@@ -6420,8 +8255,14 @@
       <c r="C97" t="n" s="8">
         <v>110.0</v>
       </c>
+      <c r="D97" t="s" s="7">
+        <v>210</v>
+      </c>
+      <c r="E97" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F97" t="s" s="197">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G97" t="n" s="9">
         <v>2.0</v>
@@ -6444,11 +8285,17 @@
       <c r="M97" t="n" s="12">
         <v>0.9583333333333334</v>
       </c>
+      <c r="N97" t="s" s="10">
+        <v>211</v>
+      </c>
       <c r="O97" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
       <c r="P97" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q97" t="s" s="10">
+        <v>61</v>
       </c>
       <c r="R97" t="n" s="12">
         <v>0.9166666666666666</v>
@@ -6467,8 +8314,14 @@
       <c r="C98" t="n" s="8">
         <v>112.0</v>
       </c>
+      <c r="D98" t="s" s="7">
+        <v>212</v>
+      </c>
+      <c r="E98" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F98" t="s" s="199">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G98" t="n" s="9">
         <v>3.0</v>
@@ -6491,11 +8344,17 @@
       <c r="M98" t="n" s="12">
         <v>0.9631944444444445</v>
       </c>
+      <c r="N98" t="s" s="10">
+        <v>213</v>
+      </c>
       <c r="O98" t="n" s="12">
         <v>0.89375</v>
       </c>
       <c r="P98" t="n" s="12">
         <v>0.9215277777777777</v>
+      </c>
+      <c r="Q98" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R98" t="n" s="12">
         <v>0.8541666666666666</v>
@@ -6514,8 +8373,14 @@
       <c r="C99" t="n" s="8">
         <v>121.0</v>
       </c>
+      <c r="D99" t="s" s="7">
+        <v>214</v>
+      </c>
+      <c r="E99" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F99" t="s" s="201">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G99" t="n" s="9">
         <v>5.0</v>
@@ -6538,11 +8403,17 @@
       <c r="M99" t="n" s="12">
         <v>0.9756944444444444</v>
       </c>
+      <c r="N99" t="s" s="10">
+        <v>50</v>
+      </c>
       <c r="O99" t="n" s="12">
         <v>0.925</v>
       </c>
       <c r="P99" t="n" s="12">
         <v>0.9472222222222222</v>
+      </c>
+      <c r="Q99" t="s" s="10">
+        <v>42</v>
       </c>
       <c r="R99" t="n" s="12">
         <v>0.93125</v>
@@ -6561,8 +8432,14 @@
       <c r="C100" t="n" s="8">
         <v>122.0</v>
       </c>
+      <c r="D100" t="s" s="7">
+        <v>215</v>
+      </c>
+      <c r="E100" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F100" t="s" s="203">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G100" t="n" s="9">
         <v>2.0</v>
@@ -6585,11 +8462,17 @@
       <c r="M100" t="n" s="12">
         <v>0.9479166666666666</v>
       </c>
+      <c r="N100" t="s" s="10">
+        <v>216</v>
+      </c>
       <c r="O100" t="n" s="12">
         <v>0.8993055555555556</v>
       </c>
       <c r="P100" t="n" s="12">
         <v>0.9236111111111112</v>
+      </c>
+      <c r="Q100" t="s" s="10">
+        <v>45</v>
       </c>
       <c r="R100" t="n" s="12">
         <v>0.8986111111111111</v>
@@ -6608,8 +8491,14 @@
       <c r="C101" t="n" s="8">
         <v>124.0</v>
       </c>
+      <c r="D101" t="s" s="7">
+        <v>217</v>
+      </c>
+      <c r="E101" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F101" t="s" s="205">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G101" t="n" s="9">
         <v>3.0</v>
@@ -6632,11 +8521,17 @@
       <c r="M101" t="n" s="12">
         <v>0.9770833333333333</v>
       </c>
+      <c r="N101" t="s" s="10">
+        <v>218</v>
+      </c>
       <c r="O101" t="n" s="12">
         <v>0.9131944444444444</v>
       </c>
       <c r="P101" t="n" s="12">
         <v>0.9291666666666667</v>
+      </c>
+      <c r="Q101" t="s" s="10">
+        <v>219</v>
       </c>
       <c r="R101" t="n" s="12">
         <v>0.9368055555555556</v>
@@ -6655,8 +8550,14 @@
       <c r="C102" t="n" s="8">
         <v>150.0</v>
       </c>
+      <c r="D102" t="s" s="7">
+        <v>220</v>
+      </c>
+      <c r="E102" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F102" t="s" s="207">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G102" t="n" s="9">
         <v>10.0</v>
@@ -6679,11 +8580,17 @@
       <c r="M102" t="n" s="12">
         <v>0.9826388888888888</v>
       </c>
+      <c r="N102" t="s" s="10">
+        <v>28</v>
+      </c>
       <c r="O102" t="n" s="12">
         <v>0.9375</v>
       </c>
       <c r="P102" t="n" s="12">
         <v>0.9451388888888889</v>
+      </c>
+      <c r="Q102" t="s" s="10">
+        <v>67</v>
       </c>
       <c r="R102" t="n" s="12">
         <v>0.9215277777777777</v>
@@ -6702,8 +8609,14 @@
       <c r="C103" t="n" s="8">
         <v>301.0</v>
       </c>
+      <c r="D103" t="s" s="7">
+        <v>221</v>
+      </c>
+      <c r="E103" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F103" t="s" s="209">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G103" t="n" s="9">
         <v>16.0</v>
@@ -6726,11 +8639,17 @@
       <c r="M103" t="n" s="12">
         <v>1.011111111111111</v>
       </c>
+      <c r="N103" t="s" s="10">
+        <v>160</v>
+      </c>
       <c r="O103" t="n" s="12">
         <v>0.9354166666666667</v>
       </c>
       <c r="P103" t="n" s="12">
         <v>0.9451388888888889</v>
+      </c>
+      <c r="Q103" t="s" s="10">
+        <v>39</v>
       </c>
       <c r="R103" t="n" s="12">
         <v>0.9305555555555556</v>
@@ -6749,8 +8668,14 @@
       <c r="C104" t="n" s="8">
         <v>321.0</v>
       </c>
+      <c r="D104" t="s" s="7">
+        <v>222</v>
+      </c>
+      <c r="E104" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F104" t="s" s="211">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G104" t="n" s="9">
         <v>4.0</v>
@@ -6773,11 +8698,17 @@
       <c r="M104" t="n" s="12">
         <v>0.9652777777777778</v>
       </c>
+      <c r="N104" t="s" s="10">
+        <v>55</v>
+      </c>
       <c r="O104" t="n" s="12">
         <v>0.9305555555555556</v>
       </c>
       <c r="P104" t="n" s="12">
         <v>0.9444444444444444</v>
+      </c>
+      <c r="Q104" t="s" s="10">
+        <v>164</v>
       </c>
       <c r="R104" t="n" s="12">
         <v>0.9236111111111112</v>
@@ -6796,8 +8727,14 @@
       <c r="C105" t="n" s="8">
         <v>332.0</v>
       </c>
+      <c r="D105" t="s" s="7">
+        <v>223</v>
+      </c>
+      <c r="E105" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F105" t="s" s="213">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G105" t="n" s="9">
         <v>8.0</v>
@@ -6820,11 +8757,17 @@
       <c r="M105" t="n" s="12">
         <v>0.9861111111111112</v>
       </c>
+      <c r="N105" t="s" s="10">
+        <v>182</v>
+      </c>
       <c r="O105" t="n" s="12">
         <v>0.9305555555555556</v>
       </c>
       <c r="P105" t="n" s="12">
         <v>0.9444444444444444</v>
+      </c>
+      <c r="Q105" t="s" s="10">
+        <v>45</v>
       </c>
       <c r="R105" t="n" s="12">
         <v>0.9305555555555556</v>
@@ -6843,8 +8786,14 @@
       <c r="C106" t="n" s="8">
         <v>334.0</v>
       </c>
+      <c r="D106" t="s" s="7">
+        <v>224</v>
+      </c>
+      <c r="E106" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F106" t="s" s="215">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G106" t="n" s="9">
         <v>8.0</v>
@@ -6867,11 +8816,17 @@
       <c r="M106" t="n" s="12">
         <v>0.9729166666666667</v>
       </c>
+      <c r="N106" t="s" s="10">
+        <v>36</v>
+      </c>
       <c r="O106" t="n" s="12">
         <v>0.9256944444444445</v>
       </c>
       <c r="P106" t="n" s="12">
         <v>0.9375</v>
+      </c>
+      <c r="Q106" t="s" s="10">
+        <v>37</v>
       </c>
       <c r="R106" t="n" s="12">
         <v>0.9256944444444445</v>
@@ -6890,8 +8845,14 @@
       <c r="C107" t="n" s="8">
         <v>339.0</v>
       </c>
+      <c r="D107" t="s" s="7">
+        <v>225</v>
+      </c>
+      <c r="E107" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F107" t="s" s="217">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G107" t="n" s="9">
         <v>4.0</v>
@@ -6914,11 +8875,17 @@
       <c r="M107" t="n" s="12">
         <v>0.9673611111111111</v>
       </c>
+      <c r="N107" t="s" s="10">
+        <v>71</v>
+      </c>
       <c r="O107" t="n" s="12">
         <v>0.9430555555555555</v>
       </c>
       <c r="P107" t="n" s="12">
         <v>0.9479166666666666</v>
+      </c>
+      <c r="Q107" t="s" s="10">
+        <v>103</v>
       </c>
       <c r="R107" t="s" s="12">
         <v>20</v>
@@ -6937,8 +8904,14 @@
       <c r="C108" t="n" s="8">
         <v>343.0</v>
       </c>
+      <c r="D108" t="s" s="7">
+        <v>226</v>
+      </c>
+      <c r="E108" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F108" t="s" s="219">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G108" t="n" s="9">
         <v>9.0</v>
@@ -6961,11 +8934,17 @@
       <c r="M108" t="n" s="12">
         <v>0.9916666666666667</v>
       </c>
+      <c r="N108" t="s" s="10">
+        <v>74</v>
+      </c>
       <c r="O108" t="n" s="12">
         <v>0.9291666666666667</v>
       </c>
       <c r="P108" t="n" s="12">
         <v>0.9395833333333333</v>
+      </c>
+      <c r="Q108" t="s" s="10">
+        <v>227</v>
       </c>
       <c r="R108" t="n" s="12">
         <v>0.9340277777777778</v>
@@ -6984,8 +8963,14 @@
       <c r="C109" t="n" s="8">
         <v>344.0</v>
       </c>
+      <c r="D109" t="s" s="7">
+        <v>228</v>
+      </c>
+      <c r="E109" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F109" t="s" s="221">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G109" t="n" s="9">
         <v>9.0</v>
@@ -7008,11 +8993,17 @@
       <c r="M109" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
+      <c r="N109" t="s" s="10">
+        <v>28</v>
+      </c>
       <c r="O109" t="n" s="12">
         <v>0.9347222222222222</v>
       </c>
       <c r="P109" t="n" s="12">
         <v>0.9416666666666667</v>
+      </c>
+      <c r="Q109" t="s" s="10">
+        <v>227</v>
       </c>
       <c r="R109" t="n" s="12">
         <v>0.9305555555555556</v>
@@ -7031,8 +9022,14 @@
       <c r="C110" t="n" s="8">
         <v>345.0</v>
       </c>
+      <c r="D110" t="s" s="7">
+        <v>229</v>
+      </c>
+      <c r="E110" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F110" t="s" s="223">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G110" t="n" s="9">
         <v>15.0</v>
@@ -7055,11 +9052,17 @@
       <c r="M110" t="n" s="12">
         <v>0.9930555555555556</v>
       </c>
+      <c r="N110" t="s" s="10">
+        <v>230</v>
+      </c>
       <c r="O110" t="n" s="12">
         <v>0.9305555555555556</v>
       </c>
       <c r="P110" t="n" s="12">
         <v>0.9409722222222222</v>
+      </c>
+      <c r="Q110" t="s" s="10">
+        <v>46</v>
       </c>
       <c r="R110" t="n" s="12">
         <v>0.9305555555555556</v>
@@ -7078,8 +9081,14 @@
       <c r="C111" t="n" s="8">
         <v>346.0</v>
       </c>
+      <c r="D111" t="s" s="7">
+        <v>231</v>
+      </c>
+      <c r="E111" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F111" t="s" s="225">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G111" t="n" s="9">
         <v>10.0</v>
@@ -7102,11 +9111,17 @@
       <c r="M111" t="n" s="12">
         <v>0.9868055555555556</v>
       </c>
+      <c r="N111" t="s" s="10">
+        <v>230</v>
+      </c>
       <c r="O111" t="n" s="12">
         <v>0.9326388888888889</v>
       </c>
       <c r="P111" t="n" s="12">
         <v>0.9416666666666667</v>
+      </c>
+      <c r="Q111" t="s" s="10">
+        <v>232</v>
       </c>
       <c r="R111" t="n" s="12">
         <v>0.9326388888888889</v>
@@ -7125,8 +9140,14 @@
       <c r="C112" t="n" s="8">
         <v>363.0</v>
       </c>
+      <c r="D112" t="s" s="7">
+        <v>233</v>
+      </c>
+      <c r="E112" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F112" t="s" s="227">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G112" t="n" s="9">
         <v>8.0</v>
@@ -7149,11 +9170,17 @@
       <c r="M112" t="n" s="12">
         <v>0.9777777777777777</v>
       </c>
+      <c r="N112" t="s" s="10">
+        <v>234</v>
+      </c>
       <c r="O112" t="n" s="12">
         <v>0.9263888888888889</v>
       </c>
       <c r="P112" t="n" s="12">
         <v>0.9388888888888889</v>
+      </c>
+      <c r="Q112" t="s" s="10">
+        <v>67</v>
       </c>
       <c r="R112" t="n" s="12">
         <v>0.9263888888888889</v>
@@ -7172,8 +9199,14 @@
       <c r="C113" t="n" s="8">
         <v>383.0</v>
       </c>
+      <c r="D113" t="s" s="7">
+        <v>235</v>
+      </c>
+      <c r="E113" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F113" t="s" s="229">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G113" t="n" s="9">
         <v>8.0</v>
@@ -7196,11 +9229,17 @@
       <c r="M113" t="n" s="12">
         <v>0.9784722222222222</v>
       </c>
+      <c r="N113" t="s" s="10">
+        <v>185</v>
+      </c>
       <c r="O113" t="n" s="12">
         <v>0.9333333333333333</v>
       </c>
       <c r="P113" t="n" s="12">
         <v>0.9423611111111111</v>
+      </c>
+      <c r="Q113" t="s" s="10">
+        <v>28</v>
       </c>
       <c r="R113" t="n" s="12">
         <v>0.9326388888888889</v>
@@ -7219,8 +9258,14 @@
       <c r="C114" t="n" s="8">
         <v>385.0</v>
       </c>
+      <c r="D114" t="s" s="7">
+        <v>236</v>
+      </c>
+      <c r="E114" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F114" t="s" s="231">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G114" t="n" s="9">
         <v>3.0</v>
@@ -7243,11 +9288,17 @@
       <c r="M114" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
+      <c r="N114" t="s" s="10">
+        <v>237</v>
+      </c>
       <c r="O114" t="n" s="12">
         <v>0.9333333333333333</v>
       </c>
       <c r="P114" t="n" s="12">
         <v>0.9430555555555555</v>
+      </c>
+      <c r="Q114" t="s" s="10">
+        <v>103</v>
       </c>
       <c r="R114" t="s" s="12">
         <v>20</v>
@@ -7266,8 +9317,14 @@
       <c r="C115" t="n" s="8">
         <v>387.0</v>
       </c>
+      <c r="D115" t="s" s="7">
+        <v>238</v>
+      </c>
+      <c r="E115" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="F115" t="s" s="233">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G115" t="n" s="9">
         <v>4.0</v>
@@ -7290,11 +9347,17 @@
       <c r="M115" t="n" s="12">
         <v>0.9701388888888889</v>
       </c>
+      <c r="N115" t="s" s="10">
+        <v>239</v>
+      </c>
       <c r="O115" t="n" s="12">
         <v>0.9298611111111111</v>
       </c>
       <c r="P115" t="n" s="12">
         <v>0.9402777777777778</v>
+      </c>
+      <c r="Q115" t="s" s="10">
+        <v>103</v>
       </c>
       <c r="R115" t="s" s="12">
         <v>20</v>

</xml_diff>

<commit_message>
Starting working on Excel Fomr classes
</commit_message>
<xml_diff>
--- a/downloads/მარაბდა.xlsx
+++ b/downloads/მარაბდა.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="241">
   <si>
     <t xml:space="preserve">მარშრუტის. № </t>
   </si>
@@ -77,10 +77,20 @@
     <t>გასვლები "B" პუნქტიდან</t>
   </si>
   <si>
+    <t>როსტომ აბრამიშვილის ქ. #1-3 კორპუსის  მიმდებარედ (მოედანთან) - როსტომ აბრამიშვილის ქ. -  ლილოს დასახლება (ჭირნახულის ქ. - მეფრინველეთა ქ. - თენზიგ სტურუას ქ. - ზურაბ ნამორაძის ქ. - ევგენი აფხაზავას II შესახვევი - ევგენი აფხაზავას ქ. - ჭირნახულის ქ.) - ივანე იუმაშევის ქ. - კახეთის გზატკეცილი - ჯავახეთის ქ. - მოსკოვის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - ქეთევან დედოფლის გამზირი - მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ). 
+უკუმიმართულებით: მ/ს 'ისანი'(ქეთევან დედოფლის გამზირი #67'ა'-ს მოპირდაპირედ)  - ვაჟა ჩაჩავას ქ. - აწყურის ქ. - კახეთის I შესახვევი - ქეთევან დედოფლის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - მოსკოვის გამზირი - ჯავახეთის ქ. - კახეთის გზატკეცილი - ივანე იუმაშევის ქ. - ლილოს დასახლება (ჭირნახულის ქ. - ევგენი აფხაზავას ქ. - ევგენი აფხაზავას II შესახვევი - ევგენი აფხაზავას IV შესახვევი -  ევგენი აფხაზავას ქ. - თენზიგ სტურუას ქ. - მეფრინველეთა ქ. - ჭირნახულის ქ. ) - როსტომ აბრამიშვილის ქ. - როსტომ აბრამიშვილის ქ. #1-3 კორპუსის  მიმდებარედ (მოედანთან))</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
     <t>MAN A-47</t>
+  </si>
+  <si>
+    <t> ლილო-ლოჭინი</t>
+  </si>
+  <si>
+    <t>მ/ს ისანი</t>
   </si>
   <si>
     <t>ქიზიყის ქ. (#5 კორპუსის მიმდებარედ) - ქიზიყის ქ. - პოლიციის ქ. - აბელ ენუქიძის ქ. - ბესარიონ ჭიჭინაძის ქ. - გუმათჰესის ქ. - ქინძმარაულის ქ. - მოსკოვის გამზირი - მ/ს 'სამგორი' (ქვედა გასასვლელი) - ქეთევან დედოფლის გამზირი - ნიკოლოზ ბარათაშვილის აღმართი – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. (გაჩერება „კონკის“ მხარეს).
@@ -155,6 +165,13 @@
     <t>ვაკე-ბაგები</t>
   </si>
   <si>
+    <t xml:space="preserve">დაბა კოჯორი (ვაჟა ფშაველას ქ. #33-ის მიმდებარედ) - დაბა კოჯორი (ვაჟა ფშაველას ქ. - ალექსანდრე ჩხეიძის ქ. (მობრუნება ალექსანდრე ჩხეიძის ქ. #16-თან) - გრიგოლ ორბელიანის ქ. - ამაღლების ქ. - ზაქარია ბაქრაძის ქ. - იუნკერთა ქ.) - თბილისი-კოჯრის ქ. (სოფ. ტაბახმელას, სოფ. შინდისის, სოფელი წავკისის, წავკისის ველის გავლით) - კოჯრის გზატკეცილი - მარო მაყაშვილის აღმართი - მარო მაყაშვილის ქ. - ამაღლების ქ. - ლადო ასათიანის შესახვევი - ლადო ასათიანის ქ. - შალვა დადიანის ქ. - თავისუფლების მოედანი -ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).
+უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – გიორგი ლეონიძის ქ. – მიხეილ ლერმონტოვის ქ. – პაოლო იაშვილის ქ. – ამაღლების ქ. – მარო მაყაშვილის ქ. – მარო მაყაშვილის აღმართი –  კოჯრის გზატკეცილი -  თბილისი-კოჯრის ქ. (წავკისის ველის, სოფ. წავკისის, სოფ. შინდისის, სოფ. ტაბახმელას გავლით) - დაბა კოჯორი (იუნკერთა ქ. - ზაქარია ბაქრაძის ქ. -  ამაღლების ქ. - გრიგოლ ორბელიანის ქ. - ალექსანდრე ჩხეიძის ქ. (მობრუნება ალექსანდრე ჩხეიძის ქ. #16-თან) - ვაჟა ფშაველას ქ. - აზეულას ქ. (მობრუნება ნიკო კეცხოველის ქუჩის გადაკვეთასთან) - ვჟა ფშაველას ქ. - ვაჟა ფშაველას ქ.#33-ის მიმდებარედ). </t>
+  </si>
+  <si>
+    <t>კოჯორი </t>
+  </si>
+  <si>
     <t xml:space="preserve">დაბა ზაჰესის დასახლება (ავჭალის ქ., ბენზინ გასამართი სადგურის მიმდებარე ტერიტორია) - ავჭალის ქ. - ელეფთერ ანდრონიკაშვილის ქ. - უწერის ქ. - ლიბანის ქ. - დავით სარაჯიშვილის ქ. - დავით გურამიშვილის გამზირი - თორნიკე ერისთავის ქ. - აკაკი წერეთლის გამზირი - აკაკი წერეთლის გამზირი #2-ის მიმდებარედ (ბორის პაიჭაძის სახ. ეროვნული სტადიონი)
 უკუმიმართულებით:  აკაკი წერეთლის გამზირი #2-ის მიმდებარედ (ბორის პაიჭაძის სახ. ეროვნული სტადიონი) - აკაკი წერეთლის გამზირი (მობრუნება გიორგი ცაბაძის ქუჩის გადაკვეთასთან) - შემდეგ იგივე სქემით. </t>
   </si>
@@ -170,9 +187,6 @@
   </si>
   <si>
     <t>დიდი ლილო</t>
-  </si>
-  <si>
-    <t>მ/ს ისანი</t>
   </si>
   <si>
     <t xml:space="preserve">დიდი დიღმის IV მ/რაიონი, კორპუსი #6-ის მიმდებარედ (დემეტრე თავდადებულის ქ.) - დიდი დიღომი  IV მ/რაიონი (დემეტრე თავდადებულის ქ. - არჩილ მეფის ქ.) - დიდი დიღმის III მ/რაიონი (მირიან მეფის ქ.) - პეტრე იბერის ქ. - იოანე პეტრიწის ქ. - ფარნავაზ მეფის გამზირი - დავით აღმაშენებლის ხეივანი  - მარშალ გელოვანის გამზირი - იური გაგარინის ქ. - ზურაბ ჟვანიას მოედანი - სიმონ კანდელაკის ქ. - ჟიული შარტავას ქ. - გიორგი სააკაძის მოედანი - მერაბ კოსტავას ქ. - გიორგი მიროტაძის ქ. - პეკინის გამზირი - მერაბ კოსტავას ქ. - ვარაზისხევის ქ. - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი -  თავისუფლების მოედანი-ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).                                                                                                                                                                                              უკუმიმართულებით:  ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – შოთა რუსთაველის გამზირი – მერაბ კოსტავას ქ. – გმირთა მოედანი – მერაბ კოსტავას ქ. – გიორგი სააკაძის მოედანი – ჟიული შარტავას ქუჩა -  შემდეგ იგივე სქემით. </t>
@@ -689,6 +703,13 @@
   </si>
   <si>
     <t>სოფელი დიღომი</t>
+  </si>
+  <si>
+    <t>დაბა კიკეთი - თბილისი-კოჯრის გზა (სოფ. დიდება, დაბა კოჯორი, სოფ. ტაბახმელა, სოფ. შინდისი, სოფ. წავკისი, წავკისის ველის გავლით) - კოჯრის გზატკეცილი - მარო მაყაშვილის აღმართი - მარო მაყაშვილის ქ. - ამაღლების ქ. - ლადო ასათიანის შესახვევი - ლადო ასათიანის ქ. - შალვა დადიანის ქ. - თავისუფლების მოედანი -ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ)
+უკუმიმართულებით:  ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – გიორგი ლეონიძის ქ. – მიხეილ ლერმონტოვის ქ. – პაოლო იაშვილის ქ. – ამაღლების ქ. – მარო მაყაშვილის ქ. – მარო მაყაშვილის აღმართი – კოჯრის გზატკეცილი – შემდეგ არსებული სქემით.</t>
+  </si>
+  <si>
+    <t>კიკეთი</t>
   </si>
   <si>
     <t>სოფ. ლისი - სოფ. თხინვალი - ახალი იპოდრომი -  ნუცუბიძის IV-II მ/რ - ჟღენტის ქ. - ნუცუბიძის ქ. - თავაძის ქ. - ზაქარიაძის ქ. - ვაჟა ფშაველას ჩიხი - მ/ს 'დელისი' (მიმდებარედ) 
@@ -2811,12 +2832,14 @@
       <c r="B5" t="n" s="6">
         <v>1.0</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" t="s" s="6">
+        <v>21</v>
+      </c>
       <c r="D5" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s" s="13">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" t="n" s="8">
         <v>8.0</v>
@@ -2845,14 +2868,18 @@
       <c r="N5" t="n" s="11">
         <v>0.9930555555555556</v>
       </c>
-      <c r="O5" s="9"/>
+      <c r="O5" t="s" s="9">
+        <v>24</v>
+      </c>
       <c r="P5" t="n" s="11">
         <v>0.925</v>
       </c>
       <c r="Q5" t="n" s="11">
         <v>0.9423611111111111</v>
       </c>
-      <c r="R5" s="9"/>
+      <c r="R5" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="S5" t="n" s="11">
         <v>0.9236111111111112</v>
       </c>
@@ -2860,7 +2887,7 @@
         <v>0.9409722222222222</v>
       </c>
       <c r="U5" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" ht="30.0" customHeight="true">
@@ -2871,13 +2898,13 @@
         <v>2.0</v>
       </c>
       <c r="C6" t="s" s="6">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s" s="15">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F6" t="n" s="8">
         <v>11.0</v>
@@ -2907,7 +2934,7 @@
         <v>1.007638888888889</v>
       </c>
       <c r="O6" t="s" s="9">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P6" t="n" s="11">
         <v>0.9340277777777778</v>
@@ -2916,7 +2943,7 @@
         <v>0.9409722222222222</v>
       </c>
       <c r="R6" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S6" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -2925,7 +2952,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="U6" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" ht="30.0" customHeight="true">
@@ -2936,13 +2963,13 @@
         <v>2.0</v>
       </c>
       <c r="C7" t="s" s="6">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s" s="17">
         <v>27</v>
-      </c>
-      <c r="D7" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s" s="17">
-        <v>24</v>
       </c>
       <c r="F7" t="n" s="8">
         <v>6.0</v>
@@ -2972,7 +2999,7 @@
         <v>0.9826388888888888</v>
       </c>
       <c r="O7" t="s" s="9">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P7" t="n" s="11">
         <v>0.9180555555555555</v>
@@ -2981,7 +3008,7 @@
         <v>0.9402777777777778</v>
       </c>
       <c r="R7" t="s" s="9">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="S7" t="n" s="11">
         <v>0.9180555555555555</v>
@@ -2990,7 +3017,7 @@
         <v>0.9402777777777778</v>
       </c>
       <c r="U7" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" ht="30.0" customHeight="true">
@@ -3001,13 +3028,13 @@
         <v>1.0</v>
       </c>
       <c r="C8" t="s" s="6">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s" s="19">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F8" t="n" s="8">
         <v>3.0</v>
@@ -3037,7 +3064,7 @@
         <v>0.9951388888888889</v>
       </c>
       <c r="O8" t="s" s="9">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="P8" t="n" s="11">
         <v>0.9145833333333333</v>
@@ -3046,7 +3073,7 @@
         <v>0.9423611111111111</v>
       </c>
       <c r="R8" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S8" t="n" s="11">
         <v>0.875</v>
@@ -3055,7 +3082,7 @@
         <v>0.9027777777777778</v>
       </c>
       <c r="U8" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" ht="30.0" customHeight="true">
@@ -3066,13 +3093,13 @@
         <v>1.0</v>
       </c>
       <c r="C9" t="s" s="6">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s" s="21">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F9" t="n" s="8">
         <v>2.0</v>
@@ -3102,7 +3129,7 @@
         <v>0.9770833333333333</v>
       </c>
       <c r="O9" t="s" s="9">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="P9" t="n" s="11">
         <v>0.875</v>
@@ -3111,7 +3138,7 @@
         <v>0.9166666666666666</v>
       </c>
       <c r="R9" t="s" s="9">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="S9" t="n" s="11">
         <v>0.8333333333333334</v>
@@ -3120,7 +3147,7 @@
         <v>0.875</v>
       </c>
       <c r="U9" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" ht="30.0" customHeight="true">
@@ -3131,13 +3158,13 @@
         <v>2.0</v>
       </c>
       <c r="C10" t="s" s="6">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s" s="23">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F10" t="n" s="8">
         <v>7.0</v>
@@ -3167,7 +3194,7 @@
         <v>1.0229166666666667</v>
       </c>
       <c r="O10" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="P10" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -3176,7 +3203,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="R10" t="s" s="9">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="S10" t="n" s="11">
         <v>0.9215277777777777</v>
@@ -3185,7 +3212,7 @@
         <v>0.9493055555555555</v>
       </c>
       <c r="U10" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" ht="30.0" customHeight="true">
@@ -3196,13 +3223,13 @@
         <v>3.0</v>
       </c>
       <c r="C11" t="s" s="6">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s" s="25">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F11" t="n" s="8">
         <v>3.0</v>
@@ -3232,7 +3259,7 @@
         <v>0.9770833333333333</v>
       </c>
       <c r="O11" t="s" s="9">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P11" t="n" s="11">
         <v>0.9375</v>
@@ -3241,7 +3268,7 @@
         <v>0.9513888888888888</v>
       </c>
       <c r="R11" t="s" s="9">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="S11" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -3250,7 +3277,7 @@
         <v>0.9340277777777778</v>
       </c>
       <c r="U11" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" ht="30.0" customHeight="true">
@@ -3261,13 +3288,13 @@
         <v>2.0</v>
       </c>
       <c r="C12" t="s" s="6">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s" s="27">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F12" t="n" s="8">
         <v>5.0</v>
@@ -3297,7 +3324,7 @@
         <v>0.9868055555555556</v>
       </c>
       <c r="O12" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="P12" t="n" s="11">
         <v>0.9215277777777777</v>
@@ -3306,7 +3333,7 @@
         <v>0.9423611111111111</v>
       </c>
       <c r="R12" t="s" s="9">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="S12" t="n" s="11">
         <v>0.9270833333333334</v>
@@ -3315,7 +3342,7 @@
         <v>0.9479166666666666</v>
       </c>
       <c r="U12" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" ht="30.0" customHeight="true">
@@ -3325,12 +3352,14 @@
       <c r="B13" t="n" s="6">
         <v>3.0</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" t="s" s="6">
+        <v>48</v>
+      </c>
       <c r="D13" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s" s="29">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F13" t="n" s="8">
         <v>4.0</v>
@@ -3359,14 +3388,18 @@
       <c r="N13" t="n" s="11">
         <v>1.0263888888888888</v>
       </c>
-      <c r="O13" s="9"/>
+      <c r="O13" t="s" s="9">
+        <v>49</v>
+      </c>
       <c r="P13" t="n" s="11">
         <v>0.9097222222222222</v>
       </c>
       <c r="Q13" t="n" s="11">
         <v>0.9368055555555556</v>
       </c>
-      <c r="R13" s="9"/>
+      <c r="R13" t="s" s="9">
+        <v>29</v>
+      </c>
       <c r="S13" t="n" s="11">
         <v>0.8840277777777777</v>
       </c>
@@ -3374,7 +3407,7 @@
         <v>0.9375</v>
       </c>
       <c r="U13" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" ht="30.0" customHeight="true">
@@ -3385,13 +3418,13 @@
         <v>2.0</v>
       </c>
       <c r="C14" t="s" s="6">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s" s="31">
         <v>45</v>
-      </c>
-      <c r="D14" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s" s="31">
-        <v>42</v>
       </c>
       <c r="F14" t="n" s="8">
         <v>7.0</v>
@@ -3421,7 +3454,7 @@
         <v>1.00625</v>
       </c>
       <c r="O14" t="s" s="9">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="P14" t="n" s="11">
         <v>0.9236111111111112</v>
@@ -3430,7 +3463,7 @@
         <v>0.9486111111111111</v>
       </c>
       <c r="R14" t="s" s="9">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="S14" t="n" s="11">
         <v>0.9173611111111111</v>
@@ -3439,7 +3472,7 @@
         <v>0.9423611111111111</v>
       </c>
       <c r="U14" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" ht="30.0" customHeight="true">
@@ -3450,13 +3483,13 @@
         <v>1.0</v>
       </c>
       <c r="C15" t="s" s="6">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s" s="33">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F15" t="n" s="8">
         <v>4.0</v>
@@ -3486,7 +3519,7 @@
         <v>1.0041666666666667</v>
       </c>
       <c r="O15" t="s" s="9">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P15" t="n" s="11">
         <v>0.8986111111111111</v>
@@ -3495,7 +3528,7 @@
         <v>0.9173611111111111</v>
       </c>
       <c r="R15" t="s" s="9">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="S15" t="n" s="11">
         <v>0.9347222222222222</v>
@@ -3504,7 +3537,7 @@
         <v>0.9534722222222223</v>
       </c>
       <c r="U15" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" ht="30.0" customHeight="true">
@@ -3515,13 +3548,13 @@
         <v>2.0</v>
       </c>
       <c r="C16" t="s" s="6">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s" s="35">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F16" t="n" s="8">
         <v>11.0</v>
@@ -3551,7 +3584,7 @@
         <v>1.0055555555555555</v>
       </c>
       <c r="O16" t="s" s="9">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="P16" t="n" s="11">
         <v>0.9055555555555556</v>
@@ -3560,7 +3593,7 @@
         <v>0.9416666666666667</v>
       </c>
       <c r="R16" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S16" t="n" s="11">
         <v>0.9368055555555556</v>
@@ -3569,7 +3602,7 @@
         <v>0.9458333333333333</v>
       </c>
       <c r="U16" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" ht="30.0" customHeight="true">
@@ -3580,13 +3613,13 @@
         <v>2.0</v>
       </c>
       <c r="C17" t="s" s="6">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s" s="37">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F17" t="n" s="8">
         <v>6.0</v>
@@ -3616,7 +3649,7 @@
         <v>0.9916666666666667</v>
       </c>
       <c r="O17" t="s" s="9">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="P17" t="n" s="11">
         <v>0.9097222222222222</v>
@@ -3625,7 +3658,7 @@
         <v>0.9375</v>
       </c>
       <c r="R17" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="S17" t="n" s="11">
         <v>0.9236111111111112</v>
@@ -3634,7 +3667,7 @@
         <v>0.9375</v>
       </c>
       <c r="U17" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" ht="30.0" customHeight="true">
@@ -3645,13 +3678,13 @@
         <v>3.0</v>
       </c>
       <c r="C18" t="s" s="6">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s" s="39">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F18" t="n" s="8">
         <v>1.0</v>
@@ -3681,7 +3714,7 @@
         <v>0.9215277777777777</v>
       </c>
       <c r="O18" t="s" s="9">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="P18" t="n" s="11">
         <v>0.8125</v>
@@ -3690,7 +3723,7 @@
         <v>0.8854166666666666</v>
       </c>
       <c r="R18" t="s" s="9">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="S18" t="n" s="11">
         <v>0.7708333333333334</v>
@@ -3699,7 +3732,7 @@
         <v>0.8541666666666666</v>
       </c>
       <c r="U18" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" ht="30.0" customHeight="true">
@@ -3710,13 +3743,13 @@
         <v>2.0</v>
       </c>
       <c r="C19" t="s" s="6">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E19" t="s" s="41">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F19" t="n" s="8">
         <v>7.0</v>
@@ -3746,7 +3779,7 @@
         <v>0.9902777777777778</v>
       </c>
       <c r="O19" t="s" s="9">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="P19" t="n" s="11">
         <v>0.90625</v>
@@ -3755,7 +3788,7 @@
         <v>0.9375</v>
       </c>
       <c r="R19" t="s" s="9">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="S19" t="n" s="11">
         <v>0.9201388888888888</v>
@@ -3764,7 +3797,7 @@
         <v>0.9409722222222222</v>
       </c>
       <c r="U19" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" ht="30.0" customHeight="true">
@@ -3775,13 +3808,13 @@
         <v>1.0</v>
       </c>
       <c r="C20" t="s" s="6">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s" s="43">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F20" t="n" s="8">
         <v>3.0</v>
@@ -3811,7 +3844,7 @@
         <v>0.9965277777777778</v>
       </c>
       <c r="O20" t="s" s="9">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="P20" t="n" s="11">
         <v>0.9027777777777778</v>
@@ -3820,7 +3853,7 @@
         <v>0.9305555555555556</v>
       </c>
       <c r="R20" t="s" s="9">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="S20" t="n" s="11">
         <v>0.8888888888888888</v>
@@ -3829,7 +3862,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="U20" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" ht="30.0" customHeight="true">
@@ -3840,13 +3873,13 @@
         <v>1.0</v>
       </c>
       <c r="C21" t="s" s="6">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D21" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E21" t="s" s="45">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F21" t="n" s="8">
         <v>10.0</v>
@@ -3876,7 +3909,7 @@
         <v>1.0083333333333333</v>
       </c>
       <c r="O21" t="s" s="9">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="P21" t="n" s="11">
         <v>0.9333333333333333</v>
@@ -3885,7 +3918,7 @@
         <v>0.9409722222222222</v>
       </c>
       <c r="R21" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S21" t="n" s="11">
         <v>0.9333333333333333</v>
@@ -3894,7 +3927,7 @@
         <v>0.9486111111111111</v>
       </c>
       <c r="U21" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" ht="30.0" customHeight="true">
@@ -3905,13 +3938,13 @@
         <v>2.0</v>
       </c>
       <c r="C22" t="s" s="6">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E22" t="s" s="47">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F22" t="n" s="8">
         <v>11.0</v>
@@ -3941,7 +3974,7 @@
         <v>1.0208333333333333</v>
       </c>
       <c r="O22" t="s" s="9">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="P22" t="n" s="11">
         <v>0.89375</v>
@@ -3950,7 +3983,7 @@
         <v>0.9409722222222222</v>
       </c>
       <c r="R22" t="s" s="9">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="S22" t="n" s="11">
         <v>0.9347222222222222</v>
@@ -3959,7 +3992,7 @@
         <v>0.9465277777777777</v>
       </c>
       <c r="U22" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" ht="30.0" customHeight="true">
@@ -3970,13 +4003,13 @@
         <v>1.0</v>
       </c>
       <c r="C23" t="s" s="6">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s" s="49">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F23" t="n" s="8">
         <v>3.0</v>
@@ -4006,7 +4039,7 @@
         <v>1.0013888888888889</v>
       </c>
       <c r="O23" t="s" s="9">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="P23" t="n" s="11">
         <v>0.875</v>
@@ -4015,7 +4048,7 @@
         <v>0.9027777777777778</v>
       </c>
       <c r="R23" t="s" s="9">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="S23" t="n" s="11">
         <v>0.9159722222222222</v>
@@ -4024,7 +4057,7 @@
         <v>0.94375</v>
       </c>
       <c r="U23" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" ht="30.0" customHeight="true">
@@ -4035,13 +4068,13 @@
         <v>2.0</v>
       </c>
       <c r="C24" t="s" s="6">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s" s="51">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F24" t="n" s="8">
         <v>9.0</v>
@@ -4071,7 +4104,7 @@
         <v>1.007638888888889</v>
       </c>
       <c r="O24" t="s" s="9">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="P24" t="n" s="11">
         <v>0.9152777777777777</v>
@@ -4080,7 +4113,7 @@
         <v>0.9458333333333333</v>
       </c>
       <c r="R24" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S24" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -4089,7 +4122,7 @@
         <v>0.9402777777777778</v>
       </c>
       <c r="U24" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" ht="30.0" customHeight="true">
@@ -4100,13 +4133,13 @@
         <v>2.0</v>
       </c>
       <c r="C25" t="s" s="6">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s" s="53">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F25" t="n" s="8">
         <v>10.0</v>
@@ -4136,7 +4169,7 @@
         <v>1.0131944444444445</v>
       </c>
       <c r="O25" t="s" s="9">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="P25" t="n" s="11">
         <v>0.9097222222222222</v>
@@ -4145,7 +4178,7 @@
         <v>0.9430555555555555</v>
       </c>
       <c r="R25" t="s" s="9">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="S25" t="n" s="11">
         <v>0.9319444444444445</v>
@@ -4154,7 +4187,7 @@
         <v>0.9430555555555555</v>
       </c>
       <c r="U25" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" ht="30.0" customHeight="true">
@@ -4165,13 +4198,13 @@
         <v>1.0</v>
       </c>
       <c r="C26" t="s" s="6">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E26" t="s" s="55">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F26" t="n" s="8">
         <v>8.0</v>
@@ -4201,7 +4234,7 @@
         <v>0.9881944444444445</v>
       </c>
       <c r="O26" t="s" s="9">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="P26" t="n" s="11">
         <v>0.9243055555555556</v>
@@ -4210,7 +4243,7 @@
         <v>0.9423611111111111</v>
       </c>
       <c r="R26" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S26" t="n" s="11">
         <v>0.9243055555555556</v>
@@ -4219,7 +4252,7 @@
         <v>0.9423611111111111</v>
       </c>
       <c r="U26" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" ht="30.0" customHeight="true">
@@ -4230,13 +4263,13 @@
         <v>3.0</v>
       </c>
       <c r="C27" t="s" s="6">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E27" t="s" s="57">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F27" t="n" s="8">
         <v>1.0</v>
@@ -4266,7 +4299,7 @@
         <v>0.91875</v>
       </c>
       <c r="O27" t="s" s="9">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P27" t="n" s="11">
         <v>0.8402777777777778</v>
@@ -4275,7 +4308,7 @@
         <v>0.8888888888888888</v>
       </c>
       <c r="R27" t="s" s="9">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="S27" t="n" s="11">
         <v>0.8159722222222222</v>
@@ -4284,7 +4317,7 @@
         <v>0.8645833333333334</v>
       </c>
       <c r="U27" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" ht="30.0" customHeight="true">
@@ -4295,13 +4328,13 @@
         <v>3.0</v>
       </c>
       <c r="C28" t="s" s="6">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D28" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E28" t="s" s="59">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F28" t="n" s="8">
         <v>6.0</v>
@@ -4331,7 +4364,7 @@
         <v>0.9854166666666667</v>
       </c>
       <c r="O28" t="s" s="9">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="P28" t="n" s="11">
         <v>0.9256944444444445</v>
@@ -4340,7 +4373,7 @@
         <v>0.9458333333333333</v>
       </c>
       <c r="R28" t="s" s="9">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="S28" t="n" s="11">
         <v>0.9347222222222222</v>
@@ -4349,7 +4382,7 @@
         <v>0.9451388888888889</v>
       </c>
       <c r="U28" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" ht="30.0" customHeight="true">
@@ -4360,13 +4393,13 @@
         <v>3.0</v>
       </c>
       <c r="C29" t="s" s="6">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D29" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E29" t="s" s="61">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F29" t="n" s="8">
         <v>4.0</v>
@@ -4396,7 +4429,7 @@
         <v>0.9805555555555555</v>
       </c>
       <c r="O29" t="s" s="9">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="P29" t="n" s="11">
         <v>0.9270833333333334</v>
@@ -4405,7 +4438,7 @@
         <v>0.9479166666666666</v>
       </c>
       <c r="R29" t="s" s="9">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="S29" t="n" s="11">
         <v>0.9270833333333334</v>
@@ -4414,7 +4447,7 @@
         <v>0.9479166666666666</v>
       </c>
       <c r="U29" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" ht="30.0" customHeight="true">
@@ -4425,13 +4458,13 @@
         <v>3.0</v>
       </c>
       <c r="C30" t="s" s="6">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D30" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E30" t="s" s="63">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F30" t="n" s="8">
         <v>3.0</v>
@@ -4461,7 +4494,7 @@
         <v>0.9902777777777778</v>
       </c>
       <c r="O30" t="s" s="9">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="P30" t="n" s="11">
         <v>0.8986111111111111</v>
@@ -4470,7 +4503,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="R30" t="s" s="9">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="S30" t="n" s="11">
         <v>0.9104166666666667</v>
@@ -4479,7 +4512,7 @@
         <v>0.9375</v>
       </c>
       <c r="U30" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" ht="30.0" customHeight="true">
@@ -4490,13 +4523,13 @@
         <v>1.0</v>
       </c>
       <c r="C31" t="s" s="6">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D31" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E31" t="s" s="65">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F31" t="n" s="8">
         <v>3.0</v>
@@ -4526,7 +4559,7 @@
         <v>0.98125</v>
       </c>
       <c r="O31" t="s" s="9">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P31" t="n" s="11">
         <v>0.90625</v>
@@ -4535,7 +4568,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="R31" t="s" s="9">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="S31" t="n" s="11">
         <v>0.9131944444444444</v>
@@ -4544,7 +4577,7 @@
         <v>0.9375</v>
       </c>
       <c r="U31" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" ht="30.0" customHeight="true">
@@ -4555,13 +4588,13 @@
         <v>1.0</v>
       </c>
       <c r="C32" t="s" s="6">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E32" t="s" s="67">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F32" t="n" s="8">
         <v>5.0</v>
@@ -4591,7 +4624,7 @@
         <v>0.9930555555555556</v>
       </c>
       <c r="O32" t="s" s="9">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="P32" t="n" s="11">
         <v>0.9138888888888889</v>
@@ -4600,7 +4633,7 @@
         <v>0.9416666666666667</v>
       </c>
       <c r="R32" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="S32" t="n" s="11">
         <v>0.91875</v>
@@ -4609,7 +4642,7 @@
         <v>0.9465277777777777</v>
       </c>
       <c r="U32" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" ht="30.0" customHeight="true">
@@ -4620,13 +4653,13 @@
         <v>2.0</v>
       </c>
       <c r="C33" t="s" s="6">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D33" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E33" t="s" s="69">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F33" t="n" s="8">
         <v>4.0</v>
@@ -4656,7 +4689,7 @@
         <v>0.9791666666666666</v>
       </c>
       <c r="O33" t="s" s="9">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="P33" t="n" s="11">
         <v>0.9215277777777777</v>
@@ -4665,7 +4698,7 @@
         <v>0.9375</v>
       </c>
       <c r="R33" t="s" s="9">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="S33" t="n" s="11">
         <v>0.90625</v>
@@ -4674,7 +4707,7 @@
         <v>0.9375</v>
       </c>
       <c r="U33" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" ht="30.0" customHeight="true">
@@ -4685,13 +4718,13 @@
         <v>2.0</v>
       </c>
       <c r="C34" t="s" s="6">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D34" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E34" t="s" s="71">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F34" t="n" s="8">
         <v>9.0</v>
@@ -4721,7 +4754,7 @@
         <v>1.0069444444444444</v>
       </c>
       <c r="O34" t="s" s="9">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="P34" t="n" s="11">
         <v>0.8951388888888889</v>
@@ -4730,7 +4763,7 @@
         <v>0.9395833333333333</v>
       </c>
       <c r="R34" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S34" t="n" s="11">
         <v>0.9340277777777778</v>
@@ -4739,7 +4772,7 @@
         <v>0.9451388888888889</v>
       </c>
       <c r="U34" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" ht="30.0" customHeight="true">
@@ -4750,13 +4783,13 @@
         <v>3.0</v>
       </c>
       <c r="C35" t="s" s="6">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D35" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E35" t="s" s="73">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F35" t="n" s="8">
         <v>9.0</v>
@@ -4786,7 +4819,7 @@
         <v>1.0138888888888888</v>
       </c>
       <c r="O35" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="P35" t="n" s="11">
         <v>0.9215277777777777</v>
@@ -4795,7 +4828,7 @@
         <v>0.9416666666666667</v>
       </c>
       <c r="R35" t="s" s="9">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="S35" t="n" s="11">
         <v>0.9263888888888889</v>
@@ -4804,7 +4837,7 @@
         <v>0.9465277777777777</v>
       </c>
       <c r="U35" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" ht="30.0" customHeight="true">
@@ -4815,13 +4848,13 @@
         <v>3.0</v>
       </c>
       <c r="C36" t="s" s="6">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D36" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E36" t="s" s="75">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F36" t="n" s="8">
         <v>1.0</v>
@@ -4851,7 +4884,7 @@
         <v>0.9513888888888888</v>
       </c>
       <c r="O36" t="s" s="9">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="P36" t="n" s="11">
         <v>0.8541666666666666</v>
@@ -4860,7 +4893,7 @@
         <v>0.8958333333333334</v>
       </c>
       <c r="R36" t="s" s="9">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="S36" t="n" s="11">
         <v>0.875</v>
@@ -4869,7 +4902,7 @@
         <v>0.9166666666666666</v>
       </c>
       <c r="U36" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" ht="30.0" customHeight="true">
@@ -4880,13 +4913,13 @@
         <v>3.0</v>
       </c>
       <c r="C37" t="s" s="6">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D37" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E37" t="s" s="77">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F37" t="n" s="8">
         <v>6.0</v>
@@ -4916,7 +4949,7 @@
         <v>0.9736111111111111</v>
       </c>
       <c r="O37" t="s" s="9">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="P37" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -4925,7 +4958,7 @@
         <v>0.9375</v>
       </c>
       <c r="R37" t="s" s="9">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="S37" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -4934,7 +4967,7 @@
         <v>0.9375</v>
       </c>
       <c r="U37" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" ht="30.0" customHeight="true">
@@ -4945,13 +4978,13 @@
         <v>2.0</v>
       </c>
       <c r="C38" t="s" s="6">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D38" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E38" t="s" s="79">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F38" t="n" s="8">
         <v>10.0</v>
@@ -4981,7 +5014,7 @@
         <v>1.023611111111111</v>
       </c>
       <c r="O38" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="P38" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -4990,7 +5023,7 @@
         <v>0.9375</v>
       </c>
       <c r="R38" t="s" s="9">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="S38" t="n" s="11">
         <v>0.9368055555555556</v>
@@ -4999,7 +5032,7 @@
         <v>0.9472222222222222</v>
       </c>
       <c r="U38" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" ht="30.0" customHeight="true">
@@ -5010,13 +5043,13 @@
         <v>2.0</v>
       </c>
       <c r="C39" t="s" s="6">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D39" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E39" t="s" s="81">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F39" t="n" s="8">
         <v>6.0</v>
@@ -5046,7 +5079,7 @@
         <v>0.9819444444444444</v>
       </c>
       <c r="O39" t="s" s="9">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="P39" t="n" s="11">
         <v>0.925</v>
@@ -5055,16 +5088,16 @@
         <v>0.9416666666666667</v>
       </c>
       <c r="R39" t="s" s="9">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="S39" t="s" s="11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T39" t="s" s="11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U39" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" ht="30.0" customHeight="true">
@@ -5075,13 +5108,13 @@
         <v>1.0</v>
       </c>
       <c r="C40" t="s" s="6">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D40" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E40" t="s" s="83">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F40" t="n" s="8">
         <v>10.0</v>
@@ -5111,7 +5144,7 @@
         <v>0.9826388888888888</v>
       </c>
       <c r="O40" t="s" s="9">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="P40" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -5120,7 +5153,7 @@
         <v>0.9375</v>
       </c>
       <c r="R40" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S40" t="n" s="11">
         <v>0.9243055555555556</v>
@@ -5129,7 +5162,7 @@
         <v>0.9381944444444444</v>
       </c>
       <c r="U40" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" ht="30.0" customHeight="true">
@@ -5140,13 +5173,13 @@
         <v>1.0</v>
       </c>
       <c r="C41" t="s" s="6">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D41" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E41" t="s" s="85">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F41" t="n" s="8">
         <v>3.0</v>
@@ -5176,7 +5209,7 @@
         <v>0.9791666666666666</v>
       </c>
       <c r="O41" t="s" s="9">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="P41" t="n" s="11">
         <v>0.9097222222222222</v>
@@ -5185,7 +5218,7 @@
         <v>0.9430555555555555</v>
       </c>
       <c r="R41" t="s" s="9">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="S41" t="n" s="11">
         <v>0.9180555555555555</v>
@@ -5194,7 +5227,7 @@
         <v>0.9340277777777778</v>
       </c>
       <c r="U41" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" ht="30.0" customHeight="true">
@@ -5205,13 +5238,13 @@
         <v>1.0</v>
       </c>
       <c r="C42" t="s" s="6">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D42" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E42" t="s" s="87">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F42" t="n" s="8">
         <v>3.0</v>
@@ -5241,7 +5274,7 @@
         <v>1.0069444444444444</v>
       </c>
       <c r="O42" t="s" s="9">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="P42" t="n" s="11">
         <v>0.9097222222222222</v>
@@ -5250,7 +5283,7 @@
         <v>0.9375</v>
       </c>
       <c r="R42" t="s" s="9">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="S42" t="n" s="11">
         <v>0.9222222222222223</v>
@@ -5259,7 +5292,7 @@
         <v>0.95</v>
       </c>
       <c r="U42" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" ht="30.0" customHeight="true">
@@ -5270,13 +5303,13 @@
         <v>3.0</v>
       </c>
       <c r="C43" t="s" s="6">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D43" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E43" t="s" s="89">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F43" t="n" s="8">
         <v>4.0</v>
@@ -5306,7 +5339,7 @@
         <v>0.9902777777777778</v>
       </c>
       <c r="O43" t="s" s="9">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="P43" t="n" s="11">
         <v>0.9208333333333333</v>
@@ -5315,7 +5348,7 @@
         <v>0.9465277777777777</v>
       </c>
       <c r="R43" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S43" t="n" s="11">
         <v>0.9340277777777778</v>
@@ -5324,7 +5357,7 @@
         <v>0.9472222222222222</v>
       </c>
       <c r="U43" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" ht="30.0" customHeight="true">
@@ -5335,13 +5368,13 @@
         <v>1.0</v>
       </c>
       <c r="C44" t="s" s="6">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D44" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E44" t="s" s="91">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F44" t="n" s="8">
         <v>3.0</v>
@@ -5371,7 +5404,7 @@
         <v>0.975</v>
       </c>
       <c r="O44" t="s" s="9">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="P44" t="n" s="11">
         <v>0.8854166666666666</v>
@@ -5380,7 +5413,7 @@
         <v>0.9270833333333334</v>
       </c>
       <c r="R44" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S44" t="n" s="11">
         <v>0.90625</v>
@@ -5389,7 +5422,7 @@
         <v>0.9479166666666666</v>
       </c>
       <c r="U44" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" ht="30.0" customHeight="true">
@@ -5400,13 +5433,13 @@
         <v>3.0</v>
       </c>
       <c r="C45" t="s" s="6">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D45" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E45" t="s" s="93">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F45" t="n" s="8">
         <v>2.0</v>
@@ -5436,7 +5469,7 @@
         <v>0.9597222222222223</v>
       </c>
       <c r="O45" t="s" s="9">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="P45" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -5445,7 +5478,7 @@
         <v>0.9319444444444445</v>
       </c>
       <c r="R45" t="s" s="9">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="S45" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -5454,7 +5487,7 @@
         <v>0.9375</v>
       </c>
       <c r="U45" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" ht="30.0" customHeight="true">
@@ -5465,13 +5498,13 @@
         <v>3.0</v>
       </c>
       <c r="C46" t="s" s="6">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D46" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E46" t="s" s="95">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F46" t="n" s="8">
         <v>1.0</v>
@@ -5501,7 +5534,7 @@
         <v>0.96875</v>
       </c>
       <c r="O46" t="s" s="9">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P46" t="n" s="11">
         <v>0.9027777777777778</v>
@@ -5517,7 +5550,7 @@
         <v>0.9236111111111112</v>
       </c>
       <c r="U46" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" ht="30.0" customHeight="true">
@@ -5528,13 +5561,13 @@
         <v>3.0</v>
       </c>
       <c r="C47" t="s" s="6">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D47" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E47" t="s" s="97">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F47" t="n" s="8">
         <v>2.0</v>
@@ -5564,7 +5597,7 @@
         <v>0.9791666666666666</v>
       </c>
       <c r="O47" t="s" s="9">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P47" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -5580,7 +5613,7 @@
         <v>0.9513888888888888</v>
       </c>
       <c r="U47" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" ht="30.0" customHeight="true">
@@ -5591,13 +5624,13 @@
         <v>2.0</v>
       </c>
       <c r="C48" t="s" s="6">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D48" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E48" t="s" s="99">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F48" t="n" s="8">
         <v>8.0</v>
@@ -5627,7 +5660,7 @@
         <v>1.0097222222222222</v>
       </c>
       <c r="O48" t="s" s="9">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="P48" t="n" s="11">
         <v>0.9027777777777778</v>
@@ -5636,7 +5669,7 @@
         <v>0.9472222222222222</v>
       </c>
       <c r="R48" t="s" s="9">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="S48" t="n" s="11">
         <v>0.9243055555555556</v>
@@ -5645,7 +5678,7 @@
         <v>0.9465277777777777</v>
       </c>
       <c r="U48" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" ht="30.0" customHeight="true">
@@ -5656,13 +5689,13 @@
         <v>3.0</v>
       </c>
       <c r="C49" t="s" s="6">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D49" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E49" t="s" s="101">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F49" t="n" s="8">
         <v>4.0</v>
@@ -5692,7 +5725,7 @@
         <v>0.9875</v>
       </c>
       <c r="O49" t="s" s="9">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="P49" t="n" s="11">
         <v>0.9027777777777778</v>
@@ -5701,7 +5734,7 @@
         <v>0.9375</v>
       </c>
       <c r="R49" t="s" s="9">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="S49" t="n" s="11">
         <v>0.9201388888888888</v>
@@ -5710,7 +5743,7 @@
         <v>0.9375</v>
       </c>
       <c r="U49" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" ht="30.0" customHeight="true">
@@ -5721,13 +5754,13 @@
         <v>3.0</v>
       </c>
       <c r="C50" t="s" s="6">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D50" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E50" t="s" s="103">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F50" t="n" s="8">
         <v>6.0</v>
@@ -5757,7 +5790,7 @@
         <v>0.9909722222222223</v>
       </c>
       <c r="O50" t="s" s="9">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="P50" t="n" s="11">
         <v>0.9263888888888889</v>
@@ -5766,7 +5799,7 @@
         <v>0.9479166666666666</v>
       </c>
       <c r="R50" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="S50" t="n" s="11">
         <v>0.9201388888888888</v>
@@ -5775,7 +5808,7 @@
         <v>0.9375</v>
       </c>
       <c r="U50" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" ht="30.0" customHeight="true">
@@ -5786,13 +5819,13 @@
         <v>1.0</v>
       </c>
       <c r="C51" t="s" s="6">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D51" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E51" t="s" s="105">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F51" t="n" s="8">
         <v>8.0</v>
@@ -5822,7 +5855,7 @@
         <v>0.9951388888888889</v>
       </c>
       <c r="O51" t="s" s="9">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="P51" t="n" s="11">
         <v>0.9236111111111112</v>
@@ -5831,7 +5864,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="R51" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S51" t="n" s="11">
         <v>0.9229166666666667</v>
@@ -5840,7 +5873,7 @@
         <v>0.94375</v>
       </c>
       <c r="U51" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" ht="30.0" customHeight="true">
@@ -5851,13 +5884,13 @@
         <v>2.0</v>
       </c>
       <c r="C52" t="s" s="6">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D52" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E52" t="s" s="107">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F52" t="n" s="8">
         <v>13.0</v>
@@ -5887,7 +5920,7 @@
         <v>1.0229166666666667</v>
       </c>
       <c r="O52" t="s" s="9">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="P52" t="n" s="11">
         <v>0.8854166666666666</v>
@@ -5896,7 +5929,7 @@
         <v>0.9375</v>
       </c>
       <c r="R52" t="s" s="9">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="S52" t="n" s="11">
         <v>0.9326388888888889</v>
@@ -5905,7 +5938,7 @@
         <v>0.9430555555555555</v>
       </c>
       <c r="U52" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" ht="30.0" customHeight="true">
@@ -5916,13 +5949,13 @@
         <v>3.0</v>
       </c>
       <c r="C53" t="s" s="6">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D53" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E53" t="s" s="109">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F53" t="n" s="8">
         <v>3.0</v>
@@ -5952,7 +5985,7 @@
         <v>0.98125</v>
       </c>
       <c r="O53" t="s" s="9">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="P53" t="n" s="11">
         <v>0.9270833333333334</v>
@@ -5961,7 +5994,7 @@
         <v>0.9409722222222222</v>
       </c>
       <c r="R53" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S53" t="n" s="11">
         <v>0.9208333333333333</v>
@@ -5970,7 +6003,7 @@
         <v>0.9486111111111111</v>
       </c>
       <c r="U53" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" ht="30.0" customHeight="true">
@@ -5981,13 +6014,13 @@
         <v>3.0</v>
       </c>
       <c r="C54" t="s" s="6">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D54" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E54" t="s" s="111">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F54" t="n" s="8">
         <v>3.0</v>
@@ -6017,7 +6050,7 @@
         <v>0.9875</v>
       </c>
       <c r="O54" t="s" s="9">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="P54" t="n" s="11">
         <v>0.9194444444444444</v>
@@ -6026,7 +6059,7 @@
         <v>0.9513888888888888</v>
       </c>
       <c r="R54" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="S54" t="n" s="11">
         <v>0.9277777777777778</v>
@@ -6035,7 +6068,7 @@
         <v>0.94375</v>
       </c>
       <c r="U54" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" ht="30.0" customHeight="true">
@@ -6046,13 +6079,13 @@
         <v>2.0</v>
       </c>
       <c r="C55" t="s" s="6">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D55" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E55" t="s" s="113">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F55" t="n" s="8">
         <v>6.0</v>
@@ -6082,7 +6115,7 @@
         <v>0.9986111111111111</v>
       </c>
       <c r="O55" t="s" s="9">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="P55" t="n" s="11">
         <v>0.9020833333333333</v>
@@ -6091,7 +6124,7 @@
         <v>0.9340277777777778</v>
       </c>
       <c r="R55" t="s" s="9">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="S55" t="n" s="11">
         <v>0.9333333333333333</v>
@@ -6100,7 +6133,7 @@
         <v>0.9493055555555555</v>
       </c>
       <c r="U55" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" ht="30.0" customHeight="true">
@@ -6111,13 +6144,13 @@
         <v>1.0</v>
       </c>
       <c r="C56" t="s" s="6">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D56" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E56" t="s" s="115">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F56" t="n" s="8">
         <v>5.0</v>
@@ -6147,7 +6180,7 @@
         <v>0.9909722222222223</v>
       </c>
       <c r="O56" t="s" s="9">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="P56" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -6156,7 +6189,7 @@
         <v>0.9430555555555555</v>
       </c>
       <c r="R56" t="s" s="9">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="S56" t="n" s="11">
         <v>0.9243055555555556</v>
@@ -6165,7 +6198,7 @@
         <v>0.9493055555555555</v>
       </c>
       <c r="U56" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" ht="30.0" customHeight="true">
@@ -6176,13 +6209,13 @@
         <v>1.0</v>
       </c>
       <c r="C57" t="s" s="6">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D57" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E57" t="s" s="117">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F57" t="n" s="8">
         <v>1.0</v>
@@ -6212,7 +6245,7 @@
         <v>0.9798611111111111</v>
       </c>
       <c r="O57" t="s" s="9">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="P57" t="n" s="11">
         <v>0.9131944444444444</v>
@@ -6221,7 +6254,7 @@
         <v>0.9548611111111112</v>
       </c>
       <c r="R57" t="s" s="9">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="S57" t="n" s="11">
         <v>0.8923611111111112</v>
@@ -6230,7 +6263,7 @@
         <v>0.9340277777777778</v>
       </c>
       <c r="U57" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" ht="30.0" customHeight="true">
@@ -6241,13 +6274,13 @@
         <v>1.0</v>
       </c>
       <c r="C58" t="s" s="6">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D58" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E58" t="s" s="119">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F58" t="n" s="8">
         <v>4.0</v>
@@ -6277,7 +6310,7 @@
         <v>0.9895833333333334</v>
       </c>
       <c r="O58" t="s" s="9">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="P58" t="n" s="11">
         <v>0.9027777777777778</v>
@@ -6286,7 +6319,7 @@
         <v>0.9375</v>
       </c>
       <c r="R58" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S58" t="n" s="11">
         <v>0.9027777777777778</v>
@@ -6295,7 +6328,7 @@
         <v>0.9375</v>
       </c>
       <c r="U58" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" ht="30.0" customHeight="true">
@@ -6306,13 +6339,13 @@
         <v>1.0</v>
       </c>
       <c r="C59" t="s" s="6">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D59" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E59" t="s" s="121">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F59" t="n" s="8">
         <v>7.0</v>
@@ -6342,7 +6375,7 @@
         <v>0.9986111111111111</v>
       </c>
       <c r="O59" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="P59" t="n" s="11">
         <v>0.9243055555555556</v>
@@ -6351,7 +6384,7 @@
         <v>0.94375</v>
       </c>
       <c r="R59" t="s" s="9">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="S59" t="n" s="11">
         <v>0.9201388888888888</v>
@@ -6360,7 +6393,7 @@
         <v>0.9395833333333333</v>
       </c>
       <c r="U59" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" ht="30.0" customHeight="true">
@@ -6371,13 +6404,13 @@
         <v>3.0</v>
       </c>
       <c r="C60" t="s" s="6">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D60" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E60" t="s" s="123">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F60" t="n" s="8">
         <v>6.0</v>
@@ -6407,7 +6440,7 @@
         <v>0.9916666666666667</v>
       </c>
       <c r="O60" t="s" s="9">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="P60" t="n" s="11">
         <v>0.9083333333333333</v>
@@ -6416,7 +6449,7 @@
         <v>0.9458333333333333</v>
       </c>
       <c r="R60" t="s" s="9">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="S60" t="n" s="11">
         <v>0.9208333333333333</v>
@@ -6425,7 +6458,7 @@
         <v>0.9458333333333333</v>
       </c>
       <c r="U60" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" ht="30.0" customHeight="true">
@@ -6436,13 +6469,13 @@
         <v>3.0</v>
       </c>
       <c r="C61" t="s" s="6">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D61" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E61" t="s" s="125">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F61" t="n" s="8">
         <v>7.0</v>
@@ -6472,7 +6505,7 @@
         <v>0.99375</v>
       </c>
       <c r="O61" t="s" s="9">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="P61" t="n" s="11">
         <v>0.9055555555555556</v>
@@ -6481,7 +6514,7 @@
         <v>0.9409722222222222</v>
       </c>
       <c r="R61" t="s" s="9">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="S61" t="n" s="11">
         <v>0.9347222222222222</v>
@@ -6490,7 +6523,7 @@
         <v>0.9465277777777777</v>
       </c>
       <c r="U61" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" ht="30.0" customHeight="true">
@@ -6501,13 +6534,13 @@
         <v>1.0</v>
       </c>
       <c r="C62" t="s" s="6">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D62" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E62" t="s" s="127">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F62" t="n" s="8">
         <v>1.0</v>
@@ -6537,7 +6570,7 @@
         <v>0.9659722222222222</v>
       </c>
       <c r="O62" t="s" s="9">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="P62" t="n" s="11">
         <v>0.8958333333333334</v>
@@ -6546,7 +6579,7 @@
         <v>0.9375</v>
       </c>
       <c r="R62" t="s" s="9">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="S62" t="n" s="11">
         <v>0.875</v>
@@ -6555,7 +6588,7 @@
         <v>0.9166666666666666</v>
       </c>
       <c r="U62" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63" ht="30.0" customHeight="true">
@@ -6566,13 +6599,13 @@
         <v>3.0</v>
       </c>
       <c r="C63" t="s" s="6">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D63" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E63" t="s" s="129">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F63" t="n" s="8">
         <v>2.0</v>
@@ -6602,7 +6635,7 @@
         <v>0.9583333333333334</v>
       </c>
       <c r="O63" t="s" s="9">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="P63" t="n" s="11">
         <v>0.9125</v>
@@ -6611,7 +6644,7 @@
         <v>0.9291666666666667</v>
       </c>
       <c r="R63" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="S63" t="n" s="11">
         <v>0.9125</v>
@@ -6620,7 +6653,7 @@
         <v>0.9291666666666667</v>
       </c>
       <c r="U63" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" ht="30.0" customHeight="true">
@@ -6631,13 +6664,13 @@
         <v>1.0</v>
       </c>
       <c r="C64" t="s" s="6">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D64" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E64" t="s" s="131">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F64" t="n" s="8">
         <v>1.0</v>
@@ -6667,7 +6700,7 @@
         <v>0.9368055555555556</v>
       </c>
       <c r="O64" t="s" s="9">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="P64" t="n" s="11">
         <v>0.8854166666666666</v>
@@ -6676,7 +6709,7 @@
         <v>0.9166666666666666</v>
       </c>
       <c r="R64" t="s" s="9">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="S64" t="n" s="11">
         <v>0.8701388888888889</v>
@@ -6685,7 +6718,7 @@
         <v>0.9013888888888889</v>
       </c>
       <c r="U64" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65" ht="30.0" customHeight="true">
@@ -6696,13 +6729,13 @@
         <v>3.0</v>
       </c>
       <c r="C65" t="s" s="6">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D65" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E65" t="s" s="133">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F65" t="n" s="8">
         <v>3.0</v>
@@ -6732,7 +6765,7 @@
         <v>0.9729166666666667</v>
       </c>
       <c r="O65" t="s" s="9">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="P65" t="n" s="11">
         <v>0.9215277777777777</v>
@@ -6741,7 +6774,7 @@
         <v>0.9451388888888889</v>
       </c>
       <c r="R65" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="S65" t="n" s="11">
         <v>0.9270833333333334</v>
@@ -6750,7 +6783,7 @@
         <v>0.9388888888888889</v>
       </c>
       <c r="U65" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" ht="30.0" customHeight="true">
@@ -6761,13 +6794,13 @@
         <v>2.0</v>
       </c>
       <c r="C66" t="s" s="6">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D66" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E66" t="s" s="135">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F66" t="n" s="8">
         <v>7.0</v>
@@ -6797,7 +6830,7 @@
         <v>1.0027777777777778</v>
       </c>
       <c r="O66" t="s" s="9">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="P66" t="n" s="11">
         <v>0.9236111111111112</v>
@@ -6806,7 +6839,7 @@
         <v>0.9479166666666666</v>
       </c>
       <c r="R66" t="s" s="9">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="S66" t="n" s="11">
         <v>0.9263888888888889</v>
@@ -6815,7 +6848,7 @@
         <v>0.9381944444444444</v>
       </c>
       <c r="U66" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" ht="30.0" customHeight="true">
@@ -6826,13 +6859,13 @@
         <v>1.0</v>
       </c>
       <c r="C67" t="s" s="6">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D67" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E67" t="s" s="137">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F67" t="n" s="8">
         <v>9.0</v>
@@ -6862,7 +6895,7 @@
         <v>0.9979166666666667</v>
       </c>
       <c r="O67" t="s" s="9">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="P67" t="n" s="11">
         <v>0.9138888888888889</v>
@@ -6871,7 +6904,7 @@
         <v>0.9430555555555555</v>
       </c>
       <c r="R67" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S67" t="n" s="11">
         <v>0.9201388888888888</v>
@@ -6880,7 +6913,7 @@
         <v>0.9395833333333333</v>
       </c>
       <c r="U67" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" ht="30.0" customHeight="true">
@@ -6891,13 +6924,13 @@
         <v>1.0</v>
       </c>
       <c r="C68" t="s" s="6">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D68" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E68" t="s" s="139">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F68" t="n" s="8">
         <v>6.0</v>
@@ -6927,7 +6960,7 @@
         <v>0.9791666666666666</v>
       </c>
       <c r="O68" t="s" s="9">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="P68" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -6936,7 +6969,7 @@
         <v>0.9381944444444444</v>
       </c>
       <c r="R68" t="s" s="9">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="S68" t="n" s="11">
         <v>0.9277777777777778</v>
@@ -6945,7 +6978,7 @@
         <v>0.9381944444444444</v>
       </c>
       <c r="U68" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" ht="30.0" customHeight="true">
@@ -6956,13 +6989,13 @@
         <v>3.0</v>
       </c>
       <c r="C69" t="s" s="6">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D69" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E69" t="s" s="141">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F69" t="n" s="8">
         <v>3.0</v>
@@ -6992,7 +7025,7 @@
         <v>0.9680555555555556</v>
       </c>
       <c r="O69" t="s" s="9">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="P69" t="n" s="11">
         <v>0.9333333333333333</v>
@@ -7001,7 +7034,7 @@
         <v>0.9430555555555555</v>
       </c>
       <c r="R69" t="s" s="9">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="S69" t="n" s="11">
         <v>0.9284722222222223</v>
@@ -7010,7 +7043,7 @@
         <v>0.9479166666666666</v>
       </c>
       <c r="U69" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" ht="30.0" customHeight="true">
@@ -7021,13 +7054,13 @@
         <v>3.0</v>
       </c>
       <c r="C70" t="s" s="6">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D70" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E70" t="s" s="143">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F70" t="n" s="8">
         <v>1.0</v>
@@ -7057,7 +7090,7 @@
         <v>0.9395833333333333</v>
       </c>
       <c r="O70" t="s" s="9">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="P70" t="n" s="11">
         <v>0.8541666666666666</v>
@@ -7066,7 +7099,7 @@
         <v>0.8958333333333334</v>
       </c>
       <c r="R70" t="s" s="9">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="S70" t="n" s="11">
         <v>0.875</v>
@@ -7075,7 +7108,7 @@
         <v>0.9166666666666666</v>
       </c>
       <c r="U70" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="71" ht="30.0" customHeight="true">
@@ -7086,13 +7119,13 @@
         <v>3.0</v>
       </c>
       <c r="C71" t="s" s="6">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D71" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E71" t="s" s="145">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F71" t="n" s="8">
         <v>2.0</v>
@@ -7122,7 +7155,7 @@
         <v>0.9777777777777777</v>
       </c>
       <c r="O71" t="s" s="9">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="P71" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -7131,7 +7164,7 @@
         <v>0.9513888888888888</v>
       </c>
       <c r="R71" t="s" s="9">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="S71" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -7140,7 +7173,7 @@
         <v>0.9513888888888888</v>
       </c>
       <c r="U71" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72" ht="30.0" customHeight="true">
@@ -7151,13 +7184,13 @@
         <v>3.0</v>
       </c>
       <c r="C72" t="s" s="6">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D72" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E72" t="s" s="147">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F72" t="n" s="8">
         <v>1.0</v>
@@ -7187,7 +7220,7 @@
         <v>0.9722222222222222</v>
       </c>
       <c r="O72" t="s" s="9">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="P72" t="n" s="11">
         <v>0.9097222222222222</v>
@@ -7196,7 +7229,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="R72" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="S72" t="n" s="11">
         <v>0.8923611111111112</v>
@@ -7205,7 +7238,7 @@
         <v>0.9270833333333334</v>
       </c>
       <c r="U72" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="73" ht="30.0" customHeight="true">
@@ -7216,13 +7249,13 @@
         <v>3.0</v>
       </c>
       <c r="C73" t="s" s="6">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D73" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E73" t="s" s="149">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F73" t="n" s="8">
         <v>4.0</v>
@@ -7252,7 +7285,7 @@
         <v>0.9715277777777778</v>
       </c>
       <c r="O73" t="s" s="9">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="P73" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -7261,7 +7294,7 @@
         <v>0.9375</v>
       </c>
       <c r="R73" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="S73" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -7270,7 +7303,7 @@
         <v>0.9375</v>
       </c>
       <c r="U73" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74" ht="30.0" customHeight="true">
@@ -7281,13 +7314,13 @@
         <v>2.0</v>
       </c>
       <c r="C74" t="s" s="6">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D74" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E74" t="s" s="151">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F74" t="n" s="8">
         <v>2.0</v>
@@ -7317,7 +7350,7 @@
         <v>0.9673611111111111</v>
       </c>
       <c r="O74" t="s" s="9">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="P74" t="n" s="11">
         <v>0.9361111111111111</v>
@@ -7326,7 +7359,7 @@
         <v>0.9472222222222222</v>
       </c>
       <c r="R74" t="s" s="9">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="S74" t="n" s="11">
         <v>0.9361111111111111</v>
@@ -7335,7 +7368,7 @@
         <v>0.9472222222222222</v>
       </c>
       <c r="U74" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="75" ht="30.0" customHeight="true">
@@ -7346,13 +7379,13 @@
         <v>1.0</v>
       </c>
       <c r="C75" t="s" s="6">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D75" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E75" t="s" s="152">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F75" t="n" s="8">
         <v>1.0</v>
@@ -7382,7 +7415,7 @@
         <v>0.9694444444444444</v>
       </c>
       <c r="O75" t="s" s="9">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="P75" t="n" s="11">
         <v>0.8854166666666666</v>
@@ -7391,7 +7424,7 @@
         <v>0.9340277777777778</v>
       </c>
       <c r="R75" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S75" t="n" s="11">
         <v>0.8631944444444445</v>
@@ -7400,7 +7433,7 @@
         <v>0.9118055555555555</v>
       </c>
       <c r="U75" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="76" ht="30.0" customHeight="true">
@@ -7411,13 +7444,13 @@
         <v>1.0</v>
       </c>
       <c r="C76" t="s" s="6">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D76" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E76" t="s" s="154">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F76" t="n" s="8">
         <v>1.0</v>
@@ -7447,7 +7480,7 @@
         <v>0.9319444444444445</v>
       </c>
       <c r="O76" t="s" s="9">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="P76" t="n" s="11">
         <v>0.8118055555555556</v>
@@ -7456,7 +7489,7 @@
         <v>0.8743055555555556</v>
       </c>
       <c r="R76" t="s" s="9">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="S76" t="n" s="11">
         <v>0.7805555555555556</v>
@@ -7465,7 +7498,7 @@
         <v>0.8430555555555556</v>
       </c>
       <c r="U76" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="77" ht="30.0" customHeight="true">
@@ -7476,13 +7509,13 @@
         <v>1.0</v>
       </c>
       <c r="C77" t="s" s="6">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D77" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E77" t="s" s="156">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F77" t="n" s="8">
         <v>2.0</v>
@@ -7512,7 +7545,7 @@
         <v>0.9458333333333333</v>
       </c>
       <c r="O77" t="s" s="9">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="P77" t="n" s="11">
         <v>0.84375</v>
@@ -7521,7 +7554,7 @@
         <v>0.8854166666666666</v>
       </c>
       <c r="R77" t="s" s="9">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="S77" t="n" s="11">
         <v>0.8020833333333334</v>
@@ -7530,7 +7563,7 @@
         <v>0.84375</v>
       </c>
       <c r="U77" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="78" ht="30.0" customHeight="true">
@@ -7541,13 +7574,13 @@
         <v>3.0</v>
       </c>
       <c r="C78" t="s" s="6">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D78" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E78" t="s" s="158">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F78" t="n" s="8">
         <v>4.0</v>
@@ -7577,7 +7610,7 @@
         <v>0.9944444444444445</v>
       </c>
       <c r="O78" t="s" s="9">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="P78" t="n" s="11">
         <v>0.9041666666666667</v>
@@ -7586,7 +7619,7 @@
         <v>0.9416666666666667</v>
       </c>
       <c r="R78" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="S78" t="n" s="11">
         <v>0.9090277777777778</v>
@@ -7595,7 +7628,7 @@
         <v>0.9465277777777777</v>
       </c>
       <c r="U78" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="79" ht="30.0" customHeight="true">
@@ -7606,13 +7639,13 @@
         <v>2.0</v>
       </c>
       <c r="C79" t="s" s="6">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D79" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E79" t="s" s="160">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F79" t="n" s="8">
         <v>8.0</v>
@@ -7642,7 +7675,7 @@
         <v>0.9993055555555556</v>
       </c>
       <c r="O79" t="s" s="9">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="P79" t="n" s="11">
         <v>0.8951388888888889</v>
@@ -7651,7 +7684,7 @@
         <v>0.9395833333333333</v>
       </c>
       <c r="R79" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="S79" t="n" s="11">
         <v>0.9173611111111111</v>
@@ -7660,7 +7693,7 @@
         <v>0.9395833333333333</v>
       </c>
       <c r="U79" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="80" ht="30.0" customHeight="true">
@@ -7671,13 +7704,13 @@
         <v>2.0</v>
       </c>
       <c r="C80" t="s" s="6">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D80" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E80" t="s" s="162">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F80" t="n" s="8">
         <v>3.0</v>
@@ -7707,7 +7740,7 @@
         <v>0.9972222222222222</v>
       </c>
       <c r="O80" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="P80" t="n" s="11">
         <v>0.9083333333333333</v>
@@ -7716,16 +7749,16 @@
         <v>0.9375</v>
       </c>
       <c r="R80" t="s" s="9">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="S80" t="s" s="11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T80" t="s" s="11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U80" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" ht="30.0" customHeight="true">
@@ -7736,13 +7769,13 @@
         <v>2.0</v>
       </c>
       <c r="C81" t="s" s="6">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D81" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E81" t="s" s="164">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F81" t="n" s="8">
         <v>10.0</v>
@@ -7772,7 +7805,7 @@
         <v>0.9972222222222222</v>
       </c>
       <c r="O81" t="s" s="9">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="P81" t="n" s="11">
         <v>0.9111111111111111</v>
@@ -7781,7 +7814,7 @@
         <v>0.9375</v>
       </c>
       <c r="R81" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S81" t="n" s="11">
         <v>0.9291666666666667</v>
@@ -7790,7 +7823,7 @@
         <v>0.9375</v>
       </c>
       <c r="U81" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" ht="30.0" customHeight="true">
@@ -7801,13 +7834,13 @@
         <v>3.0</v>
       </c>
       <c r="C82" t="s" s="6">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D82" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E82" t="s" s="166">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F82" t="n" s="8">
         <v>2.0</v>
@@ -7837,7 +7870,7 @@
         <v>0.9722222222222222</v>
       </c>
       <c r="O82" t="s" s="9">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="P82" t="n" s="11">
         <v>0.9090277777777778</v>
@@ -7846,7 +7879,7 @@
         <v>0.9375</v>
       </c>
       <c r="R82" t="s" s="9">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="S82" t="n" s="11">
         <v>0.9083333333333333</v>
@@ -7855,7 +7888,7 @@
         <v>0.9375</v>
       </c>
       <c r="U82" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83" ht="30.0" customHeight="true">
@@ -7866,13 +7899,13 @@
         <v>3.0</v>
       </c>
       <c r="C83" t="s" s="6">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D83" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E83" t="s" s="168">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F83" t="n" s="8">
         <v>5.0</v>
@@ -7902,7 +7935,7 @@
         <v>0.9930555555555556</v>
       </c>
       <c r="O83" t="s" s="9">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="P83" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -7911,7 +7944,7 @@
         <v>0.9479166666666666</v>
       </c>
       <c r="R83" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S83" t="n" s="11">
         <v>0.9229166666666667</v>
@@ -7920,7 +7953,7 @@
         <v>0.94375</v>
       </c>
       <c r="U83" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84" ht="30.0" customHeight="true">
@@ -7931,13 +7964,13 @@
         <v>1.0</v>
       </c>
       <c r="C84" t="s" s="6">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D84" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E84" t="s" s="170">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F84" t="n" s="8">
         <v>3.0</v>
@@ -7967,7 +8000,7 @@
         <v>0.9826388888888888</v>
       </c>
       <c r="O84" t="s" s="9">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="P84" t="n" s="11">
         <v>0.9020833333333333</v>
@@ -7976,7 +8009,7 @@
         <v>0.9388888888888889</v>
       </c>
       <c r="R84" t="s" s="9">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="S84" t="n" s="11">
         <v>0.9111111111111111</v>
@@ -7985,7 +8018,7 @@
         <v>0.9298611111111111</v>
       </c>
       <c r="U84" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85" ht="30.0" customHeight="true">
@@ -7996,13 +8029,13 @@
         <v>1.0</v>
       </c>
       <c r="C85" t="s" s="6">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D85" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E85" t="s" s="172">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F85" t="n" s="8">
         <v>5.0</v>
@@ -8032,7 +8065,7 @@
         <v>0.99375</v>
       </c>
       <c r="O85" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="P85" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -8041,7 +8074,7 @@
         <v>0.9416666666666667</v>
       </c>
       <c r="R85" t="s" s="9">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="S85" t="n" s="11">
         <v>0.9229166666666667</v>
@@ -8050,7 +8083,7 @@
         <v>0.9479166666666666</v>
       </c>
       <c r="U85" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" ht="30.0" customHeight="true">
@@ -8061,13 +8094,13 @@
         <v>2.0</v>
       </c>
       <c r="C86" t="s" s="6">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="D86" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E86" t="s" s="174">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F86" t="n" s="8">
         <v>4.0</v>
@@ -8097,7 +8130,7 @@
         <v>0.975</v>
       </c>
       <c r="O86" t="s" s="9">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="P86" t="n" s="11">
         <v>0.9173611111111111</v>
@@ -8106,7 +8139,7 @@
         <v>0.9409722222222222</v>
       </c>
       <c r="R86" t="s" s="9">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="S86" t="n" s="11">
         <v>0.9173611111111111</v>
@@ -8115,7 +8148,7 @@
         <v>0.9409722222222222</v>
       </c>
       <c r="U86" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87" ht="30.0" customHeight="true">
@@ -8126,13 +8159,13 @@
         <v>2.0</v>
       </c>
       <c r="C87" t="s" s="6">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D87" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E87" t="s" s="176">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F87" t="n" s="8">
         <v>7.0</v>
@@ -8162,7 +8195,7 @@
         <v>1.0055555555555555</v>
       </c>
       <c r="O87" t="s" s="9">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="P87" t="n" s="11">
         <v>0.8965277777777778</v>
@@ -8171,7 +8204,7 @@
         <v>0.9388888888888889</v>
       </c>
       <c r="R87" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S87" t="n" s="11">
         <v>0.9173611111111111</v>
@@ -8180,7 +8213,7 @@
         <v>0.9458333333333333</v>
       </c>
       <c r="U87" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88" ht="30.0" customHeight="true">
@@ -8191,13 +8224,13 @@
         <v>3.0</v>
       </c>
       <c r="C88" t="s" s="6">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D88" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E88" t="s" s="178">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F88" t="n" s="8">
         <v>4.0</v>
@@ -8227,7 +8260,7 @@
         <v>0.9784722222222222</v>
       </c>
       <c r="O88" t="s" s="9">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="P88" t="n" s="11">
         <v>0.9236111111111112</v>
@@ -8236,7 +8269,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="R88" t="s" s="9">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="S88" t="n" s="11">
         <v>0.9236111111111112</v>
@@ -8245,7 +8278,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="U88" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="89" ht="30.0" customHeight="true">
@@ -8256,13 +8289,13 @@
         <v>1.0</v>
       </c>
       <c r="C89" t="s" s="6">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D89" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E89" t="s" s="180">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F89" t="n" s="8">
         <v>5.0</v>
@@ -8292,7 +8325,7 @@
         <v>1.0125</v>
       </c>
       <c r="O89" t="s" s="9">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="P89" t="n" s="11">
         <v>0.9159722222222222</v>
@@ -8301,7 +8334,7 @@
         <v>0.9534722222222223</v>
       </c>
       <c r="R89" t="s" s="9">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="S89" t="n" s="11">
         <v>0.9069444444444444</v>
@@ -8310,7 +8343,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="U89" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="90" ht="30.0" customHeight="true">
@@ -8321,13 +8354,13 @@
         <v>1.0</v>
       </c>
       <c r="C90" t="s" s="6">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D90" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E90" t="s" s="182">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F90" t="n" s="8">
         <v>5.0</v>
@@ -8357,7 +8390,7 @@
         <v>1.0215277777777778</v>
       </c>
       <c r="O90" t="s" s="9">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="P90" t="n" s="11">
         <v>0.9055555555555556</v>
@@ -8366,7 +8399,7 @@
         <v>0.9416666666666667</v>
       </c>
       <c r="R90" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S90" t="n" s="11">
         <v>0.9145833333333333</v>
@@ -8375,7 +8408,7 @@
         <v>0.9506944444444444</v>
       </c>
       <c r="U90" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91" ht="30.0" customHeight="true">
@@ -8386,13 +8419,13 @@
         <v>1.0</v>
       </c>
       <c r="C91" t="s" s="6">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D91" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E91" t="s" s="184">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F91" t="n" s="8">
         <v>3.0</v>
@@ -8422,7 +8455,7 @@
         <v>0.98125</v>
       </c>
       <c r="O91" t="s" s="9">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="P91" t="n" s="11">
         <v>0.9020833333333333</v>
@@ -8431,7 +8464,7 @@
         <v>0.9298611111111111</v>
       </c>
       <c r="R91" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S91" t="n" s="11">
         <v>0.8611111111111112</v>
@@ -8440,7 +8473,7 @@
         <v>0.8888888888888888</v>
       </c>
       <c r="U91" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92" ht="30.0" customHeight="true">
@@ -8451,13 +8484,13 @@
         <v>3.0</v>
       </c>
       <c r="C92" t="s" s="6">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D92" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E92" t="s" s="186">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F92" t="n" s="8">
         <v>2.0</v>
@@ -8487,7 +8520,7 @@
         <v>0.9527777777777777</v>
       </c>
       <c r="O92" t="s" s="9">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="P92" t="n" s="11">
         <v>0.8993055555555556</v>
@@ -8496,7 +8529,7 @@
         <v>0.9236111111111112</v>
       </c>
       <c r="R92" t="s" s="9">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="S92" t="n" s="11">
         <v>0.875</v>
@@ -8505,7 +8538,7 @@
         <v>0.8993055555555556</v>
       </c>
       <c r="U92" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="93" ht="30.0" customHeight="true">
@@ -8515,12 +8548,14 @@
       <c r="B93" t="n" s="6">
         <v>3.0</v>
       </c>
-      <c r="C93" s="6"/>
+      <c r="C93" t="s" s="6">
+        <v>205</v>
+      </c>
       <c r="D93" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E93" t="s" s="188">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F93" t="n" s="8">
         <v>4.0</v>
@@ -8549,14 +8584,18 @@
       <c r="N93" t="n" s="11">
         <v>1.0034722222222223</v>
       </c>
-      <c r="O93" s="9"/>
+      <c r="O93" t="s" s="9">
+        <v>29</v>
+      </c>
       <c r="P93" t="n" s="11">
         <v>0.8756944444444444</v>
       </c>
       <c r="Q93" t="n" s="11">
         <v>0.9104166666666667</v>
       </c>
-      <c r="R93" s="9"/>
+      <c r="R93" t="s" s="9">
+        <v>206</v>
+      </c>
       <c r="S93" t="n" s="11">
         <v>0.9027777777777778</v>
       </c>
@@ -8564,7 +8603,7 @@
         <v>0.9305555555555556</v>
       </c>
       <c r="U93" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94" ht="30.0" customHeight="true">
@@ -8575,13 +8614,13 @@
         <v>3.0</v>
       </c>
       <c r="C94" t="s" s="6">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D94" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E94" t="s" s="190">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F94" t="n" s="8">
         <v>1.0</v>
@@ -8611,7 +8650,7 @@
         <v>0.9944444444444445</v>
       </c>
       <c r="O94" t="s" s="9">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="P94" t="n" s="11">
         <v>0.8680555555555556</v>
@@ -8620,7 +8659,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="R94" t="s" s="9">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="S94" t="n" s="11">
         <v>0.8298611111111112</v>
@@ -8629,7 +8668,7 @@
         <v>0.90625</v>
       </c>
       <c r="U94" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95" ht="30.0" customHeight="true">
@@ -8640,13 +8679,13 @@
         <v>3.0</v>
       </c>
       <c r="C95" t="s" s="6">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D95" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E95" t="s" s="192">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F95" t="n" s="8">
         <v>4.0</v>
@@ -8676,7 +8715,7 @@
         <v>0.9930555555555556</v>
       </c>
       <c r="O95" t="s" s="9">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="P95" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -8685,7 +8724,7 @@
         <v>0.9340277777777778</v>
       </c>
       <c r="R95" t="s" s="9">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="S95" t="n" s="11">
         <v>0.9173611111111111</v>
@@ -8694,7 +8733,7 @@
         <v>0.9520833333333333</v>
       </c>
       <c r="U95" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96" ht="30.0" customHeight="true">
@@ -8705,13 +8744,13 @@
         <v>3.0</v>
       </c>
       <c r="C96" t="s" s="6">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="D96" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E96" t="s" s="194">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F96" t="n" s="8">
         <v>1.0</v>
@@ -8741,7 +8780,7 @@
         <v>0.9722222222222222</v>
       </c>
       <c r="O96" t="s" s="9">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P96" t="n" s="11">
         <v>0.8958333333333334</v>
@@ -8750,7 +8789,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="R96" t="s" s="9">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="S96" t="n" s="11">
         <v>0.8694444444444445</v>
@@ -8759,7 +8798,7 @@
         <v>0.9180555555555555</v>
       </c>
       <c r="U96" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97" ht="30.0" customHeight="true">
@@ -8770,13 +8809,13 @@
         <v>3.0</v>
       </c>
       <c r="C97" t="s" s="6">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D97" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E97" t="s" s="196">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F97" t="n" s="8">
         <v>2.0</v>
@@ -8806,7 +8845,7 @@
         <v>0.9722222222222222</v>
       </c>
       <c r="O97" t="s" s="9">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="P97" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -8815,7 +8854,7 @@
         <v>0.9375</v>
       </c>
       <c r="R97" t="s" s="9">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="S97" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -8824,7 +8863,7 @@
         <v>0.9375</v>
       </c>
       <c r="U97" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98" ht="30.0" customHeight="true">
@@ -8835,13 +8874,13 @@
         <v>1.0</v>
       </c>
       <c r="C98" t="s" s="6">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="D98" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E98" t="s" s="198">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F98" t="n" s="8">
         <v>3.0</v>
@@ -8871,7 +8910,7 @@
         <v>0.9743055555555555</v>
       </c>
       <c r="O98" t="s" s="9">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="P98" t="n" s="11">
         <v>0.89375</v>
@@ -8880,7 +8919,7 @@
         <v>0.9215277777777777</v>
       </c>
       <c r="R98" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S98" t="n" s="11">
         <v>0.8541666666666666</v>
@@ -8889,7 +8928,7 @@
         <v>0.8819444444444444</v>
       </c>
       <c r="U98" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99" ht="30.0" customHeight="true">
@@ -8900,13 +8939,13 @@
         <v>3.0</v>
       </c>
       <c r="C99" t="s" s="6">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="D99" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E99" t="s" s="200">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F99" t="n" s="8">
         <v>5.0</v>
@@ -8936,7 +8975,7 @@
         <v>0.9805555555555555</v>
       </c>
       <c r="O99" t="s" s="9">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="P99" t="n" s="11">
         <v>0.925</v>
@@ -8945,7 +8984,7 @@
         <v>0.9472222222222222</v>
       </c>
       <c r="R99" t="s" s="9">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="S99" t="n" s="11">
         <v>0.93125</v>
@@ -8954,7 +8993,7 @@
         <v>0.9423611111111111</v>
       </c>
       <c r="U99" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100" ht="30.0" customHeight="true">
@@ -8965,13 +9004,13 @@
         <v>1.0</v>
       </c>
       <c r="C100" t="s" s="6">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D100" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E100" t="s" s="202">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F100" t="n" s="8">
         <v>2.0</v>
@@ -9001,7 +9040,7 @@
         <v>0.9618055555555556</v>
       </c>
       <c r="O100" t="s" s="9">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="P100" t="n" s="11">
         <v>0.8993055555555556</v>
@@ -9010,7 +9049,7 @@
         <v>0.9236111111111112</v>
       </c>
       <c r="R100" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="S100" t="n" s="11">
         <v>0.8986111111111111</v>
@@ -9019,7 +9058,7 @@
         <v>0.9229166666666667</v>
       </c>
       <c r="U100" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="101" ht="30.0" customHeight="true">
@@ -9030,13 +9069,13 @@
         <v>3.0</v>
       </c>
       <c r="C101" t="s" s="6">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="D101" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E101" t="s" s="204">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F101" t="n" s="8">
         <v>3.0</v>
@@ -9066,7 +9105,7 @@
         <v>0.9902777777777778</v>
       </c>
       <c r="O101" t="s" s="9">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="P101" t="n" s="11">
         <v>0.9131944444444444</v>
@@ -9075,7 +9114,7 @@
         <v>0.9291666666666667</v>
       </c>
       <c r="R101" t="s" s="9">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="S101" t="n" s="11">
         <v>0.9368055555555556</v>
@@ -9084,7 +9123,7 @@
         <v>0.9527777777777777</v>
       </c>
       <c r="U101" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="102" ht="30.0" customHeight="true">
@@ -9095,13 +9134,13 @@
         <v>2.0</v>
       </c>
       <c r="C102" t="s" s="6">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="D102" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E102" t="s" s="206">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F102" t="n" s="8">
         <v>10.0</v>
@@ -9131,7 +9170,7 @@
         <v>0.9979166666666667</v>
       </c>
       <c r="O102" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="P102" t="n" s="11">
         <v>0.9375</v>
@@ -9140,7 +9179,7 @@
         <v>0.9451388888888889</v>
       </c>
       <c r="R102" t="s" s="9">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="S102" t="n" s="11">
         <v>0.9215277777777777</v>
@@ -9149,7 +9188,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="U102" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="103" ht="30.0" customHeight="true">
@@ -9160,13 +9199,13 @@
         <v>2.0</v>
       </c>
       <c r="C103" t="s" s="6">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="D103" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E103" t="s" s="208">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F103" t="n" s="8">
         <v>16.0</v>
@@ -9196,7 +9235,7 @@
         <v>1.0347222222222223</v>
       </c>
       <c r="O103" t="s" s="9">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="P103" t="n" s="11">
         <v>0.9354166666666667</v>
@@ -9205,7 +9244,7 @@
         <v>0.9451388888888889</v>
       </c>
       <c r="R103" t="s" s="9">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="S103" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -9214,7 +9253,7 @@
         <v>0.9409722222222222</v>
       </c>
       <c r="U103" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="104" ht="30.0" customHeight="true">
@@ -9225,13 +9264,13 @@
         <v>2.0</v>
       </c>
       <c r="C104" t="s" s="6">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="D104" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E104" t="s" s="210">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F104" t="n" s="8">
         <v>4.0</v>
@@ -9261,7 +9300,7 @@
         <v>0.9729166666666667</v>
       </c>
       <c r="O104" t="s" s="9">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="P104" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -9270,7 +9309,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="R104" t="s" s="9">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="S104" t="n" s="11">
         <v>0.9236111111111112</v>
@@ -9279,7 +9318,7 @@
         <v>0.9375</v>
       </c>
       <c r="U104" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="105" ht="30.0" customHeight="true">
@@ -9290,13 +9329,13 @@
         <v>2.0</v>
       </c>
       <c r="C105" t="s" s="6">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D105" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E105" t="s" s="212">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F105" t="n" s="8">
         <v>8.0</v>
@@ -9326,7 +9365,7 @@
         <v>1.0048611111111112</v>
       </c>
       <c r="O105" t="s" s="9">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="P105" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -9335,7 +9374,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="R105" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="S105" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -9344,7 +9383,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="U105" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="106" ht="30.0" customHeight="true">
@@ -9355,13 +9394,13 @@
         <v>1.0</v>
       </c>
       <c r="C106" t="s" s="6">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="D106" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E106" t="s" s="214">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F106" t="n" s="8">
         <v>8.0</v>
@@ -9391,7 +9430,7 @@
         <v>0.9993055555555556</v>
       </c>
       <c r="O106" t="s" s="9">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="P106" t="n" s="11">
         <v>0.9256944444444445</v>
@@ -9400,7 +9439,7 @@
         <v>0.9375</v>
       </c>
       <c r="R106" t="s" s="9">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="S106" t="n" s="11">
         <v>0.9256944444444445</v>
@@ -9409,7 +9448,7 @@
         <v>0.9375</v>
       </c>
       <c r="U106" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="107" ht="30.0" customHeight="true">
@@ -9420,13 +9459,13 @@
         <v>2.0</v>
       </c>
       <c r="C107" t="s" s="6">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="D107" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E107" t="s" s="216">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F107" t="n" s="8">
         <v>4.0</v>
@@ -9454,7 +9493,7 @@
         <v>0.9791666666666666</v>
       </c>
       <c r="O107" t="s" s="9">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="P107" t="n" s="11">
         <v>0.9430555555555555</v>
@@ -9463,16 +9502,16 @@
         <v>0.9479166666666666</v>
       </c>
       <c r="R107" t="s" s="9">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="S107" t="s" s="11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T107" t="s" s="11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U107" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="108" ht="30.0" customHeight="true">
@@ -9483,13 +9522,13 @@
         <v>2.0</v>
       </c>
       <c r="C108" t="s" s="6">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="D108" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E108" t="s" s="218">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F108" t="n" s="8">
         <v>9.0</v>
@@ -9519,7 +9558,7 @@
         <v>1.020138888888889</v>
       </c>
       <c r="O108" t="s" s="9">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="P108" t="n" s="11">
         <v>0.9291666666666667</v>
@@ -9528,7 +9567,7 @@
         <v>0.9395833333333333</v>
       </c>
       <c r="R108" t="s" s="9">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="S108" t="n" s="11">
         <v>0.9340277777777778</v>
@@ -9537,7 +9576,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="U108" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="109" ht="30.0" customHeight="true">
@@ -9548,13 +9587,13 @@
         <v>2.0</v>
       </c>
       <c r="C109" t="s" s="6">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="D109" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E109" t="s" s="220">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F109" t="n" s="8">
         <v>9.0</v>
@@ -9584,7 +9623,7 @@
         <v>1.0027777777777778</v>
       </c>
       <c r="O109" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="P109" t="n" s="11">
         <v>0.9347222222222222</v>
@@ -9593,7 +9632,7 @@
         <v>0.9416666666666667</v>
       </c>
       <c r="R109" t="s" s="9">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="S109" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -9602,7 +9641,7 @@
         <v>0.9375</v>
       </c>
       <c r="U109" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="110" ht="30.0" customHeight="true">
@@ -9613,13 +9652,13 @@
         <v>2.0</v>
       </c>
       <c r="C110" t="s" s="6">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="D110" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E110" t="s" s="222">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F110" t="n" s="8">
         <v>15.0</v>
@@ -9649,7 +9688,7 @@
         <v>1.0256944444444445</v>
       </c>
       <c r="O110" t="s" s="9">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="P110" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -9658,7 +9697,7 @@
         <v>0.9409722222222222</v>
       </c>
       <c r="R110" t="s" s="9">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="S110" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -9667,7 +9706,7 @@
         <v>0.9409722222222222</v>
       </c>
       <c r="U110" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="111" ht="30.0" customHeight="true">
@@ -9678,13 +9717,13 @@
         <v>2.0</v>
       </c>
       <c r="C111" t="s" s="6">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="D111" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E111" t="s" s="224">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F111" t="n" s="8">
         <v>10.0</v>
@@ -9714,7 +9753,7 @@
         <v>1.0208333333333333</v>
       </c>
       <c r="O111" t="s" s="9">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="P111" t="n" s="11">
         <v>0.9326388888888889</v>
@@ -9723,7 +9762,7 @@
         <v>0.9416666666666667</v>
       </c>
       <c r="R111" t="s" s="9">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="S111" t="n" s="11">
         <v>0.9326388888888889</v>
@@ -9732,7 +9771,7 @@
         <v>0.9416666666666667</v>
       </c>
       <c r="U111" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="112" ht="30.0" customHeight="true">
@@ -9743,13 +9782,13 @@
         <v>3.0</v>
       </c>
       <c r="C112" t="s" s="6">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="D112" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E112" t="s" s="226">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F112" t="n" s="8">
         <v>8.0</v>
@@ -9779,7 +9818,7 @@
         <v>0.99375</v>
       </c>
       <c r="O112" t="s" s="9">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="P112" t="n" s="11">
         <v>0.9263888888888889</v>
@@ -9788,7 +9827,7 @@
         <v>0.9388888888888889</v>
       </c>
       <c r="R112" t="s" s="9">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="S112" t="n" s="11">
         <v>0.9263888888888889</v>
@@ -9797,7 +9836,7 @@
         <v>0.9388888888888889</v>
       </c>
       <c r="U112" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="113" ht="30.0" customHeight="true">
@@ -9808,13 +9847,13 @@
         <v>1.0</v>
       </c>
       <c r="C113" t="s" s="6">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="D113" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E113" t="s" s="228">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F113" t="n" s="8">
         <v>8.0</v>
@@ -9844,7 +9883,7 @@
         <v>0.9986111111111111</v>
       </c>
       <c r="O113" t="s" s="9">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="P113" t="n" s="11">
         <v>0.9333333333333333</v>
@@ -9853,7 +9892,7 @@
         <v>0.9423611111111111</v>
       </c>
       <c r="R113" t="s" s="9">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S113" t="n" s="11">
         <v>0.9326388888888889</v>
@@ -9862,7 +9901,7 @@
         <v>0.9416666666666667</v>
       </c>
       <c r="U113" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="114" ht="30.0" customHeight="true">
@@ -9873,13 +9912,13 @@
         <v>2.0</v>
       </c>
       <c r="C114" t="s" s="6">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="D114" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E114" t="s" s="230">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F114" t="n" s="8">
         <v>3.0</v>
@@ -9907,7 +9946,7 @@
         <v>0.9875</v>
       </c>
       <c r="O114" t="s" s="9">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="P114" t="n" s="11">
         <v>0.9333333333333333</v>
@@ -9916,16 +9955,16 @@
         <v>0.9430555555555555</v>
       </c>
       <c r="R114" t="s" s="9">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="S114" t="s" s="11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T114" t="s" s="11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U114" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="115" ht="30.0" customHeight="true">
@@ -9936,13 +9975,13 @@
         <v>2.0</v>
       </c>
       <c r="C115" t="s" s="6">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="D115" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E115" t="s" s="232">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F115" t="n" s="8">
         <v>4.0</v>
@@ -9970,7 +10009,7 @@
         <v>0.9861111111111112</v>
       </c>
       <c r="O115" t="s" s="9">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="P115" t="n" s="11">
         <v>0.9298611111111111</v>
@@ -9979,16 +10018,16 @@
         <v>0.9402777777777778</v>
       </c>
       <c r="R115" t="s" s="9">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="S115" t="s" s="11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T115" t="s" s="11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U115" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now i need only to filter tripPeriodsFilter
</commit_message>
<xml_diff>
--- a/downloads/მარაბდა.xlsx
+++ b/downloads/მარაბდა.xlsx
@@ -2727,67 +2727,67 @@
     </row>
     <row r="4">
       <c r="A4" t="n" s="5">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B4" t="n" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C4" t="n" s="5">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D4" t="n" s="5">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E4" t="n" s="5">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="F4" t="n" s="5">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="G4" t="n" s="5">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="H4" t="n" s="5">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="I4" t="n" s="5">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="J4" t="n" s="5">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="K4" t="n" s="5">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="L4" t="n" s="5">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="M4" t="n" s="5">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="N4" t="n" s="5">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="O4" t="n" s="5">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="P4" t="n" s="5">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="Q4" t="n" s="5">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
       <c r="R4" t="n" s="5">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
       <c r="S4" t="n" s="5">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="T4" t="n" s="5">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
       <c r="U4" t="n" s="5">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="5" ht="30.0" customHeight="true">

</xml_diff>

<commit_message>
intervals excel export links, dilemma, 65 000 max links
</commit_message>
<xml_diff>
--- a/downloads/მარაბდა.xlsx
+++ b/downloads/მარაბდა.xlsx
@@ -268,7 +268,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
@@ -81476,6 +81476,2160 @@
     <mergeCell ref="W1:AB1"/>
     <mergeCell ref="AC1:AM1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="Z3" r:id="rId3"/>
+    <hyperlink ref="AA3" r:id="rId4"/>
+    <hyperlink ref="H4" r:id="rId5"/>
+    <hyperlink ref="I4" r:id="rId6"/>
+    <hyperlink ref="Z4" r:id="rId7"/>
+    <hyperlink ref="AA4" r:id="rId8"/>
+    <hyperlink ref="H5" r:id="rId9"/>
+    <hyperlink ref="I5" r:id="rId10"/>
+    <hyperlink ref="Z5" r:id="rId11"/>
+    <hyperlink ref="AA5" r:id="rId12"/>
+    <hyperlink ref="H6" r:id="rId13"/>
+    <hyperlink ref="I6" r:id="rId14"/>
+    <hyperlink ref="Z6" r:id="rId15"/>
+    <hyperlink ref="AA6" r:id="rId16"/>
+    <hyperlink ref="H7" r:id="rId17"/>
+    <hyperlink ref="I7" r:id="rId18"/>
+    <hyperlink ref="Z7" r:id="rId19"/>
+    <hyperlink ref="AA7" r:id="rId20"/>
+    <hyperlink ref="H8" r:id="rId21"/>
+    <hyperlink ref="I8" r:id="rId22"/>
+    <hyperlink ref="Z8" r:id="rId23"/>
+    <hyperlink ref="AA8" r:id="rId24"/>
+    <hyperlink ref="H9" r:id="rId25"/>
+    <hyperlink ref="I9" r:id="rId26"/>
+    <hyperlink ref="Z9" r:id="rId27"/>
+    <hyperlink ref="AA9" r:id="rId28"/>
+    <hyperlink ref="H10" r:id="rId29"/>
+    <hyperlink ref="I10" r:id="rId30"/>
+    <hyperlink ref="Z10" r:id="rId31"/>
+    <hyperlink ref="AA10" r:id="rId32"/>
+    <hyperlink ref="H11" r:id="rId33"/>
+    <hyperlink ref="I11" r:id="rId34"/>
+    <hyperlink ref="Z11" r:id="rId35"/>
+    <hyperlink ref="AA11" r:id="rId36"/>
+    <hyperlink ref="H12" r:id="rId37"/>
+    <hyperlink ref="I12" r:id="rId38"/>
+    <hyperlink ref="Z12" r:id="rId39"/>
+    <hyperlink ref="AA12" r:id="rId40"/>
+    <hyperlink ref="H13" r:id="rId41"/>
+    <hyperlink ref="I13" r:id="rId42"/>
+    <hyperlink ref="Z13" r:id="rId43"/>
+    <hyperlink ref="AA13" r:id="rId44"/>
+    <hyperlink ref="H14" r:id="rId45"/>
+    <hyperlink ref="I14" r:id="rId46"/>
+    <hyperlink ref="Z14" r:id="rId47"/>
+    <hyperlink ref="AA14" r:id="rId48"/>
+    <hyperlink ref="H15" r:id="rId49"/>
+    <hyperlink ref="I15" r:id="rId50"/>
+    <hyperlink ref="Z15" r:id="rId51"/>
+    <hyperlink ref="AA15" r:id="rId52"/>
+    <hyperlink ref="H16" r:id="rId53"/>
+    <hyperlink ref="I16" r:id="rId54"/>
+    <hyperlink ref="Z16" r:id="rId55"/>
+    <hyperlink ref="AA16" r:id="rId56"/>
+    <hyperlink ref="H17" r:id="rId57"/>
+    <hyperlink ref="I17" r:id="rId58"/>
+    <hyperlink ref="Z17" r:id="rId59"/>
+    <hyperlink ref="AA17" r:id="rId60"/>
+    <hyperlink ref="H18" r:id="rId61"/>
+    <hyperlink ref="I18" r:id="rId62"/>
+    <hyperlink ref="Z18" r:id="rId63"/>
+    <hyperlink ref="AA18" r:id="rId64"/>
+    <hyperlink ref="H19" r:id="rId65"/>
+    <hyperlink ref="I19" r:id="rId66"/>
+    <hyperlink ref="Z19" r:id="rId67"/>
+    <hyperlink ref="AA19" r:id="rId68"/>
+    <hyperlink ref="H20" r:id="rId69"/>
+    <hyperlink ref="I20" r:id="rId70"/>
+    <hyperlink ref="Z20" r:id="rId71"/>
+    <hyperlink ref="AA20" r:id="rId72"/>
+    <hyperlink ref="H21" r:id="rId73"/>
+    <hyperlink ref="I21" r:id="rId74"/>
+    <hyperlink ref="Z21" r:id="rId75"/>
+    <hyperlink ref="AA21" r:id="rId76"/>
+    <hyperlink ref="H22" r:id="rId77"/>
+    <hyperlink ref="I22" r:id="rId78"/>
+    <hyperlink ref="Z22" r:id="rId79"/>
+    <hyperlink ref="AA22" r:id="rId80"/>
+    <hyperlink ref="H23" r:id="rId81"/>
+    <hyperlink ref="I23" r:id="rId82"/>
+    <hyperlink ref="Z23" r:id="rId83"/>
+    <hyperlink ref="AA23" r:id="rId84"/>
+    <hyperlink ref="H24" r:id="rId85"/>
+    <hyperlink ref="I24" r:id="rId86"/>
+    <hyperlink ref="Z24" r:id="rId87"/>
+    <hyperlink ref="AA24" r:id="rId88"/>
+    <hyperlink ref="H25" r:id="rId89"/>
+    <hyperlink ref="I25" r:id="rId90"/>
+    <hyperlink ref="Z25" r:id="rId91"/>
+    <hyperlink ref="AA25" r:id="rId92"/>
+    <hyperlink ref="H26" r:id="rId93"/>
+    <hyperlink ref="I26" r:id="rId94"/>
+    <hyperlink ref="Z26" r:id="rId95"/>
+    <hyperlink ref="AA26" r:id="rId96"/>
+    <hyperlink ref="H27" r:id="rId97"/>
+    <hyperlink ref="I27" r:id="rId98"/>
+    <hyperlink ref="Z27" r:id="rId99"/>
+    <hyperlink ref="AA27" r:id="rId100"/>
+    <hyperlink ref="H28" r:id="rId101"/>
+    <hyperlink ref="I28" r:id="rId102"/>
+    <hyperlink ref="Z28" r:id="rId103"/>
+    <hyperlink ref="AA28" r:id="rId104"/>
+    <hyperlink ref="H29" r:id="rId105"/>
+    <hyperlink ref="I29" r:id="rId106"/>
+    <hyperlink ref="Z29" r:id="rId107"/>
+    <hyperlink ref="AA29" r:id="rId108"/>
+    <hyperlink ref="H30" r:id="rId109"/>
+    <hyperlink ref="I30" r:id="rId110"/>
+    <hyperlink ref="Z30" r:id="rId111"/>
+    <hyperlink ref="AA30" r:id="rId112"/>
+    <hyperlink ref="H31" r:id="rId113"/>
+    <hyperlink ref="I31" r:id="rId114"/>
+    <hyperlink ref="Z31" r:id="rId115"/>
+    <hyperlink ref="AA31" r:id="rId116"/>
+    <hyperlink ref="H32" r:id="rId117"/>
+    <hyperlink ref="I32" r:id="rId118"/>
+    <hyperlink ref="Z32" r:id="rId119"/>
+    <hyperlink ref="AA32" r:id="rId120"/>
+    <hyperlink ref="H33" r:id="rId121"/>
+    <hyperlink ref="I33" r:id="rId122"/>
+    <hyperlink ref="Z33" r:id="rId123"/>
+    <hyperlink ref="AA33" r:id="rId124"/>
+    <hyperlink ref="H34" r:id="rId125"/>
+    <hyperlink ref="I34" r:id="rId126"/>
+    <hyperlink ref="Z34" r:id="rId127"/>
+    <hyperlink ref="AA34" r:id="rId128"/>
+    <hyperlink ref="H35" r:id="rId129"/>
+    <hyperlink ref="I35" r:id="rId130"/>
+    <hyperlink ref="Z35" r:id="rId131"/>
+    <hyperlink ref="AA35" r:id="rId132"/>
+    <hyperlink ref="H36" r:id="rId133"/>
+    <hyperlink ref="I36" r:id="rId134"/>
+    <hyperlink ref="Z36" r:id="rId135"/>
+    <hyperlink ref="AA36" r:id="rId136"/>
+    <hyperlink ref="H37" r:id="rId137"/>
+    <hyperlink ref="I37" r:id="rId138"/>
+    <hyperlink ref="Z37" r:id="rId139"/>
+    <hyperlink ref="AA37" r:id="rId140"/>
+    <hyperlink ref="H38" r:id="rId141"/>
+    <hyperlink ref="I38" r:id="rId142"/>
+    <hyperlink ref="Z38" r:id="rId143"/>
+    <hyperlink ref="AA38" r:id="rId144"/>
+    <hyperlink ref="H39" r:id="rId145"/>
+    <hyperlink ref="I39" r:id="rId146"/>
+    <hyperlink ref="Z39" r:id="rId147"/>
+    <hyperlink ref="AA39" r:id="rId148"/>
+    <hyperlink ref="H40" r:id="rId149"/>
+    <hyperlink ref="I40" r:id="rId150"/>
+    <hyperlink ref="Z40" r:id="rId151"/>
+    <hyperlink ref="AA40" r:id="rId152"/>
+    <hyperlink ref="H41" r:id="rId153"/>
+    <hyperlink ref="I41" r:id="rId154"/>
+    <hyperlink ref="Z41" r:id="rId155"/>
+    <hyperlink ref="AA41" r:id="rId156"/>
+    <hyperlink ref="H42" r:id="rId157"/>
+    <hyperlink ref="I42" r:id="rId158"/>
+    <hyperlink ref="Z42" r:id="rId159"/>
+    <hyperlink ref="AA42" r:id="rId160"/>
+    <hyperlink ref="H43" r:id="rId161"/>
+    <hyperlink ref="I43" r:id="rId162"/>
+    <hyperlink ref="Z43" r:id="rId163"/>
+    <hyperlink ref="AA43" r:id="rId164"/>
+    <hyperlink ref="H44" r:id="rId165"/>
+    <hyperlink ref="I44" r:id="rId166"/>
+    <hyperlink ref="Z44" r:id="rId167"/>
+    <hyperlink ref="AA44" r:id="rId168"/>
+    <hyperlink ref="H45" r:id="rId169"/>
+    <hyperlink ref="I45" r:id="rId170"/>
+    <hyperlink ref="Z45" r:id="rId171"/>
+    <hyperlink ref="AA45" r:id="rId172"/>
+    <hyperlink ref="H46" r:id="rId173"/>
+    <hyperlink ref="I46" r:id="rId174"/>
+    <hyperlink ref="Z46" r:id="rId175"/>
+    <hyperlink ref="AA46" r:id="rId176"/>
+    <hyperlink ref="H47" r:id="rId177"/>
+    <hyperlink ref="I47" r:id="rId178"/>
+    <hyperlink ref="Z47" r:id="rId179"/>
+    <hyperlink ref="AA47" r:id="rId180"/>
+    <hyperlink ref="H48" r:id="rId181"/>
+    <hyperlink ref="I48" r:id="rId182"/>
+    <hyperlink ref="Z48" r:id="rId183"/>
+    <hyperlink ref="AA48" r:id="rId184"/>
+    <hyperlink ref="H49" r:id="rId185"/>
+    <hyperlink ref="I49" r:id="rId186"/>
+    <hyperlink ref="Z49" r:id="rId187"/>
+    <hyperlink ref="AA49" r:id="rId188"/>
+    <hyperlink ref="H50" r:id="rId189"/>
+    <hyperlink ref="I50" r:id="rId190"/>
+    <hyperlink ref="Z50" r:id="rId191"/>
+    <hyperlink ref="AA50" r:id="rId192"/>
+    <hyperlink ref="H51" r:id="rId193"/>
+    <hyperlink ref="I51" r:id="rId194"/>
+    <hyperlink ref="Z51" r:id="rId195"/>
+    <hyperlink ref="AA51" r:id="rId196"/>
+    <hyperlink ref="H52" r:id="rId197"/>
+    <hyperlink ref="I52" r:id="rId198"/>
+    <hyperlink ref="Z52" r:id="rId199"/>
+    <hyperlink ref="AA52" r:id="rId200"/>
+    <hyperlink ref="H53" r:id="rId201"/>
+    <hyperlink ref="I53" r:id="rId202"/>
+    <hyperlink ref="Z53" r:id="rId203"/>
+    <hyperlink ref="AA53" r:id="rId204"/>
+    <hyperlink ref="H54" r:id="rId205"/>
+    <hyperlink ref="I54" r:id="rId206"/>
+    <hyperlink ref="Z54" r:id="rId207"/>
+    <hyperlink ref="AA54" r:id="rId208"/>
+    <hyperlink ref="H55" r:id="rId209"/>
+    <hyperlink ref="I55" r:id="rId210"/>
+    <hyperlink ref="Z55" r:id="rId211"/>
+    <hyperlink ref="AA55" r:id="rId212"/>
+    <hyperlink ref="H56" r:id="rId213"/>
+    <hyperlink ref="I56" r:id="rId214"/>
+    <hyperlink ref="Z56" r:id="rId215"/>
+    <hyperlink ref="AA56" r:id="rId216"/>
+    <hyperlink ref="H57" r:id="rId217"/>
+    <hyperlink ref="I57" r:id="rId218"/>
+    <hyperlink ref="Z57" r:id="rId219"/>
+    <hyperlink ref="AA57" r:id="rId220"/>
+    <hyperlink ref="H58" r:id="rId221"/>
+    <hyperlink ref="I58" r:id="rId222"/>
+    <hyperlink ref="Z58" r:id="rId223"/>
+    <hyperlink ref="AA58" r:id="rId224"/>
+    <hyperlink ref="H59" r:id="rId225"/>
+    <hyperlink ref="I59" r:id="rId226"/>
+    <hyperlink ref="Z59" r:id="rId227"/>
+    <hyperlink ref="AA59" r:id="rId228"/>
+    <hyperlink ref="H60" r:id="rId229"/>
+    <hyperlink ref="I60" r:id="rId230"/>
+    <hyperlink ref="Z60" r:id="rId231"/>
+    <hyperlink ref="AA60" r:id="rId232"/>
+    <hyperlink ref="H61" r:id="rId233"/>
+    <hyperlink ref="I61" r:id="rId234"/>
+    <hyperlink ref="Z61" r:id="rId235"/>
+    <hyperlink ref="AA61" r:id="rId236"/>
+    <hyperlink ref="H62" r:id="rId237"/>
+    <hyperlink ref="I62" r:id="rId238"/>
+    <hyperlink ref="Z62" r:id="rId239"/>
+    <hyperlink ref="AA62" r:id="rId240"/>
+    <hyperlink ref="H63" r:id="rId241"/>
+    <hyperlink ref="I63" r:id="rId242"/>
+    <hyperlink ref="Z63" r:id="rId243"/>
+    <hyperlink ref="AA63" r:id="rId244"/>
+    <hyperlink ref="H64" r:id="rId245"/>
+    <hyperlink ref="I64" r:id="rId246"/>
+    <hyperlink ref="Z64" r:id="rId247"/>
+    <hyperlink ref="AA64" r:id="rId248"/>
+    <hyperlink ref="H65" r:id="rId249"/>
+    <hyperlink ref="I65" r:id="rId250"/>
+    <hyperlink ref="Z65" r:id="rId251"/>
+    <hyperlink ref="AA65" r:id="rId252"/>
+    <hyperlink ref="H66" r:id="rId253"/>
+    <hyperlink ref="I66" r:id="rId254"/>
+    <hyperlink ref="Z66" r:id="rId255"/>
+    <hyperlink ref="AA66" r:id="rId256"/>
+    <hyperlink ref="H67" r:id="rId257"/>
+    <hyperlink ref="Z67" r:id="rId258"/>
+    <hyperlink ref="AA67" r:id="rId259"/>
+    <hyperlink ref="H68" r:id="rId260"/>
+    <hyperlink ref="Z68" r:id="rId261"/>
+    <hyperlink ref="H69" r:id="rId262"/>
+    <hyperlink ref="Z69" r:id="rId263"/>
+    <hyperlink ref="H70" r:id="rId264"/>
+    <hyperlink ref="Z70" r:id="rId265"/>
+    <hyperlink ref="H71" r:id="rId266"/>
+    <hyperlink ref="Z71" r:id="rId267"/>
+    <hyperlink ref="H72" r:id="rId268"/>
+    <hyperlink ref="Z72" r:id="rId269"/>
+    <hyperlink ref="H73" r:id="rId270"/>
+    <hyperlink ref="Z73" r:id="rId271"/>
+    <hyperlink ref="Z74" r:id="rId272"/>
+    <hyperlink ref="Z75" r:id="rId273"/>
+    <hyperlink ref="H77" r:id="rId274"/>
+    <hyperlink ref="I77" r:id="rId275"/>
+    <hyperlink ref="Z77" r:id="rId276"/>
+    <hyperlink ref="AA77" r:id="rId277"/>
+    <hyperlink ref="H78" r:id="rId278"/>
+    <hyperlink ref="I78" r:id="rId279"/>
+    <hyperlink ref="Z78" r:id="rId280"/>
+    <hyperlink ref="AA78" r:id="rId281"/>
+    <hyperlink ref="H79" r:id="rId282"/>
+    <hyperlink ref="I79" r:id="rId283"/>
+    <hyperlink ref="Z79" r:id="rId284"/>
+    <hyperlink ref="AA79" r:id="rId285"/>
+    <hyperlink ref="H80" r:id="rId286"/>
+    <hyperlink ref="I80" r:id="rId287"/>
+    <hyperlink ref="Z80" r:id="rId288"/>
+    <hyperlink ref="AA80" r:id="rId289"/>
+    <hyperlink ref="H81" r:id="rId290"/>
+    <hyperlink ref="I81" r:id="rId291"/>
+    <hyperlink ref="Z81" r:id="rId292"/>
+    <hyperlink ref="AA81" r:id="rId293"/>
+    <hyperlink ref="H82" r:id="rId294"/>
+    <hyperlink ref="I82" r:id="rId295"/>
+    <hyperlink ref="Z82" r:id="rId296"/>
+    <hyperlink ref="AA82" r:id="rId297"/>
+    <hyperlink ref="H83" r:id="rId298"/>
+    <hyperlink ref="I83" r:id="rId299"/>
+    <hyperlink ref="Z83" r:id="rId300"/>
+    <hyperlink ref="AA83" r:id="rId301"/>
+    <hyperlink ref="H84" r:id="rId302"/>
+    <hyperlink ref="I84" r:id="rId303"/>
+    <hyperlink ref="Z84" r:id="rId304"/>
+    <hyperlink ref="AA84" r:id="rId305"/>
+    <hyperlink ref="H85" r:id="rId306"/>
+    <hyperlink ref="I85" r:id="rId307"/>
+    <hyperlink ref="Z85" r:id="rId308"/>
+    <hyperlink ref="AA85" r:id="rId309"/>
+    <hyperlink ref="H86" r:id="rId310"/>
+    <hyperlink ref="I86" r:id="rId311"/>
+    <hyperlink ref="Z86" r:id="rId312"/>
+    <hyperlink ref="AA86" r:id="rId313"/>
+    <hyperlink ref="H87" r:id="rId314"/>
+    <hyperlink ref="I87" r:id="rId315"/>
+    <hyperlink ref="Z87" r:id="rId316"/>
+    <hyperlink ref="AA87" r:id="rId317"/>
+    <hyperlink ref="H88" r:id="rId318"/>
+    <hyperlink ref="I88" r:id="rId319"/>
+    <hyperlink ref="Z88" r:id="rId320"/>
+    <hyperlink ref="AA88" r:id="rId321"/>
+    <hyperlink ref="H89" r:id="rId322"/>
+    <hyperlink ref="I89" r:id="rId323"/>
+    <hyperlink ref="Z89" r:id="rId324"/>
+    <hyperlink ref="AA89" r:id="rId325"/>
+    <hyperlink ref="H90" r:id="rId326"/>
+    <hyperlink ref="I90" r:id="rId327"/>
+    <hyperlink ref="Z90" r:id="rId328"/>
+    <hyperlink ref="AA90" r:id="rId329"/>
+    <hyperlink ref="H91" r:id="rId330"/>
+    <hyperlink ref="I91" r:id="rId331"/>
+    <hyperlink ref="Z91" r:id="rId332"/>
+    <hyperlink ref="AA91" r:id="rId333"/>
+    <hyperlink ref="H92" r:id="rId334"/>
+    <hyperlink ref="I92" r:id="rId335"/>
+    <hyperlink ref="Z92" r:id="rId336"/>
+    <hyperlink ref="AA92" r:id="rId337"/>
+    <hyperlink ref="H93" r:id="rId338"/>
+    <hyperlink ref="I93" r:id="rId339"/>
+    <hyperlink ref="Z93" r:id="rId340"/>
+    <hyperlink ref="AA93" r:id="rId341"/>
+    <hyperlink ref="H94" r:id="rId342"/>
+    <hyperlink ref="I94" r:id="rId343"/>
+    <hyperlink ref="Z94" r:id="rId344"/>
+    <hyperlink ref="AA94" r:id="rId345"/>
+    <hyperlink ref="H95" r:id="rId346"/>
+    <hyperlink ref="I95" r:id="rId347"/>
+    <hyperlink ref="Z95" r:id="rId348"/>
+    <hyperlink ref="AA95" r:id="rId349"/>
+    <hyperlink ref="H96" r:id="rId350"/>
+    <hyperlink ref="I96" r:id="rId351"/>
+    <hyperlink ref="Z96" r:id="rId352"/>
+    <hyperlink ref="AA96" r:id="rId353"/>
+    <hyperlink ref="H97" r:id="rId354"/>
+    <hyperlink ref="I97" r:id="rId355"/>
+    <hyperlink ref="Z97" r:id="rId356"/>
+    <hyperlink ref="AA97" r:id="rId357"/>
+    <hyperlink ref="H98" r:id="rId358"/>
+    <hyperlink ref="I98" r:id="rId359"/>
+    <hyperlink ref="Z98" r:id="rId360"/>
+    <hyperlink ref="AA98" r:id="rId361"/>
+    <hyperlink ref="H99" r:id="rId362"/>
+    <hyperlink ref="I99" r:id="rId363"/>
+    <hyperlink ref="Z99" r:id="rId364"/>
+    <hyperlink ref="AA99" r:id="rId365"/>
+    <hyperlink ref="H100" r:id="rId366"/>
+    <hyperlink ref="I100" r:id="rId367"/>
+    <hyperlink ref="Z100" r:id="rId368"/>
+    <hyperlink ref="AA100" r:id="rId369"/>
+    <hyperlink ref="H101" r:id="rId370"/>
+    <hyperlink ref="I101" r:id="rId371"/>
+    <hyperlink ref="Z101" r:id="rId372"/>
+    <hyperlink ref="AA101" r:id="rId373"/>
+    <hyperlink ref="H102" r:id="rId374"/>
+    <hyperlink ref="I102" r:id="rId375"/>
+    <hyperlink ref="Z102" r:id="rId376"/>
+    <hyperlink ref="AA102" r:id="rId377"/>
+    <hyperlink ref="H103" r:id="rId378"/>
+    <hyperlink ref="I103" r:id="rId379"/>
+    <hyperlink ref="Z103" r:id="rId380"/>
+    <hyperlink ref="AA103" r:id="rId381"/>
+    <hyperlink ref="H104" r:id="rId382"/>
+    <hyperlink ref="I104" r:id="rId383"/>
+    <hyperlink ref="Z104" r:id="rId384"/>
+    <hyperlink ref="AA104" r:id="rId385"/>
+    <hyperlink ref="H105" r:id="rId386"/>
+    <hyperlink ref="I105" r:id="rId387"/>
+    <hyperlink ref="Z105" r:id="rId388"/>
+    <hyperlink ref="AA105" r:id="rId389"/>
+    <hyperlink ref="H106" r:id="rId390"/>
+    <hyperlink ref="I106" r:id="rId391"/>
+    <hyperlink ref="Z106" r:id="rId392"/>
+    <hyperlink ref="AA106" r:id="rId393"/>
+    <hyperlink ref="H107" r:id="rId394"/>
+    <hyperlink ref="I107" r:id="rId395"/>
+    <hyperlink ref="Z107" r:id="rId396"/>
+    <hyperlink ref="AA107" r:id="rId397"/>
+    <hyperlink ref="H108" r:id="rId398"/>
+    <hyperlink ref="I108" r:id="rId399"/>
+    <hyperlink ref="Z108" r:id="rId400"/>
+    <hyperlink ref="AA108" r:id="rId401"/>
+    <hyperlink ref="H109" r:id="rId402"/>
+    <hyperlink ref="I109" r:id="rId403"/>
+    <hyperlink ref="Z109" r:id="rId404"/>
+    <hyperlink ref="AA109" r:id="rId405"/>
+    <hyperlink ref="H110" r:id="rId406"/>
+    <hyperlink ref="I110" r:id="rId407"/>
+    <hyperlink ref="Z110" r:id="rId408"/>
+    <hyperlink ref="AA110" r:id="rId409"/>
+    <hyperlink ref="H111" r:id="rId410"/>
+    <hyperlink ref="I111" r:id="rId411"/>
+    <hyperlink ref="Z111" r:id="rId412"/>
+    <hyperlink ref="AA111" r:id="rId413"/>
+    <hyperlink ref="H112" r:id="rId414"/>
+    <hyperlink ref="I112" r:id="rId415"/>
+    <hyperlink ref="Z112" r:id="rId416"/>
+    <hyperlink ref="AA112" r:id="rId417"/>
+    <hyperlink ref="H113" r:id="rId418"/>
+    <hyperlink ref="I113" r:id="rId419"/>
+    <hyperlink ref="Z113" r:id="rId420"/>
+    <hyperlink ref="AA113" r:id="rId421"/>
+    <hyperlink ref="H114" r:id="rId422"/>
+    <hyperlink ref="I114" r:id="rId423"/>
+    <hyperlink ref="Z114" r:id="rId424"/>
+    <hyperlink ref="AA114" r:id="rId425"/>
+    <hyperlink ref="H115" r:id="rId426"/>
+    <hyperlink ref="I115" r:id="rId427"/>
+    <hyperlink ref="Z115" r:id="rId428"/>
+    <hyperlink ref="AA115" r:id="rId429"/>
+    <hyperlink ref="H116" r:id="rId430"/>
+    <hyperlink ref="I116" r:id="rId431"/>
+    <hyperlink ref="Z116" r:id="rId432"/>
+    <hyperlink ref="AA116" r:id="rId433"/>
+    <hyperlink ref="H117" r:id="rId434"/>
+    <hyperlink ref="I117" r:id="rId435"/>
+    <hyperlink ref="Z117" r:id="rId436"/>
+    <hyperlink ref="AA117" r:id="rId437"/>
+    <hyperlink ref="H118" r:id="rId438"/>
+    <hyperlink ref="I118" r:id="rId439"/>
+    <hyperlink ref="Z118" r:id="rId440"/>
+    <hyperlink ref="AA118" r:id="rId441"/>
+    <hyperlink ref="H119" r:id="rId442"/>
+    <hyperlink ref="I119" r:id="rId443"/>
+    <hyperlink ref="Z119" r:id="rId444"/>
+    <hyperlink ref="AA119" r:id="rId445"/>
+    <hyperlink ref="H120" r:id="rId446"/>
+    <hyperlink ref="I120" r:id="rId447"/>
+    <hyperlink ref="Z120" r:id="rId448"/>
+    <hyperlink ref="AA120" r:id="rId449"/>
+    <hyperlink ref="H121" r:id="rId450"/>
+    <hyperlink ref="I121" r:id="rId451"/>
+    <hyperlink ref="Z121" r:id="rId452"/>
+    <hyperlink ref="AA121" r:id="rId453"/>
+    <hyperlink ref="H122" r:id="rId454"/>
+    <hyperlink ref="I122" r:id="rId455"/>
+    <hyperlink ref="Z122" r:id="rId456"/>
+    <hyperlink ref="AA122" r:id="rId457"/>
+    <hyperlink ref="H123" r:id="rId458"/>
+    <hyperlink ref="I123" r:id="rId459"/>
+    <hyperlink ref="Z123" r:id="rId460"/>
+    <hyperlink ref="AA123" r:id="rId461"/>
+    <hyperlink ref="H124" r:id="rId462"/>
+    <hyperlink ref="I124" r:id="rId463"/>
+    <hyperlink ref="Z124" r:id="rId464"/>
+    <hyperlink ref="AA124" r:id="rId465"/>
+    <hyperlink ref="H125" r:id="rId466"/>
+    <hyperlink ref="I125" r:id="rId467"/>
+    <hyperlink ref="Z125" r:id="rId468"/>
+    <hyperlink ref="AA125" r:id="rId469"/>
+    <hyperlink ref="H126" r:id="rId470"/>
+    <hyperlink ref="I126" r:id="rId471"/>
+    <hyperlink ref="Z126" r:id="rId472"/>
+    <hyperlink ref="AA126" r:id="rId473"/>
+    <hyperlink ref="H127" r:id="rId474"/>
+    <hyperlink ref="I127" r:id="rId475"/>
+    <hyperlink ref="Z127" r:id="rId476"/>
+    <hyperlink ref="AA127" r:id="rId477"/>
+    <hyperlink ref="H128" r:id="rId478"/>
+    <hyperlink ref="I128" r:id="rId479"/>
+    <hyperlink ref="Z128" r:id="rId480"/>
+    <hyperlink ref="AA128" r:id="rId481"/>
+    <hyperlink ref="H129" r:id="rId482"/>
+    <hyperlink ref="I129" r:id="rId483"/>
+    <hyperlink ref="Z129" r:id="rId484"/>
+    <hyperlink ref="AA129" r:id="rId485"/>
+    <hyperlink ref="H130" r:id="rId486"/>
+    <hyperlink ref="I130" r:id="rId487"/>
+    <hyperlink ref="Z130" r:id="rId488"/>
+    <hyperlink ref="AA130" r:id="rId489"/>
+    <hyperlink ref="H131" r:id="rId490"/>
+    <hyperlink ref="I131" r:id="rId491"/>
+    <hyperlink ref="Z131" r:id="rId492"/>
+    <hyperlink ref="AA131" r:id="rId493"/>
+    <hyperlink ref="H132" r:id="rId494"/>
+    <hyperlink ref="I132" r:id="rId495"/>
+    <hyperlink ref="Z132" r:id="rId496"/>
+    <hyperlink ref="AA132" r:id="rId497"/>
+    <hyperlink ref="H133" r:id="rId498"/>
+    <hyperlink ref="I133" r:id="rId499"/>
+    <hyperlink ref="Z133" r:id="rId500"/>
+    <hyperlink ref="AA133" r:id="rId501"/>
+    <hyperlink ref="H134" r:id="rId502"/>
+    <hyperlink ref="I134" r:id="rId503"/>
+    <hyperlink ref="Z134" r:id="rId504"/>
+    <hyperlink ref="AA134" r:id="rId505"/>
+    <hyperlink ref="H135" r:id="rId506"/>
+    <hyperlink ref="I135" r:id="rId507"/>
+    <hyperlink ref="Z135" r:id="rId508"/>
+    <hyperlink ref="AA135" r:id="rId509"/>
+    <hyperlink ref="H136" r:id="rId510"/>
+    <hyperlink ref="I136" r:id="rId511"/>
+    <hyperlink ref="Z136" r:id="rId512"/>
+    <hyperlink ref="AA136" r:id="rId513"/>
+    <hyperlink ref="H137" r:id="rId514"/>
+    <hyperlink ref="I137" r:id="rId515"/>
+    <hyperlink ref="Z137" r:id="rId516"/>
+    <hyperlink ref="AA137" r:id="rId517"/>
+    <hyperlink ref="H138" r:id="rId518"/>
+    <hyperlink ref="I138" r:id="rId519"/>
+    <hyperlink ref="Z138" r:id="rId520"/>
+    <hyperlink ref="AA138" r:id="rId521"/>
+    <hyperlink ref="H139" r:id="rId522"/>
+    <hyperlink ref="I139" r:id="rId523"/>
+    <hyperlink ref="Z139" r:id="rId524"/>
+    <hyperlink ref="AA139" r:id="rId525"/>
+    <hyperlink ref="H140" r:id="rId526"/>
+    <hyperlink ref="I140" r:id="rId527"/>
+    <hyperlink ref="Z140" r:id="rId528"/>
+    <hyperlink ref="AA140" r:id="rId529"/>
+    <hyperlink ref="H141" r:id="rId530"/>
+    <hyperlink ref="I141" r:id="rId531"/>
+    <hyperlink ref="Z141" r:id="rId532"/>
+    <hyperlink ref="AA141" r:id="rId533"/>
+    <hyperlink ref="H142" r:id="rId534"/>
+    <hyperlink ref="I142" r:id="rId535"/>
+    <hyperlink ref="Z142" r:id="rId536"/>
+    <hyperlink ref="AA142" r:id="rId537"/>
+    <hyperlink ref="H143" r:id="rId538"/>
+    <hyperlink ref="I143" r:id="rId539"/>
+    <hyperlink ref="Z143" r:id="rId540"/>
+    <hyperlink ref="AA143" r:id="rId541"/>
+    <hyperlink ref="H144" r:id="rId542"/>
+    <hyperlink ref="I144" r:id="rId543"/>
+    <hyperlink ref="Z144" r:id="rId544"/>
+    <hyperlink ref="AA144" r:id="rId545"/>
+    <hyperlink ref="H145" r:id="rId546"/>
+    <hyperlink ref="I145" r:id="rId547"/>
+    <hyperlink ref="Z145" r:id="rId548"/>
+    <hyperlink ref="AA145" r:id="rId549"/>
+    <hyperlink ref="H146" r:id="rId550"/>
+    <hyperlink ref="I146" r:id="rId551"/>
+    <hyperlink ref="Z146" r:id="rId552"/>
+    <hyperlink ref="AA146" r:id="rId553"/>
+    <hyperlink ref="H147" r:id="rId554"/>
+    <hyperlink ref="I147" r:id="rId555"/>
+    <hyperlink ref="Z147" r:id="rId556"/>
+    <hyperlink ref="AA147" r:id="rId557"/>
+    <hyperlink ref="Z148" r:id="rId558"/>
+    <hyperlink ref="AA148" r:id="rId559"/>
+    <hyperlink ref="Z149" r:id="rId560"/>
+    <hyperlink ref="AA149" r:id="rId561"/>
+    <hyperlink ref="H151" r:id="rId562"/>
+    <hyperlink ref="I151" r:id="rId563"/>
+    <hyperlink ref="Z151" r:id="rId564"/>
+    <hyperlink ref="AA151" r:id="rId565"/>
+    <hyperlink ref="H152" r:id="rId566"/>
+    <hyperlink ref="I152" r:id="rId567"/>
+    <hyperlink ref="Z152" r:id="rId568"/>
+    <hyperlink ref="AA152" r:id="rId569"/>
+    <hyperlink ref="H153" r:id="rId570"/>
+    <hyperlink ref="I153" r:id="rId571"/>
+    <hyperlink ref="Z153" r:id="rId572"/>
+    <hyperlink ref="AA153" r:id="rId573"/>
+    <hyperlink ref="H154" r:id="rId574"/>
+    <hyperlink ref="I154" r:id="rId575"/>
+    <hyperlink ref="Z154" r:id="rId576"/>
+    <hyperlink ref="AA154" r:id="rId577"/>
+    <hyperlink ref="H155" r:id="rId578"/>
+    <hyperlink ref="I155" r:id="rId579"/>
+    <hyperlink ref="Z155" r:id="rId580"/>
+    <hyperlink ref="AA155" r:id="rId581"/>
+    <hyperlink ref="H156" r:id="rId582"/>
+    <hyperlink ref="I156" r:id="rId583"/>
+    <hyperlink ref="Z156" r:id="rId584"/>
+    <hyperlink ref="AA156" r:id="rId585"/>
+    <hyperlink ref="H157" r:id="rId586"/>
+    <hyperlink ref="I157" r:id="rId587"/>
+    <hyperlink ref="Z157" r:id="rId588"/>
+    <hyperlink ref="AA157" r:id="rId589"/>
+    <hyperlink ref="H158" r:id="rId590"/>
+    <hyperlink ref="I158" r:id="rId591"/>
+    <hyperlink ref="Z158" r:id="rId592"/>
+    <hyperlink ref="AA158" r:id="rId593"/>
+    <hyperlink ref="H159" r:id="rId594"/>
+    <hyperlink ref="I159" r:id="rId595"/>
+    <hyperlink ref="Z159" r:id="rId596"/>
+    <hyperlink ref="AA159" r:id="rId597"/>
+    <hyperlink ref="H160" r:id="rId598"/>
+    <hyperlink ref="I160" r:id="rId599"/>
+    <hyperlink ref="Z160" r:id="rId600"/>
+    <hyperlink ref="AA160" r:id="rId601"/>
+    <hyperlink ref="H161" r:id="rId602"/>
+    <hyperlink ref="I161" r:id="rId603"/>
+    <hyperlink ref="Z161" r:id="rId604"/>
+    <hyperlink ref="AA161" r:id="rId605"/>
+    <hyperlink ref="H162" r:id="rId606"/>
+    <hyperlink ref="I162" r:id="rId607"/>
+    <hyperlink ref="Z162" r:id="rId608"/>
+    <hyperlink ref="AA162" r:id="rId609"/>
+    <hyperlink ref="H163" r:id="rId610"/>
+    <hyperlink ref="I163" r:id="rId611"/>
+    <hyperlink ref="Z163" r:id="rId612"/>
+    <hyperlink ref="AA163" r:id="rId613"/>
+    <hyperlink ref="H164" r:id="rId614"/>
+    <hyperlink ref="I164" r:id="rId615"/>
+    <hyperlink ref="Z164" r:id="rId616"/>
+    <hyperlink ref="AA164" r:id="rId617"/>
+    <hyperlink ref="H165" r:id="rId618"/>
+    <hyperlink ref="I165" r:id="rId619"/>
+    <hyperlink ref="Z165" r:id="rId620"/>
+    <hyperlink ref="AA165" r:id="rId621"/>
+    <hyperlink ref="H166" r:id="rId622"/>
+    <hyperlink ref="I166" r:id="rId623"/>
+    <hyperlink ref="Z166" r:id="rId624"/>
+    <hyperlink ref="AA166" r:id="rId625"/>
+    <hyperlink ref="H167" r:id="rId626"/>
+    <hyperlink ref="I167" r:id="rId627"/>
+    <hyperlink ref="Z167" r:id="rId628"/>
+    <hyperlink ref="AA167" r:id="rId629"/>
+    <hyperlink ref="H168" r:id="rId630"/>
+    <hyperlink ref="I168" r:id="rId631"/>
+    <hyperlink ref="Z168" r:id="rId632"/>
+    <hyperlink ref="AA168" r:id="rId633"/>
+    <hyperlink ref="H169" r:id="rId634"/>
+    <hyperlink ref="I169" r:id="rId635"/>
+    <hyperlink ref="Z169" r:id="rId636"/>
+    <hyperlink ref="AA169" r:id="rId637"/>
+    <hyperlink ref="H170" r:id="rId638"/>
+    <hyperlink ref="I170" r:id="rId639"/>
+    <hyperlink ref="Z170" r:id="rId640"/>
+    <hyperlink ref="AA170" r:id="rId641"/>
+    <hyperlink ref="H171" r:id="rId642"/>
+    <hyperlink ref="I171" r:id="rId643"/>
+    <hyperlink ref="Z171" r:id="rId644"/>
+    <hyperlink ref="AA171" r:id="rId645"/>
+    <hyperlink ref="H172" r:id="rId646"/>
+    <hyperlink ref="I172" r:id="rId647"/>
+    <hyperlink ref="Z172" r:id="rId648"/>
+    <hyperlink ref="AA172" r:id="rId649"/>
+    <hyperlink ref="H173" r:id="rId650"/>
+    <hyperlink ref="I173" r:id="rId651"/>
+    <hyperlink ref="Z173" r:id="rId652"/>
+    <hyperlink ref="AA173" r:id="rId653"/>
+    <hyperlink ref="H174" r:id="rId654"/>
+    <hyperlink ref="I174" r:id="rId655"/>
+    <hyperlink ref="Z174" r:id="rId656"/>
+    <hyperlink ref="AA174" r:id="rId657"/>
+    <hyperlink ref="H175" r:id="rId658"/>
+    <hyperlink ref="I175" r:id="rId659"/>
+    <hyperlink ref="Z175" r:id="rId660"/>
+    <hyperlink ref="AA175" r:id="rId661"/>
+    <hyperlink ref="H176" r:id="rId662"/>
+    <hyperlink ref="I176" r:id="rId663"/>
+    <hyperlink ref="Z176" r:id="rId664"/>
+    <hyperlink ref="AA176" r:id="rId665"/>
+    <hyperlink ref="H177" r:id="rId666"/>
+    <hyperlink ref="I177" r:id="rId667"/>
+    <hyperlink ref="Z177" r:id="rId668"/>
+    <hyperlink ref="AA177" r:id="rId669"/>
+    <hyperlink ref="H178" r:id="rId670"/>
+    <hyperlink ref="I178" r:id="rId671"/>
+    <hyperlink ref="Z178" r:id="rId672"/>
+    <hyperlink ref="AA178" r:id="rId673"/>
+    <hyperlink ref="H179" r:id="rId674"/>
+    <hyperlink ref="I179" r:id="rId675"/>
+    <hyperlink ref="Z179" r:id="rId676"/>
+    <hyperlink ref="AA179" r:id="rId677"/>
+    <hyperlink ref="H180" r:id="rId678"/>
+    <hyperlink ref="I180" r:id="rId679"/>
+    <hyperlink ref="Z180" r:id="rId680"/>
+    <hyperlink ref="AA180" r:id="rId681"/>
+    <hyperlink ref="H181" r:id="rId682"/>
+    <hyperlink ref="I181" r:id="rId683"/>
+    <hyperlink ref="Z181" r:id="rId684"/>
+    <hyperlink ref="AA181" r:id="rId685"/>
+    <hyperlink ref="H182" r:id="rId686"/>
+    <hyperlink ref="I182" r:id="rId687"/>
+    <hyperlink ref="Z182" r:id="rId688"/>
+    <hyperlink ref="AA182" r:id="rId689"/>
+    <hyperlink ref="H183" r:id="rId690"/>
+    <hyperlink ref="I183" r:id="rId691"/>
+    <hyperlink ref="Z183" r:id="rId692"/>
+    <hyperlink ref="AA183" r:id="rId693"/>
+    <hyperlink ref="H184" r:id="rId694"/>
+    <hyperlink ref="I184" r:id="rId695"/>
+    <hyperlink ref="Z184" r:id="rId696"/>
+    <hyperlink ref="AA184" r:id="rId697"/>
+    <hyperlink ref="H185" r:id="rId698"/>
+    <hyperlink ref="I185" r:id="rId699"/>
+    <hyperlink ref="Z185" r:id="rId700"/>
+    <hyperlink ref="AA185" r:id="rId701"/>
+    <hyperlink ref="H186" r:id="rId702"/>
+    <hyperlink ref="I186" r:id="rId703"/>
+    <hyperlink ref="Z186" r:id="rId704"/>
+    <hyperlink ref="AA186" r:id="rId705"/>
+    <hyperlink ref="H187" r:id="rId706"/>
+    <hyperlink ref="I187" r:id="rId707"/>
+    <hyperlink ref="Z187" r:id="rId708"/>
+    <hyperlink ref="AA187" r:id="rId709"/>
+    <hyperlink ref="H188" r:id="rId710"/>
+    <hyperlink ref="I188" r:id="rId711"/>
+    <hyperlink ref="Z188" r:id="rId712"/>
+    <hyperlink ref="AA188" r:id="rId713"/>
+    <hyperlink ref="H189" r:id="rId714"/>
+    <hyperlink ref="I189" r:id="rId715"/>
+    <hyperlink ref="Z189" r:id="rId716"/>
+    <hyperlink ref="AA189" r:id="rId717"/>
+    <hyperlink ref="H190" r:id="rId718"/>
+    <hyperlink ref="I190" r:id="rId719"/>
+    <hyperlink ref="Z190" r:id="rId720"/>
+    <hyperlink ref="AA190" r:id="rId721"/>
+    <hyperlink ref="H191" r:id="rId722"/>
+    <hyperlink ref="I191" r:id="rId723"/>
+    <hyperlink ref="Z191" r:id="rId724"/>
+    <hyperlink ref="AA191" r:id="rId725"/>
+    <hyperlink ref="H192" r:id="rId726"/>
+    <hyperlink ref="I192" r:id="rId727"/>
+    <hyperlink ref="Z192" r:id="rId728"/>
+    <hyperlink ref="AA192" r:id="rId729"/>
+    <hyperlink ref="H193" r:id="rId730"/>
+    <hyperlink ref="I193" r:id="rId731"/>
+    <hyperlink ref="Z193" r:id="rId732"/>
+    <hyperlink ref="AA193" r:id="rId733"/>
+    <hyperlink ref="H194" r:id="rId734"/>
+    <hyperlink ref="I194" r:id="rId735"/>
+    <hyperlink ref="Z194" r:id="rId736"/>
+    <hyperlink ref="AA194" r:id="rId737"/>
+    <hyperlink ref="H195" r:id="rId738"/>
+    <hyperlink ref="I195" r:id="rId739"/>
+    <hyperlink ref="Z195" r:id="rId740"/>
+    <hyperlink ref="AA195" r:id="rId741"/>
+    <hyperlink ref="H196" r:id="rId742"/>
+    <hyperlink ref="I196" r:id="rId743"/>
+    <hyperlink ref="Z196" r:id="rId744"/>
+    <hyperlink ref="AA196" r:id="rId745"/>
+    <hyperlink ref="H197" r:id="rId746"/>
+    <hyperlink ref="I197" r:id="rId747"/>
+    <hyperlink ref="Z197" r:id="rId748"/>
+    <hyperlink ref="AA197" r:id="rId749"/>
+    <hyperlink ref="H198" r:id="rId750"/>
+    <hyperlink ref="I198" r:id="rId751"/>
+    <hyperlink ref="Z198" r:id="rId752"/>
+    <hyperlink ref="AA198" r:id="rId753"/>
+    <hyperlink ref="H199" r:id="rId754"/>
+    <hyperlink ref="I199" r:id="rId755"/>
+    <hyperlink ref="Z199" r:id="rId756"/>
+    <hyperlink ref="AA199" r:id="rId757"/>
+    <hyperlink ref="H200" r:id="rId758"/>
+    <hyperlink ref="I200" r:id="rId759"/>
+    <hyperlink ref="Z200" r:id="rId760"/>
+    <hyperlink ref="AA200" r:id="rId761"/>
+    <hyperlink ref="H201" r:id="rId762"/>
+    <hyperlink ref="I201" r:id="rId763"/>
+    <hyperlink ref="Z201" r:id="rId764"/>
+    <hyperlink ref="AA201" r:id="rId765"/>
+    <hyperlink ref="H202" r:id="rId766"/>
+    <hyperlink ref="I202" r:id="rId767"/>
+    <hyperlink ref="Z202" r:id="rId768"/>
+    <hyperlink ref="AA202" r:id="rId769"/>
+    <hyperlink ref="H203" r:id="rId770"/>
+    <hyperlink ref="I203" r:id="rId771"/>
+    <hyperlink ref="Z203" r:id="rId772"/>
+    <hyperlink ref="AA203" r:id="rId773"/>
+    <hyperlink ref="H204" r:id="rId774"/>
+    <hyperlink ref="I204" r:id="rId775"/>
+    <hyperlink ref="Z204" r:id="rId776"/>
+    <hyperlink ref="AA204" r:id="rId777"/>
+    <hyperlink ref="H205" r:id="rId778"/>
+    <hyperlink ref="I205" r:id="rId779"/>
+    <hyperlink ref="Z205" r:id="rId780"/>
+    <hyperlink ref="AA205" r:id="rId781"/>
+    <hyperlink ref="H206" r:id="rId782"/>
+    <hyperlink ref="I206" r:id="rId783"/>
+    <hyperlink ref="Z206" r:id="rId784"/>
+    <hyperlink ref="AA206" r:id="rId785"/>
+    <hyperlink ref="H207" r:id="rId786"/>
+    <hyperlink ref="I207" r:id="rId787"/>
+    <hyperlink ref="Z207" r:id="rId788"/>
+    <hyperlink ref="AA207" r:id="rId789"/>
+    <hyperlink ref="H208" r:id="rId790"/>
+    <hyperlink ref="I208" r:id="rId791"/>
+    <hyperlink ref="Z208" r:id="rId792"/>
+    <hyperlink ref="AA208" r:id="rId793"/>
+    <hyperlink ref="H209" r:id="rId794"/>
+    <hyperlink ref="I209" r:id="rId795"/>
+    <hyperlink ref="Z209" r:id="rId796"/>
+    <hyperlink ref="AA209" r:id="rId797"/>
+    <hyperlink ref="H210" r:id="rId798"/>
+    <hyperlink ref="I210" r:id="rId799"/>
+    <hyperlink ref="Z210" r:id="rId800"/>
+    <hyperlink ref="AA210" r:id="rId801"/>
+    <hyperlink ref="H211" r:id="rId802"/>
+    <hyperlink ref="I211" r:id="rId803"/>
+    <hyperlink ref="Z211" r:id="rId804"/>
+    <hyperlink ref="AA211" r:id="rId805"/>
+    <hyperlink ref="H212" r:id="rId806"/>
+    <hyperlink ref="I212" r:id="rId807"/>
+    <hyperlink ref="Z212" r:id="rId808"/>
+    <hyperlink ref="AA212" r:id="rId809"/>
+    <hyperlink ref="H213" r:id="rId810"/>
+    <hyperlink ref="I213" r:id="rId811"/>
+    <hyperlink ref="Z213" r:id="rId812"/>
+    <hyperlink ref="AA213" r:id="rId813"/>
+    <hyperlink ref="H214" r:id="rId814"/>
+    <hyperlink ref="I214" r:id="rId815"/>
+    <hyperlink ref="Z214" r:id="rId816"/>
+    <hyperlink ref="AA214" r:id="rId817"/>
+    <hyperlink ref="H215" r:id="rId818"/>
+    <hyperlink ref="I215" r:id="rId819"/>
+    <hyperlink ref="Z215" r:id="rId820"/>
+    <hyperlink ref="AA215" r:id="rId821"/>
+    <hyperlink ref="H216" r:id="rId822"/>
+    <hyperlink ref="I216" r:id="rId823"/>
+    <hyperlink ref="Z216" r:id="rId824"/>
+    <hyperlink ref="AA216" r:id="rId825"/>
+    <hyperlink ref="H217" r:id="rId826"/>
+    <hyperlink ref="I217" r:id="rId827"/>
+    <hyperlink ref="Z217" r:id="rId828"/>
+    <hyperlink ref="AA217" r:id="rId829"/>
+    <hyperlink ref="H218" r:id="rId830"/>
+    <hyperlink ref="I218" r:id="rId831"/>
+    <hyperlink ref="Z218" r:id="rId832"/>
+    <hyperlink ref="AA218" r:id="rId833"/>
+    <hyperlink ref="H219" r:id="rId834"/>
+    <hyperlink ref="I219" r:id="rId835"/>
+    <hyperlink ref="Z219" r:id="rId836"/>
+    <hyperlink ref="AA219" r:id="rId837"/>
+    <hyperlink ref="H220" r:id="rId838"/>
+    <hyperlink ref="I220" r:id="rId839"/>
+    <hyperlink ref="Z220" r:id="rId840"/>
+    <hyperlink ref="AA220" r:id="rId841"/>
+    <hyperlink ref="H221" r:id="rId842"/>
+    <hyperlink ref="I221" r:id="rId843"/>
+    <hyperlink ref="Z221" r:id="rId844"/>
+    <hyperlink ref="AA221" r:id="rId845"/>
+    <hyperlink ref="Z222" r:id="rId846"/>
+    <hyperlink ref="AA222" r:id="rId847"/>
+    <hyperlink ref="Z223" r:id="rId848"/>
+    <hyperlink ref="AA223" r:id="rId849"/>
+    <hyperlink ref="H225" r:id="rId850"/>
+    <hyperlink ref="I225" r:id="rId851"/>
+    <hyperlink ref="Z225" r:id="rId852"/>
+    <hyperlink ref="AA225" r:id="rId853"/>
+    <hyperlink ref="H226" r:id="rId854"/>
+    <hyperlink ref="I226" r:id="rId855"/>
+    <hyperlink ref="Z226" r:id="rId856"/>
+    <hyperlink ref="AA226" r:id="rId857"/>
+    <hyperlink ref="H227" r:id="rId858"/>
+    <hyperlink ref="I227" r:id="rId859"/>
+    <hyperlink ref="Z227" r:id="rId860"/>
+    <hyperlink ref="AA227" r:id="rId861"/>
+    <hyperlink ref="H228" r:id="rId862"/>
+    <hyperlink ref="I228" r:id="rId863"/>
+    <hyperlink ref="Z228" r:id="rId864"/>
+    <hyperlink ref="AA228" r:id="rId865"/>
+    <hyperlink ref="H229" r:id="rId866"/>
+    <hyperlink ref="I229" r:id="rId867"/>
+    <hyperlink ref="Z229" r:id="rId868"/>
+    <hyperlink ref="AA229" r:id="rId869"/>
+    <hyperlink ref="H230" r:id="rId870"/>
+    <hyperlink ref="I230" r:id="rId871"/>
+    <hyperlink ref="Z230" r:id="rId872"/>
+    <hyperlink ref="AA230" r:id="rId873"/>
+    <hyperlink ref="H231" r:id="rId874"/>
+    <hyperlink ref="I231" r:id="rId875"/>
+    <hyperlink ref="Z231" r:id="rId876"/>
+    <hyperlink ref="AA231" r:id="rId877"/>
+    <hyperlink ref="H232" r:id="rId878"/>
+    <hyperlink ref="I232" r:id="rId879"/>
+    <hyperlink ref="Z232" r:id="rId880"/>
+    <hyperlink ref="AA232" r:id="rId881"/>
+    <hyperlink ref="H233" r:id="rId882"/>
+    <hyperlink ref="I233" r:id="rId883"/>
+    <hyperlink ref="Z233" r:id="rId884"/>
+    <hyperlink ref="AA233" r:id="rId885"/>
+    <hyperlink ref="H234" r:id="rId886"/>
+    <hyperlink ref="I234" r:id="rId887"/>
+    <hyperlink ref="Z234" r:id="rId888"/>
+    <hyperlink ref="AA234" r:id="rId889"/>
+    <hyperlink ref="H235" r:id="rId890"/>
+    <hyperlink ref="I235" r:id="rId891"/>
+    <hyperlink ref="Z235" r:id="rId892"/>
+    <hyperlink ref="AA235" r:id="rId893"/>
+    <hyperlink ref="H236" r:id="rId894"/>
+    <hyperlink ref="I236" r:id="rId895"/>
+    <hyperlink ref="Z236" r:id="rId896"/>
+    <hyperlink ref="AA236" r:id="rId897"/>
+    <hyperlink ref="H237" r:id="rId898"/>
+    <hyperlink ref="I237" r:id="rId899"/>
+    <hyperlink ref="Z237" r:id="rId900"/>
+    <hyperlink ref="AA237" r:id="rId901"/>
+    <hyperlink ref="H238" r:id="rId902"/>
+    <hyperlink ref="I238" r:id="rId903"/>
+    <hyperlink ref="Z238" r:id="rId904"/>
+    <hyperlink ref="AA238" r:id="rId905"/>
+    <hyperlink ref="H239" r:id="rId906"/>
+    <hyperlink ref="I239" r:id="rId907"/>
+    <hyperlink ref="Z239" r:id="rId908"/>
+    <hyperlink ref="AA239" r:id="rId909"/>
+    <hyperlink ref="H240" r:id="rId910"/>
+    <hyperlink ref="I240" r:id="rId911"/>
+    <hyperlink ref="Z240" r:id="rId912"/>
+    <hyperlink ref="AA240" r:id="rId913"/>
+    <hyperlink ref="H241" r:id="rId914"/>
+    <hyperlink ref="I241" r:id="rId915"/>
+    <hyperlink ref="Z241" r:id="rId916"/>
+    <hyperlink ref="AA241" r:id="rId917"/>
+    <hyperlink ref="H242" r:id="rId918"/>
+    <hyperlink ref="I242" r:id="rId919"/>
+    <hyperlink ref="Z242" r:id="rId920"/>
+    <hyperlink ref="AA242" r:id="rId921"/>
+    <hyperlink ref="H243" r:id="rId922"/>
+    <hyperlink ref="I243" r:id="rId923"/>
+    <hyperlink ref="Z243" r:id="rId924"/>
+    <hyperlink ref="AA243" r:id="rId925"/>
+    <hyperlink ref="H244" r:id="rId926"/>
+    <hyperlink ref="I244" r:id="rId927"/>
+    <hyperlink ref="Z244" r:id="rId928"/>
+    <hyperlink ref="AA244" r:id="rId929"/>
+    <hyperlink ref="H245" r:id="rId930"/>
+    <hyperlink ref="I245" r:id="rId931"/>
+    <hyperlink ref="Z245" r:id="rId932"/>
+    <hyperlink ref="AA245" r:id="rId933"/>
+    <hyperlink ref="H246" r:id="rId934"/>
+    <hyperlink ref="I246" r:id="rId935"/>
+    <hyperlink ref="Z246" r:id="rId936"/>
+    <hyperlink ref="AA246" r:id="rId937"/>
+    <hyperlink ref="H247" r:id="rId938"/>
+    <hyperlink ref="I247" r:id="rId939"/>
+    <hyperlink ref="Z247" r:id="rId940"/>
+    <hyperlink ref="AA247" r:id="rId941"/>
+    <hyperlink ref="H248" r:id="rId942"/>
+    <hyperlink ref="I248" r:id="rId943"/>
+    <hyperlink ref="Z248" r:id="rId944"/>
+    <hyperlink ref="AA248" r:id="rId945"/>
+    <hyperlink ref="H249" r:id="rId946"/>
+    <hyperlink ref="I249" r:id="rId947"/>
+    <hyperlink ref="Z249" r:id="rId948"/>
+    <hyperlink ref="AA249" r:id="rId949"/>
+    <hyperlink ref="H250" r:id="rId950"/>
+    <hyperlink ref="I250" r:id="rId951"/>
+    <hyperlink ref="Z250" r:id="rId952"/>
+    <hyperlink ref="AA250" r:id="rId953"/>
+    <hyperlink ref="H251" r:id="rId954"/>
+    <hyperlink ref="I251" r:id="rId955"/>
+    <hyperlink ref="Z251" r:id="rId956"/>
+    <hyperlink ref="AA251" r:id="rId957"/>
+    <hyperlink ref="H252" r:id="rId958"/>
+    <hyperlink ref="I252" r:id="rId959"/>
+    <hyperlink ref="Z252" r:id="rId960"/>
+    <hyperlink ref="AA252" r:id="rId961"/>
+    <hyperlink ref="H253" r:id="rId962"/>
+    <hyperlink ref="I253" r:id="rId963"/>
+    <hyperlink ref="Z253" r:id="rId964"/>
+    <hyperlink ref="AA253" r:id="rId965"/>
+    <hyperlink ref="H254" r:id="rId966"/>
+    <hyperlink ref="I254" r:id="rId967"/>
+    <hyperlink ref="Z254" r:id="rId968"/>
+    <hyperlink ref="AA254" r:id="rId969"/>
+    <hyperlink ref="H255" r:id="rId970"/>
+    <hyperlink ref="I255" r:id="rId971"/>
+    <hyperlink ref="Z255" r:id="rId972"/>
+    <hyperlink ref="AA255" r:id="rId973"/>
+    <hyperlink ref="H256" r:id="rId974"/>
+    <hyperlink ref="I256" r:id="rId975"/>
+    <hyperlink ref="Z256" r:id="rId976"/>
+    <hyperlink ref="AA256" r:id="rId977"/>
+    <hyperlink ref="H257" r:id="rId978"/>
+    <hyperlink ref="I257" r:id="rId979"/>
+    <hyperlink ref="Z257" r:id="rId980"/>
+    <hyperlink ref="AA257" r:id="rId981"/>
+    <hyperlink ref="H258" r:id="rId982"/>
+    <hyperlink ref="I258" r:id="rId983"/>
+    <hyperlink ref="Z258" r:id="rId984"/>
+    <hyperlink ref="AA258" r:id="rId985"/>
+    <hyperlink ref="H259" r:id="rId986"/>
+    <hyperlink ref="I259" r:id="rId987"/>
+    <hyperlink ref="Z259" r:id="rId988"/>
+    <hyperlink ref="AA259" r:id="rId989"/>
+    <hyperlink ref="H260" r:id="rId990"/>
+    <hyperlink ref="I260" r:id="rId991"/>
+    <hyperlink ref="Z260" r:id="rId992"/>
+    <hyperlink ref="AA260" r:id="rId993"/>
+    <hyperlink ref="H261" r:id="rId994"/>
+    <hyperlink ref="I261" r:id="rId995"/>
+    <hyperlink ref="Z261" r:id="rId996"/>
+    <hyperlink ref="AA261" r:id="rId997"/>
+    <hyperlink ref="H262" r:id="rId998"/>
+    <hyperlink ref="I262" r:id="rId999"/>
+    <hyperlink ref="Z262" r:id="rId1000"/>
+    <hyperlink ref="AA262" r:id="rId1001"/>
+    <hyperlink ref="H263" r:id="rId1002"/>
+    <hyperlink ref="I263" r:id="rId1003"/>
+    <hyperlink ref="Z263" r:id="rId1004"/>
+    <hyperlink ref="AA263" r:id="rId1005"/>
+    <hyperlink ref="H264" r:id="rId1006"/>
+    <hyperlink ref="I264" r:id="rId1007"/>
+    <hyperlink ref="Z264" r:id="rId1008"/>
+    <hyperlink ref="AA264" r:id="rId1009"/>
+    <hyperlink ref="H265" r:id="rId1010"/>
+    <hyperlink ref="I265" r:id="rId1011"/>
+    <hyperlink ref="Z265" r:id="rId1012"/>
+    <hyperlink ref="AA265" r:id="rId1013"/>
+    <hyperlink ref="H266" r:id="rId1014"/>
+    <hyperlink ref="I266" r:id="rId1015"/>
+    <hyperlink ref="Z266" r:id="rId1016"/>
+    <hyperlink ref="AA266" r:id="rId1017"/>
+    <hyperlink ref="H267" r:id="rId1018"/>
+    <hyperlink ref="I267" r:id="rId1019"/>
+    <hyperlink ref="Z267" r:id="rId1020"/>
+    <hyperlink ref="AA267" r:id="rId1021"/>
+    <hyperlink ref="H268" r:id="rId1022"/>
+    <hyperlink ref="I268" r:id="rId1023"/>
+    <hyperlink ref="Z268" r:id="rId1024"/>
+    <hyperlink ref="AA268" r:id="rId1025"/>
+    <hyperlink ref="H269" r:id="rId1026"/>
+    <hyperlink ref="I269" r:id="rId1027"/>
+    <hyperlink ref="Z269" r:id="rId1028"/>
+    <hyperlink ref="AA269" r:id="rId1029"/>
+    <hyperlink ref="H270" r:id="rId1030"/>
+    <hyperlink ref="I270" r:id="rId1031"/>
+    <hyperlink ref="Z270" r:id="rId1032"/>
+    <hyperlink ref="AA270" r:id="rId1033"/>
+    <hyperlink ref="H271" r:id="rId1034"/>
+    <hyperlink ref="I271" r:id="rId1035"/>
+    <hyperlink ref="Z271" r:id="rId1036"/>
+    <hyperlink ref="AA271" r:id="rId1037"/>
+    <hyperlink ref="H272" r:id="rId1038"/>
+    <hyperlink ref="I272" r:id="rId1039"/>
+    <hyperlink ref="Z272" r:id="rId1040"/>
+    <hyperlink ref="AA272" r:id="rId1041"/>
+    <hyperlink ref="H273" r:id="rId1042"/>
+    <hyperlink ref="I273" r:id="rId1043"/>
+    <hyperlink ref="Z273" r:id="rId1044"/>
+    <hyperlink ref="AA273" r:id="rId1045"/>
+    <hyperlink ref="H274" r:id="rId1046"/>
+    <hyperlink ref="I274" r:id="rId1047"/>
+    <hyperlink ref="Z274" r:id="rId1048"/>
+    <hyperlink ref="AA274" r:id="rId1049"/>
+    <hyperlink ref="H275" r:id="rId1050"/>
+    <hyperlink ref="I275" r:id="rId1051"/>
+    <hyperlink ref="Z275" r:id="rId1052"/>
+    <hyperlink ref="AA275" r:id="rId1053"/>
+    <hyperlink ref="H276" r:id="rId1054"/>
+    <hyperlink ref="I276" r:id="rId1055"/>
+    <hyperlink ref="Z276" r:id="rId1056"/>
+    <hyperlink ref="AA276" r:id="rId1057"/>
+    <hyperlink ref="H277" r:id="rId1058"/>
+    <hyperlink ref="I277" r:id="rId1059"/>
+    <hyperlink ref="Z277" r:id="rId1060"/>
+    <hyperlink ref="AA277" r:id="rId1061"/>
+    <hyperlink ref="H278" r:id="rId1062"/>
+    <hyperlink ref="I278" r:id="rId1063"/>
+    <hyperlink ref="Z278" r:id="rId1064"/>
+    <hyperlink ref="AA278" r:id="rId1065"/>
+    <hyperlink ref="H279" r:id="rId1066"/>
+    <hyperlink ref="I279" r:id="rId1067"/>
+    <hyperlink ref="Z279" r:id="rId1068"/>
+    <hyperlink ref="AA279" r:id="rId1069"/>
+    <hyperlink ref="H280" r:id="rId1070"/>
+    <hyperlink ref="I280" r:id="rId1071"/>
+    <hyperlink ref="Z280" r:id="rId1072"/>
+    <hyperlink ref="AA280" r:id="rId1073"/>
+    <hyperlink ref="H281" r:id="rId1074"/>
+    <hyperlink ref="I281" r:id="rId1075"/>
+    <hyperlink ref="Z281" r:id="rId1076"/>
+    <hyperlink ref="AA281" r:id="rId1077"/>
+    <hyperlink ref="H282" r:id="rId1078"/>
+    <hyperlink ref="I282" r:id="rId1079"/>
+    <hyperlink ref="Z282" r:id="rId1080"/>
+    <hyperlink ref="AA282" r:id="rId1081"/>
+    <hyperlink ref="H283" r:id="rId1082"/>
+    <hyperlink ref="I283" r:id="rId1083"/>
+    <hyperlink ref="Z283" r:id="rId1084"/>
+    <hyperlink ref="AA283" r:id="rId1085"/>
+    <hyperlink ref="H284" r:id="rId1086"/>
+    <hyperlink ref="I284" r:id="rId1087"/>
+    <hyperlink ref="Z284" r:id="rId1088"/>
+    <hyperlink ref="AA284" r:id="rId1089"/>
+    <hyperlink ref="H285" r:id="rId1090"/>
+    <hyperlink ref="I285" r:id="rId1091"/>
+    <hyperlink ref="Z285" r:id="rId1092"/>
+    <hyperlink ref="AA285" r:id="rId1093"/>
+    <hyperlink ref="H286" r:id="rId1094"/>
+    <hyperlink ref="I286" r:id="rId1095"/>
+    <hyperlink ref="Z286" r:id="rId1096"/>
+    <hyperlink ref="AA286" r:id="rId1097"/>
+    <hyperlink ref="H287" r:id="rId1098"/>
+    <hyperlink ref="I287" r:id="rId1099"/>
+    <hyperlink ref="Z287" r:id="rId1100"/>
+    <hyperlink ref="AA287" r:id="rId1101"/>
+    <hyperlink ref="H288" r:id="rId1102"/>
+    <hyperlink ref="I288" r:id="rId1103"/>
+    <hyperlink ref="Z288" r:id="rId1104"/>
+    <hyperlink ref="AA288" r:id="rId1105"/>
+    <hyperlink ref="H289" r:id="rId1106"/>
+    <hyperlink ref="I289" r:id="rId1107"/>
+    <hyperlink ref="Z289" r:id="rId1108"/>
+    <hyperlink ref="AA289" r:id="rId1109"/>
+    <hyperlink ref="H290" r:id="rId1110"/>
+    <hyperlink ref="I290" r:id="rId1111"/>
+    <hyperlink ref="Z290" r:id="rId1112"/>
+    <hyperlink ref="AA290" r:id="rId1113"/>
+    <hyperlink ref="H291" r:id="rId1114"/>
+    <hyperlink ref="I291" r:id="rId1115"/>
+    <hyperlink ref="Z291" r:id="rId1116"/>
+    <hyperlink ref="AA291" r:id="rId1117"/>
+    <hyperlink ref="H292" r:id="rId1118"/>
+    <hyperlink ref="I292" r:id="rId1119"/>
+    <hyperlink ref="Z292" r:id="rId1120"/>
+    <hyperlink ref="AA292" r:id="rId1121"/>
+    <hyperlink ref="H293" r:id="rId1122"/>
+    <hyperlink ref="I293" r:id="rId1123"/>
+    <hyperlink ref="Z293" r:id="rId1124"/>
+    <hyperlink ref="AA293" r:id="rId1125"/>
+    <hyperlink ref="H294" r:id="rId1126"/>
+    <hyperlink ref="I294" r:id="rId1127"/>
+    <hyperlink ref="Z294" r:id="rId1128"/>
+    <hyperlink ref="AA294" r:id="rId1129"/>
+    <hyperlink ref="H295" r:id="rId1130"/>
+    <hyperlink ref="I295" r:id="rId1131"/>
+    <hyperlink ref="Z295" r:id="rId1132"/>
+    <hyperlink ref="AA295" r:id="rId1133"/>
+    <hyperlink ref="Z296" r:id="rId1134"/>
+    <hyperlink ref="AA296" r:id="rId1135"/>
+    <hyperlink ref="Z297" r:id="rId1136"/>
+    <hyperlink ref="AA297" r:id="rId1137"/>
+    <hyperlink ref="H299" r:id="rId1138"/>
+    <hyperlink ref="I299" r:id="rId1139"/>
+    <hyperlink ref="Z299" r:id="rId1140"/>
+    <hyperlink ref="AA299" r:id="rId1141"/>
+    <hyperlink ref="H300" r:id="rId1142"/>
+    <hyperlink ref="I300" r:id="rId1143"/>
+    <hyperlink ref="Z300" r:id="rId1144"/>
+    <hyperlink ref="AA300" r:id="rId1145"/>
+    <hyperlink ref="H301" r:id="rId1146"/>
+    <hyperlink ref="I301" r:id="rId1147"/>
+    <hyperlink ref="Z301" r:id="rId1148"/>
+    <hyperlink ref="AA301" r:id="rId1149"/>
+    <hyperlink ref="H302" r:id="rId1150"/>
+    <hyperlink ref="I302" r:id="rId1151"/>
+    <hyperlink ref="Z302" r:id="rId1152"/>
+    <hyperlink ref="AA302" r:id="rId1153"/>
+    <hyperlink ref="H303" r:id="rId1154"/>
+    <hyperlink ref="I303" r:id="rId1155"/>
+    <hyperlink ref="Z303" r:id="rId1156"/>
+    <hyperlink ref="AA303" r:id="rId1157"/>
+    <hyperlink ref="H304" r:id="rId1158"/>
+    <hyperlink ref="I304" r:id="rId1159"/>
+    <hyperlink ref="Z304" r:id="rId1160"/>
+    <hyperlink ref="AA304" r:id="rId1161"/>
+    <hyperlink ref="H305" r:id="rId1162"/>
+    <hyperlink ref="I305" r:id="rId1163"/>
+    <hyperlink ref="Z305" r:id="rId1164"/>
+    <hyperlink ref="AA305" r:id="rId1165"/>
+    <hyperlink ref="H306" r:id="rId1166"/>
+    <hyperlink ref="I306" r:id="rId1167"/>
+    <hyperlink ref="Z306" r:id="rId1168"/>
+    <hyperlink ref="AA306" r:id="rId1169"/>
+    <hyperlink ref="H307" r:id="rId1170"/>
+    <hyperlink ref="I307" r:id="rId1171"/>
+    <hyperlink ref="Z307" r:id="rId1172"/>
+    <hyperlink ref="AA307" r:id="rId1173"/>
+    <hyperlink ref="H308" r:id="rId1174"/>
+    <hyperlink ref="I308" r:id="rId1175"/>
+    <hyperlink ref="Z308" r:id="rId1176"/>
+    <hyperlink ref="AA308" r:id="rId1177"/>
+    <hyperlink ref="H309" r:id="rId1178"/>
+    <hyperlink ref="I309" r:id="rId1179"/>
+    <hyperlink ref="Z309" r:id="rId1180"/>
+    <hyperlink ref="AA309" r:id="rId1181"/>
+    <hyperlink ref="H310" r:id="rId1182"/>
+    <hyperlink ref="I310" r:id="rId1183"/>
+    <hyperlink ref="Z310" r:id="rId1184"/>
+    <hyperlink ref="AA310" r:id="rId1185"/>
+    <hyperlink ref="H311" r:id="rId1186"/>
+    <hyperlink ref="I311" r:id="rId1187"/>
+    <hyperlink ref="Z311" r:id="rId1188"/>
+    <hyperlink ref="AA311" r:id="rId1189"/>
+    <hyperlink ref="H312" r:id="rId1190"/>
+    <hyperlink ref="I312" r:id="rId1191"/>
+    <hyperlink ref="Z312" r:id="rId1192"/>
+    <hyperlink ref="AA312" r:id="rId1193"/>
+    <hyperlink ref="H313" r:id="rId1194"/>
+    <hyperlink ref="I313" r:id="rId1195"/>
+    <hyperlink ref="Z313" r:id="rId1196"/>
+    <hyperlink ref="AA313" r:id="rId1197"/>
+    <hyperlink ref="H314" r:id="rId1198"/>
+    <hyperlink ref="I314" r:id="rId1199"/>
+    <hyperlink ref="Z314" r:id="rId1200"/>
+    <hyperlink ref="AA314" r:id="rId1201"/>
+    <hyperlink ref="H315" r:id="rId1202"/>
+    <hyperlink ref="I315" r:id="rId1203"/>
+    <hyperlink ref="Z315" r:id="rId1204"/>
+    <hyperlink ref="AA315" r:id="rId1205"/>
+    <hyperlink ref="H316" r:id="rId1206"/>
+    <hyperlink ref="I316" r:id="rId1207"/>
+    <hyperlink ref="Z316" r:id="rId1208"/>
+    <hyperlink ref="AA316" r:id="rId1209"/>
+    <hyperlink ref="H317" r:id="rId1210"/>
+    <hyperlink ref="I317" r:id="rId1211"/>
+    <hyperlink ref="Z317" r:id="rId1212"/>
+    <hyperlink ref="AA317" r:id="rId1213"/>
+    <hyperlink ref="H318" r:id="rId1214"/>
+    <hyperlink ref="I318" r:id="rId1215"/>
+    <hyperlink ref="Z318" r:id="rId1216"/>
+    <hyperlink ref="AA318" r:id="rId1217"/>
+    <hyperlink ref="H319" r:id="rId1218"/>
+    <hyperlink ref="I319" r:id="rId1219"/>
+    <hyperlink ref="Z319" r:id="rId1220"/>
+    <hyperlink ref="AA319" r:id="rId1221"/>
+    <hyperlink ref="H320" r:id="rId1222"/>
+    <hyperlink ref="I320" r:id="rId1223"/>
+    <hyperlink ref="Z320" r:id="rId1224"/>
+    <hyperlink ref="AA320" r:id="rId1225"/>
+    <hyperlink ref="H321" r:id="rId1226"/>
+    <hyperlink ref="I321" r:id="rId1227"/>
+    <hyperlink ref="Z321" r:id="rId1228"/>
+    <hyperlink ref="AA321" r:id="rId1229"/>
+    <hyperlink ref="H322" r:id="rId1230"/>
+    <hyperlink ref="I322" r:id="rId1231"/>
+    <hyperlink ref="Z322" r:id="rId1232"/>
+    <hyperlink ref="AA322" r:id="rId1233"/>
+    <hyperlink ref="H323" r:id="rId1234"/>
+    <hyperlink ref="I323" r:id="rId1235"/>
+    <hyperlink ref="Z323" r:id="rId1236"/>
+    <hyperlink ref="AA323" r:id="rId1237"/>
+    <hyperlink ref="H324" r:id="rId1238"/>
+    <hyperlink ref="I324" r:id="rId1239"/>
+    <hyperlink ref="Z324" r:id="rId1240"/>
+    <hyperlink ref="AA324" r:id="rId1241"/>
+    <hyperlink ref="H325" r:id="rId1242"/>
+    <hyperlink ref="I325" r:id="rId1243"/>
+    <hyperlink ref="Z325" r:id="rId1244"/>
+    <hyperlink ref="AA325" r:id="rId1245"/>
+    <hyperlink ref="H326" r:id="rId1246"/>
+    <hyperlink ref="I326" r:id="rId1247"/>
+    <hyperlink ref="Z326" r:id="rId1248"/>
+    <hyperlink ref="AA326" r:id="rId1249"/>
+    <hyperlink ref="H327" r:id="rId1250"/>
+    <hyperlink ref="I327" r:id="rId1251"/>
+    <hyperlink ref="Z327" r:id="rId1252"/>
+    <hyperlink ref="AA327" r:id="rId1253"/>
+    <hyperlink ref="H328" r:id="rId1254"/>
+    <hyperlink ref="I328" r:id="rId1255"/>
+    <hyperlink ref="Z328" r:id="rId1256"/>
+    <hyperlink ref="AA328" r:id="rId1257"/>
+    <hyperlink ref="H329" r:id="rId1258"/>
+    <hyperlink ref="I329" r:id="rId1259"/>
+    <hyperlink ref="Z329" r:id="rId1260"/>
+    <hyperlink ref="AA329" r:id="rId1261"/>
+    <hyperlink ref="H330" r:id="rId1262"/>
+    <hyperlink ref="I330" r:id="rId1263"/>
+    <hyperlink ref="Z330" r:id="rId1264"/>
+    <hyperlink ref="AA330" r:id="rId1265"/>
+    <hyperlink ref="H331" r:id="rId1266"/>
+    <hyperlink ref="I331" r:id="rId1267"/>
+    <hyperlink ref="Z331" r:id="rId1268"/>
+    <hyperlink ref="AA331" r:id="rId1269"/>
+    <hyperlink ref="H332" r:id="rId1270"/>
+    <hyperlink ref="I332" r:id="rId1271"/>
+    <hyperlink ref="Z332" r:id="rId1272"/>
+    <hyperlink ref="AA332" r:id="rId1273"/>
+    <hyperlink ref="H333" r:id="rId1274"/>
+    <hyperlink ref="I333" r:id="rId1275"/>
+    <hyperlink ref="Z333" r:id="rId1276"/>
+    <hyperlink ref="AA333" r:id="rId1277"/>
+    <hyperlink ref="H334" r:id="rId1278"/>
+    <hyperlink ref="I334" r:id="rId1279"/>
+    <hyperlink ref="Z334" r:id="rId1280"/>
+    <hyperlink ref="AA334" r:id="rId1281"/>
+    <hyperlink ref="H335" r:id="rId1282"/>
+    <hyperlink ref="I335" r:id="rId1283"/>
+    <hyperlink ref="Z335" r:id="rId1284"/>
+    <hyperlink ref="AA335" r:id="rId1285"/>
+    <hyperlink ref="H336" r:id="rId1286"/>
+    <hyperlink ref="I336" r:id="rId1287"/>
+    <hyperlink ref="Z336" r:id="rId1288"/>
+    <hyperlink ref="AA336" r:id="rId1289"/>
+    <hyperlink ref="H337" r:id="rId1290"/>
+    <hyperlink ref="I337" r:id="rId1291"/>
+    <hyperlink ref="Z337" r:id="rId1292"/>
+    <hyperlink ref="AA337" r:id="rId1293"/>
+    <hyperlink ref="H338" r:id="rId1294"/>
+    <hyperlink ref="I338" r:id="rId1295"/>
+    <hyperlink ref="Z338" r:id="rId1296"/>
+    <hyperlink ref="AA338" r:id="rId1297"/>
+    <hyperlink ref="H339" r:id="rId1298"/>
+    <hyperlink ref="I339" r:id="rId1299"/>
+    <hyperlink ref="Z339" r:id="rId1300"/>
+    <hyperlink ref="AA339" r:id="rId1301"/>
+    <hyperlink ref="H340" r:id="rId1302"/>
+    <hyperlink ref="I340" r:id="rId1303"/>
+    <hyperlink ref="Z340" r:id="rId1304"/>
+    <hyperlink ref="AA340" r:id="rId1305"/>
+    <hyperlink ref="H341" r:id="rId1306"/>
+    <hyperlink ref="I341" r:id="rId1307"/>
+    <hyperlink ref="Z341" r:id="rId1308"/>
+    <hyperlink ref="AA341" r:id="rId1309"/>
+    <hyperlink ref="H342" r:id="rId1310"/>
+    <hyperlink ref="I342" r:id="rId1311"/>
+    <hyperlink ref="Z342" r:id="rId1312"/>
+    <hyperlink ref="AA342" r:id="rId1313"/>
+    <hyperlink ref="H343" r:id="rId1314"/>
+    <hyperlink ref="I343" r:id="rId1315"/>
+    <hyperlink ref="Z343" r:id="rId1316"/>
+    <hyperlink ref="AA343" r:id="rId1317"/>
+    <hyperlink ref="H344" r:id="rId1318"/>
+    <hyperlink ref="I344" r:id="rId1319"/>
+    <hyperlink ref="Z344" r:id="rId1320"/>
+    <hyperlink ref="AA344" r:id="rId1321"/>
+    <hyperlink ref="H345" r:id="rId1322"/>
+    <hyperlink ref="I345" r:id="rId1323"/>
+    <hyperlink ref="Z345" r:id="rId1324"/>
+    <hyperlink ref="AA345" r:id="rId1325"/>
+    <hyperlink ref="H346" r:id="rId1326"/>
+    <hyperlink ref="I346" r:id="rId1327"/>
+    <hyperlink ref="Z346" r:id="rId1328"/>
+    <hyperlink ref="AA346" r:id="rId1329"/>
+    <hyperlink ref="H347" r:id="rId1330"/>
+    <hyperlink ref="I347" r:id="rId1331"/>
+    <hyperlink ref="Z347" r:id="rId1332"/>
+    <hyperlink ref="AA347" r:id="rId1333"/>
+    <hyperlink ref="H348" r:id="rId1334"/>
+    <hyperlink ref="I348" r:id="rId1335"/>
+    <hyperlink ref="Z348" r:id="rId1336"/>
+    <hyperlink ref="AA348" r:id="rId1337"/>
+    <hyperlink ref="H349" r:id="rId1338"/>
+    <hyperlink ref="I349" r:id="rId1339"/>
+    <hyperlink ref="Z349" r:id="rId1340"/>
+    <hyperlink ref="AA349" r:id="rId1341"/>
+    <hyperlink ref="H350" r:id="rId1342"/>
+    <hyperlink ref="I350" r:id="rId1343"/>
+    <hyperlink ref="Z350" r:id="rId1344"/>
+    <hyperlink ref="AA350" r:id="rId1345"/>
+    <hyperlink ref="H351" r:id="rId1346"/>
+    <hyperlink ref="I351" r:id="rId1347"/>
+    <hyperlink ref="Z351" r:id="rId1348"/>
+    <hyperlink ref="AA351" r:id="rId1349"/>
+    <hyperlink ref="H352" r:id="rId1350"/>
+    <hyperlink ref="I352" r:id="rId1351"/>
+    <hyperlink ref="Z352" r:id="rId1352"/>
+    <hyperlink ref="AA352" r:id="rId1353"/>
+    <hyperlink ref="H353" r:id="rId1354"/>
+    <hyperlink ref="I353" r:id="rId1355"/>
+    <hyperlink ref="Z353" r:id="rId1356"/>
+    <hyperlink ref="AA353" r:id="rId1357"/>
+    <hyperlink ref="H354" r:id="rId1358"/>
+    <hyperlink ref="I354" r:id="rId1359"/>
+    <hyperlink ref="Z354" r:id="rId1360"/>
+    <hyperlink ref="AA354" r:id="rId1361"/>
+    <hyperlink ref="H355" r:id="rId1362"/>
+    <hyperlink ref="I355" r:id="rId1363"/>
+    <hyperlink ref="Z355" r:id="rId1364"/>
+    <hyperlink ref="AA355" r:id="rId1365"/>
+    <hyperlink ref="H356" r:id="rId1366"/>
+    <hyperlink ref="I356" r:id="rId1367"/>
+    <hyperlink ref="Z356" r:id="rId1368"/>
+    <hyperlink ref="AA356" r:id="rId1369"/>
+    <hyperlink ref="H357" r:id="rId1370"/>
+    <hyperlink ref="I357" r:id="rId1371"/>
+    <hyperlink ref="Z357" r:id="rId1372"/>
+    <hyperlink ref="AA357" r:id="rId1373"/>
+    <hyperlink ref="H358" r:id="rId1374"/>
+    <hyperlink ref="I358" r:id="rId1375"/>
+    <hyperlink ref="Z358" r:id="rId1376"/>
+    <hyperlink ref="AA358" r:id="rId1377"/>
+    <hyperlink ref="H359" r:id="rId1378"/>
+    <hyperlink ref="I359" r:id="rId1379"/>
+    <hyperlink ref="Z359" r:id="rId1380"/>
+    <hyperlink ref="AA359" r:id="rId1381"/>
+    <hyperlink ref="H360" r:id="rId1382"/>
+    <hyperlink ref="I360" r:id="rId1383"/>
+    <hyperlink ref="Z360" r:id="rId1384"/>
+    <hyperlink ref="AA360" r:id="rId1385"/>
+    <hyperlink ref="H361" r:id="rId1386"/>
+    <hyperlink ref="I361" r:id="rId1387"/>
+    <hyperlink ref="Z361" r:id="rId1388"/>
+    <hyperlink ref="AA361" r:id="rId1389"/>
+    <hyperlink ref="H362" r:id="rId1390"/>
+    <hyperlink ref="I362" r:id="rId1391"/>
+    <hyperlink ref="Z362" r:id="rId1392"/>
+    <hyperlink ref="AA362" r:id="rId1393"/>
+    <hyperlink ref="H363" r:id="rId1394"/>
+    <hyperlink ref="I363" r:id="rId1395"/>
+    <hyperlink ref="Z363" r:id="rId1396"/>
+    <hyperlink ref="AA363" r:id="rId1397"/>
+    <hyperlink ref="H364" r:id="rId1398"/>
+    <hyperlink ref="I364" r:id="rId1399"/>
+    <hyperlink ref="Z364" r:id="rId1400"/>
+    <hyperlink ref="AA364" r:id="rId1401"/>
+    <hyperlink ref="H365" r:id="rId1402"/>
+    <hyperlink ref="I365" r:id="rId1403"/>
+    <hyperlink ref="Z365" r:id="rId1404"/>
+    <hyperlink ref="AA365" r:id="rId1405"/>
+    <hyperlink ref="H366" r:id="rId1406"/>
+    <hyperlink ref="I366" r:id="rId1407"/>
+    <hyperlink ref="Z366" r:id="rId1408"/>
+    <hyperlink ref="AA366" r:id="rId1409"/>
+    <hyperlink ref="H367" r:id="rId1410"/>
+    <hyperlink ref="I367" r:id="rId1411"/>
+    <hyperlink ref="Z367" r:id="rId1412"/>
+    <hyperlink ref="AA367" r:id="rId1413"/>
+    <hyperlink ref="H368" r:id="rId1414"/>
+    <hyperlink ref="I368" r:id="rId1415"/>
+    <hyperlink ref="Z368" r:id="rId1416"/>
+    <hyperlink ref="AA368" r:id="rId1417"/>
+    <hyperlink ref="Z369" r:id="rId1418"/>
+    <hyperlink ref="AA369" r:id="rId1419"/>
+    <hyperlink ref="Z370" r:id="rId1420"/>
+    <hyperlink ref="AA370" r:id="rId1421"/>
+    <hyperlink ref="Z371" r:id="rId1422"/>
+    <hyperlink ref="AA371" r:id="rId1423"/>
+    <hyperlink ref="H373" r:id="rId1424"/>
+    <hyperlink ref="I373" r:id="rId1425"/>
+    <hyperlink ref="Z373" r:id="rId1426"/>
+    <hyperlink ref="AA373" r:id="rId1427"/>
+    <hyperlink ref="H374" r:id="rId1428"/>
+    <hyperlink ref="I374" r:id="rId1429"/>
+    <hyperlink ref="Z374" r:id="rId1430"/>
+    <hyperlink ref="AA374" r:id="rId1431"/>
+    <hyperlink ref="H375" r:id="rId1432"/>
+    <hyperlink ref="I375" r:id="rId1433"/>
+    <hyperlink ref="Z375" r:id="rId1434"/>
+    <hyperlink ref="AA375" r:id="rId1435"/>
+    <hyperlink ref="H376" r:id="rId1436"/>
+    <hyperlink ref="I376" r:id="rId1437"/>
+    <hyperlink ref="Z376" r:id="rId1438"/>
+    <hyperlink ref="AA376" r:id="rId1439"/>
+    <hyperlink ref="H377" r:id="rId1440"/>
+    <hyperlink ref="I377" r:id="rId1441"/>
+    <hyperlink ref="Z377" r:id="rId1442"/>
+    <hyperlink ref="AA377" r:id="rId1443"/>
+    <hyperlink ref="H378" r:id="rId1444"/>
+    <hyperlink ref="I378" r:id="rId1445"/>
+    <hyperlink ref="Z378" r:id="rId1446"/>
+    <hyperlink ref="AA378" r:id="rId1447"/>
+    <hyperlink ref="H379" r:id="rId1448"/>
+    <hyperlink ref="I379" r:id="rId1449"/>
+    <hyperlink ref="Z379" r:id="rId1450"/>
+    <hyperlink ref="AA379" r:id="rId1451"/>
+    <hyperlink ref="H380" r:id="rId1452"/>
+    <hyperlink ref="I380" r:id="rId1453"/>
+    <hyperlink ref="Z380" r:id="rId1454"/>
+    <hyperlink ref="AA380" r:id="rId1455"/>
+    <hyperlink ref="H381" r:id="rId1456"/>
+    <hyperlink ref="I381" r:id="rId1457"/>
+    <hyperlink ref="Z381" r:id="rId1458"/>
+    <hyperlink ref="AA381" r:id="rId1459"/>
+    <hyperlink ref="H382" r:id="rId1460"/>
+    <hyperlink ref="I382" r:id="rId1461"/>
+    <hyperlink ref="Z382" r:id="rId1462"/>
+    <hyperlink ref="AA382" r:id="rId1463"/>
+    <hyperlink ref="H383" r:id="rId1464"/>
+    <hyperlink ref="I383" r:id="rId1465"/>
+    <hyperlink ref="Z383" r:id="rId1466"/>
+    <hyperlink ref="AA383" r:id="rId1467"/>
+    <hyperlink ref="H384" r:id="rId1468"/>
+    <hyperlink ref="I384" r:id="rId1469"/>
+    <hyperlink ref="Z384" r:id="rId1470"/>
+    <hyperlink ref="AA384" r:id="rId1471"/>
+    <hyperlink ref="H385" r:id="rId1472"/>
+    <hyperlink ref="I385" r:id="rId1473"/>
+    <hyperlink ref="Z385" r:id="rId1474"/>
+    <hyperlink ref="AA385" r:id="rId1475"/>
+    <hyperlink ref="H386" r:id="rId1476"/>
+    <hyperlink ref="I386" r:id="rId1477"/>
+    <hyperlink ref="Z386" r:id="rId1478"/>
+    <hyperlink ref="AA386" r:id="rId1479"/>
+    <hyperlink ref="H387" r:id="rId1480"/>
+    <hyperlink ref="I387" r:id="rId1481"/>
+    <hyperlink ref="Z387" r:id="rId1482"/>
+    <hyperlink ref="AA387" r:id="rId1483"/>
+    <hyperlink ref="H388" r:id="rId1484"/>
+    <hyperlink ref="I388" r:id="rId1485"/>
+    <hyperlink ref="Z388" r:id="rId1486"/>
+    <hyperlink ref="AA388" r:id="rId1487"/>
+    <hyperlink ref="H389" r:id="rId1488"/>
+    <hyperlink ref="I389" r:id="rId1489"/>
+    <hyperlink ref="Z389" r:id="rId1490"/>
+    <hyperlink ref="AA389" r:id="rId1491"/>
+    <hyperlink ref="H390" r:id="rId1492"/>
+    <hyperlink ref="I390" r:id="rId1493"/>
+    <hyperlink ref="Z390" r:id="rId1494"/>
+    <hyperlink ref="AA390" r:id="rId1495"/>
+    <hyperlink ref="H391" r:id="rId1496"/>
+    <hyperlink ref="I391" r:id="rId1497"/>
+    <hyperlink ref="Z391" r:id="rId1498"/>
+    <hyperlink ref="AA391" r:id="rId1499"/>
+    <hyperlink ref="H392" r:id="rId1500"/>
+    <hyperlink ref="I392" r:id="rId1501"/>
+    <hyperlink ref="Z392" r:id="rId1502"/>
+    <hyperlink ref="AA392" r:id="rId1503"/>
+    <hyperlink ref="H393" r:id="rId1504"/>
+    <hyperlink ref="I393" r:id="rId1505"/>
+    <hyperlink ref="Z393" r:id="rId1506"/>
+    <hyperlink ref="AA393" r:id="rId1507"/>
+    <hyperlink ref="H394" r:id="rId1508"/>
+    <hyperlink ref="I394" r:id="rId1509"/>
+    <hyperlink ref="Z394" r:id="rId1510"/>
+    <hyperlink ref="AA394" r:id="rId1511"/>
+    <hyperlink ref="H395" r:id="rId1512"/>
+    <hyperlink ref="I395" r:id="rId1513"/>
+    <hyperlink ref="Z395" r:id="rId1514"/>
+    <hyperlink ref="AA395" r:id="rId1515"/>
+    <hyperlink ref="H396" r:id="rId1516"/>
+    <hyperlink ref="I396" r:id="rId1517"/>
+    <hyperlink ref="Z396" r:id="rId1518"/>
+    <hyperlink ref="AA396" r:id="rId1519"/>
+    <hyperlink ref="H397" r:id="rId1520"/>
+    <hyperlink ref="I397" r:id="rId1521"/>
+    <hyperlink ref="Z397" r:id="rId1522"/>
+    <hyperlink ref="AA397" r:id="rId1523"/>
+    <hyperlink ref="H398" r:id="rId1524"/>
+    <hyperlink ref="I398" r:id="rId1525"/>
+    <hyperlink ref="Z398" r:id="rId1526"/>
+    <hyperlink ref="AA398" r:id="rId1527"/>
+    <hyperlink ref="H399" r:id="rId1528"/>
+    <hyperlink ref="I399" r:id="rId1529"/>
+    <hyperlink ref="Z399" r:id="rId1530"/>
+    <hyperlink ref="AA399" r:id="rId1531"/>
+    <hyperlink ref="H400" r:id="rId1532"/>
+    <hyperlink ref="I400" r:id="rId1533"/>
+    <hyperlink ref="Z400" r:id="rId1534"/>
+    <hyperlink ref="AA400" r:id="rId1535"/>
+    <hyperlink ref="H401" r:id="rId1536"/>
+    <hyperlink ref="I401" r:id="rId1537"/>
+    <hyperlink ref="Z401" r:id="rId1538"/>
+    <hyperlink ref="AA401" r:id="rId1539"/>
+    <hyperlink ref="H402" r:id="rId1540"/>
+    <hyperlink ref="I402" r:id="rId1541"/>
+    <hyperlink ref="Z402" r:id="rId1542"/>
+    <hyperlink ref="AA402" r:id="rId1543"/>
+    <hyperlink ref="H403" r:id="rId1544"/>
+    <hyperlink ref="I403" r:id="rId1545"/>
+    <hyperlink ref="Z403" r:id="rId1546"/>
+    <hyperlink ref="AA403" r:id="rId1547"/>
+    <hyperlink ref="H404" r:id="rId1548"/>
+    <hyperlink ref="I404" r:id="rId1549"/>
+    <hyperlink ref="Z404" r:id="rId1550"/>
+    <hyperlink ref="AA404" r:id="rId1551"/>
+    <hyperlink ref="H405" r:id="rId1552"/>
+    <hyperlink ref="I405" r:id="rId1553"/>
+    <hyperlink ref="Z405" r:id="rId1554"/>
+    <hyperlink ref="AA405" r:id="rId1555"/>
+    <hyperlink ref="H406" r:id="rId1556"/>
+    <hyperlink ref="I406" r:id="rId1557"/>
+    <hyperlink ref="Z406" r:id="rId1558"/>
+    <hyperlink ref="AA406" r:id="rId1559"/>
+    <hyperlink ref="H407" r:id="rId1560"/>
+    <hyperlink ref="I407" r:id="rId1561"/>
+    <hyperlink ref="Z407" r:id="rId1562"/>
+    <hyperlink ref="AA407" r:id="rId1563"/>
+    <hyperlink ref="H408" r:id="rId1564"/>
+    <hyperlink ref="I408" r:id="rId1565"/>
+    <hyperlink ref="Z408" r:id="rId1566"/>
+    <hyperlink ref="AA408" r:id="rId1567"/>
+    <hyperlink ref="H409" r:id="rId1568"/>
+    <hyperlink ref="I409" r:id="rId1569"/>
+    <hyperlink ref="Z409" r:id="rId1570"/>
+    <hyperlink ref="AA409" r:id="rId1571"/>
+    <hyperlink ref="H410" r:id="rId1572"/>
+    <hyperlink ref="I410" r:id="rId1573"/>
+    <hyperlink ref="Z410" r:id="rId1574"/>
+    <hyperlink ref="AA410" r:id="rId1575"/>
+    <hyperlink ref="H411" r:id="rId1576"/>
+    <hyperlink ref="I411" r:id="rId1577"/>
+    <hyperlink ref="Z411" r:id="rId1578"/>
+    <hyperlink ref="AA411" r:id="rId1579"/>
+    <hyperlink ref="H412" r:id="rId1580"/>
+    <hyperlink ref="I412" r:id="rId1581"/>
+    <hyperlink ref="Z412" r:id="rId1582"/>
+    <hyperlink ref="AA412" r:id="rId1583"/>
+    <hyperlink ref="H413" r:id="rId1584"/>
+    <hyperlink ref="I413" r:id="rId1585"/>
+    <hyperlink ref="Z413" r:id="rId1586"/>
+    <hyperlink ref="AA413" r:id="rId1587"/>
+    <hyperlink ref="H414" r:id="rId1588"/>
+    <hyperlink ref="I414" r:id="rId1589"/>
+    <hyperlink ref="Z414" r:id="rId1590"/>
+    <hyperlink ref="AA414" r:id="rId1591"/>
+    <hyperlink ref="H415" r:id="rId1592"/>
+    <hyperlink ref="I415" r:id="rId1593"/>
+    <hyperlink ref="Z415" r:id="rId1594"/>
+    <hyperlink ref="AA415" r:id="rId1595"/>
+    <hyperlink ref="H416" r:id="rId1596"/>
+    <hyperlink ref="I416" r:id="rId1597"/>
+    <hyperlink ref="Z416" r:id="rId1598"/>
+    <hyperlink ref="AA416" r:id="rId1599"/>
+    <hyperlink ref="H417" r:id="rId1600"/>
+    <hyperlink ref="I417" r:id="rId1601"/>
+    <hyperlink ref="Z417" r:id="rId1602"/>
+    <hyperlink ref="AA417" r:id="rId1603"/>
+    <hyperlink ref="H418" r:id="rId1604"/>
+    <hyperlink ref="I418" r:id="rId1605"/>
+    <hyperlink ref="Z418" r:id="rId1606"/>
+    <hyperlink ref="AA418" r:id="rId1607"/>
+    <hyperlink ref="H419" r:id="rId1608"/>
+    <hyperlink ref="I419" r:id="rId1609"/>
+    <hyperlink ref="Z419" r:id="rId1610"/>
+    <hyperlink ref="AA419" r:id="rId1611"/>
+    <hyperlink ref="H420" r:id="rId1612"/>
+    <hyperlink ref="I420" r:id="rId1613"/>
+    <hyperlink ref="Z420" r:id="rId1614"/>
+    <hyperlink ref="AA420" r:id="rId1615"/>
+    <hyperlink ref="H421" r:id="rId1616"/>
+    <hyperlink ref="I421" r:id="rId1617"/>
+    <hyperlink ref="Z421" r:id="rId1618"/>
+    <hyperlink ref="AA421" r:id="rId1619"/>
+    <hyperlink ref="H422" r:id="rId1620"/>
+    <hyperlink ref="I422" r:id="rId1621"/>
+    <hyperlink ref="Z422" r:id="rId1622"/>
+    <hyperlink ref="AA422" r:id="rId1623"/>
+    <hyperlink ref="H423" r:id="rId1624"/>
+    <hyperlink ref="I423" r:id="rId1625"/>
+    <hyperlink ref="Z423" r:id="rId1626"/>
+    <hyperlink ref="AA423" r:id="rId1627"/>
+    <hyperlink ref="H424" r:id="rId1628"/>
+    <hyperlink ref="I424" r:id="rId1629"/>
+    <hyperlink ref="Z424" r:id="rId1630"/>
+    <hyperlink ref="AA424" r:id="rId1631"/>
+    <hyperlink ref="H425" r:id="rId1632"/>
+    <hyperlink ref="I425" r:id="rId1633"/>
+    <hyperlink ref="Z425" r:id="rId1634"/>
+    <hyperlink ref="AA425" r:id="rId1635"/>
+    <hyperlink ref="H426" r:id="rId1636"/>
+    <hyperlink ref="I426" r:id="rId1637"/>
+    <hyperlink ref="Z426" r:id="rId1638"/>
+    <hyperlink ref="AA426" r:id="rId1639"/>
+    <hyperlink ref="H427" r:id="rId1640"/>
+    <hyperlink ref="I427" r:id="rId1641"/>
+    <hyperlink ref="Z427" r:id="rId1642"/>
+    <hyperlink ref="AA427" r:id="rId1643"/>
+    <hyperlink ref="H428" r:id="rId1644"/>
+    <hyperlink ref="I428" r:id="rId1645"/>
+    <hyperlink ref="Z428" r:id="rId1646"/>
+    <hyperlink ref="AA428" r:id="rId1647"/>
+    <hyperlink ref="H429" r:id="rId1648"/>
+    <hyperlink ref="I429" r:id="rId1649"/>
+    <hyperlink ref="Z429" r:id="rId1650"/>
+    <hyperlink ref="AA429" r:id="rId1651"/>
+    <hyperlink ref="H430" r:id="rId1652"/>
+    <hyperlink ref="I430" r:id="rId1653"/>
+    <hyperlink ref="Z430" r:id="rId1654"/>
+    <hyperlink ref="AA430" r:id="rId1655"/>
+    <hyperlink ref="H431" r:id="rId1656"/>
+    <hyperlink ref="I431" r:id="rId1657"/>
+    <hyperlink ref="Z431" r:id="rId1658"/>
+    <hyperlink ref="AA431" r:id="rId1659"/>
+    <hyperlink ref="H432" r:id="rId1660"/>
+    <hyperlink ref="I432" r:id="rId1661"/>
+    <hyperlink ref="Z432" r:id="rId1662"/>
+    <hyperlink ref="AA432" r:id="rId1663"/>
+    <hyperlink ref="H433" r:id="rId1664"/>
+    <hyperlink ref="I433" r:id="rId1665"/>
+    <hyperlink ref="Z433" r:id="rId1666"/>
+    <hyperlink ref="H434" r:id="rId1667"/>
+    <hyperlink ref="H436" r:id="rId1668"/>
+    <hyperlink ref="I436" r:id="rId1669"/>
+    <hyperlink ref="Z436" r:id="rId1670"/>
+    <hyperlink ref="AA436" r:id="rId1671"/>
+    <hyperlink ref="H437" r:id="rId1672"/>
+    <hyperlink ref="I437" r:id="rId1673"/>
+    <hyperlink ref="Z437" r:id="rId1674"/>
+    <hyperlink ref="AA437" r:id="rId1675"/>
+    <hyperlink ref="H438" r:id="rId1676"/>
+    <hyperlink ref="I438" r:id="rId1677"/>
+    <hyperlink ref="Z438" r:id="rId1678"/>
+    <hyperlink ref="AA438" r:id="rId1679"/>
+    <hyperlink ref="H439" r:id="rId1680"/>
+    <hyperlink ref="I439" r:id="rId1681"/>
+    <hyperlink ref="Z439" r:id="rId1682"/>
+    <hyperlink ref="AA439" r:id="rId1683"/>
+    <hyperlink ref="H440" r:id="rId1684"/>
+    <hyperlink ref="I440" r:id="rId1685"/>
+    <hyperlink ref="Z440" r:id="rId1686"/>
+    <hyperlink ref="AA440" r:id="rId1687"/>
+    <hyperlink ref="H441" r:id="rId1688"/>
+    <hyperlink ref="I441" r:id="rId1689"/>
+    <hyperlink ref="Z441" r:id="rId1690"/>
+    <hyperlink ref="AA441" r:id="rId1691"/>
+    <hyperlink ref="H442" r:id="rId1692"/>
+    <hyperlink ref="I442" r:id="rId1693"/>
+    <hyperlink ref="Z442" r:id="rId1694"/>
+    <hyperlink ref="AA442" r:id="rId1695"/>
+    <hyperlink ref="H443" r:id="rId1696"/>
+    <hyperlink ref="I443" r:id="rId1697"/>
+    <hyperlink ref="Z443" r:id="rId1698"/>
+    <hyperlink ref="AA443" r:id="rId1699"/>
+    <hyperlink ref="H444" r:id="rId1700"/>
+    <hyperlink ref="I444" r:id="rId1701"/>
+    <hyperlink ref="Z444" r:id="rId1702"/>
+    <hyperlink ref="AA444" r:id="rId1703"/>
+    <hyperlink ref="H445" r:id="rId1704"/>
+    <hyperlink ref="I445" r:id="rId1705"/>
+    <hyperlink ref="Z445" r:id="rId1706"/>
+    <hyperlink ref="AA445" r:id="rId1707"/>
+    <hyperlink ref="H446" r:id="rId1708"/>
+    <hyperlink ref="I446" r:id="rId1709"/>
+    <hyperlink ref="Z446" r:id="rId1710"/>
+    <hyperlink ref="AA446" r:id="rId1711"/>
+    <hyperlink ref="H447" r:id="rId1712"/>
+    <hyperlink ref="I447" r:id="rId1713"/>
+    <hyperlink ref="Z447" r:id="rId1714"/>
+    <hyperlink ref="AA447" r:id="rId1715"/>
+    <hyperlink ref="H448" r:id="rId1716"/>
+    <hyperlink ref="I448" r:id="rId1717"/>
+    <hyperlink ref="Z448" r:id="rId1718"/>
+    <hyperlink ref="AA448" r:id="rId1719"/>
+    <hyperlink ref="H449" r:id="rId1720"/>
+    <hyperlink ref="I449" r:id="rId1721"/>
+    <hyperlink ref="Z449" r:id="rId1722"/>
+    <hyperlink ref="AA449" r:id="rId1723"/>
+    <hyperlink ref="H450" r:id="rId1724"/>
+    <hyperlink ref="I450" r:id="rId1725"/>
+    <hyperlink ref="Z450" r:id="rId1726"/>
+    <hyperlink ref="AA450" r:id="rId1727"/>
+    <hyperlink ref="H451" r:id="rId1728"/>
+    <hyperlink ref="I451" r:id="rId1729"/>
+    <hyperlink ref="Z451" r:id="rId1730"/>
+    <hyperlink ref="AA451" r:id="rId1731"/>
+    <hyperlink ref="H452" r:id="rId1732"/>
+    <hyperlink ref="I452" r:id="rId1733"/>
+    <hyperlink ref="Z452" r:id="rId1734"/>
+    <hyperlink ref="AA452" r:id="rId1735"/>
+    <hyperlink ref="H453" r:id="rId1736"/>
+    <hyperlink ref="I453" r:id="rId1737"/>
+    <hyperlink ref="Z453" r:id="rId1738"/>
+    <hyperlink ref="AA453" r:id="rId1739"/>
+    <hyperlink ref="H454" r:id="rId1740"/>
+    <hyperlink ref="I454" r:id="rId1741"/>
+    <hyperlink ref="Z454" r:id="rId1742"/>
+    <hyperlink ref="AA454" r:id="rId1743"/>
+    <hyperlink ref="H455" r:id="rId1744"/>
+    <hyperlink ref="I455" r:id="rId1745"/>
+    <hyperlink ref="Z455" r:id="rId1746"/>
+    <hyperlink ref="AA455" r:id="rId1747"/>
+    <hyperlink ref="H456" r:id="rId1748"/>
+    <hyperlink ref="I456" r:id="rId1749"/>
+    <hyperlink ref="Z456" r:id="rId1750"/>
+    <hyperlink ref="AA456" r:id="rId1751"/>
+    <hyperlink ref="H457" r:id="rId1752"/>
+    <hyperlink ref="I457" r:id="rId1753"/>
+    <hyperlink ref="Z457" r:id="rId1754"/>
+    <hyperlink ref="AA457" r:id="rId1755"/>
+    <hyperlink ref="H458" r:id="rId1756"/>
+    <hyperlink ref="I458" r:id="rId1757"/>
+    <hyperlink ref="Z458" r:id="rId1758"/>
+    <hyperlink ref="AA458" r:id="rId1759"/>
+    <hyperlink ref="H459" r:id="rId1760"/>
+    <hyperlink ref="I459" r:id="rId1761"/>
+    <hyperlink ref="Z459" r:id="rId1762"/>
+    <hyperlink ref="AA459" r:id="rId1763"/>
+    <hyperlink ref="H460" r:id="rId1764"/>
+    <hyperlink ref="I460" r:id="rId1765"/>
+    <hyperlink ref="Z460" r:id="rId1766"/>
+    <hyperlink ref="AA460" r:id="rId1767"/>
+    <hyperlink ref="H461" r:id="rId1768"/>
+    <hyperlink ref="I461" r:id="rId1769"/>
+    <hyperlink ref="Z461" r:id="rId1770"/>
+    <hyperlink ref="AA461" r:id="rId1771"/>
+    <hyperlink ref="H462" r:id="rId1772"/>
+    <hyperlink ref="I462" r:id="rId1773"/>
+    <hyperlink ref="Z462" r:id="rId1774"/>
+    <hyperlink ref="AA462" r:id="rId1775"/>
+    <hyperlink ref="H463" r:id="rId1776"/>
+    <hyperlink ref="I463" r:id="rId1777"/>
+    <hyperlink ref="Z463" r:id="rId1778"/>
+    <hyperlink ref="AA463" r:id="rId1779"/>
+    <hyperlink ref="H464" r:id="rId1780"/>
+    <hyperlink ref="I464" r:id="rId1781"/>
+    <hyperlink ref="Z464" r:id="rId1782"/>
+    <hyperlink ref="AA464" r:id="rId1783"/>
+    <hyperlink ref="H465" r:id="rId1784"/>
+    <hyperlink ref="I465" r:id="rId1785"/>
+    <hyperlink ref="Z465" r:id="rId1786"/>
+    <hyperlink ref="AA465" r:id="rId1787"/>
+    <hyperlink ref="H466" r:id="rId1788"/>
+    <hyperlink ref="I466" r:id="rId1789"/>
+    <hyperlink ref="Z466" r:id="rId1790"/>
+    <hyperlink ref="AA466" r:id="rId1791"/>
+    <hyperlink ref="H467" r:id="rId1792"/>
+    <hyperlink ref="I467" r:id="rId1793"/>
+    <hyperlink ref="Z467" r:id="rId1794"/>
+    <hyperlink ref="AA467" r:id="rId1795"/>
+    <hyperlink ref="H468" r:id="rId1796"/>
+    <hyperlink ref="I468" r:id="rId1797"/>
+    <hyperlink ref="Z468" r:id="rId1798"/>
+    <hyperlink ref="AA468" r:id="rId1799"/>
+    <hyperlink ref="H469" r:id="rId1800"/>
+    <hyperlink ref="I469" r:id="rId1801"/>
+    <hyperlink ref="Z469" r:id="rId1802"/>
+    <hyperlink ref="AA469" r:id="rId1803"/>
+    <hyperlink ref="H470" r:id="rId1804"/>
+    <hyperlink ref="I470" r:id="rId1805"/>
+    <hyperlink ref="Z470" r:id="rId1806"/>
+    <hyperlink ref="AA470" r:id="rId1807"/>
+    <hyperlink ref="H471" r:id="rId1808"/>
+    <hyperlink ref="I471" r:id="rId1809"/>
+    <hyperlink ref="Z471" r:id="rId1810"/>
+    <hyperlink ref="AA471" r:id="rId1811"/>
+    <hyperlink ref="H472" r:id="rId1812"/>
+    <hyperlink ref="I472" r:id="rId1813"/>
+    <hyperlink ref="Z472" r:id="rId1814"/>
+    <hyperlink ref="AA472" r:id="rId1815"/>
+    <hyperlink ref="H473" r:id="rId1816"/>
+    <hyperlink ref="I473" r:id="rId1817"/>
+    <hyperlink ref="Z473" r:id="rId1818"/>
+    <hyperlink ref="AA473" r:id="rId1819"/>
+    <hyperlink ref="H474" r:id="rId1820"/>
+    <hyperlink ref="I474" r:id="rId1821"/>
+    <hyperlink ref="Z474" r:id="rId1822"/>
+    <hyperlink ref="AA474" r:id="rId1823"/>
+    <hyperlink ref="H475" r:id="rId1824"/>
+    <hyperlink ref="I475" r:id="rId1825"/>
+    <hyperlink ref="Z475" r:id="rId1826"/>
+    <hyperlink ref="AA475" r:id="rId1827"/>
+    <hyperlink ref="H476" r:id="rId1828"/>
+    <hyperlink ref="I476" r:id="rId1829"/>
+    <hyperlink ref="Z476" r:id="rId1830"/>
+    <hyperlink ref="AA476" r:id="rId1831"/>
+    <hyperlink ref="H477" r:id="rId1832"/>
+    <hyperlink ref="I477" r:id="rId1833"/>
+    <hyperlink ref="Z477" r:id="rId1834"/>
+    <hyperlink ref="AA477" r:id="rId1835"/>
+    <hyperlink ref="H478" r:id="rId1836"/>
+    <hyperlink ref="I478" r:id="rId1837"/>
+    <hyperlink ref="Z478" r:id="rId1838"/>
+    <hyperlink ref="AA478" r:id="rId1839"/>
+    <hyperlink ref="H479" r:id="rId1840"/>
+    <hyperlink ref="I479" r:id="rId1841"/>
+    <hyperlink ref="Z479" r:id="rId1842"/>
+    <hyperlink ref="AA479" r:id="rId1843"/>
+    <hyperlink ref="H480" r:id="rId1844"/>
+    <hyperlink ref="I480" r:id="rId1845"/>
+    <hyperlink ref="Z480" r:id="rId1846"/>
+    <hyperlink ref="AA480" r:id="rId1847"/>
+    <hyperlink ref="H481" r:id="rId1848"/>
+    <hyperlink ref="I481" r:id="rId1849"/>
+    <hyperlink ref="Z481" r:id="rId1850"/>
+    <hyperlink ref="AA481" r:id="rId1851"/>
+    <hyperlink ref="H482" r:id="rId1852"/>
+    <hyperlink ref="I482" r:id="rId1853"/>
+    <hyperlink ref="Z482" r:id="rId1854"/>
+    <hyperlink ref="AA482" r:id="rId1855"/>
+    <hyperlink ref="H483" r:id="rId1856"/>
+    <hyperlink ref="I483" r:id="rId1857"/>
+    <hyperlink ref="Z483" r:id="rId1858"/>
+    <hyperlink ref="AA483" r:id="rId1859"/>
+    <hyperlink ref="H484" r:id="rId1860"/>
+    <hyperlink ref="I484" r:id="rId1861"/>
+    <hyperlink ref="Z484" r:id="rId1862"/>
+    <hyperlink ref="AA484" r:id="rId1863"/>
+    <hyperlink ref="H485" r:id="rId1864"/>
+    <hyperlink ref="I485" r:id="rId1865"/>
+    <hyperlink ref="Z485" r:id="rId1866"/>
+    <hyperlink ref="AA485" r:id="rId1867"/>
+    <hyperlink ref="H486" r:id="rId1868"/>
+    <hyperlink ref="I486" r:id="rId1869"/>
+    <hyperlink ref="Z486" r:id="rId1870"/>
+    <hyperlink ref="AA486" r:id="rId1871"/>
+    <hyperlink ref="H487" r:id="rId1872"/>
+    <hyperlink ref="I487" r:id="rId1873"/>
+    <hyperlink ref="Z487" r:id="rId1874"/>
+    <hyperlink ref="AA487" r:id="rId1875"/>
+    <hyperlink ref="H488" r:id="rId1876"/>
+    <hyperlink ref="I488" r:id="rId1877"/>
+    <hyperlink ref="Z488" r:id="rId1878"/>
+    <hyperlink ref="AA488" r:id="rId1879"/>
+    <hyperlink ref="H489" r:id="rId1880"/>
+    <hyperlink ref="H491" r:id="rId1881"/>
+    <hyperlink ref="I491" r:id="rId1882"/>
+    <hyperlink ref="Z491" r:id="rId1883"/>
+    <hyperlink ref="AA491" r:id="rId1884"/>
+    <hyperlink ref="H492" r:id="rId1885"/>
+    <hyperlink ref="I492" r:id="rId1886"/>
+    <hyperlink ref="Z492" r:id="rId1887"/>
+    <hyperlink ref="AA492" r:id="rId1888"/>
+    <hyperlink ref="H493" r:id="rId1889"/>
+    <hyperlink ref="I493" r:id="rId1890"/>
+    <hyperlink ref="Z493" r:id="rId1891"/>
+    <hyperlink ref="AA493" r:id="rId1892"/>
+    <hyperlink ref="H494" r:id="rId1893"/>
+    <hyperlink ref="I494" r:id="rId1894"/>
+    <hyperlink ref="Z494" r:id="rId1895"/>
+    <hyperlink ref="AA494" r:id="rId1896"/>
+    <hyperlink ref="H495" r:id="rId1897"/>
+    <hyperlink ref="I495" r:id="rId1898"/>
+    <hyperlink ref="Z495" r:id="rId1899"/>
+    <hyperlink ref="AA495" r:id="rId1900"/>
+    <hyperlink ref="H496" r:id="rId1901"/>
+    <hyperlink ref="I496" r:id="rId1902"/>
+    <hyperlink ref="Z496" r:id="rId1903"/>
+    <hyperlink ref="AA496" r:id="rId1904"/>
+    <hyperlink ref="H497" r:id="rId1905"/>
+    <hyperlink ref="I497" r:id="rId1906"/>
+    <hyperlink ref="Z497" r:id="rId1907"/>
+    <hyperlink ref="AA497" r:id="rId1908"/>
+    <hyperlink ref="H498" r:id="rId1909"/>
+    <hyperlink ref="I498" r:id="rId1910"/>
+    <hyperlink ref="Z498" r:id="rId1911"/>
+    <hyperlink ref="AA498" r:id="rId1912"/>
+    <hyperlink ref="H499" r:id="rId1913"/>
+    <hyperlink ref="I499" r:id="rId1914"/>
+    <hyperlink ref="Z499" r:id="rId1915"/>
+    <hyperlink ref="AA499" r:id="rId1916"/>
+    <hyperlink ref="H500" r:id="rId1917"/>
+    <hyperlink ref="I500" r:id="rId1918"/>
+    <hyperlink ref="Z500" r:id="rId1919"/>
+    <hyperlink ref="AA500" r:id="rId1920"/>
+    <hyperlink ref="H501" r:id="rId1921"/>
+    <hyperlink ref="I501" r:id="rId1922"/>
+    <hyperlink ref="Z501" r:id="rId1923"/>
+    <hyperlink ref="AA501" r:id="rId1924"/>
+    <hyperlink ref="H502" r:id="rId1925"/>
+    <hyperlink ref="I502" r:id="rId1926"/>
+    <hyperlink ref="Z502" r:id="rId1927"/>
+    <hyperlink ref="AA502" r:id="rId1928"/>
+    <hyperlink ref="H503" r:id="rId1929"/>
+    <hyperlink ref="I503" r:id="rId1930"/>
+    <hyperlink ref="Z503" r:id="rId1931"/>
+    <hyperlink ref="AA503" r:id="rId1932"/>
+    <hyperlink ref="H504" r:id="rId1933"/>
+    <hyperlink ref="I504" r:id="rId1934"/>
+    <hyperlink ref="Z504" r:id="rId1935"/>
+    <hyperlink ref="AA504" r:id="rId1936"/>
+    <hyperlink ref="H505" r:id="rId1937"/>
+    <hyperlink ref="I505" r:id="rId1938"/>
+    <hyperlink ref="Z505" r:id="rId1939"/>
+    <hyperlink ref="AA505" r:id="rId1940"/>
+    <hyperlink ref="H506" r:id="rId1941"/>
+    <hyperlink ref="I506" r:id="rId1942"/>
+    <hyperlink ref="Z506" r:id="rId1943"/>
+    <hyperlink ref="AA506" r:id="rId1944"/>
+    <hyperlink ref="H507" r:id="rId1945"/>
+    <hyperlink ref="I507" r:id="rId1946"/>
+    <hyperlink ref="Z507" r:id="rId1947"/>
+    <hyperlink ref="AA507" r:id="rId1948"/>
+    <hyperlink ref="H508" r:id="rId1949"/>
+    <hyperlink ref="I508" r:id="rId1950"/>
+    <hyperlink ref="Z508" r:id="rId1951"/>
+    <hyperlink ref="AA508" r:id="rId1952"/>
+    <hyperlink ref="H509" r:id="rId1953"/>
+    <hyperlink ref="I509" r:id="rId1954"/>
+    <hyperlink ref="Z509" r:id="rId1955"/>
+    <hyperlink ref="AA509" r:id="rId1956"/>
+    <hyperlink ref="H510" r:id="rId1957"/>
+    <hyperlink ref="I510" r:id="rId1958"/>
+    <hyperlink ref="Z510" r:id="rId1959"/>
+    <hyperlink ref="AA510" r:id="rId1960"/>
+    <hyperlink ref="H511" r:id="rId1961"/>
+    <hyperlink ref="I511" r:id="rId1962"/>
+    <hyperlink ref="Z511" r:id="rId1963"/>
+    <hyperlink ref="AA511" r:id="rId1964"/>
+    <hyperlink ref="H512" r:id="rId1965"/>
+    <hyperlink ref="I512" r:id="rId1966"/>
+    <hyperlink ref="Z512" r:id="rId1967"/>
+    <hyperlink ref="AA512" r:id="rId1968"/>
+    <hyperlink ref="H513" r:id="rId1969"/>
+    <hyperlink ref="I513" r:id="rId1970"/>
+    <hyperlink ref="Z513" r:id="rId1971"/>
+    <hyperlink ref="AA513" r:id="rId1972"/>
+    <hyperlink ref="H514" r:id="rId1973"/>
+    <hyperlink ref="I514" r:id="rId1974"/>
+    <hyperlink ref="Z514" r:id="rId1975"/>
+    <hyperlink ref="AA514" r:id="rId1976"/>
+    <hyperlink ref="H515" r:id="rId1977"/>
+    <hyperlink ref="I515" r:id="rId1978"/>
+    <hyperlink ref="Z515" r:id="rId1979"/>
+    <hyperlink ref="AA515" r:id="rId1980"/>
+    <hyperlink ref="H516" r:id="rId1981"/>
+    <hyperlink ref="I516" r:id="rId1982"/>
+    <hyperlink ref="Z516" r:id="rId1983"/>
+    <hyperlink ref="AA516" r:id="rId1984"/>
+    <hyperlink ref="H517" r:id="rId1985"/>
+    <hyperlink ref="I517" r:id="rId1986"/>
+    <hyperlink ref="Z517" r:id="rId1987"/>
+    <hyperlink ref="AA517" r:id="rId1988"/>
+    <hyperlink ref="H518" r:id="rId1989"/>
+    <hyperlink ref="I518" r:id="rId1990"/>
+    <hyperlink ref="Z518" r:id="rId1991"/>
+    <hyperlink ref="AA518" r:id="rId1992"/>
+    <hyperlink ref="H519" r:id="rId1993"/>
+    <hyperlink ref="I519" r:id="rId1994"/>
+    <hyperlink ref="Z519" r:id="rId1995"/>
+    <hyperlink ref="AA519" r:id="rId1996"/>
+    <hyperlink ref="H520" r:id="rId1997"/>
+    <hyperlink ref="I520" r:id="rId1998"/>
+    <hyperlink ref="Z520" r:id="rId1999"/>
+    <hyperlink ref="AA520" r:id="rId2000"/>
+    <hyperlink ref="H521" r:id="rId2001"/>
+    <hyperlink ref="I521" r:id="rId2002"/>
+    <hyperlink ref="Z521" r:id="rId2003"/>
+    <hyperlink ref="AA521" r:id="rId2004"/>
+    <hyperlink ref="H522" r:id="rId2005"/>
+    <hyperlink ref="I522" r:id="rId2006"/>
+    <hyperlink ref="Z522" r:id="rId2007"/>
+    <hyperlink ref="AA522" r:id="rId2008"/>
+    <hyperlink ref="H523" r:id="rId2009"/>
+    <hyperlink ref="I523" r:id="rId2010"/>
+    <hyperlink ref="Z523" r:id="rId2011"/>
+    <hyperlink ref="AA523" r:id="rId2012"/>
+    <hyperlink ref="H524" r:id="rId2013"/>
+    <hyperlink ref="I524" r:id="rId2014"/>
+    <hyperlink ref="Z524" r:id="rId2015"/>
+    <hyperlink ref="AA524" r:id="rId2016"/>
+    <hyperlink ref="H525" r:id="rId2017"/>
+    <hyperlink ref="I525" r:id="rId2018"/>
+    <hyperlink ref="Z525" r:id="rId2019"/>
+    <hyperlink ref="AA525" r:id="rId2020"/>
+    <hyperlink ref="H526" r:id="rId2021"/>
+    <hyperlink ref="I526" r:id="rId2022"/>
+    <hyperlink ref="Z526" r:id="rId2023"/>
+    <hyperlink ref="AA526" r:id="rId2024"/>
+    <hyperlink ref="H527" r:id="rId2025"/>
+    <hyperlink ref="I527" r:id="rId2026"/>
+    <hyperlink ref="Z527" r:id="rId2027"/>
+    <hyperlink ref="AA527" r:id="rId2028"/>
+    <hyperlink ref="H528" r:id="rId2029"/>
+    <hyperlink ref="I528" r:id="rId2030"/>
+    <hyperlink ref="Z528" r:id="rId2031"/>
+    <hyperlink ref="AA528" r:id="rId2032"/>
+    <hyperlink ref="H529" r:id="rId2033"/>
+    <hyperlink ref="I529" r:id="rId2034"/>
+    <hyperlink ref="Z529" r:id="rId2035"/>
+    <hyperlink ref="AA529" r:id="rId2036"/>
+    <hyperlink ref="H530" r:id="rId2037"/>
+    <hyperlink ref="I530" r:id="rId2038"/>
+    <hyperlink ref="Z530" r:id="rId2039"/>
+    <hyperlink ref="AA530" r:id="rId2040"/>
+    <hyperlink ref="H531" r:id="rId2041"/>
+    <hyperlink ref="I531" r:id="rId2042"/>
+    <hyperlink ref="Z531" r:id="rId2043"/>
+    <hyperlink ref="AA531" r:id="rId2044"/>
+    <hyperlink ref="H532" r:id="rId2045"/>
+    <hyperlink ref="I532" r:id="rId2046"/>
+    <hyperlink ref="Z532" r:id="rId2047"/>
+    <hyperlink ref="AA532" r:id="rId2048"/>
+    <hyperlink ref="H533" r:id="rId2049"/>
+    <hyperlink ref="I533" r:id="rId2050"/>
+    <hyperlink ref="Z533" r:id="rId2051"/>
+    <hyperlink ref="AA533" r:id="rId2052"/>
+    <hyperlink ref="H534" r:id="rId2053"/>
+    <hyperlink ref="I534" r:id="rId2054"/>
+    <hyperlink ref="Z534" r:id="rId2055"/>
+    <hyperlink ref="AA534" r:id="rId2056"/>
+    <hyperlink ref="H535" r:id="rId2057"/>
+    <hyperlink ref="I535" r:id="rId2058"/>
+    <hyperlink ref="Z535" r:id="rId2059"/>
+    <hyperlink ref="AA535" r:id="rId2060"/>
+    <hyperlink ref="H536" r:id="rId2061"/>
+    <hyperlink ref="I536" r:id="rId2062"/>
+    <hyperlink ref="Z536" r:id="rId2063"/>
+    <hyperlink ref="AA536" r:id="rId2064"/>
+    <hyperlink ref="H537" r:id="rId2065"/>
+    <hyperlink ref="I537" r:id="rId2066"/>
+    <hyperlink ref="Z537" r:id="rId2067"/>
+    <hyperlink ref="AA537" r:id="rId2068"/>
+    <hyperlink ref="H538" r:id="rId2069"/>
+    <hyperlink ref="I538" r:id="rId2070"/>
+    <hyperlink ref="Z538" r:id="rId2071"/>
+    <hyperlink ref="AA538" r:id="rId2072"/>
+    <hyperlink ref="H539" r:id="rId2073"/>
+    <hyperlink ref="I539" r:id="rId2074"/>
+    <hyperlink ref="Z539" r:id="rId2075"/>
+    <hyperlink ref="AA539" r:id="rId2076"/>
+    <hyperlink ref="H540" r:id="rId2077"/>
+    <hyperlink ref="I540" r:id="rId2078"/>
+    <hyperlink ref="Z540" r:id="rId2079"/>
+    <hyperlink ref="AA540" r:id="rId2080"/>
+    <hyperlink ref="H541" r:id="rId2081"/>
+    <hyperlink ref="I541" r:id="rId2082"/>
+    <hyperlink ref="Z541" r:id="rId2083"/>
+    <hyperlink ref="AA541" r:id="rId2084"/>
+    <hyperlink ref="H542" r:id="rId2085"/>
+    <hyperlink ref="I542" r:id="rId2086"/>
+    <hyperlink ref="Z542" r:id="rId2087"/>
+    <hyperlink ref="AA542" r:id="rId2088"/>
+    <hyperlink ref="H543" r:id="rId2089"/>
+    <hyperlink ref="I543" r:id="rId2090"/>
+    <hyperlink ref="Z543" r:id="rId2091"/>
+    <hyperlink ref="AA543" r:id="rId2092"/>
+    <hyperlink ref="H544" r:id="rId2093"/>
+    <hyperlink ref="I544" r:id="rId2094"/>
+    <hyperlink ref="Z544" r:id="rId2095"/>
+    <hyperlink ref="AA544" r:id="rId2096"/>
+    <hyperlink ref="H545" r:id="rId2097"/>
+    <hyperlink ref="I545" r:id="rId2098"/>
+    <hyperlink ref="Z545" r:id="rId2099"/>
+    <hyperlink ref="AA545" r:id="rId2100"/>
+    <hyperlink ref="H546" r:id="rId2101"/>
+    <hyperlink ref="I546" r:id="rId2102"/>
+    <hyperlink ref="Z546" r:id="rId2103"/>
+    <hyperlink ref="AA546" r:id="rId2104"/>
+    <hyperlink ref="H547" r:id="rId2105"/>
+    <hyperlink ref="I547" r:id="rId2106"/>
+    <hyperlink ref="Z547" r:id="rId2107"/>
+    <hyperlink ref="AA547" r:id="rId2108"/>
+    <hyperlink ref="H548" r:id="rId2109"/>
+    <hyperlink ref="I548" r:id="rId2110"/>
+    <hyperlink ref="Z548" r:id="rId2111"/>
+    <hyperlink ref="AA548" r:id="rId2112"/>
+    <hyperlink ref="H549" r:id="rId2113"/>
+    <hyperlink ref="I549" r:id="rId2114"/>
+    <hyperlink ref="Z549" r:id="rId2115"/>
+    <hyperlink ref="AA549" r:id="rId2116"/>
+    <hyperlink ref="H550" r:id="rId2117"/>
+    <hyperlink ref="I550" r:id="rId2118"/>
+    <hyperlink ref="Z550" r:id="rId2119"/>
+    <hyperlink ref="AA550" r:id="rId2120"/>
+    <hyperlink ref="H551" r:id="rId2121"/>
+    <hyperlink ref="I551" r:id="rId2122"/>
+    <hyperlink ref="Z551" r:id="rId2123"/>
+    <hyperlink ref="AA551" r:id="rId2124"/>
+    <hyperlink ref="H552" r:id="rId2125"/>
+    <hyperlink ref="I552" r:id="rId2126"/>
+    <hyperlink ref="Z552" r:id="rId2127"/>
+    <hyperlink ref="AA552" r:id="rId2128"/>
+    <hyperlink ref="H553" r:id="rId2129"/>
+    <hyperlink ref="I553" r:id="rId2130"/>
+    <hyperlink ref="Z553" r:id="rId2131"/>
+    <hyperlink ref="AA553" r:id="rId2132"/>
+    <hyperlink ref="H554" r:id="rId2133"/>
+    <hyperlink ref="I554" r:id="rId2134"/>
+    <hyperlink ref="Z554" r:id="rId2135"/>
+    <hyperlink ref="H555" r:id="rId2136"/>
+    <hyperlink ref="I555" r:id="rId2137"/>
+    <hyperlink ref="Z555" r:id="rId2138"/>
+    <hyperlink ref="H556" r:id="rId2139"/>
+    <hyperlink ref="Z556" r:id="rId2140"/>
+    <hyperlink ref="H557" r:id="rId2141"/>
+    <hyperlink ref="Z557" r:id="rId2142"/>
+    <hyperlink ref="H558" r:id="rId2143"/>
+    <hyperlink ref="Z558" r:id="rId2144"/>
+    <hyperlink ref="H559" r:id="rId2145"/>
+    <hyperlink ref="Z559" r:id="rId2146"/>
+    <hyperlink ref="H560" r:id="rId2147"/>
+    <hyperlink ref="Z560" r:id="rId2148"/>
+    <hyperlink ref="H561" r:id="rId2149"/>
+    <hyperlink ref="Z561" r:id="rId2150"/>
+    <hyperlink ref="Z562" r:id="rId2151"/>
+    <hyperlink ref="Z563" r:id="rId2152"/>
+  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>